<commit_message>
working on indirect cost
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannbn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D053BFA-EC9D-1449-98E1-F487820FBFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EBA101-A52C-1349-AD93-4B99B67931F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="407">
   <si>
     <t>Account</t>
   </si>
@@ -1509,17 +1509,30 @@
   <si>
     <t>Total Capital Investment</t>
   </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>Total Field Direct Cost</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="37" x14ac:knownFonts="1">
     <font>
@@ -1986,7 +1999,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2255,6 +2268,24 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2263,10 +2294,37 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2296,51 +2354,6 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2362,6 +2375,9 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2370,7 +2386,7 @@
     <cellStyle name="Normal 2" xfId="4" xr:uid="{E15291B7-9068-3147-AE9D-D55638463741}"/>
     <cellStyle name="Normal 2 5" xfId="3" xr:uid="{D5427F60-54E8-014E-9224-5454BAE094F2}"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="96">
     <dxf>
       <font>
         <b/>
@@ -2397,141 +2413,6 @@
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2588,9 +2469,15 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2604,15 +2491,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2669,33 +2550,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2719,54 +2573,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2802,6 +2608,405 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3250,9 +3455,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
   <dimension ref="A1:Z126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="63" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
+    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="63" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P102" sqref="P102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3432,10 +3637,10 @@
       <c r="Q3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="113" t="s">
+      <c r="R3" s="119" t="s">
         <v>142</v>
       </c>
-      <c r="S3" s="129" t="s">
+      <c r="S3" s="123" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="26"/>
@@ -3485,8 +3690,8 @@
       <c r="Q4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="113"/>
-      <c r="S4" s="129"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="123"/>
       <c r="T4" s="26"/>
     </row>
     <row r="5" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3528,10 +3733,10 @@
       <c r="Q5" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="113" t="s">
+      <c r="R5" s="119" t="s">
         <v>143</v>
       </c>
-      <c r="S5" s="129" t="s">
+      <c r="S5" s="123" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="26"/>
@@ -3574,8 +3779,8 @@
       <c r="Q6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="113"/>
-      <c r="S6" s="129"/>
+      <c r="R6" s="119"/>
+      <c r="S6" s="123"/>
       <c r="T6" s="26"/>
     </row>
     <row r="7" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3763,13 +3968,13 @@
       <c r="P11" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="125" t="s">
+      <c r="Q11" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="113" t="s">
+      <c r="R11" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="114" t="s">
+      <c r="S11" s="124" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="26"/>
@@ -3823,9 +4028,9 @@
       <c r="P12" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="125"/>
-      <c r="R12" s="113"/>
-      <c r="S12" s="115"/>
+      <c r="Q12" s="115"/>
+      <c r="R12" s="119"/>
+      <c r="S12" s="125"/>
       <c r="T12" s="26"/>
     </row>
     <row r="13" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3870,9 +4075,9 @@
       <c r="P13" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="125"/>
-      <c r="R13" s="113"/>
-      <c r="S13" s="115"/>
+      <c r="Q13" s="115"/>
+      <c r="R13" s="119"/>
+      <c r="S13" s="125"/>
       <c r="T13" s="26"/>
     </row>
     <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3948,13 +4153,13 @@
       <c r="P15" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="125" t="s">
+      <c r="Q15" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="113" t="s">
+      <c r="R15" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="114" t="s">
+      <c r="S15" s="124" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="26"/>
@@ -4001,9 +4206,9 @@
       <c r="P16" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="125"/>
-      <c r="R16" s="113"/>
-      <c r="S16" s="115"/>
+      <c r="Q16" s="115"/>
+      <c r="R16" s="119"/>
+      <c r="S16" s="125"/>
       <c r="T16" s="26"/>
     </row>
     <row r="17" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -4048,9 +4253,9 @@
       <c r="P17" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="125"/>
-      <c r="R17" s="113"/>
-      <c r="S17" s="115"/>
+      <c r="Q17" s="115"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="125"/>
       <c r="T17" s="26"/>
     </row>
     <row r="18" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4159,13 +4364,13 @@
       <c r="P20" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q20" s="125" t="s">
+      <c r="Q20" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="113" t="s">
+      <c r="R20" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="S20" s="114" t="s">
+      <c r="S20" s="124" t="s">
         <v>84</v>
       </c>
       <c r="T20" s="26"/>
@@ -4212,9 +4417,9 @@
       <c r="P21" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q21" s="125"/>
-      <c r="R21" s="113"/>
-      <c r="S21" s="115"/>
+      <c r="Q21" s="115"/>
+      <c r="R21" s="119"/>
+      <c r="S21" s="125"/>
       <c r="T21" s="26"/>
     </row>
     <row r="22" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -4259,9 +4464,9 @@
       <c r="P22" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="125"/>
-      <c r="R22" s="113"/>
-      <c r="S22" s="115"/>
+      <c r="Q22" s="115"/>
+      <c r="R22" s="119"/>
+      <c r="S22" s="125"/>
       <c r="T22" s="26"/>
     </row>
     <row r="23" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4338,13 +4543,13 @@
       <c r="P24" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="125" t="s">
+      <c r="Q24" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="R24" s="113" t="s">
+      <c r="R24" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="S24" s="114" t="s">
+      <c r="S24" s="124" t="s">
         <v>84</v>
       </c>
       <c r="T24" s="26"/>
@@ -4391,9 +4596,9 @@
       <c r="P25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q25" s="125"/>
-      <c r="R25" s="113"/>
-      <c r="S25" s="115"/>
+      <c r="Q25" s="115"/>
+      <c r="R25" s="119"/>
+      <c r="S25" s="125"/>
       <c r="T25" s="26"/>
     </row>
     <row r="26" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -4438,9 +4643,9 @@
       <c r="P26" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="125"/>
-      <c r="R26" s="113"/>
-      <c r="S26" s="115"/>
+      <c r="Q26" s="115"/>
+      <c r="R26" s="119"/>
+      <c r="S26" s="125"/>
       <c r="T26" s="26"/>
     </row>
     <row r="27" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4581,13 +4786,13 @@
       <c r="P30" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="136" t="s">
+      <c r="Q30" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="135" t="s">
+      <c r="R30" s="120" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="133" t="s">
+      <c r="S30" s="129" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="85"/>
@@ -4634,9 +4839,9 @@
       <c r="P31" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="136"/>
-      <c r="R31" s="135"/>
-      <c r="S31" s="134"/>
+      <c r="Q31" s="114"/>
+      <c r="R31" s="120"/>
+      <c r="S31" s="130"/>
       <c r="T31" s="85"/>
     </row>
     <row r="32" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
@@ -4681,9 +4886,9 @@
       <c r="P32" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="136"/>
-      <c r="R32" s="135"/>
-      <c r="S32" s="134"/>
+      <c r="Q32" s="114"/>
+      <c r="R32" s="120"/>
+      <c r="S32" s="130"/>
       <c r="T32" s="85"/>
     </row>
     <row r="33" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4760,13 +4965,13 @@
       <c r="P34" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="136" t="s">
+      <c r="Q34" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="R34" s="135" t="s">
+      <c r="R34" s="120" t="s">
         <v>83</v>
       </c>
-      <c r="S34" s="133" t="s">
+      <c r="S34" s="129" t="s">
         <v>84</v>
       </c>
       <c r="T34" s="85"/>
@@ -4813,9 +5018,9 @@
       <c r="P35" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q35" s="136"/>
-      <c r="R35" s="135"/>
-      <c r="S35" s="134"/>
+      <c r="Q35" s="114"/>
+      <c r="R35" s="120"/>
+      <c r="S35" s="130"/>
       <c r="T35" s="85"/>
     </row>
     <row r="36" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
@@ -4860,9 +5065,9 @@
       <c r="P36" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q36" s="136"/>
-      <c r="R36" s="135"/>
-      <c r="S36" s="134"/>
+      <c r="Q36" s="114"/>
+      <c r="R36" s="120"/>
+      <c r="S36" s="130"/>
       <c r="T36" s="85"/>
     </row>
     <row r="37" spans="1:20" ht="30" thickBot="1" x14ac:dyDescent="0.25">
@@ -4971,13 +5176,13 @@
       <c r="P39" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="136" t="s">
+      <c r="Q39" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="R39" s="135" t="s">
+      <c r="R39" s="120" t="s">
         <v>83</v>
       </c>
-      <c r="S39" s="133" t="s">
+      <c r="S39" s="129" t="s">
         <v>84</v>
       </c>
       <c r="T39" s="85"/>
@@ -5024,9 +5229,9 @@
       <c r="P40" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q40" s="136"/>
-      <c r="R40" s="135"/>
-      <c r="S40" s="134"/>
+      <c r="Q40" s="114"/>
+      <c r="R40" s="120"/>
+      <c r="S40" s="130"/>
       <c r="T40" s="85"/>
     </row>
     <row r="41" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
@@ -5071,9 +5276,9 @@
       <c r="P41" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="136"/>
-      <c r="R41" s="135"/>
-      <c r="S41" s="134"/>
+      <c r="Q41" s="114"/>
+      <c r="R41" s="120"/>
+      <c r="S41" s="130"/>
       <c r="T41" s="85"/>
     </row>
     <row r="42" spans="1:20" ht="104" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5240,13 +5445,13 @@
       <c r="P45" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q45" s="125" t="s">
+      <c r="Q45" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="R45" s="113" t="s">
+      <c r="R45" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="S45" s="114" t="s">
+      <c r="S45" s="124" t="s">
         <v>84</v>
       </c>
       <c r="T45" s="26"/>
@@ -5293,9 +5498,9 @@
       <c r="P46" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="125"/>
-      <c r="R46" s="113"/>
-      <c r="S46" s="115"/>
+      <c r="Q46" s="115"/>
+      <c r="R46" s="119"/>
+      <c r="S46" s="125"/>
       <c r="T46" s="26"/>
     </row>
     <row r="47" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -5340,9 +5545,9 @@
       <c r="P47" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="125"/>
-      <c r="R47" s="113"/>
-      <c r="S47" s="115"/>
+      <c r="Q47" s="115"/>
+      <c r="R47" s="119"/>
+      <c r="S47" s="125"/>
       <c r="T47" s="26"/>
     </row>
     <row r="48" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5419,13 +5624,13 @@
       <c r="P49" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q49" s="125" t="s">
+      <c r="Q49" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="R49" s="113" t="s">
+      <c r="R49" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="S49" s="114" t="s">
+      <c r="S49" s="124" t="s">
         <v>84</v>
       </c>
       <c r="T49" s="26"/>
@@ -5472,9 +5677,9 @@
       <c r="P50" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q50" s="125"/>
-      <c r="R50" s="113"/>
-      <c r="S50" s="115"/>
+      <c r="Q50" s="115"/>
+      <c r="R50" s="119"/>
+      <c r="S50" s="125"/>
       <c r="T50" s="26"/>
     </row>
     <row r="51" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -5519,9 +5724,9 @@
       <c r="P51" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q51" s="125"/>
-      <c r="R51" s="113"/>
-      <c r="S51" s="115"/>
+      <c r="Q51" s="115"/>
+      <c r="R51" s="119"/>
+      <c r="S51" s="125"/>
       <c r="T51" s="26"/>
     </row>
     <row r="52" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5670,10 +5875,10 @@
       <c r="Q55" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R55" s="130" t="s">
+      <c r="R55" s="126" t="s">
         <v>179</v>
       </c>
-      <c r="S55" s="116" t="s">
+      <c r="S55" s="131" t="s">
         <v>183</v>
       </c>
       <c r="T55" s="42" t="s">
@@ -5730,8 +5935,8 @@
       <c r="Q56" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R56" s="131"/>
-      <c r="S56" s="117"/>
+      <c r="R56" s="127"/>
+      <c r="S56" s="132"/>
       <c r="T56" s="26"/>
     </row>
     <row r="57" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5787,8 +5992,8 @@
       <c r="Q57" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R57" s="132"/>
-      <c r="S57" s="118"/>
+      <c r="R57" s="128"/>
+      <c r="S57" s="133"/>
       <c r="T57" s="42" t="s">
         <v>182</v>
       </c>
@@ -5898,10 +6103,10 @@
       <c r="Q60" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R60" s="119" t="s">
+      <c r="R60" s="134" t="s">
         <v>179</v>
       </c>
-      <c r="S60" s="122" t="s">
+      <c r="S60" s="137" t="s">
         <v>352</v>
       </c>
       <c r="T60" s="90" t="s">
@@ -5947,8 +6152,8 @@
       <c r="Q61" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R61" s="120"/>
-      <c r="S61" s="123"/>
+      <c r="R61" s="135"/>
+      <c r="S61" s="138"/>
       <c r="T61" s="85"/>
     </row>
     <row r="62" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6005,8 +6210,8 @@
       <c r="Q62" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R62" s="120"/>
-      <c r="S62" s="123"/>
+      <c r="R62" s="135"/>
+      <c r="S62" s="138"/>
       <c r="T62" s="85"/>
     </row>
     <row r="63" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6063,8 +6268,8 @@
       <c r="Q63" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R63" s="121"/>
-      <c r="S63" s="124"/>
+      <c r="R63" s="136"/>
+      <c r="S63" s="139"/>
       <c r="T63" s="85"/>
     </row>
     <row r="64" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6154,10 +6359,10 @@
       <c r="Q65" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R65" s="130" t="s">
+      <c r="R65" s="126" t="s">
         <v>179</v>
       </c>
-      <c r="S65" s="116" t="s">
+      <c r="S65" s="131" t="s">
         <v>183</v>
       </c>
       <c r="T65" s="26"/>
@@ -6190,8 +6395,8 @@
       <c r="O66" s="26"/>
       <c r="P66" s="26"/>
       <c r="Q66" s="42"/>
-      <c r="R66" s="131"/>
-      <c r="S66" s="117"/>
+      <c r="R66" s="127"/>
+      <c r="S66" s="132"/>
       <c r="T66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6251,8 +6456,8 @@
       <c r="Q67" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R67" s="131"/>
-      <c r="S67" s="117"/>
+      <c r="R67" s="127"/>
+      <c r="S67" s="132"/>
       <c r="T67" s="85"/>
     </row>
     <row r="68" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6308,8 +6513,8 @@
       <c r="Q68" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R68" s="132"/>
-      <c r="S68" s="118"/>
+      <c r="R68" s="128"/>
+      <c r="S68" s="133"/>
       <c r="T68" s="85"/>
     </row>
     <row r="69" spans="1:20" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6534,13 +6739,13 @@
       <c r="Q73" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="R73" s="111" t="s">
+      <c r="R73" s="116" t="s">
         <v>353</v>
       </c>
-      <c r="S73" s="127" t="s">
+      <c r="S73" s="121" t="s">
         <v>355</v>
       </c>
-      <c r="T73" s="111"/>
+      <c r="T73" s="116"/>
     </row>
     <row r="74" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
@@ -6590,9 +6795,9 @@
       <c r="Q74" s="42" t="s">
         <v>348</v>
       </c>
-      <c r="R74" s="112"/>
-      <c r="S74" s="128"/>
-      <c r="T74" s="112"/>
+      <c r="R74" s="118"/>
+      <c r="S74" s="122"/>
+      <c r="T74" s="118"/>
     </row>
     <row r="75" spans="1:20" ht="76" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
@@ -7544,10 +7749,10 @@
       <c r="P95" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q95" s="111" t="s">
+      <c r="Q95" s="116" t="s">
         <v>388</v>
       </c>
-      <c r="R95" s="111" t="s">
+      <c r="R95" s="116" t="s">
         <v>389</v>
       </c>
       <c r="S95" s="26"/>
@@ -7592,8 +7797,8 @@
       <c r="P96" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q96" s="126"/>
-      <c r="R96" s="126"/>
+      <c r="Q96" s="117"/>
+      <c r="R96" s="117"/>
       <c r="S96" s="26"/>
       <c r="T96" s="26"/>
     </row>
@@ -7638,8 +7843,8 @@
       <c r="P97" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q97" s="126"/>
-      <c r="R97" s="126"/>
+      <c r="Q97" s="117"/>
+      <c r="R97" s="117"/>
       <c r="S97" s="26"/>
       <c r="T97" s="26"/>
     </row>
@@ -7686,8 +7891,8 @@
       <c r="P98" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q98" s="126"/>
-      <c r="R98" s="126"/>
+      <c r="Q98" s="117"/>
+      <c r="R98" s="117"/>
       <c r="S98" s="26"/>
       <c r="T98" s="26"/>
     </row>
@@ -7741,8 +7946,8 @@
       <c r="P99" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q99" s="112"/>
-      <c r="R99" s="112"/>
+      <c r="Q99" s="118"/>
+      <c r="R99" s="118"/>
       <c r="S99" s="26"/>
       <c r="T99" s="26"/>
     </row>
@@ -7836,18 +8041,33 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve">      Factory &amp; field indirect costs</v>
       </c>
-      <c r="E102" s="19"/>
+      <c r="E102" s="19" t="s">
+        <v>351</v>
+      </c>
       <c r="F102" s="19"/>
       <c r="G102" s="19"/>
       <c r="H102" s="29"/>
-      <c r="I102" s="20"/>
-      <c r="J102" s="29"/>
-      <c r="K102" s="29"/>
+      <c r="I102" s="147">
+        <f>MARVEL_Cost!C56/(MARVEL_Cost!C6+MARVEL_Cost!C13+MARVEL_Cost!C45)</f>
+        <v>6.5389932052543287E-2</v>
+      </c>
+      <c r="J102" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="K102" s="42" t="s">
+        <v>404</v>
+      </c>
       <c r="L102" s="29"/>
-      <c r="M102" s="29"/>
+      <c r="M102" s="29" t="s">
+        <v>405</v>
+      </c>
       <c r="N102" s="29"/>
-      <c r="O102" s="29"/>
-      <c r="P102" s="29"/>
+      <c r="O102" s="26">
+        <v>2024</v>
+      </c>
+      <c r="P102" s="26" t="s">
+        <v>406</v>
+      </c>
       <c r="Q102" s="98"/>
       <c r="R102" s="29"/>
       <c r="S102" s="29"/>
@@ -7920,7 +8140,7 @@
       <c r="P104" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="Q104" s="137" t="s">
+      <c r="Q104" s="111" t="s">
         <v>380</v>
       </c>
       <c r="R104" s="24"/>
@@ -7969,7 +8189,7 @@
       <c r="P105" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="Q105" s="138"/>
+      <c r="Q105" s="112"/>
       <c r="R105" s="24"/>
       <c r="S105" s="24"/>
       <c r="T105" s="24"/>
@@ -8016,7 +8236,7 @@
       <c r="P106" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="Q106" s="138"/>
+      <c r="Q106" s="112"/>
       <c r="R106" s="26"/>
       <c r="S106" s="26"/>
       <c r="T106" s="26"/>
@@ -8058,7 +8278,7 @@
       <c r="P107" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="Q107" s="139"/>
+      <c r="Q107" s="113"/>
       <c r="R107" s="26"/>
       <c r="S107" s="26"/>
       <c r="T107" s="26"/>
@@ -8683,19 +8903,20 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="Q104:Q107"/>
-    <mergeCell ref="Q39:Q41"/>
-    <mergeCell ref="Q45:Q47"/>
-    <mergeCell ref="Q49:Q51"/>
-    <mergeCell ref="Q95:Q99"/>
-    <mergeCell ref="R24:R26"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="R34:R36"/>
-    <mergeCell ref="R39:R41"/>
-    <mergeCell ref="Q20:Q22"/>
-    <mergeCell ref="Q24:Q26"/>
-    <mergeCell ref="Q30:Q32"/>
-    <mergeCell ref="Q34:Q36"/>
+    <mergeCell ref="T73:T74"/>
+    <mergeCell ref="R45:R47"/>
+    <mergeCell ref="R49:R51"/>
+    <mergeCell ref="S45:S47"/>
+    <mergeCell ref="S49:S51"/>
+    <mergeCell ref="S65:S68"/>
+    <mergeCell ref="R60:R63"/>
+    <mergeCell ref="S60:S63"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
     <mergeCell ref="R95:R99"/>
     <mergeCell ref="R73:R74"/>
     <mergeCell ref="S73:S74"/>
@@ -8712,163 +8933,162 @@
     <mergeCell ref="S55:S57"/>
     <mergeCell ref="S39:S41"/>
     <mergeCell ref="R20:R22"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="T73:T74"/>
-    <mergeCell ref="R45:R47"/>
-    <mergeCell ref="R49:R51"/>
-    <mergeCell ref="S45:S47"/>
-    <mergeCell ref="S49:S51"/>
-    <mergeCell ref="S65:S68"/>
-    <mergeCell ref="R60:R63"/>
-    <mergeCell ref="S60:S63"/>
+    <mergeCell ref="R24:R26"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="R34:R36"/>
+    <mergeCell ref="R39:R41"/>
+    <mergeCell ref="Q20:Q22"/>
+    <mergeCell ref="Q24:Q26"/>
+    <mergeCell ref="Q30:Q32"/>
+    <mergeCell ref="Q34:Q36"/>
+    <mergeCell ref="Q104:Q107"/>
+    <mergeCell ref="Q39:Q41"/>
+    <mergeCell ref="Q45:Q47"/>
+    <mergeCell ref="Q49:Q51"/>
+    <mergeCell ref="Q95:Q99"/>
   </mergeCells>
-  <conditionalFormatting sqref="A124">
-    <cfRule type="expression" dxfId="67" priority="5">
-      <formula>$B124=3</formula>
+  <conditionalFormatting sqref="A124 L102:N102 Q102:T102">
+    <cfRule type="expression" dxfId="95" priority="29">
+      <formula>$B102=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="6">
-      <formula>$B124=2</formula>
+    <cfRule type="expression" dxfId="94" priority="30">
+      <formula>$B102=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="7">
-      <formula>$B124&lt;2</formula>
+    <cfRule type="expression" dxfId="93" priority="31">
+      <formula>$B102&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="8">
-      <formula>$B124=0</formula>
+    <cfRule type="expression" dxfId="92" priority="32">
+      <formula>$B102=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A73:F75 L95:T95 L96:P96 S96:T100 I97:P97 A100:R100 A101:T103 A104:P109 R104:T109">
-    <cfRule type="expression" dxfId="63" priority="76">
-      <formula>$B73=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="73">
+  <conditionalFormatting sqref="A73:F75 L95:T95 L96:P96 S96:T100 I97:P97 A100:R100 A101:T101 A104:P109 R104:T109 A103:T103 A102:H102">
+    <cfRule type="expression" dxfId="91" priority="97">
       <formula>$B73=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="74">
+    <cfRule type="expression" dxfId="90" priority="98">
       <formula>$B73=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="75">
+    <cfRule type="expression" dxfId="89" priority="99">
       <formula>$B73&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="100">
+      <formula>$B73=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:H97">
-    <cfRule type="expression" dxfId="59" priority="40">
-      <formula>$B95=0</formula>
+    <cfRule type="expression" dxfId="87" priority="61">
+      <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="39">
+    <cfRule type="expression" dxfId="86" priority="62">
+      <formula>$B95=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="63">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="38">
-      <formula>$B95=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="37">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="84" priority="64">
+      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:I81">
-    <cfRule type="expression" dxfId="55" priority="61">
+    <cfRule type="expression" dxfId="83" priority="85">
       <formula>$B77=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="64">
-      <formula>$B77=0</formula>
+    <cfRule type="expression" dxfId="82" priority="86">
+      <formula>$B77=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="63">
+    <cfRule type="expression" dxfId="81" priority="87">
       <formula>$B77&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="62">
-      <formula>$B77=2</formula>
+    <cfRule type="expression" dxfId="80" priority="88">
+      <formula>$B77=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:P99">
-    <cfRule type="expression" dxfId="51" priority="21">
+    <cfRule type="expression" dxfId="79" priority="45">
       <formula>$B98=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="22">
+    <cfRule type="expression" dxfId="78" priority="46">
       <formula>$B98=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="23">
+    <cfRule type="expression" dxfId="77" priority="47">
       <formula>$B98&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="24">
+    <cfRule type="expression" dxfId="76" priority="48">
       <formula>$B98=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:S72">
-    <cfRule type="expression" dxfId="47" priority="80">
-      <formula>$B72=0</formula>
+    <cfRule type="expression" dxfId="75" priority="101">
+      <formula>$B72=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="79">
+    <cfRule type="expression" dxfId="74" priority="102">
+      <formula>$B72=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="103">
       <formula>$B72&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="78">
-      <formula>$B72=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="77">
-      <formula>$B72=3</formula>
+    <cfRule type="expression" dxfId="72" priority="104">
+      <formula>$B72=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T71 T72:T75 H73:R73 H74:Q74 G75:Q75 A76:T76 K77:T77 S78:T81">
-    <cfRule type="expression" dxfId="43" priority="81">
+    <cfRule type="expression" dxfId="71" priority="105">
       <formula>$B1=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="82">
+    <cfRule type="expression" dxfId="70" priority="106">
       <formula>$B1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="83">
+    <cfRule type="expression" dxfId="69" priority="107">
       <formula>$B1&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="84">
+    <cfRule type="expression" dxfId="68" priority="108">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:T94">
-    <cfRule type="expression" dxfId="39" priority="41">
+    <cfRule type="expression" dxfId="67" priority="65">
       <formula>$B82=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="42">
+    <cfRule type="expression" dxfId="66" priority="66">
       <formula>$B82=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="43">
+    <cfRule type="expression" dxfId="65" priority="67">
       <formula>$B82&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="44">
+    <cfRule type="expression" dxfId="64" priority="68">
       <formula>$B82=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:T123">
-    <cfRule type="expression" dxfId="35" priority="12">
-      <formula>$B110=0</formula>
+    <cfRule type="expression" dxfId="63" priority="33">
+      <formula>$B110=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="62" priority="34">
+      <formula>$B110=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="35">
       <formula>$B110&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="10">
-      <formula>$B110=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="9">
-      <formula>$B110=3</formula>
+    <cfRule type="expression" dxfId="60" priority="36">
+      <formula>$B110=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C124:D124">
-    <cfRule type="expression" dxfId="31" priority="1">
+    <cfRule type="expression" dxfId="59" priority="25">
       <formula>$B124=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="58" priority="26">
       <formula>$B124=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="3">
+    <cfRule type="expression" dxfId="57" priority="27">
       <formula>$B124&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="56" priority="28">
       <formula>$B124=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D123">
-    <cfRule type="colorScale" priority="128">
+    <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8878,108 +9098,178 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G73:G74">
-    <cfRule type="expression" dxfId="27" priority="69">
+    <cfRule type="expression" dxfId="55" priority="93">
       <formula>$B73=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="70">
+    <cfRule type="expression" dxfId="54" priority="94">
       <formula>$B73=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="71">
+    <cfRule type="expression" dxfId="53" priority="95">
       <formula>$B73&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="72">
+    <cfRule type="expression" dxfId="52" priority="96">
       <formula>$B73=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I95:K96">
-    <cfRule type="expression" dxfId="23" priority="36">
+    <cfRule type="expression" dxfId="51" priority="57">
+      <formula>$B95=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="58">
+      <formula>$B95=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="59">
+      <formula>$B95&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="60">
       <formula>$B95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="35">
-      <formula>$B95&lt;2</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77 O101">
+    <cfRule type="expression" dxfId="47" priority="114">
+      <formula>$B78=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="34">
-      <formula>$B95=2</formula>
+    <cfRule type="expression" dxfId="46" priority="115">
+      <formula>$B78=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="33">
-      <formula>$B95=3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J77">
-    <cfRule type="expression" dxfId="19" priority="93">
-      <formula>$B78=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="92">
+    <cfRule type="expression" dxfId="45" priority="116">
       <formula>$B78&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="91">
-      <formula>$B78=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="90">
-      <formula>$B78=3</formula>
+    <cfRule type="expression" dxfId="44" priority="117">
+      <formula>$B78=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:Q81">
-    <cfRule type="expression" dxfId="15" priority="58">
+    <cfRule type="expression" dxfId="43" priority="81">
+      <formula>$B78=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="82">
       <formula>$B78=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="57">
-      <formula>$B78=3</formula>
+    <cfRule type="expression" dxfId="41" priority="83">
+      <formula>$B78&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="60">
+    <cfRule type="expression" dxfId="40" priority="84">
       <formula>$B78=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="59">
-      <formula>$B78&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q104">
-    <cfRule type="expression" dxfId="11" priority="17">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>$B104=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="18">
+    <cfRule type="expression" dxfId="38" priority="42">
       <formula>$B104=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="19">
+    <cfRule type="expression" dxfId="37" priority="43">
       <formula>$B104&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="20">
+    <cfRule type="expression" dxfId="36" priority="44">
       <formula>$B104=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q108:Q109">
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>$B108=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>$B108=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
       <formula>$B108&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14">
-      <formula>$B108=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13">
-      <formula>$B108=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="16">
+    <cfRule type="expression" dxfId="32" priority="40">
       <formula>$B108=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S73">
-    <cfRule type="expression" dxfId="3" priority="98">
+    <cfRule type="expression" dxfId="31" priority="122">
       <formula>$B72=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="99">
+    <cfRule type="expression" dxfId="30" priority="123">
       <formula>$B72=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="100">
+    <cfRule type="expression" dxfId="29" priority="124">
       <formula>$B72&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="101">
+    <cfRule type="expression" dxfId="28" priority="125">
       <formula>$B72=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="13">
+  <conditionalFormatting sqref="I102">
+    <cfRule type="expression" dxfId="27" priority="21">
+      <formula>$B102=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="22">
+      <formula>$B102=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="23">
+      <formula>$B102&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="24">
+      <formula>$B102=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J102">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>$B102=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>$B102=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>$B102&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>$B102=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K102">
+    <cfRule type="expression" dxfId="19" priority="13">
+      <formula>$B102=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>$B102=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="15">
+      <formula>$B102&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>$B102=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P102">
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>$B102=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>$B102=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>$B102&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>$B102=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O102">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>$B102=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>$B102=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>$B102&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>$B102=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="14">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I157:I186 H124:H148" xr:uid="{0D656B1C-36BB-D24C-9DF1-8575D533B58B}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P171:P215 O2:O215" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P171:P215 O2:O101 O103:O215" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
       <formula1>1950</formula1>
       <formula2>2025</formula2>
     </dataValidation>
@@ -9010,13 +9300,16 @@
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M123" xr:uid="{127B7473-9D01-354E-A3BD-12180E660A5C}">
-      <formula1>"acres, MWe, m^3, MWt, Kg, Drums, kW"</formula1>
+      <formula1>"acres, MWe, m^3, MWt, Kg, Drums, kW, $"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P123" xr:uid="{7E44D5D7-AB3F-D340-AE9A-F65BCE5B6A48}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P123" xr:uid="{7E44D5D7-AB3F-D340-AE9A-F65BCE5B6A48}">
       <formula1>"General, Labor, Material, Equipment,Lab and Mat and Equip, 'Lab and Equip"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J123" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
       <formula1>"$/acres, $/MWe, $/m^3, $/MWt, $/Kg, $/Drum, $/(kg.sec), $/SWU, unitless"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P122" xr:uid="{17DDFD40-D97D-B64B-BD3B-AEAF52F6302C}">
+      <formula1>"N/A, General, Labor, Material, Equipment,Lab and Mat and Equip, 'Lab and Equip"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -9034,7 +9327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAED81D3-2E1E-EB42-8F84-3B0F01FD7CDC}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="183" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="183" workbookViewId="0">
       <selection activeCell="A72" sqref="A72:XFD72"/>
     </sheetView>
   </sheetViews>
@@ -10630,10 +10923,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF46401-6828-1F49-B2C3-A6E5E28394B1}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10644,7 +10937,7 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -10666,8 +10959,11 @@
       <c r="G1" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1985</v>
       </c>
@@ -10691,8 +10987,11 @@
         <f>AVERAGE(C2,E2)</f>
         <v>3.5077268631057317</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f>+A2+1</f>
         <v>1986</v>
@@ -10717,8 +11016,11 @@
         <f t="shared" ref="G3:G41" si="1">AVERAGE(C3,E3)</f>
         <v>3.4091576629618658</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A39" si="2">+A3+1</f>
         <v>1987</v>
@@ -10743,8 +11045,11 @@
         <f t="shared" si="1"/>
         <v>3.3453365939328341</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="2"/>
         <v>1988</v>
@@ -10769,8 +11074,11 @@
         <f t="shared" si="1"/>
         <v>3.1996966340937996</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="2"/>
         <v>1989</v>
@@ -10795,8 +11103,11 @@
         <f t="shared" si="1"/>
         <v>3.0469579706202397</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="2"/>
         <v>1990</v>
@@ -10821,8 +11132,11 @@
         <f t="shared" si="1"/>
         <v>2.9415018835339906</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="2"/>
         <v>1991</v>
@@ -10847,8 +11161,11 @@
         <f t="shared" si="1"/>
         <v>2.8361039998658946</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f t="shared" si="2"/>
         <v>1992</v>
@@ -10873,8 +11190,11 @@
         <f t="shared" si="1"/>
         <v>2.7325235034052247</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="2"/>
         <v>1993</v>
@@ -10899,8 +11219,11 @@
         <f t="shared" si="1"/>
         <v>2.6102364763135144</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="2"/>
         <v>1994</v>
@@ -10925,8 +11248,11 @@
         <f t="shared" si="1"/>
         <v>2.5262885305582738</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="2"/>
         <v>1995</v>
@@ -10951,8 +11277,11 @@
         <f t="shared" si="1"/>
         <v>2.4827907155103204</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="2"/>
         <v>1996</v>
@@ -10977,8 +11306,11 @@
         <f t="shared" si="1"/>
         <v>2.4262533008020304</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="2"/>
         <v>1997</v>
@@ -11003,8 +11335,11 @@
         <f t="shared" si="1"/>
         <v>2.3671474216595447</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="2"/>
         <v>1998</v>
@@ -11029,8 +11364,11 @@
         <f t="shared" si="1"/>
         <v>2.307052093528327</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="2"/>
         <v>1999</v>
@@ -11055,8 +11393,11 @@
         <f t="shared" si="1"/>
         <v>2.2643663875974873</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f t="shared" si="2"/>
         <v>2000</v>
@@ -11081,8 +11422,11 @@
         <f t="shared" si="1"/>
         <v>2.2041708998292839</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="2"/>
         <v>2001</v>
@@ -11107,8 +11451,11 @@
         <f t="shared" si="1"/>
         <v>2.1214299408402955</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="2"/>
         <v>2002</v>
@@ -11133,8 +11480,11 @@
         <f t="shared" si="1"/>
         <v>2.0800427371143604</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f t="shared" si="2"/>
         <v>2003</v>
@@ -11159,8 +11509,11 @@
         <f t="shared" si="1"/>
         <v>2.0294240285722087</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <f t="shared" si="2"/>
         <v>2004</v>
@@ -11185,8 +11538,11 @@
         <f t="shared" si="1"/>
         <v>1.9615140730224918</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <f t="shared" si="2"/>
         <v>2005</v>
@@ -11211,8 +11567,11 @@
         <f t="shared" si="1"/>
         <v>1.8908139941124174</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f t="shared" si="2"/>
         <v>2006</v>
@@ -11237,8 +11596,11 @@
         <f t="shared" si="1"/>
         <v>1.7812582023870296</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <f t="shared" si="2"/>
         <v>2007</v>
@@ -11263,8 +11625,11 @@
         <f t="shared" si="1"/>
         <v>1.6698766116056492</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <f t="shared" si="2"/>
         <v>2008</v>
@@ -11289,8 +11654,11 @@
         <f t="shared" si="1"/>
         <v>1.6212060370241057</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <f t="shared" si="2"/>
         <v>2009</v>
@@ -11315,8 +11683,11 @@
         <f t="shared" si="1"/>
         <v>1.6018382421283412</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <f t="shared" si="2"/>
         <v>2010</v>
@@ -11341,8 +11712,11 @@
         <f t="shared" si="1"/>
         <v>1.599627378088782</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <f t="shared" si="2"/>
         <v>2011</v>
@@ -11367,8 +11741,11 @@
         <f t="shared" si="1"/>
         <v>1.555513512447007</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <f t="shared" si="2"/>
         <v>2012</v>
@@ -11393,8 +11770,11 @@
         <f t="shared" si="1"/>
         <v>1.489126368714752</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <f t="shared" si="2"/>
         <v>2013</v>
@@ -11419,8 +11799,11 @@
         <f t="shared" si="1"/>
         <v>1.4468538620411944</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <f t="shared" si="2"/>
         <v>2014</v>
@@ -11445,8 +11828,11 @@
         <f t="shared" si="1"/>
         <v>1.4086050826947987</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <f t="shared" si="2"/>
         <v>2015</v>
@@ -11471,8 +11857,11 @@
         <f t="shared" si="1"/>
         <v>1.3743420273513181</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -11497,8 +11886,11 @@
         <f t="shared" si="1"/>
         <v>1.3499985236534209</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -11523,8 +11915,11 @@
         <f t="shared" si="1"/>
         <v>1.3179687370712139</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11549,8 +11944,11 @@
         <f t="shared" si="1"/>
         <v>1.276830950870623</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11575,8 +11973,11 @@
         <f t="shared" si="1"/>
         <v>1.2415770326808417</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -11601,8 +12002,11 @@
         <f t="shared" si="1"/>
         <v>1.2165134245854174</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <f t="shared" si="2"/>
         <v>2021</v>
@@ -11627,8 +12031,11 @@
         <f t="shared" si="1"/>
         <v>1.1715472467908044</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <f t="shared" si="2"/>
         <v>2022</v>
@@ -11653,8 +12060,11 @@
         <f t="shared" si="1"/>
         <v>1.0792357293864472</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>2023</v>
       </c>
@@ -11678,8 +12088,11 @@
         <f t="shared" si="1"/>
         <v>1.0172398620903442</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>2024</v>
       </c>
@@ -11701,6 +12114,9 @@
       </c>
       <c r="G41" s="4">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
review and cleanup LTMR
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannbn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692ACE91-ADA2-F441-8D30-877F9DB982BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772FDCFA-964E-6246-B56B-2622D447C2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1240,12 +1240,6 @@
     <t>WEP</t>
   </si>
   <si>
-    <t>In Vessel Shielding Mass</t>
-  </si>
-  <si>
-    <t>Out Of Vessel Shielding Mass</t>
-  </si>
-  <si>
     <t>ZrH</t>
   </si>
   <si>
@@ -1548,6 +1542,12 @@
   </si>
   <si>
     <t>Annual Electricity Production</t>
+  </si>
+  <si>
+    <t>In Vessel Shield Mass</t>
+  </si>
+  <si>
+    <t>Out Of Vessel Shield Mass</t>
   </si>
 </sst>
 </file>
@@ -2260,6 +2260,24 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2268,10 +2286,37 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2300,51 +2345,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2383,108 +2383,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2512,15 +2410,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2574,7 +2466,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2597,6 +2489,249 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2655,13 +2790,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -2671,33 +2799,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2721,26 +2822,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
@@ -2750,7 +2831,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2815,11 +2896,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2829,15 +2909,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2851,27 +2925,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2885,61 +2939,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3369,9 +3369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
   <dimension ref="A1:Z122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="63" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E124" sqref="E124"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="63" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3413,7 +3413,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>329</v>
@@ -3422,10 +3422,10 @@
         <v>330</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>50</v>
@@ -3523,7 +3523,7 @@
         <v xml:space="preserve">      Land Cost</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
@@ -3551,10 +3551,10 @@
       <c r="Q3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="106" t="s">
+      <c r="R3" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="S3" s="122" t="s">
+      <c r="S3" s="116" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="26"/>
@@ -3575,7 +3575,7 @@
         <v xml:space="preserve">      Site Permits</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -3604,8 +3604,8 @@
       <c r="Q4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="106"/>
-      <c r="S4" s="122"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="116"/>
       <c r="T4" s="26"/>
     </row>
     <row r="5" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3624,7 +3624,7 @@
         <v xml:space="preserve">      Plant Licensing</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -3647,10 +3647,10 @@
       <c r="Q5" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="106" t="s">
+      <c r="R5" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="S5" s="122" t="s">
+      <c r="S5" s="116" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="26"/>
@@ -3671,7 +3671,7 @@
         <v xml:space="preserve">      Plant Permits</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -3693,8 +3693,8 @@
       <c r="Q6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="106"/>
-      <c r="S6" s="122"/>
+      <c r="R6" s="112"/>
+      <c r="S6" s="116"/>
       <c r="T6" s="26"/>
     </row>
     <row r="7" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3713,7 +3713,7 @@
         <v xml:space="preserve">      Plant Studies</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -3865,7 +3865,7 @@
         <v xml:space="preserve">                  Cleaning and Grubbing</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
@@ -3891,13 +3891,13 @@
       <c r="P11" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="118" t="s">
+      <c r="Q11" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="106" t="s">
+      <c r="R11" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="107" t="s">
+      <c r="S11" s="117" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="26"/>
@@ -3925,7 +3925,7 @@
         <v xml:space="preserve">                  Stripping Topsoil</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
@@ -3951,9 +3951,9 @@
       <c r="P12" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="118"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="112"/>
+      <c r="S12" s="118"/>
       <c r="T12" s="26"/>
     </row>
     <row r="13" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3972,7 +3972,7 @@
         <v xml:space="preserve">                  Excavation</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -3998,9 +3998,9 @@
       <c r="P13" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="118"/>
-      <c r="R13" s="106"/>
-      <c r="S13" s="108"/>
+      <c r="Q13" s="108"/>
+      <c r="R13" s="112"/>
+      <c r="S13" s="118"/>
       <c r="T13" s="26"/>
     </row>
     <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4051,7 +4051,7 @@
         <v xml:space="preserve">                  Reactor Building Slab Roof</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="27"/>
@@ -4076,13 +4076,13 @@
       <c r="P15" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="118" t="s">
+      <c r="Q15" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="106" t="s">
+      <c r="R15" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="107" t="s">
+      <c r="S15" s="117" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="26"/>
@@ -4103,7 +4103,7 @@
         <v xml:space="preserve">                  Reactor Building Basement</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -4129,9 +4129,9 @@
       <c r="P16" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="106"/>
-      <c r="S16" s="108"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="118"/>
       <c r="T16" s="26"/>
     </row>
     <row r="17" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -4150,7 +4150,7 @@
         <v xml:space="preserve">                  Reactor Building Walls</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
@@ -4176,9 +4176,9 @@
       <c r="P17" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="106"/>
-      <c r="S17" s="108"/>
+      <c r="Q17" s="108"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="118"/>
       <c r="T17" s="26"/>
     </row>
     <row r="18" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v xml:space="preserve">                        Energy Conversion Building Slab Roof</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -4287,13 +4287,13 @@
       <c r="P20" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q20" s="118" t="s">
+      <c r="Q20" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="106" t="s">
+      <c r="R20" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="S20" s="107" t="s">
+      <c r="S20" s="117" t="s">
         <v>84</v>
       </c>
       <c r="T20" s="26"/>
@@ -4314,7 +4314,7 @@
         <v xml:space="preserve">                        Energy Conversion Building Basement</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
@@ -4340,9 +4340,9 @@
       <c r="P21" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="106"/>
-      <c r="S21" s="108"/>
+      <c r="Q21" s="108"/>
+      <c r="R21" s="112"/>
+      <c r="S21" s="118"/>
       <c r="T21" s="26"/>
     </row>
     <row r="22" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -4361,7 +4361,7 @@
         <v xml:space="preserve">                        Energy Conversion Building Walls</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -4387,9 +4387,9 @@
       <c r="P22" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="118"/>
-      <c r="R22" s="106"/>
-      <c r="S22" s="108"/>
+      <c r="Q22" s="108"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="118"/>
       <c r="T22" s="26"/>
     </row>
     <row r="23" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4440,7 +4440,7 @@
         <v xml:space="preserve">                        Control Building Slab Roof</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -4466,13 +4466,13 @@
       <c r="P24" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="118" t="s">
+      <c r="Q24" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="R24" s="106" t="s">
+      <c r="R24" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="S24" s="107" t="s">
+      <c r="S24" s="117" t="s">
         <v>84</v>
       </c>
       <c r="T24" s="26"/>
@@ -4493,7 +4493,7 @@
         <v xml:space="preserve">                        Control Building Basement</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -4519,9 +4519,9 @@
       <c r="P25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="106"/>
-      <c r="S25" s="108"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="112"/>
+      <c r="S25" s="118"/>
       <c r="T25" s="26"/>
     </row>
     <row r="26" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -4540,7 +4540,7 @@
         <v xml:space="preserve">                        Control Building Walls</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -4566,9 +4566,9 @@
       <c r="P26" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="118"/>
-      <c r="R26" s="106"/>
-      <c r="S26" s="108"/>
+      <c r="Q26" s="108"/>
+      <c r="R26" s="112"/>
+      <c r="S26" s="118"/>
       <c r="T26" s="26"/>
     </row>
     <row r="27" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4683,7 +4683,7 @@
         <v xml:space="preserve">                              Refueling Building Slab Roof</v>
       </c>
       <c r="E30" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F30" s="80"/>
       <c r="G30" s="80"/>
@@ -4709,13 +4709,13 @@
       <c r="P30" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="129" t="s">
+      <c r="Q30" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="128" t="s">
+      <c r="R30" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="126" t="s">
+      <c r="S30" s="122" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="85"/>
@@ -4736,7 +4736,7 @@
         <v xml:space="preserve">                              Refueling Building Basement</v>
       </c>
       <c r="E31" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F31" s="80"/>
       <c r="G31" s="80"/>
@@ -4762,9 +4762,9 @@
       <c r="P31" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="129"/>
-      <c r="R31" s="128"/>
-      <c r="S31" s="127"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="113"/>
+      <c r="S31" s="123"/>
       <c r="T31" s="85"/>
     </row>
     <row r="32" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
@@ -4783,7 +4783,7 @@
         <v xml:space="preserve">                              Refueling Building Walls</v>
       </c>
       <c r="E32" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F32" s="80"/>
       <c r="G32" s="80"/>
@@ -4809,9 +4809,9 @@
       <c r="P32" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="129"/>
-      <c r="R32" s="128"/>
-      <c r="S32" s="127"/>
+      <c r="Q32" s="107"/>
+      <c r="R32" s="113"/>
+      <c r="S32" s="123"/>
       <c r="T32" s="85"/>
     </row>
     <row r="33" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4862,7 +4862,7 @@
         <v xml:space="preserve">                              Spent Fuel Building Slab Roof</v>
       </c>
       <c r="E34" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F34" s="80"/>
       <c r="G34" s="80"/>
@@ -4888,13 +4888,13 @@
       <c r="P34" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="129" t="s">
+      <c r="Q34" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="R34" s="128" t="s">
+      <c r="R34" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="S34" s="126" t="s">
+      <c r="S34" s="122" t="s">
         <v>84</v>
       </c>
       <c r="T34" s="85"/>
@@ -4915,7 +4915,7 @@
         <v xml:space="preserve">                              Spent Fuel Building Basement</v>
       </c>
       <c r="E35" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F35" s="80"/>
       <c r="G35" s="80"/>
@@ -4941,9 +4941,9 @@
       <c r="P35" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q35" s="129"/>
-      <c r="R35" s="128"/>
-      <c r="S35" s="127"/>
+      <c r="Q35" s="107"/>
+      <c r="R35" s="113"/>
+      <c r="S35" s="123"/>
       <c r="T35" s="85"/>
     </row>
     <row r="36" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
@@ -4962,7 +4962,7 @@
         <v xml:space="preserve">                              Spent Fuel Building Walls</v>
       </c>
       <c r="E36" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F36" s="80"/>
       <c r="G36" s="80"/>
@@ -4988,9 +4988,9 @@
       <c r="P36" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q36" s="129"/>
-      <c r="R36" s="128"/>
-      <c r="S36" s="127"/>
+      <c r="Q36" s="107"/>
+      <c r="R36" s="113"/>
+      <c r="S36" s="123"/>
       <c r="T36" s="85"/>
     </row>
     <row r="37" spans="1:20" ht="30" thickBot="1" x14ac:dyDescent="0.25">
@@ -5073,7 +5073,7 @@
         <v xml:space="preserve">                              Emergency Building Slab Roof</v>
       </c>
       <c r="E39" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F39" s="80"/>
       <c r="G39" s="80"/>
@@ -5099,13 +5099,13 @@
       <c r="P39" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="129" t="s">
+      <c r="Q39" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="R39" s="128" t="s">
+      <c r="R39" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="S39" s="126" t="s">
+      <c r="S39" s="122" t="s">
         <v>84</v>
       </c>
       <c r="T39" s="85"/>
@@ -5126,7 +5126,7 @@
         <v xml:space="preserve">                              Emergency Building Basement</v>
       </c>
       <c r="E40" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F40" s="80"/>
       <c r="G40" s="80"/>
@@ -5152,9 +5152,9 @@
       <c r="P40" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q40" s="129"/>
-      <c r="R40" s="128"/>
-      <c r="S40" s="127"/>
+      <c r="Q40" s="107"/>
+      <c r="R40" s="113"/>
+      <c r="S40" s="123"/>
       <c r="T40" s="85"/>
     </row>
     <row r="41" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
@@ -5173,7 +5173,7 @@
         <v xml:space="preserve">                              Emergency Building Walls</v>
       </c>
       <c r="E41" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F41" s="80"/>
       <c r="G41" s="80"/>
@@ -5199,9 +5199,9 @@
       <c r="P41" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="129"/>
-      <c r="R41" s="128"/>
-      <c r="S41" s="127"/>
+      <c r="Q41" s="107"/>
+      <c r="R41" s="113"/>
+      <c r="S41" s="123"/>
       <c r="T41" s="85"/>
     </row>
     <row r="42" spans="1:20" ht="104" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5220,7 +5220,7 @@
         <v xml:space="preserve">                        Diesel Generator</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -5342,7 +5342,7 @@
         <v xml:space="preserve">                        Storage Building Slab Roof</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -5368,13 +5368,13 @@
       <c r="P45" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q45" s="118" t="s">
+      <c r="Q45" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="R45" s="106" t="s">
+      <c r="R45" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="S45" s="107" t="s">
+      <c r="S45" s="117" t="s">
         <v>84</v>
       </c>
       <c r="T45" s="26"/>
@@ -5395,7 +5395,7 @@
         <v xml:space="preserve">                        Storage Building Basement</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
@@ -5421,9 +5421,9 @@
       <c r="P46" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="118"/>
-      <c r="R46" s="106"/>
-      <c r="S46" s="108"/>
+      <c r="Q46" s="108"/>
+      <c r="R46" s="112"/>
+      <c r="S46" s="118"/>
       <c r="T46" s="26"/>
     </row>
     <row r="47" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -5442,7 +5442,7 @@
         <v xml:space="preserve">                        Storage Building Walls</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
@@ -5468,9 +5468,9 @@
       <c r="P47" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="118"/>
-      <c r="R47" s="106"/>
-      <c r="S47" s="108"/>
+      <c r="Q47" s="108"/>
+      <c r="R47" s="112"/>
+      <c r="S47" s="118"/>
       <c r="T47" s="26"/>
     </row>
     <row r="48" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5521,7 +5521,7 @@
         <v xml:space="preserve">                        Radwaste Building Slab Roof</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -5547,13 +5547,13 @@
       <c r="P49" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q49" s="118" t="s">
+      <c r="Q49" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="R49" s="106" t="s">
+      <c r="R49" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="S49" s="107" t="s">
+      <c r="S49" s="117" t="s">
         <v>84</v>
       </c>
       <c r="T49" s="26"/>
@@ -5574,7 +5574,7 @@
         <v xml:space="preserve">                        Radwaste Building Basement</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
@@ -5600,9 +5600,9 @@
       <c r="P50" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q50" s="118"/>
-      <c r="R50" s="106"/>
-      <c r="S50" s="108"/>
+      <c r="Q50" s="108"/>
+      <c r="R50" s="112"/>
+      <c r="S50" s="118"/>
       <c r="T50" s="26"/>
     </row>
     <row r="51" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
@@ -5621,7 +5621,7 @@
         <v xml:space="preserve">                        Radwaste Building Walls</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
@@ -5647,9 +5647,9 @@
       <c r="P51" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q51" s="118"/>
-      <c r="R51" s="106"/>
-      <c r="S51" s="108"/>
+      <c r="Q51" s="108"/>
+      <c r="R51" s="112"/>
+      <c r="S51" s="118"/>
       <c r="T51" s="26"/>
     </row>
     <row r="52" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5764,7 +5764,7 @@
         <v xml:space="preserve">                        Reactor Support</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
@@ -5798,10 +5798,10 @@
       <c r="Q55" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R55" s="123" t="s">
+      <c r="R55" s="119" t="s">
         <v>179</v>
       </c>
-      <c r="S55" s="109" t="s">
+      <c r="S55" s="124" t="s">
         <v>183</v>
       </c>
       <c r="T55" s="42" t="s">
@@ -5824,7 +5824,7 @@
         <v xml:space="preserve">                        Outer Vessel Structure</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F56" s="19"/>
       <c r="G56" s="19"/>
@@ -5858,8 +5858,8 @@
       <c r="Q56" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R56" s="124"/>
-      <c r="S56" s="110"/>
+      <c r="R56" s="120"/>
+      <c r="S56" s="125"/>
       <c r="T56" s="26"/>
     </row>
     <row r="57" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5878,7 +5878,7 @@
         <v xml:space="preserve">                        Inner Vessel Structure</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
@@ -5915,8 +5915,8 @@
       <c r="Q57" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R57" s="125"/>
-      <c r="S57" s="111"/>
+      <c r="R57" s="121"/>
+      <c r="S57" s="126"/>
       <c r="T57" s="42" t="s">
         <v>182</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v xml:space="preserve">                              Reactivity Control System Fabrication</v>
       </c>
       <c r="E60" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F60" s="80"/>
       <c r="G60" s="80"/>
@@ -6026,11 +6026,11 @@
       <c r="Q60" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R60" s="112" t="s">
+      <c r="R60" s="127" t="s">
         <v>179</v>
       </c>
-      <c r="S60" s="115" t="s">
-        <v>352</v>
+      <c r="S60" s="130" t="s">
+        <v>350</v>
       </c>
       <c r="T60" s="90" t="s">
         <v>188</v>
@@ -6052,7 +6052,7 @@
         <v xml:space="preserve">                              Installation</v>
       </c>
       <c r="E61" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F61" s="80"/>
       <c r="G61" s="80"/>
@@ -6075,8 +6075,8 @@
       <c r="Q61" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R61" s="113"/>
-      <c r="S61" s="116"/>
+      <c r="R61" s="128"/>
+      <c r="S61" s="131"/>
       <c r="T61" s="85"/>
     </row>
     <row r="62" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6095,7 +6095,7 @@
         <v xml:space="preserve">                              Control Drums Materials (Absorber)</v>
       </c>
       <c r="E62" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F62" s="80" t="s">
         <v>332</v>
@@ -6133,8 +6133,8 @@
       <c r="Q62" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R62" s="113"/>
-      <c r="S62" s="116"/>
+      <c r="R62" s="128"/>
+      <c r="S62" s="131"/>
       <c r="T62" s="85"/>
     </row>
     <row r="63" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6153,7 +6153,7 @@
         <v xml:space="preserve">                              Control Drums Materials (Reflector)</v>
       </c>
       <c r="E63" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F63" s="80" t="s">
         <v>331</v>
@@ -6191,8 +6191,8 @@
       <c r="Q63" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R63" s="114"/>
-      <c r="S63" s="117"/>
+      <c r="R63" s="129"/>
+      <c r="S63" s="132"/>
       <c r="T63" s="85"/>
     </row>
     <row r="64" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6211,7 +6211,7 @@
         <v xml:space="preserve">                  Non-Fuel Core Internals</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
@@ -6241,7 +6241,7 @@
         <v xml:space="preserve">                        Reflector</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F65" s="19" t="s">
         <v>13</v>
@@ -6282,10 +6282,10 @@
       <c r="Q65" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="R65" s="123" t="s">
+      <c r="R65" s="119" t="s">
         <v>179</v>
       </c>
-      <c r="S65" s="109" t="s">
+      <c r="S65" s="124" t="s">
         <v>183</v>
       </c>
       <c r="T65" s="26"/>
@@ -6318,8 +6318,8 @@
       <c r="O66" s="26"/>
       <c r="P66" s="26"/>
       <c r="Q66" s="42"/>
-      <c r="R66" s="124"/>
-      <c r="S66" s="110"/>
+      <c r="R66" s="120"/>
+      <c r="S66" s="125"/>
       <c r="T66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6338,7 +6338,7 @@
         <v xml:space="preserve">                              In Vessel Shield Materials</v>
       </c>
       <c r="E67" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F67" s="80" t="s">
         <v>335</v>
@@ -6358,7 +6358,7 @@
         <v>177</v>
       </c>
       <c r="K67" s="90" t="s">
-        <v>338</v>
+        <v>414</v>
       </c>
       <c r="L67" s="85">
         <f>L62</f>
@@ -6379,8 +6379,8 @@
       <c r="Q67" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R67" s="124"/>
-      <c r="S67" s="110"/>
+      <c r="R67" s="120"/>
+      <c r="S67" s="125"/>
       <c r="T67" s="85"/>
     </row>
     <row r="68" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -6399,7 +6399,7 @@
         <v xml:space="preserve">                              Out The Vessel Shield Materials</v>
       </c>
       <c r="E68" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F68" s="80" t="s">
         <v>336</v>
@@ -6415,7 +6415,7 @@
         <v>177</v>
       </c>
       <c r="K68" s="90" t="s">
-        <v>339</v>
+        <v>415</v>
       </c>
       <c r="L68" s="85">
         <f>'Design Variables'!B43</f>
@@ -6436,8 +6436,8 @@
       <c r="Q68" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="R68" s="125"/>
-      <c r="S68" s="111"/>
+      <c r="R68" s="121"/>
+      <c r="S68" s="126"/>
       <c r="T68" s="85"/>
     </row>
     <row r="69" spans="1:20" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6456,13 +6456,13 @@
         <v xml:space="preserve">                        Moderator</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F69" s="19" t="s">
         <v>203</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H69" s="24"/>
       <c r="I69" s="69">
@@ -6472,7 +6472,7 @@
         <v>177</v>
       </c>
       <c r="K69" s="42" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="M69" s="26" t="s">
         <v>176</v>
@@ -6485,10 +6485,10 @@
         <v>73</v>
       </c>
       <c r="Q69" s="42" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R69" s="73" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="S69" s="75"/>
       <c r="T69" s="26"/>
@@ -6509,13 +6509,13 @@
         <v xml:space="preserve">            Moderator</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F70" s="19" t="s">
         <v>203</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H70" s="24"/>
       <c r="I70" s="69">
@@ -6525,7 +6525,7 @@
         <v>177</v>
       </c>
       <c r="K70" s="42" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="M70" s="26" t="s">
         <v>176</v>
@@ -6538,7 +6538,7 @@
         <v>73</v>
       </c>
       <c r="Q70" s="76" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="R70" s="74"/>
       <c r="S70" s="75"/>
@@ -6591,7 +6591,7 @@
         <v>3</v>
       </c>
       <c r="C72" s="37" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D72" s="19" t="str">
         <f t="shared" si="1"/>
@@ -6622,20 +6622,20 @@
         <v>4</v>
       </c>
       <c r="C73" s="37" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D73" s="19" t="str">
         <f>REPT("   ", B73*2) &amp; C73</f>
         <v xml:space="preserve">                        Primary Pump</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G73" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H73" s="24"/>
       <c r="I73" s="69">
@@ -6643,10 +6643,10 @@
         <v>8818.5</v>
       </c>
       <c r="J73" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K73" s="42" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L73" s="26"/>
       <c r="M73" s="26"/>
@@ -6660,15 +6660,15 @@
         <v>74</v>
       </c>
       <c r="Q73" s="42" t="s">
-        <v>354</v>
-      </c>
-      <c r="R73" s="104" t="s">
+        <v>352</v>
+      </c>
+      <c r="R73" s="109" t="s">
+        <v>351</v>
+      </c>
+      <c r="S73" s="114" t="s">
         <v>353</v>
       </c>
-      <c r="S73" s="120" t="s">
-        <v>355</v>
-      </c>
-      <c r="T73" s="104"/>
+      <c r="T73" s="109"/>
     </row>
     <row r="74" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
@@ -6679,30 +6679,30 @@
         <v>4</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D74" s="19" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">                        Secondary Pump</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G74" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H74" s="24"/>
       <c r="I74" s="69">
         <v>705.48</v>
       </c>
       <c r="J74" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K74" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L74" s="26"/>
       <c r="M74" s="26"/>
@@ -6716,11 +6716,11 @@
         <v>74</v>
       </c>
       <c r="Q74" s="42" t="s">
-        <v>348</v>
-      </c>
-      <c r="R74" s="105"/>
-      <c r="S74" s="121"/>
-      <c r="T74" s="105"/>
+        <v>346</v>
+      </c>
+      <c r="R74" s="111"/>
+      <c r="S74" s="115"/>
+      <c r="T74" s="111"/>
     </row>
     <row r="75" spans="1:20" ht="76" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
@@ -6731,30 +6731,30 @@
         <v>4</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D75" s="19" t="str">
         <f t="shared" ref="D75" si="3">REPT("   ", B75*2) &amp; C75</f>
         <v xml:space="preserve">                        Compressor</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H75" s="24"/>
       <c r="I75" s="69">
         <v>44.71</v>
       </c>
       <c r="J75" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K75" s="42" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L75" s="26"/>
       <c r="M75" s="26"/>
@@ -6768,10 +6768,10 @@
         <v>74</v>
       </c>
       <c r="Q75" s="42" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="R75" s="93" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="S75" s="94"/>
       <c r="T75" s="93"/>
@@ -6792,7 +6792,7 @@
         <v xml:space="preserve">                  Reactor Heat Transfer Piping System</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F76" s="19"/>
       <c r="G76" s="19"/>
@@ -6816,10 +6816,10 @@
         <v>74</v>
       </c>
       <c r="Q76" s="42" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="R76" s="42" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="S76" s="26"/>
       <c r="T76" s="26"/>
@@ -6865,20 +6865,20 @@
         <v>4</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D78" s="19" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">                        Primary Heat Exchanger</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G78" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H78" s="24"/>
       <c r="I78" s="69">
@@ -6888,7 +6888,7 @@
         <v>177</v>
       </c>
       <c r="K78" s="42" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L78" s="26"/>
       <c r="M78" s="26" t="s">
@@ -6902,10 +6902,10 @@
         <v>74</v>
       </c>
       <c r="Q78" s="42" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="R78" s="93" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="S78" s="26"/>
       <c r="T78" s="26"/>
@@ -6926,20 +6926,20 @@
         <v>4</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D79" s="19" t="str">
         <f t="shared" ref="D79" si="5">REPT("   ", B79*2) &amp; C79</f>
         <v xml:space="preserve">                        Primary Heat Exchanger</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G79" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H79" s="24"/>
       <c r="I79" s="69">
@@ -6949,7 +6949,7 @@
         <v>177</v>
       </c>
       <c r="K79" s="42" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L79" s="26"/>
       <c r="M79" s="26" t="s">
@@ -6963,10 +6963,10 @@
         <v>74</v>
       </c>
       <c r="Q79" s="42" t="s">
+        <v>371</v>
+      </c>
+      <c r="R79" s="93" t="s">
         <v>373</v>
-      </c>
-      <c r="R79" s="93" t="s">
-        <v>375</v>
       </c>
       <c r="S79" s="26"/>
       <c r="T79" s="26"/>
@@ -6987,13 +6987,13 @@
         <v xml:space="preserve">                        Secondary Heat Exchanger</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H80" s="24"/>
       <c r="I80" s="69">
@@ -7003,7 +7003,7 @@
         <v>177</v>
       </c>
       <c r="K80" s="42" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L80" s="26"/>
       <c r="M80" s="26" t="s">
@@ -7017,10 +7017,10 @@
         <v>74</v>
       </c>
       <c r="Q80" s="42" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="R80" s="93" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="S80" s="26"/>
       <c r="T80" s="26"/>
@@ -7048,13 +7048,13 @@
         <v xml:space="preserve">                        Secondary Heat Exchanger</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G81" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H81" s="24"/>
       <c r="I81" s="69">
@@ -7064,7 +7064,7 @@
         <v>177</v>
       </c>
       <c r="K81" s="42" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L81" s="26"/>
       <c r="M81" s="26" t="s">
@@ -7078,10 +7078,10 @@
         <v>74</v>
       </c>
       <c r="Q81" s="42" t="s">
+        <v>371</v>
+      </c>
+      <c r="R81" s="93" t="s">
         <v>373</v>
-      </c>
-      <c r="R81" s="93" t="s">
-        <v>375</v>
       </c>
       <c r="S81" s="26"/>
       <c r="T81" s="26"/>
@@ -7166,7 +7166,7 @@
         <v xml:space="preserve">                        Rvacs (Cooling Vessel)</v>
       </c>
       <c r="E84" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F84" s="19"/>
       <c r="G84" s="23"/>
@@ -7179,7 +7179,7 @@
         <v>177</v>
       </c>
       <c r="K84" s="42" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L84" s="26">
         <f>L56</f>
@@ -7198,7 +7198,7 @@
         <v>77</v>
       </c>
       <c r="Q84" s="42" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="R84" s="26"/>
       <c r="S84" s="26"/>
@@ -7220,7 +7220,7 @@
         <v xml:space="preserve">                        Rvacs (Intake Vessel)</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F85" s="19"/>
       <c r="G85" s="23"/>
@@ -7233,7 +7233,7 @@
         <v>177</v>
       </c>
       <c r="K85" s="42" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L85" s="26">
         <f>L84</f>
@@ -7252,7 +7252,7 @@
         <v>77</v>
       </c>
       <c r="Q85" s="42" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="R85" s="26"/>
       <c r="S85" s="26"/>
@@ -7274,7 +7274,7 @@
         <v xml:space="preserve">            Other Reactor Plant Equipment</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F86" s="19"/>
       <c r="G86" s="23"/>
@@ -7295,7 +7295,7 @@
         <v>74</v>
       </c>
       <c r="Q86" s="42" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="R86" s="26"/>
       <c r="S86" s="26"/>
@@ -7324,7 +7324,7 @@
         <v xml:space="preserve">            Reactor Instrumentation and Control (I&amp;C)</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F87" s="19"/>
       <c r="G87" s="23"/>
@@ -7345,7 +7345,7 @@
         <v>74</v>
       </c>
       <c r="Q87" s="42" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="R87" s="26"/>
       <c r="S87" s="26"/>
@@ -7367,7 +7367,7 @@
         <v xml:space="preserve">            Reactor Plant Miscellaneous Items</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F88" s="19"/>
       <c r="G88" s="23"/>
@@ -7388,7 +7388,7 @@
         <v>77</v>
       </c>
       <c r="Q88" s="42" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="R88" s="26"/>
       <c r="S88" s="26"/>
@@ -7474,7 +7474,7 @@
         <v xml:space="preserve">                  Electricity Generation Systems</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F91" s="19"/>
       <c r="G91" s="23"/>
@@ -7505,10 +7505,10 @@
         <v>74</v>
       </c>
       <c r="Q91" s="42" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="R91" s="42" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S91" s="26"/>
       <c r="T91" s="26"/>
@@ -7561,7 +7561,7 @@
         <v xml:space="preserve">            Power and Control Cables and Wiring</v>
       </c>
       <c r="E93" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F93" s="19"/>
       <c r="G93" s="23"/>
@@ -7593,10 +7593,10 @@
         <v>74</v>
       </c>
       <c r="Q93" s="42" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="R93" s="42" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="S93" s="26"/>
       <c r="T93" s="26"/>
@@ -7649,7 +7649,7 @@
         <v xml:space="preserve">            First Core Mining</v>
       </c>
       <c r="E95" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F95" s="19"/>
       <c r="G95" s="23"/>
@@ -7661,7 +7661,7 @@
         <v>177</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L95" s="26"/>
       <c r="M95" s="26"/>
@@ -7672,11 +7672,11 @@
       <c r="P95" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q95" s="104" t="s">
-        <v>387</v>
-      </c>
-      <c r="R95" s="104" t="s">
-        <v>388</v>
+      <c r="Q95" s="109" t="s">
+        <v>385</v>
+      </c>
+      <c r="R95" s="109" t="s">
+        <v>386</v>
       </c>
       <c r="S95" s="26"/>
       <c r="T95" s="26"/>
@@ -7697,7 +7697,7 @@
         <v xml:space="preserve">            First Core Conversion </v>
       </c>
       <c r="E96" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F96" s="19"/>
       <c r="G96" s="23"/>
@@ -7709,7 +7709,7 @@
         <v>177</v>
       </c>
       <c r="K96" s="23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L96" s="26"/>
       <c r="M96" s="26"/>
@@ -7720,8 +7720,8 @@
       <c r="P96" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q96" s="119"/>
-      <c r="R96" s="119"/>
+      <c r="Q96" s="110"/>
+      <c r="R96" s="110"/>
       <c r="S96" s="26"/>
       <c r="T96" s="26"/>
     </row>
@@ -7741,7 +7741,7 @@
         <v xml:space="preserve">            First Core Enrichment </v>
       </c>
       <c r="E97" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F97" s="19"/>
       <c r="G97" s="23"/>
@@ -7750,10 +7750,10 @@
         <v>184.2</v>
       </c>
       <c r="J97" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="K97" s="42" t="s">
         <v>384</v>
-      </c>
-      <c r="K97" s="42" t="s">
-        <v>386</v>
       </c>
       <c r="L97" s="26"/>
       <c r="M97" s="26"/>
@@ -7766,8 +7766,8 @@
       <c r="P97" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q97" s="119"/>
-      <c r="R97" s="119"/>
+      <c r="Q97" s="110"/>
+      <c r="R97" s="110"/>
       <c r="S97" s="26"/>
       <c r="T97" s="26"/>
     </row>
@@ -7787,13 +7787,13 @@
         <v xml:space="preserve">            First Core Fuel Assembly Fabrication </v>
       </c>
       <c r="E98" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F98" s="19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G98" s="23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H98" s="23"/>
       <c r="I98" s="23">
@@ -7803,7 +7803,7 @@
         <v>177</v>
       </c>
       <c r="K98" s="42" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L98" s="26"/>
       <c r="M98" s="26"/>
@@ -7814,8 +7814,8 @@
       <c r="P98" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q98" s="119"/>
-      <c r="R98" s="119"/>
+      <c r="Q98" s="110"/>
+      <c r="R98" s="110"/>
       <c r="S98" s="26"/>
       <c r="T98" s="26"/>
     </row>
@@ -7842,13 +7842,13 @@
         <v xml:space="preserve">            First Core Fuel Assembly Fabrication </v>
       </c>
       <c r="E99" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G99" s="23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H99" s="23"/>
       <c r="I99" s="23">
@@ -7858,7 +7858,7 @@
         <v>177</v>
       </c>
       <c r="K99" s="42" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L99" s="26"/>
       <c r="M99" s="26"/>
@@ -7869,8 +7869,8 @@
       <c r="P99" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q99" s="105"/>
-      <c r="R99" s="105"/>
+      <c r="Q99" s="111"/>
+      <c r="R99" s="111"/>
       <c r="S99" s="26"/>
       <c r="T99" s="26"/>
     </row>
@@ -7890,7 +7890,7 @@
         <v xml:space="preserve">      Miscellaneous Equipment (Cranes)</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F100" s="19"/>
       <c r="G100" s="19"/>
@@ -7910,10 +7910,10 @@
         <v>74</v>
       </c>
       <c r="Q100" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="R100" s="42" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="S100" s="26"/>
       <c r="T100" s="26"/>
@@ -7965,7 +7965,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="37" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D102" s="19" t="str">
         <f t="shared" si="9"/>
@@ -7996,7 +7996,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="37" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D103" s="19" t="str">
         <f t="shared" si="9"/>
@@ -8035,7 +8035,7 @@
         <v xml:space="preserve">      Startup Costs</v>
       </c>
       <c r="E104" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F104" s="19"/>
       <c r="G104" s="19"/>
@@ -8055,8 +8055,8 @@
       <c r="P104" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="Q104" s="130" t="s">
-        <v>379</v>
+      <c r="Q104" s="104" t="s">
+        <v>377</v>
       </c>
       <c r="R104" s="24"/>
       <c r="S104" s="24"/>
@@ -8084,7 +8084,7 @@
         <v xml:space="preserve">      Shipping and Transportation Costs</v>
       </c>
       <c r="E105" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F105" s="19"/>
       <c r="G105" s="19"/>
@@ -8104,7 +8104,7 @@
       <c r="P105" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="Q105" s="131"/>
+      <c r="Q105" s="105"/>
       <c r="R105" s="24"/>
       <c r="S105" s="24"/>
       <c r="T105" s="24"/>
@@ -8131,7 +8131,7 @@
         <v xml:space="preserve">      Engineering Services</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F106" s="19"/>
       <c r="G106" s="19"/>
@@ -8151,7 +8151,7 @@
       <c r="P106" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="Q106" s="131"/>
+      <c r="Q106" s="105"/>
       <c r="R106" s="26"/>
       <c r="S106" s="26"/>
       <c r="T106" s="26"/>
@@ -8173,7 +8173,7 @@
         <v xml:space="preserve">      PM/CM Services</v>
       </c>
       <c r="E107" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F107" s="19"/>
       <c r="G107" s="19"/>
@@ -8193,7 +8193,7 @@
       <c r="P107" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="Q107" s="132"/>
+      <c r="Q107" s="106"/>
       <c r="R107" s="26"/>
       <c r="S107" s="26"/>
       <c r="T107" s="26"/>
@@ -8208,7 +8208,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="37" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D108" s="19" t="str">
         <f t="shared" si="9"/>
@@ -8241,14 +8241,14 @@
         <v>1</v>
       </c>
       <c r="C109" s="37" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D109" s="19" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">      staff recruitment and training</v>
       </c>
       <c r="E109" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F109" s="19"/>
       <c r="G109" s="19"/>
@@ -8269,7 +8269,7 @@
         <v>72</v>
       </c>
       <c r="Q109" s="99" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="R109" s="26"/>
       <c r="S109" s="26"/>
@@ -8424,7 +8424,7 @@
         <v xml:space="preserve">            Operators </v>
       </c>
       <c r="E114" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F114" s="19"/>
       <c r="G114" s="19"/>
@@ -8433,10 +8433,10 @@
         <v>178500</v>
       </c>
       <c r="J114" s="26" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K114" s="42" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L114" s="26"/>
       <c r="M114" s="26"/>
@@ -8451,7 +8451,7 @@
       </c>
       <c r="Q114" s="42"/>
       <c r="R114" s="102" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="S114" s="26"/>
       <c r="T114" s="26"/>
@@ -8473,23 +8473,23 @@
         <v xml:space="preserve">            Remote Monitoring Technicians </v>
       </c>
       <c r="E115" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F115" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G115" s="19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H115" s="24"/>
       <c r="I115" s="69">
         <v>178500</v>
       </c>
       <c r="J115" s="26" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K115" s="42" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L115" s="26"/>
       <c r="M115" s="26"/>
@@ -8504,7 +8504,7 @@
       </c>
       <c r="Q115" s="42"/>
       <c r="R115" s="102" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="S115" s="26"/>
       <c r="T115" s="26"/>
@@ -8526,7 +8526,7 @@
         <v xml:space="preserve">            Security Staff </v>
       </c>
       <c r="E116" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F116" s="19"/>
       <c r="G116" s="19"/>
@@ -8535,10 +8535,10 @@
         <v>178500</v>
       </c>
       <c r="J116" s="26" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K116" s="42" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L116" s="26"/>
       <c r="M116" s="26"/>
@@ -8553,7 +8553,7 @@
       </c>
       <c r="Q116" s="42"/>
       <c r="R116" s="102" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="S116" s="26"/>
       <c r="T116" s="26"/>
@@ -8608,7 +8608,7 @@
         <v xml:space="preserve">      Annualized Decommissioning Cost</v>
       </c>
       <c r="E118" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F118" s="19"/>
       <c r="G118" s="19"/>
@@ -8636,7 +8636,7 @@
       </c>
       <c r="Q118" s="42"/>
       <c r="R118" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="S118" s="26"/>
       <c r="T118" s="26"/>
@@ -8690,7 +8690,7 @@
         <v xml:space="preserve">      Refueling Operations</v>
       </c>
       <c r="E120" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F120" s="19"/>
       <c r="G120" s="19"/>
@@ -8699,10 +8699,10 @@
         <v>178500</v>
       </c>
       <c r="J120" s="26" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K120" s="42" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L120" s="26"/>
       <c r="M120" s="26"/>
@@ -8717,7 +8717,7 @@
       </c>
       <c r="Q120" s="42"/>
       <c r="R120" s="102" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="S120" s="26"/>
       <c r="T120" s="26"/>
@@ -8770,7 +8770,7 @@
         <v xml:space="preserve">      Spent Fuel Management</v>
       </c>
       <c r="E122" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F122" s="19"/>
       <c r="G122" s="19"/>
@@ -8779,10 +8779,10 @@
         <v>1</v>
       </c>
       <c r="J122" s="26" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K122" s="42" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L122" s="26"/>
       <c r="M122" s="26"/>
@@ -8802,19 +8802,20 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="Q104:Q107"/>
-    <mergeCell ref="Q39:Q41"/>
-    <mergeCell ref="Q45:Q47"/>
-    <mergeCell ref="Q49:Q51"/>
-    <mergeCell ref="Q95:Q99"/>
-    <mergeCell ref="R24:R26"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="R34:R36"/>
-    <mergeCell ref="R39:R41"/>
-    <mergeCell ref="Q20:Q22"/>
-    <mergeCell ref="Q24:Q26"/>
-    <mergeCell ref="Q30:Q32"/>
-    <mergeCell ref="Q34:Q36"/>
+    <mergeCell ref="T73:T74"/>
+    <mergeCell ref="R45:R47"/>
+    <mergeCell ref="R49:R51"/>
+    <mergeCell ref="S45:S47"/>
+    <mergeCell ref="S49:S51"/>
+    <mergeCell ref="S65:S68"/>
+    <mergeCell ref="R60:R63"/>
+    <mergeCell ref="S60:S63"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
     <mergeCell ref="R95:R99"/>
     <mergeCell ref="R73:R74"/>
     <mergeCell ref="S73:S74"/>
@@ -8831,61 +8832,60 @@
     <mergeCell ref="S55:S57"/>
     <mergeCell ref="S39:S41"/>
     <mergeCell ref="R20:R22"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="T73:T74"/>
-    <mergeCell ref="R45:R47"/>
-    <mergeCell ref="R49:R51"/>
-    <mergeCell ref="S45:S47"/>
-    <mergeCell ref="S49:S51"/>
-    <mergeCell ref="S65:S68"/>
-    <mergeCell ref="R60:R63"/>
-    <mergeCell ref="S60:S63"/>
+    <mergeCell ref="R24:R26"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="R34:R36"/>
+    <mergeCell ref="R39:R41"/>
+    <mergeCell ref="Q20:Q22"/>
+    <mergeCell ref="Q24:Q26"/>
+    <mergeCell ref="Q30:Q32"/>
+    <mergeCell ref="Q34:Q36"/>
+    <mergeCell ref="Q104:Q107"/>
+    <mergeCell ref="Q39:Q41"/>
+    <mergeCell ref="Q45:Q47"/>
+    <mergeCell ref="Q49:Q51"/>
+    <mergeCell ref="Q95:Q99"/>
   </mergeCells>
-  <conditionalFormatting sqref="A73:F75 L95:T95 L96:P96 S96:T100 I97:P97 A100:R100 R104:T109 A110:T113 A114:H115 A116:J116 A117:T117 S118:T118 A119:T119 A121:T122 A120:J120 L120:Q120 S120:T120">
+  <conditionalFormatting sqref="A73:F75 L95:T95 L96:P96 S96:T100 I97:P97 A100:R100 R104:T109 A110:T113 A114:H115 A116:J116 A117:T117 S118:T118 A119:T119 S120:T120 A121:T122">
     <cfRule type="expression" dxfId="84" priority="140">
       <formula>$B73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="139">
-      <formula>$B73&lt;2</formula>
+    <cfRule type="expression" dxfId="83" priority="137">
+      <formula>$B73=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="82" priority="138">
       <formula>$B73=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="137">
-      <formula>$B73=3</formula>
+    <cfRule type="expression" dxfId="81" priority="139">
+      <formula>$B73&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:H97">
-    <cfRule type="expression" dxfId="80" priority="104">
-      <formula>$B95=0</formula>
+    <cfRule type="expression" dxfId="80" priority="101">
+      <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="103">
+    <cfRule type="expression" dxfId="79" priority="102">
+      <formula>$B95=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="103">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="102">
-      <formula>$B95=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="101">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="77" priority="104">
+      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:I81">
-    <cfRule type="expression" dxfId="76" priority="128">
-      <formula>$B77=0</formula>
+    <cfRule type="expression" dxfId="76" priority="125">
+      <formula>$B77=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="127">
+    <cfRule type="expression" dxfId="75" priority="126">
+      <formula>$B77=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="127">
       <formula>$B77&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="126">
-      <formula>$B77=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="125">
-      <formula>$B77=3</formula>
+    <cfRule type="expression" dxfId="73" priority="128">
+      <formula>$B77=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:P99">
@@ -8903,86 +8903,100 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:P109">
-    <cfRule type="expression" dxfId="68" priority="33">
+    <cfRule type="expression" dxfId="68" priority="36">
+      <formula>$B102=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="33">
       <formula>$B102=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="36">
-      <formula>$B102=0</formula>
+    <cfRule type="expression" dxfId="66" priority="34">
+      <formula>$B102=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="35">
+    <cfRule type="expression" dxfId="65" priority="35">
       <formula>$B102&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="34">
-      <formula>$B102=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118:Q118">
-    <cfRule type="expression" dxfId="64" priority="5">
+    <cfRule type="expression" dxfId="64" priority="6">
+      <formula>$B118=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="5">
       <formula>$B118=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="6">
-      <formula>$B118=2</formula>
+    <cfRule type="expression" dxfId="62" priority="8">
+      <formula>$B118=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="7">
+    <cfRule type="expression" dxfId="61" priority="7">
       <formula>$B118&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="8">
-      <formula>$B118=0</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A120:Q120">
+    <cfRule type="expression" dxfId="60" priority="4">
+      <formula>$B120=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="3">
+      <formula>$B120&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="2">
+      <formula>$B120=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="1">
+      <formula>$B120=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:S72">
-    <cfRule type="expression" dxfId="60" priority="144">
-      <formula>$B72=0</formula>
+    <cfRule type="expression" dxfId="56" priority="141">
+      <formula>$B72=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="143">
+    <cfRule type="expression" dxfId="55" priority="142">
+      <formula>$B72=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="143">
       <formula>$B72&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="142">
-      <formula>$B72=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="141">
-      <formula>$B72=3</formula>
+    <cfRule type="expression" dxfId="53" priority="144">
+      <formula>$B72=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T71 T72:T75 H73:R73 H74:Q74 G75:Q75 A76:T76 K77:T77 S78:T81">
-    <cfRule type="expression" dxfId="56" priority="148">
-      <formula>$B1=0</formula>
+    <cfRule type="expression" dxfId="52" priority="145">
+      <formula>$B1=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="147">
+    <cfRule type="expression" dxfId="51" priority="146">
+      <formula>$B1=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="147">
       <formula>$B1&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="146">
-      <formula>$B1=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="145">
-      <formula>$B1=3</formula>
+    <cfRule type="expression" dxfId="49" priority="148">
+      <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:T94">
-    <cfRule type="expression" dxfId="52" priority="105">
-      <formula>$B82=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="108">
+    <cfRule type="expression" dxfId="48" priority="108">
       <formula>$B82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="107">
+    <cfRule type="expression" dxfId="47" priority="107">
       <formula>$B82&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="106">
+    <cfRule type="expression" dxfId="46" priority="106">
       <formula>$B82=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="105">
+      <formula>$B82=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:T101">
-    <cfRule type="expression" dxfId="48" priority="69">
+    <cfRule type="expression" dxfId="44" priority="69">
       <formula>$B101=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="70">
+    <cfRule type="expression" dxfId="43" priority="70">
       <formula>$B101=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="71">
+    <cfRule type="expression" dxfId="42" priority="71">
       <formula>$B101&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="72">
+    <cfRule type="expression" dxfId="41" priority="72">
       <formula>$B101=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8997,168 +9011,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G73:G74">
-    <cfRule type="expression" dxfId="44" priority="133">
+    <cfRule type="expression" dxfId="40" priority="133">
       <formula>$B73=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="136">
+    <cfRule type="expression" dxfId="39" priority="136">
       <formula>$B73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="135">
+    <cfRule type="expression" dxfId="38" priority="135">
       <formula>$B73&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="134">
+    <cfRule type="expression" dxfId="37" priority="134">
       <formula>$B73=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I114:J115">
-    <cfRule type="expression" dxfId="40" priority="20">
-      <formula>$B115=0</formula>
+    <cfRule type="expression" dxfId="36" priority="17">
+      <formula>$B115=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="19">
+    <cfRule type="expression" dxfId="35" priority="18">
+      <formula>$B115=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="19">
       <formula>$B115&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="18">
-      <formula>$B115=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="17">
-      <formula>$B115=3</formula>
+    <cfRule type="expression" dxfId="33" priority="20">
+      <formula>$B115=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I95:K96">
-    <cfRule type="expression" dxfId="36" priority="97">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="32" priority="99">
+      <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="98">
+    <cfRule type="expression" dxfId="31" priority="100">
+      <formula>$B95=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="98">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="99">
-      <formula>$B95&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="100">
-      <formula>$B95=0</formula>
+    <cfRule type="expression" dxfId="29" priority="97">
+      <formula>$B95=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J77 O101">
-    <cfRule type="expression" dxfId="32" priority="157">
+    <cfRule type="expression" dxfId="28" priority="157">
       <formula>$B78=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="156">
+    <cfRule type="expression" dxfId="27" priority="156">
       <formula>$B78&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="155">
+    <cfRule type="expression" dxfId="26" priority="155">
       <formula>$B78=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:Q81">
-    <cfRule type="expression" dxfId="29" priority="123">
+    <cfRule type="expression" dxfId="25" priority="122">
+      <formula>$B78=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="123">
       <formula>$B78&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="124">
+    <cfRule type="expression" dxfId="23" priority="124">
       <formula>$B78=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="121">
+    <cfRule type="expression" dxfId="22" priority="121">
       <formula>$B78=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="122">
-      <formula>$B78=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K114:Q116 S114:T116">
-    <cfRule type="expression" dxfId="25" priority="11">
-      <formula>$B114&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>$B114=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="10">
+    <cfRule type="expression" dxfId="20" priority="10">
       <formula>$B114=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="11">
+      <formula>$B114&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K114:Q116">
-    <cfRule type="expression" dxfId="22" priority="12">
+    <cfRule type="expression" dxfId="18" priority="12">
       <formula>$B114=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O101 J77">
-    <cfRule type="expression" dxfId="21" priority="154">
+    <cfRule type="expression" dxfId="17" priority="154">
       <formula>$B78=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q104">
-    <cfRule type="expression" dxfId="20" priority="84">
+    <cfRule type="expression" dxfId="16" priority="84">
       <formula>$B104=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="81">
-      <formula>$B104=3</formula>
+    <cfRule type="expression" dxfId="15" priority="83">
+      <formula>$B104&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="82">
+    <cfRule type="expression" dxfId="14" priority="82">
       <formula>$B104=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="83">
-      <formula>$B104&lt;2</formula>
+    <cfRule type="expression" dxfId="13" priority="81">
+      <formula>$B104=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q108:Q109">
-    <cfRule type="expression" dxfId="16" priority="80">
+    <cfRule type="expression" dxfId="12" priority="80">
       <formula>$B108=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="79">
-      <formula>$B108&lt;2</formula>
+    <cfRule type="expression" dxfId="11" priority="77">
+      <formula>$B108=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="78">
+    <cfRule type="expression" dxfId="10" priority="78">
       <formula>$B108=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="77">
-      <formula>$B108=3</formula>
+    <cfRule type="expression" dxfId="9" priority="79">
+      <formula>$B108&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q102:T103">
-    <cfRule type="expression" dxfId="12" priority="44">
+    <cfRule type="expression" dxfId="8" priority="41">
+      <formula>$B102=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="42">
+      <formula>$B102=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="44">
       <formula>$B102=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="43">
+    <cfRule type="expression" dxfId="5" priority="43">
       <formula>$B102&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="42">
-      <formula>$B102=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="41">
-      <formula>$B102=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S73">
-    <cfRule type="expression" dxfId="8" priority="162">
+    <cfRule type="expression" dxfId="4" priority="162">
       <formula>$B72=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="165">
-      <formula>$B72=0</formula>
+    <cfRule type="expression" dxfId="3" priority="163">
+      <formula>$B72=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="164">
+    <cfRule type="expression" dxfId="2" priority="164">
       <formula>$B72&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="163">
-      <formula>$B72=2</formula>
+    <cfRule type="expression" dxfId="1" priority="165">
+      <formula>$B72=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S114:T116">
-    <cfRule type="expression" dxfId="4" priority="28">
+    <cfRule type="expression" dxfId="0" priority="28">
       <formula>$B114=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K120">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$B120=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$B120=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>$B120&lt;2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K120">
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$B120=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">
@@ -11945,7 +11943,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="101" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="101" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B1" s="101" t="s">
         <v>242</v>
@@ -11953,7 +11951,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B2" s="4">
         <f>MARVEL_Cost!C56/(MARVEL_Cost!C6+MARVEL_Cost!C13+MARVEL_Cost!C45)</f>
@@ -11962,7 +11960,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -11970,7 +11968,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -11978,7 +11976,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -11986,7 +11984,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B6">
         <v>1800</v>
@@ -11994,7 +11992,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -12002,7 +12000,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B8">
         <v>0.01</v>

</xml_diff>

<commit_message>
FOAK to NOAK Cost Multipliers
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannbn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A2598A-FF6D-554C-AA6E-51CFD281026F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E81F21-968A-EC4F-B5F1-97401D01F92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -57,6 +57,7 @@
     <author>tc={F26C2C60-5554-7C46-A2DA-9CC485CDD5A5}</author>
     <author>tc={6A4E3BDC-584F-1346-BF51-598A89836273}</author>
     <author>tc={368934F8-D933-024D-9355-5B191B79D6E7}</author>
+    <author>tc={6E7B8F31-3BA2-6E43-928D-71FCFDC70463}</author>
   </authors>
   <commentList>
     <comment ref="L63" authorId="0" shapeId="0" xr:uid="{1B3BEBC6-8301-0940-8823-166952F6D7FC}">
@@ -94,12 +95,21 @@
 </t>
       </text>
     </comment>
+    <comment ref="H107" authorId="4" shapeId="0" xr:uid="{6E7B8F31-3BA2-6E43-928D-71FCFDC70463}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The cost is multiplied by 0.5 since the
+ shipping included international shipping</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="431">
   <si>
     <t>Account</t>
   </si>
@@ -1567,6 +1577,42 @@
   </si>
   <si>
     <t>https://papers.ssrn.com/sol3/papers.cfm?abstract_id=5163464</t>
+  </si>
+  <si>
+    <t>FOAK to NOAK Multiplier Type</t>
+  </si>
+  <si>
+    <t>No Learning</t>
+  </si>
+  <si>
+    <t>Onsite Learning</t>
+  </si>
+  <si>
+    <t>Factory Primary Structure</t>
+  </si>
+  <si>
+    <t>Factory Drums</t>
+  </si>
+  <si>
+    <t>Factory Other</t>
+  </si>
+  <si>
+    <t>NRC Website</t>
+  </si>
+  <si>
+    <t>https://www.nrc.gov/about-nrc/regulatory/licensing/general-fee-questions.pdf</t>
+  </si>
+  <si>
+    <t>Licensing Learning</t>
+  </si>
+  <si>
+    <t>Assumed Onsite Learning Rate</t>
+  </si>
+  <si>
+    <t>FOAK to NOAK Multipliers</t>
+  </si>
+  <si>
+    <t>Assumed Number Of Units For Onsite Learning</t>
   </si>
 </sst>
 </file>
@@ -2019,7 +2065,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2275,6 +2321,9 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2383,6 +2432,9 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2391,12 +2443,13 @@
     <cellStyle name="Normal 2" xfId="4" xr:uid="{E15291B7-9068-3147-AE9D-D55638463741}"/>
     <cellStyle name="Normal 2 5" xfId="3" xr:uid="{D5427F60-54E8-014E-9224-5454BAE094F2}"/>
   </cellStyles>
-  <dxfs count="81">
+  <dxfs count="85">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2419,11 +2472,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2487,10 +2539,348 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2549,7 +2939,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2559,6 +2949,19 @@
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2588,15 +2991,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2610,7 +3007,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2619,324 +3016,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3355,16 +3434,20 @@
     <text xml:space="preserve">The primary pump needs to be expensive!!
 </text>
   </threadedComment>
+  <threadedComment ref="H107" dT="2025-06-19T23:17:33.50" personId="{84112BF8-C915-7B4B-BE8E-B816F75B981C}" id="{6E7B8F31-3BA2-6E43-928D-71FCFDC70463}">
+    <text>The cost is multiplied by 0.5 since the
+ shipping included international shipping</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
-  <dimension ref="A1:Z124"/>
+  <dimension ref="A1:X124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="63" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="150" zoomScaleNormal="63" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U122" sqref="U122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3389,10 +3472,11 @@
     <col min="18" max="18" width="37.1640625" style="6" customWidth="1"/>
     <col min="19" max="19" width="81.1640625" style="6" customWidth="1"/>
     <col min="20" max="20" width="18.6640625" style="6" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="6"/>
+    <col min="21" max="21" width="16" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="10" customFormat="1" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="10" customFormat="1" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3453,8 +3537,11 @@
       <c r="T1" s="13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" s="11" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U1" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="11" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>10</v>
       </c>
@@ -3492,8 +3579,9 @@
       <c r="R2" s="17"/>
       <c r="S2" s="17"/>
       <c r="T2" s="17"/>
-    </row>
-    <row r="3" spans="1:20" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U2" s="6"/>
+    </row>
+    <row r="3" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>11</v>
       </c>
@@ -3544,15 +3632,18 @@
       <c r="Q3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="107" t="s">
+      <c r="R3" s="108" t="s">
         <v>141</v>
       </c>
-      <c r="S3" s="123" t="s">
+      <c r="S3" s="124" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="26"/>
-    </row>
-    <row r="4" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U3" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>12</v>
       </c>
@@ -3597,11 +3688,14 @@
       <c r="Q4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="107"/>
-      <c r="S4" s="123"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="124"/>
       <c r="T4" s="26"/>
-    </row>
-    <row r="5" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U4" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>13</v>
       </c>
@@ -3622,8 +3716,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="27">
-        <f>50*1000000</f>
-        <v>50000000</v>
+        <v>45000000</v>
       </c>
       <c r="I5" s="66"/>
       <c r="J5" s="24"/>
@@ -3632,23 +3725,26 @@
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
       <c r="O5" s="23">
-        <v>2009</v>
+        <v>2024</v>
       </c>
       <c r="P5" s="23" t="s">
         <v>72</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="R5" s="107" t="s">
-        <v>142</v>
-      </c>
-      <c r="S5" s="123" t="s">
-        <v>59</v>
+        <v>425</v>
+      </c>
+      <c r="R5" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>426</v>
       </c>
       <c r="T5" s="26"/>
-    </row>
-    <row r="6" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="76" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>14</v>
       </c>
@@ -3686,11 +3782,18 @@
       <c r="Q6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="107"/>
-      <c r="S6" s="123"/>
+      <c r="R6" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="S6" s="105" t="s">
+        <v>59</v>
+      </c>
       <c r="T6" s="26"/>
-    </row>
-    <row r="7" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>15</v>
       </c>
@@ -3738,8 +3841,11 @@
       <c r="T7" s="23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>20</v>
       </c>
@@ -3778,7 +3884,7 @@
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>21</v>
       </c>
@@ -3810,7 +3916,7 @@
       <c r="S9" s="5"/>
       <c r="T9" s="26"/>
     </row>
-    <row r="10" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32">
         <v>211</v>
       </c>
@@ -3842,7 +3948,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="26"/>
     </row>
-    <row r="11" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
         <v>211.1</v>
       </c>
@@ -3884,18 +3990,21 @@
       <c r="P11" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="119" t="s">
+      <c r="Q11" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="107" t="s">
+      <c r="R11" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="108" t="s">
+      <c r="S11" s="109" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="26"/>
-    </row>
-    <row r="12" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
         <v>211.2</v>
       </c>
@@ -3944,12 +4053,15 @@
       <c r="P12" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="119"/>
-      <c r="R12" s="107"/>
-      <c r="S12" s="109"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="110"/>
       <c r="T12" s="26"/>
-    </row>
-    <row r="13" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>211.3</v>
       </c>
@@ -3991,12 +4103,15 @@
       <c r="P13" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="119"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="109"/>
+      <c r="Q13" s="120"/>
+      <c r="R13" s="108"/>
+      <c r="S13" s="110"/>
       <c r="T13" s="26"/>
-    </row>
-    <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32">
         <v>212</v>
       </c>
@@ -4028,7 +4143,7 @@
       <c r="S14" s="26"/>
       <c r="T14" s="26"/>
     </row>
-    <row r="15" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36">
         <v>212.1</v>
       </c>
@@ -4069,18 +4184,21 @@
       <c r="P15" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="119" t="s">
+      <c r="Q15" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="107" t="s">
+      <c r="R15" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="108" t="s">
+      <c r="S15" s="109" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="26"/>
-    </row>
-    <row r="16" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>212.2</v>
       </c>
@@ -4122,12 +4240,15 @@
       <c r="P16" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="119"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="109"/>
+      <c r="Q16" s="120"/>
+      <c r="R16" s="108"/>
+      <c r="S16" s="110"/>
       <c r="T16" s="26"/>
-    </row>
-    <row r="17" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <v>212.3</v>
       </c>
@@ -4169,12 +4290,15 @@
       <c r="P17" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="119"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="109"/>
+      <c r="Q17" s="120"/>
+      <c r="R17" s="108"/>
+      <c r="S17" s="110"/>
       <c r="T17" s="26"/>
-    </row>
-    <row r="18" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36">
         <v>213</v>
       </c>
@@ -4206,7 +4330,7 @@
       <c r="S18" s="35"/>
       <c r="T18" s="26"/>
     </row>
-    <row r="19" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
         <v>213.1</v>
       </c>
@@ -4238,7 +4362,7 @@
       <c r="S19" s="35"/>
       <c r="T19" s="26"/>
     </row>
-    <row r="20" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <v>213.11</v>
       </c>
@@ -4280,18 +4404,21 @@
       <c r="P20" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q20" s="119" t="s">
+      <c r="Q20" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="107" t="s">
+      <c r="R20" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="S20" s="108" t="s">
+      <c r="S20" s="109" t="s">
         <v>84</v>
       </c>
       <c r="T20" s="26"/>
-    </row>
-    <row r="21" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U20" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>213.12</v>
       </c>
@@ -4333,12 +4460,15 @@
       <c r="P21" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q21" s="119"/>
-      <c r="R21" s="107"/>
-      <c r="S21" s="109"/>
+      <c r="Q21" s="120"/>
+      <c r="R21" s="108"/>
+      <c r="S21" s="110"/>
       <c r="T21" s="26"/>
-    </row>
-    <row r="22" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>213.13</v>
       </c>
@@ -4380,12 +4510,15 @@
       <c r="P22" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="119"/>
-      <c r="R22" s="107"/>
-      <c r="S22" s="109"/>
+      <c r="Q22" s="120"/>
+      <c r="R22" s="108"/>
+      <c r="S22" s="110"/>
       <c r="T22" s="26"/>
-    </row>
-    <row r="23" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U22" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36">
         <v>213.2</v>
       </c>
@@ -4417,7 +4550,7 @@
       <c r="S23" s="35"/>
       <c r="T23" s="26"/>
     </row>
-    <row r="24" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36">
         <v>213.21</v>
       </c>
@@ -4459,18 +4592,21 @@
       <c r="P24" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="119" t="s">
+      <c r="Q24" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="R24" s="107" t="s">
+      <c r="R24" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="S24" s="108" t="s">
+      <c r="S24" s="109" t="s">
         <v>84</v>
       </c>
       <c r="T24" s="26"/>
-    </row>
-    <row r="25" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U24" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="36">
         <v>213.22</v>
       </c>
@@ -4512,12 +4648,15 @@
       <c r="P25" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q25" s="119"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="109"/>
+      <c r="Q25" s="120"/>
+      <c r="R25" s="108"/>
+      <c r="S25" s="110"/>
       <c r="T25" s="26"/>
-    </row>
-    <row r="26" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U25" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36">
         <v>213.23</v>
       </c>
@@ -4559,12 +4698,15 @@
       <c r="P26" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="119"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="109"/>
+      <c r="Q26" s="120"/>
+      <c r="R26" s="108"/>
+      <c r="S26" s="110"/>
       <c r="T26" s="26"/>
-    </row>
-    <row r="27" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U26" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36">
         <v>214</v>
       </c>
@@ -4596,7 +4738,7 @@
       <c r="S27" s="26"/>
       <c r="T27" s="26"/>
     </row>
-    <row r="28" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36">
         <v>214.1</v>
       </c>
@@ -4628,7 +4770,7 @@
       <c r="S28" s="26"/>
       <c r="T28" s="26"/>
     </row>
-    <row r="29" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="36">
         <v>214.11</v>
       </c>
@@ -4660,7 +4802,7 @@
       <c r="S29" s="26"/>
       <c r="T29" s="26"/>
     </row>
-    <row r="30" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77">
         <v>214.11099999999999</v>
       </c>
@@ -4702,18 +4844,21 @@
       <c r="P30" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="130" t="s">
+      <c r="Q30" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="129" t="s">
+      <c r="R30" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="127" t="s">
+      <c r="S30" s="128" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="85"/>
-    </row>
-    <row r="31" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U30" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="77">
         <v>214.11199999999999</v>
       </c>
@@ -4755,12 +4900,15 @@
       <c r="P31" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="130"/>
-      <c r="R31" s="129"/>
-      <c r="S31" s="128"/>
+      <c r="Q31" s="131"/>
+      <c r="R31" s="130"/>
+      <c r="S31" s="129"/>
       <c r="T31" s="85"/>
-    </row>
-    <row r="32" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U31" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="77">
         <v>214.113</v>
       </c>
@@ -4802,12 +4950,15 @@
       <c r="P32" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="130"/>
-      <c r="R32" s="129"/>
-      <c r="S32" s="128"/>
+      <c r="Q32" s="131"/>
+      <c r="R32" s="130"/>
+      <c r="S32" s="129"/>
       <c r="T32" s="85"/>
-    </row>
-    <row r="33" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U32" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="36">
         <v>214.12</v>
       </c>
@@ -4839,7 +4990,7 @@
       <c r="S33" s="26"/>
       <c r="T33" s="26"/>
     </row>
-    <row r="34" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="77">
         <v>214.12100000000001</v>
       </c>
@@ -4881,18 +5032,21 @@
       <c r="P34" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="130" t="s">
+      <c r="Q34" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="R34" s="129" t="s">
+      <c r="R34" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="S34" s="127" t="s">
+      <c r="S34" s="128" t="s">
         <v>84</v>
       </c>
       <c r="T34" s="85"/>
-    </row>
-    <row r="35" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U34" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="77">
         <v>214.12200000000001</v>
       </c>
@@ -4934,12 +5088,15 @@
       <c r="P35" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q35" s="130"/>
-      <c r="R35" s="129"/>
-      <c r="S35" s="128"/>
+      <c r="Q35" s="131"/>
+      <c r="R35" s="130"/>
+      <c r="S35" s="129"/>
       <c r="T35" s="85"/>
-    </row>
-    <row r="36" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U35" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="77">
         <v>214.12299999999999</v>
       </c>
@@ -4981,12 +5138,15 @@
       <c r="P36" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q36" s="130"/>
-      <c r="R36" s="129"/>
-      <c r="S36" s="128"/>
+      <c r="Q36" s="131"/>
+      <c r="R36" s="130"/>
+      <c r="S36" s="129"/>
       <c r="T36" s="85"/>
-    </row>
-    <row r="37" spans="1:20" ht="30" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U36" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="36">
         <v>214.7</v>
       </c>
@@ -5018,7 +5178,7 @@
       <c r="S37" s="26"/>
       <c r="T37" s="26"/>
     </row>
-    <row r="38" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="36">
         <v>214.71</v>
       </c>
@@ -5050,7 +5210,7 @@
       <c r="S38" s="26"/>
       <c r="T38" s="26"/>
     </row>
-    <row r="39" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77">
         <v>214.71100000000001</v>
       </c>
@@ -5092,18 +5252,21 @@
       <c r="P39" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="130" t="s">
+      <c r="Q39" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="R39" s="129" t="s">
+      <c r="R39" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="S39" s="127" t="s">
+      <c r="S39" s="128" t="s">
         <v>84</v>
       </c>
       <c r="T39" s="85"/>
-    </row>
-    <row r="40" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U39" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="77">
         <v>214.71199999999999</v>
       </c>
@@ -5145,12 +5308,15 @@
       <c r="P40" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="Q40" s="130"/>
-      <c r="R40" s="129"/>
-      <c r="S40" s="128"/>
+      <c r="Q40" s="131"/>
+      <c r="R40" s="130"/>
+      <c r="S40" s="129"/>
       <c r="T40" s="85"/>
-    </row>
-    <row r="41" spans="1:20" s="86" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U40" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" s="86" customFormat="1" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="77">
         <v>214.71299999999999</v>
       </c>
@@ -5192,12 +5358,15 @@
       <c r="P41" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="130"/>
-      <c r="R41" s="129"/>
-      <c r="S41" s="128"/>
+      <c r="Q41" s="131"/>
+      <c r="R41" s="130"/>
+      <c r="S41" s="129"/>
       <c r="T41" s="85"/>
-    </row>
-    <row r="42" spans="1:20" ht="104" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U41" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="104" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="36">
         <v>214.72</v>
       </c>
@@ -5254,8 +5423,11 @@
         <v>159</v>
       </c>
       <c r="T42" s="26"/>
-    </row>
-    <row r="43" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U42" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="36">
         <v>215</v>
       </c>
@@ -5287,7 +5459,7 @@
       <c r="S43" s="39"/>
       <c r="T43" s="26"/>
     </row>
-    <row r="44" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="36">
         <v>215.1</v>
       </c>
@@ -5319,7 +5491,7 @@
       <c r="S44" s="39"/>
       <c r="T44" s="26"/>
     </row>
-    <row r="45" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="36">
         <v>215.11</v>
       </c>
@@ -5361,18 +5533,21 @@
       <c r="P45" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q45" s="119" t="s">
+      <c r="Q45" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="R45" s="107" t="s">
+      <c r="R45" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="S45" s="108" t="s">
+      <c r="S45" s="109" t="s">
         <v>84</v>
       </c>
       <c r="T45" s="26"/>
-    </row>
-    <row r="46" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U45" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="36">
         <v>215.12</v>
       </c>
@@ -5414,12 +5589,15 @@
       <c r="P46" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="119"/>
-      <c r="R46" s="107"/>
-      <c r="S46" s="109"/>
+      <c r="Q46" s="120"/>
+      <c r="R46" s="108"/>
+      <c r="S46" s="110"/>
       <c r="T46" s="26"/>
-    </row>
-    <row r="47" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U46" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36">
         <v>215.13</v>
       </c>
@@ -5461,12 +5639,15 @@
       <c r="P47" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="119"/>
-      <c r="R47" s="107"/>
-      <c r="S47" s="109"/>
+      <c r="Q47" s="120"/>
+      <c r="R47" s="108"/>
+      <c r="S47" s="110"/>
       <c r="T47" s="26"/>
-    </row>
-    <row r="48" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U47" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="36">
         <v>215.4</v>
       </c>
@@ -5498,7 +5679,7 @@
       <c r="S48" s="39"/>
       <c r="T48" s="26"/>
     </row>
-    <row r="49" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="36">
         <v>215.41</v>
       </c>
@@ -5540,18 +5721,21 @@
       <c r="P49" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q49" s="119" t="s">
+      <c r="Q49" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="R49" s="107" t="s">
+      <c r="R49" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="S49" s="108" t="s">
+      <c r="S49" s="109" t="s">
         <v>84</v>
       </c>
       <c r="T49" s="26"/>
-    </row>
-    <row r="50" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U49" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="36">
         <v>215.42</v>
       </c>
@@ -5593,12 +5777,15 @@
       <c r="P50" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q50" s="119"/>
-      <c r="R50" s="107"/>
-      <c r="S50" s="109"/>
+      <c r="Q50" s="120"/>
+      <c r="R50" s="108"/>
+      <c r="S50" s="110"/>
       <c r="T50" s="26"/>
-    </row>
-    <row r="51" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U50" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="36">
         <v>215.43</v>
       </c>
@@ -5640,12 +5827,15 @@
       <c r="P51" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Q51" s="119"/>
-      <c r="R51" s="107"/>
-      <c r="S51" s="109"/>
+      <c r="Q51" s="120"/>
+      <c r="R51" s="108"/>
+      <c r="S51" s="110"/>
       <c r="T51" s="26"/>
-    </row>
-    <row r="52" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U51" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>22</v>
       </c>
@@ -5677,7 +5867,7 @@
       <c r="S52" s="26"/>
       <c r="T52" s="26"/>
     </row>
-    <row r="53" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="36">
         <v>221</v>
       </c>
@@ -5709,7 +5899,7 @@
       <c r="S53" s="26"/>
       <c r="T53" s="26"/>
     </row>
-    <row r="54" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="36">
         <v>221.1</v>
       </c>
@@ -5741,7 +5931,7 @@
       <c r="S54" s="26"/>
       <c r="T54" s="26"/>
     </row>
-    <row r="55" spans="1:20" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="36">
         <v>221.11</v>
       </c>
@@ -5791,17 +5981,20 @@
       <c r="Q55" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="R55" s="124" t="s">
+      <c r="R55" s="125" t="s">
         <v>178</v>
       </c>
-      <c r="S55" s="110" t="s">
+      <c r="S55" s="111" t="s">
         <v>182</v>
       </c>
       <c r="T55" s="42" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U55" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="36">
         <v>221.12</v>
       </c>
@@ -5851,11 +6044,14 @@
       <c r="Q56" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="R56" s="125"/>
-      <c r="S56" s="111"/>
+      <c r="R56" s="126"/>
+      <c r="S56" s="112"/>
       <c r="T56" s="26"/>
-    </row>
-    <row r="57" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U56" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="36">
         <v>221.13</v>
       </c>
@@ -5908,13 +6104,16 @@
       <c r="Q57" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="R57" s="126"/>
-      <c r="S57" s="112"/>
+      <c r="R57" s="127"/>
+      <c r="S57" s="113"/>
       <c r="T57" s="42" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U57" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="36">
         <v>221.2</v>
       </c>
@@ -5946,7 +6145,7 @@
       <c r="S58" s="26"/>
       <c r="T58" s="26"/>
     </row>
-    <row r="59" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="36">
         <v>221.21</v>
       </c>
@@ -5978,7 +6177,7 @@
       <c r="S59" s="26"/>
       <c r="T59" s="26"/>
     </row>
-    <row r="60" spans="1:20" s="86" customFormat="1" ht="40" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" s="86" customFormat="1" ht="40" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="77">
         <v>221.21100000000001</v>
       </c>
@@ -6019,17 +6218,20 @@
       <c r="Q60" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="R60" s="113" t="s">
+      <c r="R60" s="114" t="s">
         <v>178</v>
       </c>
-      <c r="S60" s="116" t="s">
+      <c r="S60" s="117" t="s">
         <v>347</v>
       </c>
       <c r="T60" s="90" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" s="86" customFormat="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U60" s="86" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" s="86" customFormat="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="77">
         <v>221.21199999999999</v>
       </c>
@@ -6068,11 +6270,14 @@
       <c r="Q61" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="R61" s="114"/>
-      <c r="S61" s="117"/>
+      <c r="R61" s="115"/>
+      <c r="S61" s="118"/>
       <c r="T61" s="85"/>
-    </row>
-    <row r="62" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U61" s="86" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="77">
         <v>221.21299999999999</v>
       </c>
@@ -6126,11 +6331,14 @@
       <c r="Q62" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="R62" s="114"/>
-      <c r="S62" s="117"/>
+      <c r="R62" s="115"/>
+      <c r="S62" s="118"/>
       <c r="T62" s="85"/>
-    </row>
-    <row r="63" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U62" s="86" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="77">
         <v>221.214</v>
       </c>
@@ -6184,11 +6392,14 @@
       <c r="Q63" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="R63" s="115"/>
-      <c r="S63" s="118"/>
+      <c r="R63" s="116"/>
+      <c r="S63" s="119"/>
       <c r="T63" s="85"/>
-    </row>
-    <row r="64" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U63" s="86" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="77">
         <v>221.214</v>
       </c>
@@ -6252,8 +6463,11 @@
       <c r="R64" s="103"/>
       <c r="S64" s="104"/>
       <c r="T64" s="85"/>
-    </row>
-    <row r="65" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U64" s="86" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="36">
         <v>221.3</v>
       </c>
@@ -6283,7 +6497,7 @@
       <c r="S65" s="26"/>
       <c r="T65" s="26"/>
     </row>
-    <row r="66" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="36">
         <v>221.31</v>
       </c>
@@ -6340,15 +6554,18 @@
       <c r="Q66" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="R66" s="124" t="s">
+      <c r="R66" s="125" t="s">
         <v>178</v>
       </c>
-      <c r="S66" s="110" t="s">
+      <c r="S66" s="111" t="s">
         <v>182</v>
       </c>
       <c r="T66" s="26"/>
-    </row>
-    <row r="67" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U66" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="36">
         <v>221.31</v>
       </c>
@@ -6409,11 +6626,14 @@
       <c r="Q67" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="R67" s="125"/>
-      <c r="S67" s="111"/>
+      <c r="R67" s="126"/>
+      <c r="S67" s="112"/>
       <c r="T67" s="26"/>
-    </row>
-    <row r="68" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U67" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="36">
         <v>221.32</v>
       </c>
@@ -6441,11 +6661,11 @@
       <c r="O68" s="26"/>
       <c r="P68" s="26"/>
       <c r="Q68" s="42"/>
-      <c r="R68" s="125"/>
-      <c r="S68" s="111"/>
+      <c r="R68" s="126"/>
+      <c r="S68" s="112"/>
       <c r="T68" s="26"/>
     </row>
-    <row r="69" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="77">
         <v>221.321</v>
       </c>
@@ -6502,11 +6722,14 @@
       <c r="Q69" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="R69" s="125"/>
-      <c r="S69" s="111"/>
+      <c r="R69" s="126"/>
+      <c r="S69" s="112"/>
       <c r="T69" s="85"/>
-    </row>
-    <row r="70" spans="1:20" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="U69" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" s="86" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="77">
         <v>221.322</v>
       </c>
@@ -6559,11 +6782,14 @@
       <c r="Q70" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="R70" s="126"/>
-      <c r="S70" s="112"/>
+      <c r="R70" s="127"/>
+      <c r="S70" s="113"/>
       <c r="T70" s="85"/>
-    </row>
-    <row r="71" spans="1:20" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U70" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="36">
         <v>221.33</v>
       </c>
@@ -6615,8 +6841,11 @@
       </c>
       <c r="S71" s="75"/>
       <c r="T71" s="26"/>
-    </row>
-    <row r="72" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U71" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="36">
         <v>221.33</v>
       </c>
@@ -6666,8 +6895,11 @@
       <c r="R72" s="74"/>
       <c r="S72" s="75"/>
       <c r="T72" s="26"/>
-    </row>
-    <row r="73" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U72" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="36">
         <v>222</v>
       </c>
@@ -6698,7 +6930,7 @@
       <c r="S73" s="26"/>
       <c r="T73" s="26"/>
     </row>
-    <row r="74" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="36">
         <v>222.1</v>
       </c>
@@ -6736,7 +6968,7 @@
       <c r="S74" s="26"/>
       <c r="T74" s="26"/>
     </row>
-    <row r="75" spans="1:20" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>222.11</v>
       </c>
@@ -6785,15 +7017,18 @@
       <c r="Q75" s="42" t="s">
         <v>349</v>
       </c>
-      <c r="R75" s="105" t="s">
+      <c r="R75" s="106" t="s">
         <v>348</v>
       </c>
-      <c r="S75" s="121" t="s">
+      <c r="S75" s="122" t="s">
         <v>350</v>
       </c>
-      <c r="T75" s="105"/>
-    </row>
-    <row r="76" spans="1:20" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T75" s="106"/>
+      <c r="U75" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>222.12</v>
       </c>
@@ -6841,11 +7076,14 @@
       <c r="Q76" s="42" t="s">
         <v>343</v>
       </c>
-      <c r="R76" s="106"/>
-      <c r="S76" s="122"/>
-      <c r="T76" s="106"/>
-    </row>
-    <row r="77" spans="1:20" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R76" s="107"/>
+      <c r="S76" s="123"/>
+      <c r="T76" s="107"/>
+      <c r="U76" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" ht="76" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>222.13</v>
       </c>
@@ -6898,8 +7136,11 @@
       </c>
       <c r="S77" s="94"/>
       <c r="T77" s="93"/>
-    </row>
-    <row r="78" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U77" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="36">
         <v>222.2</v>
       </c>
@@ -6946,8 +7187,11 @@
       </c>
       <c r="S78" s="26"/>
       <c r="T78" s="26"/>
-    </row>
-    <row r="79" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U78" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="36">
         <v>222.3</v>
       </c>
@@ -6979,7 +7223,7 @@
       <c r="S79" s="26"/>
       <c r="T79" s="26"/>
     </row>
-    <row r="80" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="36">
         <v>222.31</v>
       </c>
@@ -7032,8 +7276,11 @@
       </c>
       <c r="S80" s="26"/>
       <c r="T80" s="26"/>
-    </row>
-    <row r="81" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U80" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="36">
         <v>222.31</v>
       </c>
@@ -7093,8 +7340,11 @@
       </c>
       <c r="S81" s="26"/>
       <c r="T81" s="26"/>
-    </row>
-    <row r="82" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U81" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="36">
         <v>222.32</v>
       </c>
@@ -7147,8 +7397,11 @@
       </c>
       <c r="S82" s="26"/>
       <c r="T82" s="26"/>
-    </row>
-    <row r="83" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U82" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="36">
         <v>222.32</v>
       </c>
@@ -7208,8 +7461,11 @@
       </c>
       <c r="S83" s="26"/>
       <c r="T83" s="26"/>
-    </row>
-    <row r="84" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U83" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="36">
         <v>223</v>
       </c>
@@ -7241,7 +7497,7 @@
       <c r="S84" s="26"/>
       <c r="T84" s="26"/>
     </row>
-    <row r="85" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="36">
         <v>223.2</v>
       </c>
@@ -7273,7 +7529,7 @@
       <c r="S85" s="26"/>
       <c r="T85" s="26"/>
     </row>
-    <row r="86" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="36">
         <v>223.21</v>
       </c>
@@ -7326,8 +7582,11 @@
       <c r="R86" s="26"/>
       <c r="S86" s="26"/>
       <c r="T86" s="26"/>
-    </row>
-    <row r="87" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U86" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="36">
         <v>223.22</v>
       </c>
@@ -7380,8 +7639,11 @@
       <c r="R87" s="26"/>
       <c r="S87" s="26"/>
       <c r="T87" s="26"/>
-    </row>
-    <row r="88" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U87" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="36">
         <v>226</v>
       </c>
@@ -7423,8 +7685,11 @@
       <c r="R88" s="26"/>
       <c r="S88" s="26"/>
       <c r="T88" s="26"/>
-    </row>
-    <row r="89" spans="1:20" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U88" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="36">
         <v>227</v>
       </c>
@@ -7473,8 +7738,11 @@
       <c r="R89" s="26"/>
       <c r="S89" s="26"/>
       <c r="T89" s="26"/>
-    </row>
-    <row r="90" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U89" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="36">
         <v>228</v>
       </c>
@@ -7516,8 +7784,11 @@
       <c r="R90" s="26"/>
       <c r="S90" s="26"/>
       <c r="T90" s="26"/>
-    </row>
-    <row r="91" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U90" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="21">
         <v>23</v>
       </c>
@@ -7549,7 +7820,7 @@
       <c r="S91" s="26"/>
       <c r="T91" s="26"/>
     </row>
-    <row r="92" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="36">
         <v>232</v>
       </c>
@@ -7581,7 +7852,7 @@
       <c r="S92" s="26"/>
       <c r="T92" s="26"/>
     </row>
-    <row r="93" spans="1:20" ht="211" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="211" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="36">
         <v>232.1</v>
       </c>
@@ -7635,8 +7906,11 @@
       </c>
       <c r="S93" s="26"/>
       <c r="T93" s="26"/>
-    </row>
-    <row r="94" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U93" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="21">
         <v>24</v>
       </c>
@@ -7668,7 +7942,7 @@
       <c r="S94" s="26"/>
       <c r="T94" s="26"/>
     </row>
-    <row r="95" spans="1:20" ht="121" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" ht="121" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="21">
         <v>246</v>
       </c>
@@ -7723,8 +7997,11 @@
       </c>
       <c r="S95" s="26"/>
       <c r="T95" s="26"/>
-    </row>
-    <row r="96" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U95" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="21">
         <v>25</v>
       </c>
@@ -7756,7 +8033,7 @@
       <c r="S96" s="26"/>
       <c r="T96" s="26"/>
     </row>
-    <row r="97" spans="1:26" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="36">
         <v>251</v>
       </c>
@@ -7795,16 +8072,19 @@
       <c r="P97" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q97" s="105" t="s">
+      <c r="Q97" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="R97" s="105" t="s">
+      <c r="R97" s="106" t="s">
         <v>383</v>
       </c>
       <c r="S97" s="26"/>
       <c r="T97" s="26"/>
-    </row>
-    <row r="98" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U97" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="36">
         <v>252</v>
       </c>
@@ -7843,12 +8123,15 @@
       <c r="P98" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q98" s="120"/>
-      <c r="R98" s="120"/>
+      <c r="Q98" s="121"/>
+      <c r="R98" s="121"/>
       <c r="S98" s="26"/>
       <c r="T98" s="26"/>
-    </row>
-    <row r="99" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U98" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="36">
         <v>253</v>
       </c>
@@ -7889,12 +8172,15 @@
       <c r="P99" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q99" s="120"/>
-      <c r="R99" s="120"/>
+      <c r="Q99" s="121"/>
+      <c r="R99" s="121"/>
       <c r="S99" s="26"/>
       <c r="T99" s="26"/>
-    </row>
-    <row r="100" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U99" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="36">
         <v>254</v>
       </c>
@@ -7937,12 +8223,15 @@
       <c r="P100" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q100" s="120"/>
-      <c r="R100" s="120"/>
+      <c r="Q100" s="121"/>
+      <c r="R100" s="121"/>
       <c r="S100" s="26"/>
       <c r="T100" s="26"/>
-    </row>
-    <row r="101" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U100" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="36">
         <v>254</v>
       </c>
@@ -7992,12 +8281,15 @@
       <c r="P101" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q101" s="106"/>
-      <c r="R101" s="106"/>
+      <c r="Q101" s="107"/>
+      <c r="R101" s="107"/>
       <c r="S101" s="26"/>
       <c r="T101" s="26"/>
-    </row>
-    <row r="102" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U101" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="21">
         <v>26</v>
       </c>
@@ -8040,8 +8332,11 @@
       </c>
       <c r="S102" s="26"/>
       <c r="T102" s="26"/>
-    </row>
-    <row r="103" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U102" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29">
         <v>30</v>
       </c>
@@ -8080,7 +8375,7 @@
       <c r="S103" s="29"/>
       <c r="T103" s="29"/>
     </row>
-    <row r="104" spans="1:26" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29">
         <v>31</v>
       </c>
@@ -8111,7 +8406,7 @@
       <c r="S104" s="29"/>
       <c r="T104" s="29"/>
     </row>
-    <row r="105" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="29">
         <v>32</v>
       </c>
@@ -8142,7 +8437,7 @@
       <c r="S105" s="29"/>
       <c r="T105" s="29"/>
     </row>
-    <row r="106" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="21">
         <v>33</v>
       </c>
@@ -8178,20 +8473,20 @@
       <c r="P106" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="Q106" s="131" t="s">
+      <c r="Q106" s="132" t="s">
         <v>374</v>
       </c>
       <c r="R106" s="24"/>
       <c r="S106" s="24"/>
       <c r="T106" s="24"/>
-      <c r="U106" s="12"/>
+      <c r="U106" s="6" t="s">
+        <v>421</v>
+      </c>
       <c r="V106" s="12"/>
       <c r="W106" s="12"/>
       <c r="X106" s="12"/>
-      <c r="Y106" s="12"/>
-      <c r="Z106" s="12"/>
-    </row>
-    <row r="107" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="21">
         <v>34</v>
       </c>
@@ -8212,8 +8507,8 @@
       <c r="F107" s="19"/>
       <c r="G107" s="19"/>
       <c r="H107" s="24">
-        <f>MARVEL_Cost!C62</f>
-        <v>1665282.7999999998</v>
+        <f>0.5*MARVEL_Cost!C62</f>
+        <v>832641.39999999991</v>
       </c>
       <c r="I107" s="66"/>
       <c r="J107" s="24"/>
@@ -8227,18 +8522,18 @@
       <c r="P107" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="Q107" s="132"/>
+      <c r="Q107" s="133"/>
       <c r="R107" s="24"/>
       <c r="S107" s="24"/>
       <c r="T107" s="24"/>
-      <c r="U107" s="12"/>
+      <c r="U107" s="6" t="s">
+        <v>421</v>
+      </c>
       <c r="V107" s="12"/>
       <c r="W107" s="12"/>
       <c r="X107" s="12"/>
-      <c r="Y107" s="12"/>
-      <c r="Z107" s="12"/>
-    </row>
-    <row r="108" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="21">
         <v>35</v>
       </c>
@@ -8274,13 +8569,15 @@
       <c r="P108" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="Q108" s="132"/>
+      <c r="Q108" s="133"/>
       <c r="R108" s="26"/>
       <c r="S108" s="26"/>
       <c r="T108" s="26"/>
-      <c r="U108" s="12"/>
-    </row>
-    <row r="109" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U108" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="21">
         <v>36</v>
       </c>
@@ -8316,13 +8613,15 @@
       <c r="P109" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="Q109" s="133"/>
+      <c r="Q109" s="134"/>
       <c r="R109" s="26"/>
       <c r="S109" s="26"/>
       <c r="T109" s="26"/>
-      <c r="U109" s="12"/>
-    </row>
-    <row r="110" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U109" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="21">
         <v>40</v>
       </c>
@@ -8355,7 +8654,7 @@
       <c r="T110" s="26"/>
       <c r="U110" s="12"/>
     </row>
-    <row r="111" spans="1:26" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="21">
         <v>41</v>
       </c>
@@ -8398,9 +8697,11 @@
         <v>418</v>
       </c>
       <c r="T111" s="26"/>
-      <c r="U111" s="12"/>
-    </row>
-    <row r="112" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U111" s="12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="29">
         <v>60</v>
       </c>
@@ -8579,7 +8880,9 @@
       </c>
       <c r="S116" s="26"/>
       <c r="T116" s="26"/>
-      <c r="U116" s="12"/>
+      <c r="U116" s="12" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="117" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="36">
@@ -8632,7 +8935,9 @@
       </c>
       <c r="S117" s="26"/>
       <c r="T117" s="26"/>
-      <c r="U117" s="12"/>
+      <c r="U117" s="12" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="118" spans="1:21" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="36">
@@ -8681,7 +8986,9 @@
       </c>
       <c r="S118" s="26"/>
       <c r="T118" s="26"/>
-      <c r="U118" s="12"/>
+      <c r="U118" s="12" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="119" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="21">
@@ -8764,7 +9071,9 @@
       </c>
       <c r="S120" s="26"/>
       <c r="T120" s="26"/>
-      <c r="U120" s="12"/>
+      <c r="U120" s="12" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="121" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="16">
@@ -8845,6 +9154,9 @@
       </c>
       <c r="S122" s="26"/>
       <c r="T122" s="26"/>
+      <c r="U122" s="6" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="123" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="21">
@@ -8877,6 +9189,9 @@
       <c r="R123" s="26"/>
       <c r="S123" s="26"/>
       <c r="T123" s="26"/>
+      <c r="U123" s="6" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="124" spans="1:21" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="21">
@@ -8923,16 +9238,17 @@
       <c r="R124" s="26"/>
       <c r="S124" s="26"/>
       <c r="T124" s="26"/>
+      <c r="U124" s="6" t="s">
+        <v>420</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="41">
     <mergeCell ref="Q106:Q109"/>
     <mergeCell ref="Q39:Q41"/>
     <mergeCell ref="Q45:Q47"/>
     <mergeCell ref="Q49:Q51"/>
     <mergeCell ref="Q97:Q101"/>
-    <mergeCell ref="R24:R26"/>
-    <mergeCell ref="R30:R32"/>
     <mergeCell ref="R34:R36"/>
     <mergeCell ref="R39:R41"/>
     <mergeCell ref="Q20:Q22"/>
@@ -8944,8 +9260,6 @@
     <mergeCell ref="S75:S76"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
     <mergeCell ref="S20:S22"/>
     <mergeCell ref="R66:R70"/>
     <mergeCell ref="S24:S26"/>
@@ -8955,6 +9269,8 @@
     <mergeCell ref="S55:S57"/>
     <mergeCell ref="S39:S41"/>
     <mergeCell ref="R20:R22"/>
+    <mergeCell ref="R24:R26"/>
+    <mergeCell ref="R30:R32"/>
     <mergeCell ref="Q15:Q17"/>
     <mergeCell ref="Q11:Q13"/>
     <mergeCell ref="R11:R13"/>
@@ -8970,162 +9286,148 @@
     <mergeCell ref="R60:R63"/>
     <mergeCell ref="S60:S63"/>
   </mergeCells>
-  <conditionalFormatting sqref="A75:F77 L97:T97 L98:P98 S98:T102 I99:P99 A102:R102 A112:T115 A116:H117 A118:J118 A119:T119 S120:T120 A121:T121 S122:T122 A123:T124 R106:T111 Q110:Q111">
-    <cfRule type="expression" dxfId="80" priority="137">
-      <formula>$B75=3</formula>
+  <conditionalFormatting sqref="A97:H99">
+    <cfRule type="expression" dxfId="84" priority="108">
+      <formula>$B97=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="138">
-      <formula>$B75=2</formula>
+    <cfRule type="expression" dxfId="83" priority="107">
+      <formula>$B97&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="139">
-      <formula>$B75&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="140">
-      <formula>$B75=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97:H99">
-    <cfRule type="expression" dxfId="76" priority="101">
-      <formula>$B97=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="102">
+    <cfRule type="expression" dxfId="82" priority="106">
       <formula>$B97=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="103">
-      <formula>$B97&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="104">
-      <formula>$B97=0</formula>
+    <cfRule type="expression" dxfId="81" priority="105">
+      <formula>$B97=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:I83">
-    <cfRule type="expression" dxfId="72" priority="125">
+    <cfRule type="expression" dxfId="80" priority="129">
       <formula>$B79=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="126">
+    <cfRule type="expression" dxfId="79" priority="130">
       <formula>$B79=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="127">
+    <cfRule type="expression" dxfId="78" priority="131">
       <formula>$B79&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="128">
+    <cfRule type="expression" dxfId="77" priority="132">
       <formula>$B79=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:P101">
-    <cfRule type="expression" dxfId="68" priority="85">
-      <formula>$B100=3</formula>
+    <cfRule type="expression" dxfId="76" priority="92">
+      <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="86">
+    <cfRule type="expression" dxfId="75" priority="91">
+      <formula>$B100&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="90">
       <formula>$B100=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="87">
-      <formula>$B100&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="88">
-      <formula>$B100=0</formula>
+    <cfRule type="expression" dxfId="73" priority="89">
+      <formula>$B100=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104:P111">
-    <cfRule type="expression" dxfId="64" priority="33">
+    <cfRule type="expression" dxfId="72" priority="40">
+      <formula>$B104=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="37">
       <formula>$B104=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="34">
+    <cfRule type="expression" dxfId="70" priority="38">
       <formula>$B104=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="35">
+    <cfRule type="expression" dxfId="69" priority="39">
       <formula>$B104&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="36">
-      <formula>$B104=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A120:Q120">
-    <cfRule type="expression" dxfId="60" priority="5">
+    <cfRule type="expression" dxfId="68" priority="12">
+      <formula>$B120=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="9">
       <formula>$B120=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="6">
+    <cfRule type="expression" dxfId="66" priority="10">
       <formula>$B120=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="7">
+    <cfRule type="expression" dxfId="65" priority="11">
       <formula>$B120&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="8">
-      <formula>$B120=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A122:Q122">
-    <cfRule type="expression" dxfId="56" priority="1">
+    <cfRule type="expression" dxfId="64" priority="5">
       <formula>$B122=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="2">
+    <cfRule type="expression" dxfId="63" priority="6">
       <formula>$B122=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="3">
+    <cfRule type="expression" dxfId="62" priority="7">
       <formula>$B122&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="4">
+    <cfRule type="expression" dxfId="61" priority="8">
       <formula>$B122=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:S74">
-    <cfRule type="expression" dxfId="52" priority="141">
+    <cfRule type="expression" dxfId="60" priority="148">
+      <formula>$B74=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="147">
+      <formula>$B74&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="146">
+      <formula>$B74=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="145">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="142">
-      <formula>$B74=2</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:T4 A5:R6 T5:T6 A7:T73 A75:F77 L97:T97 L98:P98 S98:T102 I99:P99 A102:R102 R106:T111 Q110:Q111 A112:T115 A116:H117 A118:J118 A119:T119 S120:T120 A121:T121 S122:T122 A123:T124">
+    <cfRule type="expression" dxfId="56" priority="143">
+      <formula>$B1&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="143">
-      <formula>$B74&lt;2</formula>
+    <cfRule type="expression" dxfId="55" priority="142">
+      <formula>$B1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="144">
-      <formula>$B74=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:T73 T74:T77 H75:R75 H76:Q76 G77:Q77 A78:T78 K79:T79 S80:T83">
-    <cfRule type="expression" dxfId="48" priority="145">
+    <cfRule type="expression" dxfId="54" priority="141">
       <formula>$B1=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="146">
-      <formula>$B1=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="147">
-      <formula>$B1&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="148">
+    <cfRule type="expression" dxfId="53" priority="144">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84:T96">
-    <cfRule type="expression" dxfId="44" priority="105">
+    <cfRule type="expression" dxfId="52" priority="109">
       <formula>$B84=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="106">
-      <formula>$B84=2</formula>
+    <cfRule type="expression" dxfId="51" priority="112">
+      <formula>$B84=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="107">
+    <cfRule type="expression" dxfId="50" priority="111">
       <formula>$B84&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="108">
-      <formula>$B84=0</formula>
+    <cfRule type="expression" dxfId="49" priority="110">
+      <formula>$B84=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:T103">
-    <cfRule type="expression" dxfId="40" priority="69">
+    <cfRule type="expression" dxfId="48" priority="76">
+      <formula>$B103=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="74">
+      <formula>$B103=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="73">
       <formula>$B103=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="70">
-      <formula>$B103=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="71">
+    <cfRule type="expression" dxfId="45" priority="75">
       <formula>$B103&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="72">
-      <formula>$B103=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D124">
-    <cfRule type="colorScale" priority="197">
+    <cfRule type="colorScale" priority="201">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9135,141 +9437,169 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G75:G76">
-    <cfRule type="expression" dxfId="36" priority="133">
+    <cfRule type="expression" dxfId="44" priority="137">
       <formula>$B75=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="134">
+    <cfRule type="expression" dxfId="43" priority="138">
       <formula>$B75=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="135">
+    <cfRule type="expression" dxfId="42" priority="139">
       <formula>$B75&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="136">
+    <cfRule type="expression" dxfId="41" priority="140">
       <formula>$B75=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I116:J117">
-    <cfRule type="expression" dxfId="32" priority="17">
-      <formula>$B117=3</formula>
+    <cfRule type="expression" dxfId="40" priority="24">
+      <formula>$B117=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="18">
+    <cfRule type="expression" dxfId="39" priority="23">
+      <formula>$B117&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>$B117=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="19">
-      <formula>$B117&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="20">
-      <formula>$B117=0</formula>
+    <cfRule type="expression" dxfId="37" priority="21">
+      <formula>$B117=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I97:K98">
-    <cfRule type="expression" dxfId="28" priority="97">
-      <formula>$B97=3</formula>
+    <cfRule type="expression" dxfId="36" priority="103">
+      <formula>$B97&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="98">
+    <cfRule type="expression" dxfId="35" priority="104">
+      <formula>$B97=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="102">
       <formula>$B97=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="99">
-      <formula>$B97&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="100">
-      <formula>$B97=0</formula>
+    <cfRule type="expression" dxfId="33" priority="101">
+      <formula>$B97=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J79 O103">
-    <cfRule type="expression" dxfId="24" priority="155">
-      <formula>$B80=2</formula>
+    <cfRule type="expression" dxfId="32" priority="161">
+      <formula>$B80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="156">
+    <cfRule type="expression" dxfId="31" priority="160">
       <formula>$B80&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="157">
-      <formula>$B80=0</formula>
+    <cfRule type="expression" dxfId="30" priority="159">
+      <formula>$B80=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K80:Q83">
-    <cfRule type="expression" dxfId="21" priority="121">
+    <cfRule type="expression" dxfId="29" priority="125">
       <formula>$B80=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="122">
+    <cfRule type="expression" dxfId="28" priority="126">
       <formula>$B80=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="123">
+    <cfRule type="expression" dxfId="27" priority="127">
       <formula>$B80&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="124">
+    <cfRule type="expression" dxfId="26" priority="128">
       <formula>$B80=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K116:Q118 S116:T118">
-    <cfRule type="expression" dxfId="17" priority="9">
-      <formula>$B116=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="25" priority="14">
       <formula>$B116=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="24" priority="15">
       <formula>$B116&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="13">
+      <formula>$B116=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K116:Q118">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="22" priority="16">
       <formula>$B116=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O103 J79">
-    <cfRule type="expression" dxfId="13" priority="154">
+    <cfRule type="expression" dxfId="21" priority="158">
       <formula>$B80=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q106">
-    <cfRule type="expression" dxfId="12" priority="81">
+    <cfRule type="expression" dxfId="20" priority="88">
+      <formula>$B106=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="85">
       <formula>$B106=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="82">
-      <formula>$B106=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="83">
+    <cfRule type="expression" dxfId="18" priority="87">
       <formula>$B106&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="84">
-      <formula>$B106=0</formula>
+    <cfRule type="expression" dxfId="17" priority="86">
+      <formula>$B106=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q104:T105">
-    <cfRule type="expression" dxfId="8" priority="41">
+    <cfRule type="expression" dxfId="16" priority="48">
+      <formula>$B104=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="47">
+      <formula>$B104&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="46">
+      <formula>$B104=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="45">
       <formula>$B104=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="42">
-      <formula>$B104=2</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S5">
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="43">
-      <formula>$B104&lt;2</formula>
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="44">
-      <formula>$B104=0</formula>
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>$B5&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>$B5=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S75">
-    <cfRule type="expression" dxfId="4" priority="162">
-      <formula>$B74=3</formula>
+  <conditionalFormatting sqref="S6 S75">
+    <cfRule type="expression" dxfId="8" priority="166">
+      <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="163">
-      <formula>$B74=2</formula>
+    <cfRule type="expression" dxfId="7" priority="167">
+      <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="164">
-      <formula>$B74&lt;2</formula>
+    <cfRule type="expression" dxfId="6" priority="168">
+      <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="165">
-      <formula>$B74=0</formula>
+    <cfRule type="expression" dxfId="5" priority="169">
+      <formula>$B5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S116:T118">
-    <cfRule type="expression" dxfId="0" priority="28">
+    <cfRule type="expression" dxfId="4" priority="32">
       <formula>$B116=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="10">
+  <conditionalFormatting sqref="T74:T77 H75:R75 H76:Q76 G77:Q77 A78:T78 K79:T79 S80:T83">
+    <cfRule type="expression" dxfId="3" priority="150">
+      <formula>$B74=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="151">
+      <formula>$B74&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="152">
+      <formula>$B74=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="149">
+      <formula>$B74=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="11">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O105:O124 O125:P132 O2:O103" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
       <formula1>1950</formula1>
       <formula2>2025</formula2>
@@ -9303,6 +9633,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J124" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
       <formula1>"$/MWeHour,$/FTE, $/acres, $/MWe, $/m^3, $/MWt, $/Kg, $/Drum, $/(kg.sec), $/SWU, unitless"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U124" xr:uid="{8C851931-DD22-6940-94BD-3E222B1E11BE}">
+      <formula1>"No Learning, Onsite Learning, Factory Primary Structure, Factory Drums, Factory Other, Licensing Learning"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="S3" r:id="rId1" xr:uid="{BA0D9C81-F547-414C-A28F-25DA56C7D1AB}"/>
@@ -9332,20 +9665,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="136" t="s">
+      <c r="C1" s="137" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="134"/>
-      <c r="B2" s="135"/>
-      <c r="C2" s="137"/>
+      <c r="A2" s="135"/>
+      <c r="B2" s="136"/>
+      <c r="C2" s="138"/>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="62">
@@ -10253,12 +10586,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="139" t="s">
         <v>243</v>
       </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
-      <c r="D2" s="140"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="141"/>
     </row>
     <row r="3" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
@@ -10315,12 +10648,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="138" t="s">
+      <c r="A7" s="139" t="s">
         <v>252</v>
       </c>
-      <c r="B7" s="139"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="140"/>
+      <c r="B7" s="140"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="141"/>
     </row>
     <row r="8" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
@@ -10379,12 +10712,12 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="138" t="s">
+      <c r="A12" s="139" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="140"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="141"/>
     </row>
     <row r="13" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
@@ -10483,12 +10816,12 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="138" t="s">
+      <c r="A20" s="139" t="s">
         <v>275</v>
       </c>
-      <c r="B20" s="139"/>
-      <c r="C20" s="139"/>
-      <c r="D20" s="140"/>
+      <c r="B20" s="140"/>
+      <c r="C20" s="140"/>
+      <c r="D20" s="141"/>
     </row>
     <row r="21" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="54" t="s">
@@ -10617,12 +10950,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="138" t="s">
+      <c r="A30" s="139" t="s">
         <v>288</v>
       </c>
-      <c r="B30" s="139"/>
-      <c r="C30" s="139"/>
-      <c r="D30" s="140"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="140"/>
+      <c r="D30" s="141"/>
     </row>
     <row r="31" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
@@ -10697,12 +11030,12 @@
       <c r="D36" s="60"/>
     </row>
     <row r="37" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="138" t="s">
+      <c r="A37" s="139" t="s">
         <v>295</v>
       </c>
-      <c r="B37" s="139"/>
-      <c r="C37" s="139"/>
-      <c r="D37" s="140"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="140"/>
+      <c r="D37" s="141"/>
     </row>
     <row r="38" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="54" t="s">
@@ -10789,12 +11122,12 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="138" t="s">
+      <c r="A44" s="139" t="s">
         <v>308</v>
       </c>
-      <c r="B44" s="139"/>
-      <c r="C44" s="139"/>
-      <c r="D44" s="140"/>
+      <c r="B44" s="140"/>
+      <c r="C44" s="140"/>
+      <c r="D44" s="141"/>
     </row>
     <row r="45" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
@@ -10811,12 +11144,12 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="138" t="s">
+      <c r="A46" s="139" t="s">
         <v>311</v>
       </c>
-      <c r="B46" s="139"/>
-      <c r="C46" s="139"/>
-      <c r="D46" s="140"/>
+      <c r="B46" s="140"/>
+      <c r="C46" s="140"/>
+      <c r="D46" s="141"/>
     </row>
     <row r="47" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="54" t="s">
@@ -10861,12 +11194,12 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="138" t="s">
+      <c r="A50" s="139" t="s">
         <v>318</v>
       </c>
-      <c r="B50" s="139"/>
-      <c r="C50" s="139"/>
-      <c r="D50" s="140"/>
+      <c r="B50" s="140"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="141"/>
     </row>
     <row r="51" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="54" t="s">
@@ -12039,19 +12372,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358A137-1626-9343-A399-452BA3D3C6F7}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="100" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="100" t="s">
         <v>395</v>
       </c>
@@ -12059,7 +12392,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>394</v>
       </c>
@@ -12068,7 +12401,7 @@
         <v>6.5389932052543287E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>404</v>
       </c>
@@ -12076,7 +12409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>405</v>
       </c>
@@ -12084,7 +12417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>406</v>
       </c>
@@ -12092,7 +12425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>407</v>
       </c>
@@ -12100,7 +12433,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>399</v>
       </c>
@@ -12108,7 +12441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>408</v>
       </c>
@@ -12116,7 +12449,78 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>428</v>
+      </c>
+      <c r="B9">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="142" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="142"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="B12">
+        <v>0.6</v>
+      </c>
+      <c r="C12" s="142"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="86" t="s">
+        <v>423</v>
+      </c>
+      <c r="B13">
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="142"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="142"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C10:C14"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:A14" xr:uid="{CF33C35E-6228-1344-B339-BF1C0841C758}">
+      <formula1>"No Learning, Onsite Learning, Factory Primary Structure, Factory Drums, Factory Other, Licensing Learning"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Add source and rationale on A78 implementation
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\mouse\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCF7DC-4886-46DD-8BCA-0D9D4355AFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224B1060-DDF9-48E2-8346-63E5471A3B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="491">
   <si>
     <t>Account</t>
   </si>
@@ -1834,6 +1834,13 @@
   <si>
     <t>Implemented on the python side. 
 Chosen over default due to uncertainty in compressor Pressure Ratio changes based on reactor TH</t>
+  </si>
+  <si>
+    <t>Implemented on non_direct_cost.py
+The cost is scaled as a fraction of CAPEX (15%)</t>
+  </si>
+  <si>
+    <t>Venneri, (2023) and INL/EXT-21-63067</t>
   </si>
 </sst>
 </file>
@@ -3638,10 +3645,10 @@
   <dimension ref="A1:AH141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="15" ySplit="1" topLeftCell="R78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="15" ySplit="1" topLeftCell="Q132" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A86" sqref="A86"/>
+      <selection pane="bottomRight" activeCell="Q137" sqref="Q137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -13750,7 +13757,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="136" spans="1:31">
+    <row r="136" spans="1:31" ht="25.5">
       <c r="A136" s="39">
         <v>75</v>
       </c>
@@ -13777,8 +13784,12 @@
       <c r="N136" s="51"/>
       <c r="O136" s="68"/>
       <c r="P136" s="51"/>
-      <c r="Q136" s="61"/>
-      <c r="R136" s="61"/>
+      <c r="Q136" s="61" t="s">
+        <v>490</v>
+      </c>
+      <c r="R136" s="61" t="s">
+        <v>490</v>
+      </c>
       <c r="S136" s="51"/>
       <c r="T136" s="51"/>
       <c r="U136" s="80"/>
@@ -13830,7 +13841,9 @@
       <c r="Q137" s="61"/>
       <c r="R137" s="61"/>
       <c r="S137" s="51"/>
-      <c r="T137" s="51"/>
+      <c r="T137" s="61" t="s">
+        <v>489</v>
+      </c>
       <c r="U137" s="80"/>
       <c r="V137" s="84"/>
       <c r="W137" s="84"/>

</xml_diff>

<commit_message>
Separate A75 to subaccounts to categorize costs of component replacements
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\mouse\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF79DDA8-DC2A-463C-9C57-49F346901E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363A84B1-8632-46B7-A238-8F8278EE471C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Economics Parameters" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Database'!$A$1:$Z$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Database'!$A$1:$Z$157</definedName>
     <definedName name="CRF">#REF!</definedName>
     <definedName name="DiscountRate">#REF!</definedName>
     <definedName name="FacilityLifetime">#REF!</definedName>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="518">
   <si>
     <t>Account</t>
   </si>
@@ -1905,6 +1905,24 @@
   </si>
   <si>
     <t>Integrated Heat Transfer Vessel Mass</t>
+  </si>
+  <si>
+    <t>Annualized Vessel Replacements</t>
+  </si>
+  <si>
+    <t>Annualized Moderator Replacements</t>
+  </si>
+  <si>
+    <t>Annualized Reflector Replacements</t>
+  </si>
+  <si>
+    <t>Annualized Reactivity Control Replacements</t>
+  </si>
+  <si>
+    <t>Annualized Integrated Heat Transfer System Replacements</t>
+  </si>
+  <si>
+    <t>Annualized Misc. Replacements</t>
   </si>
 </sst>
 </file>
@@ -2318,7 +2336,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2616,6 +2634,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3831,10 +3852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
-  <dimension ref="A1:AH151"/>
+  <dimension ref="A1:AH157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K103" sqref="K103"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -12020,7 +12041,7 @@
         <v>227</v>
       </c>
       <c r="B108" s="40">
-        <f t="shared" ref="B108:B151" si="44">IF(ISNUMBER(A108),
+        <f t="shared" ref="B108:B157" si="44">IF(ISNUMBER(A108),
     IF(AND(A108=INT(A108), MOD(A108, 10) = 0), 0,
         IF(AND(A108=INT(A108), LEN(A108)=2), 1,
             IF(AND(A108=INT(A108), LEN(A108)=3), 2,
@@ -12034,7 +12055,7 @@
         <v>20</v>
       </c>
       <c r="D108" s="41" t="str">
-        <f t="shared" ref="D108:D151" si="45">REPT("   ", B108*2) &amp; C108</f>
+        <f t="shared" ref="D108:D157" si="45">REPT("   ", B108*2) &amp; C108</f>
         <v xml:space="preserve">            Reactor Instrumentation and Control (I&amp;C)</v>
       </c>
       <c r="E108" s="41" t="s">
@@ -14367,22 +14388,22 @@
         <v>468</v>
       </c>
       <c r="V141" s="84">
-        <f t="shared" ref="V141:V151" si="48">0.9*$H141</f>
+        <f t="shared" ref="V141:V157" si="48">0.9*$H141</f>
         <v>0</v>
       </c>
       <c r="W141" s="84">
-        <f t="shared" ref="W141:W151" si="49">1.5*H141</f>
+        <f t="shared" ref="W141:W157" si="49">1.5*H141</f>
         <v>0</v>
       </c>
       <c r="X141" s="80" t="s">
         <v>451</v>
       </c>
       <c r="Y141" s="83">
-        <f t="shared" ref="Y141:Y151" si="50">0.9*I141</f>
+        <f t="shared" ref="Y141:Y157" si="50">0.9*I141</f>
         <v>160650</v>
       </c>
       <c r="Z141" s="83">
-        <f t="shared" ref="Z141:Z151" si="51">1.3*I141</f>
+        <f t="shared" ref="Z141:Z157" si="51">1.3*I141</f>
         <v>232050</v>
       </c>
       <c r="AA141" s="80" t="s">
@@ -14772,45 +14793,42 @@
       <c r="AD146" s="83"/>
       <c r="AE146" s="80"/>
     </row>
-    <row r="147" spans="1:31" ht="30" customHeight="1">
+    <row r="147" spans="1:31" ht="12.75" customHeight="1">
       <c r="A147" s="39">
-        <v>78</v>
+        <v>751</v>
       </c>
       <c r="B147" s="40">
-        <f t="shared" ref="B147" si="56">IF(ISNUMBER(A147),
-    IF(AND(A147=INT(A147), MOD(A147, 10) = 0), 0,
-        IF(AND(A147=INT(A147), LEN(A147)=2), 1,
-            IF(AND(A147=INT(A147), LEN(A147)=3), 2,
-                LEN(A147) - FIND(".", A147) + 2)
-        )
-    ),
-"")</f>
-        <v>1</v>
+        <f t="shared" si="44"/>
+        <v>2</v>
       </c>
       <c r="C147" s="58" t="s">
-        <v>42</v>
+        <v>512</v>
       </c>
       <c r="D147" s="41" t="str">
-        <f t="shared" ref="D147" si="57">REPT("   ", B147*2) &amp; C147</f>
-        <v xml:space="preserve">      Annualized Decommissioning Cost</v>
+        <f t="shared" si="45"/>
+        <v xml:space="preserve">            Annualized Vessel Replacements</v>
       </c>
       <c r="E147" s="41"/>
       <c r="F147" s="41"/>
       <c r="G147" s="41"/>
       <c r="H147" s="45"/>
-      <c r="I147" s="75"/>
+      <c r="I147" s="63"/>
       <c r="J147" s="51"/>
-      <c r="K147" s="47"/>
+      <c r="K147" s="61"/>
       <c r="L147" s="51"/>
       <c r="M147" s="51"/>
       <c r="N147" s="51"/>
       <c r="O147" s="68"/>
-      <c r="P147" s="76"/>
-      <c r="Q147" s="61"/>
-      <c r="R147" s="61"/>
+      <c r="P147" s="51"/>
+      <c r="Q147" s="113" t="s">
+        <v>504</v>
+      </c>
+      <c r="R147" s="113" t="s">
+        <v>504</v>
+      </c>
       <c r="S147" s="51"/>
-      <c r="T147" s="61" t="s">
-        <v>503</v>
+      <c r="T147" s="113" t="s">
+        <v>505</v>
       </c>
       <c r="U147" s="80"/>
       <c r="V147" s="84"/>
@@ -14824,37 +14842,37 @@
       <c r="AD147" s="83"/>
       <c r="AE147" s="80"/>
     </row>
-    <row r="148" spans="1:31">
+    <row r="148" spans="1:31" ht="25.5">
       <c r="A148" s="39">
-        <v>80</v>
+        <v>752</v>
       </c>
       <c r="B148" s="40">
         <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="C148" s="74" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="C148" s="58" t="s">
+        <v>513</v>
       </c>
       <c r="D148" s="41" t="str">
         <f t="shared" si="45"/>
-        <v>Annualized Fuel Cost</v>
+        <v xml:space="preserve">            Annualized Moderator Replacements</v>
       </c>
       <c r="E148" s="41"/>
       <c r="F148" s="41"/>
       <c r="G148" s="41"/>
-      <c r="H148" s="42"/>
-      <c r="I148" s="42"/>
-      <c r="J148" s="40"/>
-      <c r="K148" s="43"/>
-      <c r="L148" s="40"/>
-      <c r="M148" s="40"/>
-      <c r="N148" s="40"/>
-      <c r="O148" s="42"/>
-      <c r="P148" s="40"/>
-      <c r="Q148" s="43"/>
-      <c r="R148" s="40"/>
-      <c r="S148" s="40"/>
-      <c r="T148" s="40"/>
+      <c r="H148" s="45"/>
+      <c r="I148" s="63"/>
+      <c r="J148" s="51"/>
+      <c r="K148" s="61"/>
+      <c r="L148" s="51"/>
+      <c r="M148" s="51"/>
+      <c r="N148" s="51"/>
+      <c r="O148" s="68"/>
+      <c r="P148" s="51"/>
+      <c r="Q148" s="115"/>
+      <c r="R148" s="115"/>
+      <c r="S148" s="51"/>
+      <c r="T148" s="115"/>
       <c r="U148" s="80"/>
       <c r="V148" s="84"/>
       <c r="W148" s="84"/>
@@ -14867,105 +14885,63 @@
       <c r="AD148" s="83"/>
       <c r="AE148" s="80"/>
     </row>
-    <row r="149" spans="1:31" ht="89.25">
+    <row r="149" spans="1:31">
       <c r="A149" s="39">
-        <v>81</v>
+        <v>753</v>
       </c>
       <c r="B149" s="40">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C149" s="58" t="s">
-        <v>44</v>
+        <v>514</v>
       </c>
       <c r="D149" s="41" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">      Refueling Operations</v>
-      </c>
-      <c r="E149" s="41" t="s">
-        <v>342</v>
-      </c>
+        <v xml:space="preserve">            Annualized Reflector Replacements</v>
+      </c>
+      <c r="E149" s="41"/>
       <c r="F149" s="41"/>
       <c r="G149" s="41"/>
       <c r="H149" s="45"/>
-      <c r="I149" s="63">
-        <v>178500</v>
-      </c>
-      <c r="J149" s="51" t="s">
-        <v>383</v>
-      </c>
-      <c r="K149" s="61" t="s">
-        <v>384</v>
-      </c>
+      <c r="I149" s="63"/>
+      <c r="J149" s="51"/>
+      <c r="K149" s="61"/>
       <c r="L149" s="51"/>
       <c r="M149" s="51"/>
-      <c r="N149" s="51">
-        <v>1</v>
-      </c>
-      <c r="O149" s="68">
-        <v>2024</v>
-      </c>
-      <c r="P149" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q149" s="61"/>
-      <c r="R149" s="61" t="s">
-        <v>385</v>
-      </c>
+      <c r="N149" s="51"/>
+      <c r="O149" s="68"/>
+      <c r="P149" s="51"/>
+      <c r="Q149" s="115"/>
+      <c r="R149" s="115"/>
       <c r="S149" s="51"/>
-      <c r="T149" s="51"/>
-      <c r="U149" s="80" t="s">
-        <v>468</v>
-      </c>
-      <c r="V149" s="84">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="W149" s="84">
-        <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="X149" s="80" t="s">
-        <v>451</v>
-      </c>
-      <c r="Y149" s="83">
-        <f t="shared" si="50"/>
-        <v>160650</v>
-      </c>
-      <c r="Z149" s="83">
-        <f t="shared" si="51"/>
-        <v>232050</v>
-      </c>
-      <c r="AA149" s="80" t="s">
-        <v>451</v>
-      </c>
-      <c r="AB149" s="83" t="s">
-        <v>475</v>
-      </c>
-      <c r="AC149" s="83" t="s">
-        <v>476</v>
-      </c>
-      <c r="AD149" s="83" t="s">
-        <v>477</v>
-      </c>
-      <c r="AE149" s="80" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="150" spans="1:31">
+      <c r="T149" s="115"/>
+      <c r="U149" s="80"/>
+      <c r="V149" s="84"/>
+      <c r="W149" s="84"/>
+      <c r="X149" s="80"/>
+      <c r="Y149" s="83"/>
+      <c r="Z149" s="83"/>
+      <c r="AA149" s="80"/>
+      <c r="AB149" s="83"/>
+      <c r="AC149" s="83"/>
+      <c r="AD149" s="83"/>
+      <c r="AE149" s="80"/>
+    </row>
+    <row r="150" spans="1:31" ht="25.5">
       <c r="A150" s="39">
-        <v>82</v>
+        <v>754</v>
       </c>
       <c r="B150" s="40">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C150" s="58" t="s">
-        <v>45</v>
+        <v>515</v>
       </c>
       <c r="D150" s="41" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">      Additional Nuclear Fuel</v>
+        <v xml:space="preserve">            Annualized Reactivity Control Replacements</v>
       </c>
       <c r="E150" s="41"/>
       <c r="F150" s="41"/>
@@ -14979,10 +14955,10 @@
       <c r="N150" s="51"/>
       <c r="O150" s="68"/>
       <c r="P150" s="51"/>
-      <c r="Q150" s="61"/>
-      <c r="R150" s="51"/>
+      <c r="Q150" s="115"/>
+      <c r="R150" s="115"/>
       <c r="S150" s="51"/>
-      <c r="T150" s="51"/>
+      <c r="T150" s="115"/>
       <c r="U150" s="80"/>
       <c r="V150" s="84"/>
       <c r="W150" s="84"/>
@@ -14997,91 +14973,403 @@
     </row>
     <row r="151" spans="1:31" ht="25.5">
       <c r="A151" s="39">
-        <v>83</v>
+        <v>755</v>
       </c>
       <c r="B151" s="40">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C151" s="58" t="s">
-        <v>46</v>
+        <v>516</v>
       </c>
       <c r="D151" s="41" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">      Spent Fuel Management</v>
-      </c>
-      <c r="E151" s="41" t="s">
-        <v>341</v>
-      </c>
+        <v xml:space="preserve">            Annualized Integrated Heat Transfer System Replacements</v>
+      </c>
+      <c r="E151" s="41"/>
       <c r="F151" s="41"/>
       <c r="G151" s="41"/>
       <c r="H151" s="45"/>
-      <c r="I151" s="63">
-        <v>1</v>
-      </c>
-      <c r="J151" s="51" t="s">
-        <v>396</v>
-      </c>
-      <c r="K151" s="61" t="s">
-        <v>397</v>
-      </c>
+      <c r="I151" s="63"/>
+      <c r="J151" s="51"/>
+      <c r="K151" s="61"/>
       <c r="L151" s="51"/>
       <c r="M151" s="51"/>
-      <c r="N151" s="51">
+      <c r="N151" s="51"/>
+      <c r="O151" s="68"/>
+      <c r="P151" s="51"/>
+      <c r="Q151" s="115"/>
+      <c r="R151" s="115"/>
+      <c r="S151" s="51"/>
+      <c r="T151" s="115"/>
+      <c r="U151" s="80"/>
+      <c r="V151" s="84"/>
+      <c r="W151" s="84"/>
+      <c r="X151" s="80"/>
+      <c r="Y151" s="83"/>
+      <c r="Z151" s="83"/>
+      <c r="AA151" s="80"/>
+      <c r="AB151" s="83"/>
+      <c r="AC151" s="83"/>
+      <c r="AD151" s="83"/>
+      <c r="AE151" s="80"/>
+    </row>
+    <row r="152" spans="1:31" ht="25.5" customHeight="1">
+      <c r="A152" s="39">
+        <v>759</v>
+      </c>
+      <c r="B152" s="40">
+        <f t="shared" si="44"/>
+        <v>2</v>
+      </c>
+      <c r="C152" s="58" t="s">
+        <v>517</v>
+      </c>
+      <c r="D152" s="41" t="str">
+        <f t="shared" si="45"/>
+        <v xml:space="preserve">            Annualized Misc. Replacements</v>
+      </c>
+      <c r="E152" s="41"/>
+      <c r="F152" s="41"/>
+      <c r="G152" s="41"/>
+      <c r="H152" s="45"/>
+      <c r="I152" s="63"/>
+      <c r="J152" s="51"/>
+      <c r="K152" s="61"/>
+      <c r="L152" s="51"/>
+      <c r="M152" s="51"/>
+      <c r="N152" s="51"/>
+      <c r="O152" s="68"/>
+      <c r="P152" s="51"/>
+      <c r="Q152" s="114"/>
+      <c r="R152" s="114"/>
+      <c r="S152" s="51"/>
+      <c r="T152" s="114"/>
+      <c r="U152" s="80"/>
+      <c r="V152" s="84"/>
+      <c r="W152" s="84"/>
+      <c r="X152" s="80"/>
+      <c r="Y152" s="83"/>
+      <c r="Z152" s="83"/>
+      <c r="AA152" s="80"/>
+      <c r="AB152" s="83"/>
+      <c r="AC152" s="83"/>
+      <c r="AD152" s="83"/>
+      <c r="AE152" s="80"/>
+    </row>
+    <row r="153" spans="1:31" ht="30" customHeight="1">
+      <c r="A153" s="39">
+        <v>78</v>
+      </c>
+      <c r="B153" s="40">
+        <f t="shared" ref="B153" si="56">IF(ISNUMBER(A153),
+    IF(AND(A153=INT(A153), MOD(A153, 10) = 0), 0,
+        IF(AND(A153=INT(A153), LEN(A153)=2), 1,
+            IF(AND(A153=INT(A153), LEN(A153)=3), 2,
+                LEN(A153) - FIND(".", A153) + 2)
+        )
+    ),
+"")</f>
         <v>1</v>
       </c>
-      <c r="O151" s="68">
+      <c r="C153" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D153" s="41" t="str">
+        <f t="shared" ref="D153" si="57">REPT("   ", B153*2) &amp; C153</f>
+        <v xml:space="preserve">      Annualized Decommissioning Cost</v>
+      </c>
+      <c r="E153" s="41"/>
+      <c r="F153" s="41"/>
+      <c r="G153" s="41"/>
+      <c r="H153" s="45"/>
+      <c r="I153" s="75"/>
+      <c r="J153" s="51"/>
+      <c r="K153" s="47"/>
+      <c r="L153" s="51"/>
+      <c r="M153" s="51"/>
+      <c r="N153" s="51"/>
+      <c r="O153" s="68"/>
+      <c r="P153" s="76"/>
+      <c r="Q153" s="61"/>
+      <c r="R153" s="61"/>
+      <c r="S153" s="51"/>
+      <c r="T153" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="U153" s="80"/>
+      <c r="V153" s="84"/>
+      <c r="W153" s="84"/>
+      <c r="X153" s="80"/>
+      <c r="Y153" s="83"/>
+      <c r="Z153" s="83"/>
+      <c r="AA153" s="80"/>
+      <c r="AB153" s="83"/>
+      <c r="AC153" s="83"/>
+      <c r="AD153" s="83"/>
+      <c r="AE153" s="80"/>
+    </row>
+    <row r="154" spans="1:31">
+      <c r="A154" s="39">
+        <v>80</v>
+      </c>
+      <c r="B154" s="40">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="C154" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="D154" s="41" t="str">
+        <f t="shared" si="45"/>
+        <v>Annualized Fuel Cost</v>
+      </c>
+      <c r="E154" s="41"/>
+      <c r="F154" s="41"/>
+      <c r="G154" s="41"/>
+      <c r="H154" s="42"/>
+      <c r="I154" s="42"/>
+      <c r="J154" s="40"/>
+      <c r="K154" s="43"/>
+      <c r="L154" s="40"/>
+      <c r="M154" s="40"/>
+      <c r="N154" s="40"/>
+      <c r="O154" s="42"/>
+      <c r="P154" s="40"/>
+      <c r="Q154" s="43"/>
+      <c r="R154" s="40"/>
+      <c r="S154" s="40"/>
+      <c r="T154" s="40"/>
+      <c r="U154" s="80"/>
+      <c r="V154" s="84"/>
+      <c r="W154" s="84"/>
+      <c r="X154" s="80"/>
+      <c r="Y154" s="83"/>
+      <c r="Z154" s="83"/>
+      <c r="AA154" s="80"/>
+      <c r="AB154" s="83"/>
+      <c r="AC154" s="83"/>
+      <c r="AD154" s="83"/>
+      <c r="AE154" s="80"/>
+    </row>
+    <row r="155" spans="1:31" ht="89.25">
+      <c r="A155" s="39">
+        <v>81</v>
+      </c>
+      <c r="B155" s="40">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="C155" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="D155" s="41" t="str">
+        <f t="shared" si="45"/>
+        <v xml:space="preserve">      Refueling Operations</v>
+      </c>
+      <c r="E155" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="F155" s="41"/>
+      <c r="G155" s="41"/>
+      <c r="H155" s="45"/>
+      <c r="I155" s="63">
+        <v>178500</v>
+      </c>
+      <c r="J155" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="K155" s="61" t="s">
+        <v>384</v>
+      </c>
+      <c r="L155" s="51"/>
+      <c r="M155" s="51"/>
+      <c r="N155" s="51">
+        <v>1</v>
+      </c>
+      <c r="O155" s="68">
         <v>2024</v>
       </c>
-      <c r="P151" s="51" t="s">
+      <c r="P155" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q155" s="61"/>
+      <c r="R155" s="61" t="s">
+        <v>385</v>
+      </c>
+      <c r="S155" s="51"/>
+      <c r="T155" s="51"/>
+      <c r="U155" s="80" t="s">
+        <v>468</v>
+      </c>
+      <c r="V155" s="84">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="W155" s="84">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="X155" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y155" s="83">
+        <f t="shared" si="50"/>
+        <v>160650</v>
+      </c>
+      <c r="Z155" s="83">
+        <f t="shared" si="51"/>
+        <v>232050</v>
+      </c>
+      <c r="AA155" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="AB155" s="83" t="s">
+        <v>475</v>
+      </c>
+      <c r="AC155" s="83" t="s">
+        <v>476</v>
+      </c>
+      <c r="AD155" s="83" t="s">
+        <v>477</v>
+      </c>
+      <c r="AE155" s="80" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="156" spans="1:31">
+      <c r="A156" s="39">
+        <v>82</v>
+      </c>
+      <c r="B156" s="40">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="C156" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="D156" s="41" t="str">
+        <f t="shared" si="45"/>
+        <v xml:space="preserve">      Additional Nuclear Fuel</v>
+      </c>
+      <c r="E156" s="41"/>
+      <c r="F156" s="41"/>
+      <c r="G156" s="41"/>
+      <c r="H156" s="45"/>
+      <c r="I156" s="63"/>
+      <c r="J156" s="51"/>
+      <c r="K156" s="61"/>
+      <c r="L156" s="51"/>
+      <c r="M156" s="51"/>
+      <c r="N156" s="51"/>
+      <c r="O156" s="68"/>
+      <c r="P156" s="51"/>
+      <c r="Q156" s="61"/>
+      <c r="R156" s="51"/>
+      <c r="S156" s="51"/>
+      <c r="T156" s="51"/>
+      <c r="U156" s="80"/>
+      <c r="V156" s="84"/>
+      <c r="W156" s="84"/>
+      <c r="X156" s="80"/>
+      <c r="Y156" s="83"/>
+      <c r="Z156" s="83"/>
+      <c r="AA156" s="80"/>
+      <c r="AB156" s="83"/>
+      <c r="AC156" s="83"/>
+      <c r="AD156" s="83"/>
+      <c r="AE156" s="80"/>
+    </row>
+    <row r="157" spans="1:31" ht="25.5">
+      <c r="A157" s="39">
+        <v>83</v>
+      </c>
+      <c r="B157" s="40">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="C157" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="D157" s="41" t="str">
+        <f t="shared" si="45"/>
+        <v xml:space="preserve">      Spent Fuel Management</v>
+      </c>
+      <c r="E157" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="F157" s="41"/>
+      <c r="G157" s="41"/>
+      <c r="H157" s="45"/>
+      <c r="I157" s="63">
+        <v>1</v>
+      </c>
+      <c r="J157" s="51" t="s">
+        <v>396</v>
+      </c>
+      <c r="K157" s="61" t="s">
+        <v>397</v>
+      </c>
+      <c r="L157" s="51"/>
+      <c r="M157" s="51"/>
+      <c r="N157" s="51">
+        <v>1</v>
+      </c>
+      <c r="O157" s="68">
+        <v>2024</v>
+      </c>
+      <c r="P157" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q151" s="61"/>
-      <c r="R151" s="51"/>
-      <c r="S151" s="51"/>
-      <c r="T151" s="51"/>
-      <c r="U151" s="80" t="s">
+      <c r="Q157" s="61"/>
+      <c r="R157" s="51"/>
+      <c r="S157" s="51"/>
+      <c r="T157" s="51"/>
+      <c r="U157" s="80" t="s">
         <v>468</v>
       </c>
-      <c r="V151" s="84">
+      <c r="V157" s="84">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="W151" s="84">
+      <c r="W157" s="84">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="X151" s="80" t="s">
+      <c r="X157" s="80" t="s">
         <v>451</v>
       </c>
-      <c r="Y151" s="83">
+      <c r="Y157" s="83">
         <f t="shared" si="50"/>
         <v>0.9</v>
       </c>
-      <c r="Z151" s="83">
+      <c r="Z157" s="83">
         <f t="shared" si="51"/>
         <v>1.3</v>
       </c>
-      <c r="AA151" s="80" t="s">
+      <c r="AA157" s="80" t="s">
         <v>451</v>
       </c>
-      <c r="AB151" s="83" t="s">
+      <c r="AB157" s="83" t="s">
         <v>475</v>
       </c>
-      <c r="AC151" s="83" t="s">
+      <c r="AC157" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="AD151" s="83" t="s">
+      <c r="AD157" s="83" t="s">
         <v>477</v>
       </c>
-      <c r="AE151" s="80" t="s">
+      <c r="AE157" s="80" t="s">
         <v>452</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z151" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
-  <mergeCells count="48">
+  <autoFilter ref="A1:Z157" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
+  <mergeCells count="51">
     <mergeCell ref="T100:T101"/>
+    <mergeCell ref="R147:R152"/>
+    <mergeCell ref="Q147:Q152"/>
+    <mergeCell ref="T147:T152"/>
     <mergeCell ref="Q131:Q134"/>
     <mergeCell ref="Q39:Q41"/>
     <mergeCell ref="Q50:Q52"/>
@@ -15239,26 +15527,26 @@
       <formula>$B128=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A148:T151">
+  <conditionalFormatting sqref="A154:T157">
     <cfRule type="expression" dxfId="78" priority="90">
-      <formula>$B148=3</formula>
+      <formula>$B154=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="77" priority="91">
-      <formula>$B148=2</formula>
+      <formula>$B154=2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="76" priority="92">
-      <formula>$B148&lt;2</formula>
+      <formula>$B154&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="75" priority="93">
-      <formula>$B148=0</formula>
+      <formula>$B154=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE45 A46:S47 U46:AE47 A48:AE100 A102:AE151 U101:AE101 A101:S101">
+  <conditionalFormatting sqref="A1:AE45 A46:S47 U46:AE47 A48:AE100 U101:AE101 A101:S101 A102:AE146 A153:AE157 U148:AE152 S148:S152 A147:P152 Q147:AE147">
     <cfRule type="expression" dxfId="74" priority="193">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE45 A46:S47 U46:AE47 A48:AE100 A102:AE151 U101:AE101 A101:S101">
+  <conditionalFormatting sqref="A1:AE45 A46:S47 U46:AE47 A48:AE100 U101:AE101 A101:S101 A102:AE146 A153:AE157 U148:AE152 S148:S152 A147:P152 Q147:AE147">
     <cfRule type="expression" dxfId="73" priority="191">
       <formula>$B1=2</formula>
     </cfRule>
@@ -15266,7 +15554,7 @@
       <formula>$B1&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE45 A46:S47 U46:AE47 A48:AE100 A102:AE151 U101:AE101 A101:S101">
+  <conditionalFormatting sqref="A1:AE45 A46:S47 U46:AE47 A48:AE100 U101:AE101 A101:S101 A102:AE146 A153:AE157 U148:AE152 S148:S152 A147:P152 Q147:AE147">
     <cfRule type="expression" dxfId="71" priority="190">
       <formula>$B1=3</formula>
     </cfRule>
@@ -15315,7 +15603,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D121:D151 D2:D73 D75 D77:D114">
+  <conditionalFormatting sqref="D121:D157 D2:D73 D75 D77:D114">
     <cfRule type="colorScale" priority="478">
       <colorScale>
         <cfvo type="min"/>
@@ -15579,31 +15867,31 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O152:P159 O130:O151 O2:O128" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O158:P165 O130:O157 O2:O128" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
       <formula1>1950</formula1>
       <formula2>2025</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9 I11:I41 I50:I52 I54:I56 I77 L78:L86 I82:I87 H110:H111 H114:H121 I60:I72 L64:L76 I45:I47 L1:L60 I128:I151 H125:H151 I89:I126 H2:H107 L88:L1048576" xr:uid="{66ABF627-CC97-3E44-B6AC-09E441BED0CD}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9 I11:I41 I50:I52 I54:I56 I77 L78:L86 I82:I87 H110:H111 H114:H121 I60:I72 L64:L76 I45:I47 L1:L60 I128:I157 H125:H157 I89:I126 H2:H107 L88:L1048576" xr:uid="{66ABF627-CC97-3E44-B6AC-09E441BED0CD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K326:K336" xr:uid="{9E6037A9-5EC7-2945-A2FE-1723BA7DEE83}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K332:K342" xr:uid="{9E6037A9-5EC7-2945-A2FE-1723BA7DEE83}">
       <formula1>"Land Area, Power MWe, Excavation Volume,  Reactor Building Slab Roof Volume,	Reactor Building  Basement Volume, Reactor Building  Exterior Walls Volume,		Turbine Building Slab Roof Volume,	Turbine Building  Basement Volume,	Turbine Building  Exterior Wall"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J152:J1048576" xr:uid="{EEDF1E2A-32DC-6242-8EBD-BD01BBD19C77}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J158:J1048576" xr:uid="{EEDF1E2A-32DC-6242-8EBD-BD01BBD19C77}">
       <formula1>"$/acres, $/MWe, $/m^3, $/MWt"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N152:N305" xr:uid="{6D536505-A5B6-E145-A4B9-9C3C8E6B8527}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N158:N311" xr:uid="{6D536505-A5B6-E145-A4B9-9C3C8E6B8527}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N73 N121:N151 N75:N114" xr:uid="{1C0096F5-23AB-5A48-8F14-E27BC72A38A6}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N73 N121:N157 N75:N114" xr:uid="{1C0096F5-23AB-5A48-8F14-E27BC72A38A6}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M114 M2:M73 M121:M151 M75:M111" xr:uid="{127B7473-9D01-354E-A3BD-12180E660A5C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M114 M2:M73 M121:M157 M75:M111" xr:uid="{127B7473-9D01-354E-A3BD-12180E660A5C}">
       <formula1>"acres, MWe, m^3, MWt, Kg, Drums, kW, $, m^2, kg/s"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J73 J121:J151 J75:J114" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J73 J121:J157 J75:J114" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
       <formula1>"$/MWeHour,$/FTE, $/acres, $/MWe, $/m^3, $/MWt, $/Kg, $/Drum, $/(kg.sec), $/SWU, unitless, $/kWe"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M112:M113" xr:uid="{3DD8CB7E-F66A-4C30-8943-BB08D88ABA07}">
@@ -15619,10 +15907,10 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E151" xr:uid="{E571E7A1-C2F9-2E4D-99A9-8FA0C5D45C39}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E157" xr:uid="{E571E7A1-C2F9-2E4D-99A9-8FA0C5D45C39}">
       <formula1>"standard, nonstandard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P151" xr:uid="{17DDFD40-D97D-B64B-BD3B-AEAF52F6302C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P157" xr:uid="{17DDFD40-D97D-B64B-BD3B-AEAF52F6302C}">
       <formula1>"NA, General, Labor, Material, Equipment,Lab and Mat and Equip, 'Lab and Equip"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Replace NOAK Cost Multiplier with Learning Rate calculation which plateau's after 100th-of-a-Kind
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\mouse\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC99EAF3-93AE-44CB-987D-EE8B75DE6D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE1016C-61BA-4007-AC30-673EB317857F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{7B9AFB2B-1179-45AC-AF03-507FE361D8B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -19,6 +20,9 @@
     <sheet name="Inflation Adjustment" sheetId="3" r:id="rId4"/>
     <sheet name="Economics Parameters" sheetId="7" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Database'!$A$1:$Z$164</definedName>
     <definedName name="CRF">#REF!</definedName>
@@ -182,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="538">
   <si>
     <t>Account</t>
   </si>
@@ -1805,15 +1809,6 @@
     <t>Drum Count</t>
   </si>
   <si>
-    <t>Assumed Onsite Learning Rate</t>
-  </si>
-  <si>
-    <t>FOAK to NOAK Multipliers</t>
-  </si>
-  <si>
-    <t>Assumed Number Of Units For Onsite Learning</t>
-  </si>
-  <si>
     <t>In Vessel Shield Material</t>
   </si>
   <si>
@@ -1971,6 +1966,29 @@
   </si>
   <si>
     <t>Integrated Heat Exchanger Building Superstructure Area</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>FOAK to NOAK Learning Rates</t>
+  </si>
+  <si>
+    <t>Assessment of Factory Fabrication Considerations
+for Nuclear Microreactors
+ 10.1080/00295450.2023.2206779</t>
+  </si>
+  <si>
+    <t>Factory Be</t>
+  </si>
+  <si>
+    <t>Factory BeO</t>
+  </si>
+  <si>
+    <t>Calculated based on Refernce Paper + Gyutae's work. Refer to TEM Slides for rationale and methodology</t>
   </si>
 </sst>
 </file>
@@ -2384,7 +2402,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2690,6 +2708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2700,13 +2719,6 @@
   </cellStyles>
   <dxfs count="108">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2716,6 +2728,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2760,9 +2779,15 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2774,15 +2799,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2903,14 +2922,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2923,7 +2935,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2942,58 +2961,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3011,13 +2980,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3026,8 +2988,31 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3041,6 +3026,40 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3078,13 +3097,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3093,14 +3105,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3110,26 +3115,6 @@
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3159,18 +3144,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
-        <i/>
+        <i val="0"/>
       </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3184,8 +3173,17 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
       </fill>
     </dxf>
     <dxf>
@@ -3193,6 +3191,27 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3311,56 +3330,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3392,6 +3364,32 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3415,6 +3413,27 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3552,6 +3571,63 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="rccs_Qradiation"/>
+      <sheetName val="MIGHTR He Circulator Sizing"/>
+      <sheetName val="A13 Fitting"/>
+      <sheetName val="A21"/>
+      <sheetName val="A22"/>
+      <sheetName val="A23,24"/>
+      <sheetName val="A78"/>
+      <sheetName val="Building Dimensions"/>
+      <sheetName val="Spent Fuel StorageCask Capacity"/>
+      <sheetName val="Scaling Factory"/>
+      <sheetName val="Factory Fabricated Learning Rat"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="3">
+          <cell r="Q3">
+            <v>0.17627928659011793</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="Q4">
+            <v>0.18845943020781919</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="Q5">
+            <v>0.24138465715027702</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="Q6">
+            <v>0.23265368932625929</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3905,8 +3981,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
   <dimension ref="A1:AH164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -5230,7 +5309,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D18" s="41" t="str">
         <f>REPT("   ", B18*2) &amp; C18</f>
@@ -5251,16 +5330,16 @@
         <v>6491.9267043635973</v>
       </c>
       <c r="J18" s="47" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="K18" s="49" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="L18" s="48">
         <v>9373</v>
       </c>
       <c r="M18" s="47" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="N18" s="48">
         <v>1</v>
@@ -5272,13 +5351,13 @@
         <v>77</v>
       </c>
       <c r="Q18" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="R18" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S18" s="88" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="T18" s="51"/>
       <c r="U18" s="80" t="s">
@@ -5328,7 +5407,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D19" s="41" t="str">
         <f>REPT("   ", B19*2) &amp; C19</f>
@@ -5370,13 +5449,13 @@
         <v>77</v>
       </c>
       <c r="Q19" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="R19" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S19" s="88" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="T19" s="51"/>
       <c r="U19" s="80" t="s">
@@ -6071,7 +6150,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D29" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6114,7 +6193,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D30" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6138,7 +6217,7 @@
         <v>79</v>
       </c>
       <c r="K30" s="49" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="L30" s="48"/>
       <c r="M30" s="47" t="s">
@@ -6208,7 +6287,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D31" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6232,7 +6311,7 @@
         <v>79</v>
       </c>
       <c r="K31" s="49" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="L31" s="48"/>
       <c r="M31" s="47" t="s">
@@ -6296,7 +6375,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D32" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6320,7 +6399,7 @@
         <v>79</v>
       </c>
       <c r="K32" s="49" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="L32" s="48"/>
       <c r="M32" s="47" t="s">
@@ -6384,7 +6463,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D33" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6405,16 +6484,16 @@
         <v>6491.9267043635973</v>
       </c>
       <c r="J33" s="47" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="K33" s="49" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="L33" s="48">
         <v>9373</v>
       </c>
       <c r="M33" s="47" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="N33" s="48">
         <v>1</v>
@@ -6426,13 +6505,13 @@
         <v>77</v>
       </c>
       <c r="Q33" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="R33" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S33" s="88" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="T33" s="51"/>
       <c r="U33" s="80" t="s">
@@ -7609,7 +7688,7 @@
         <v>3</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D50" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7652,7 +7731,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D51" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7695,7 +7774,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D52" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7719,7 +7798,7 @@
         <v>79</v>
       </c>
       <c r="K52" s="58" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="L52" s="47"/>
       <c r="M52" s="47" t="s">
@@ -7742,7 +7821,7 @@
         <v>84</v>
       </c>
       <c r="T52" s="89" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="U52" s="80" t="s">
         <v>471</v>
@@ -7791,7 +7870,7 @@
         <v>5</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D53" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7815,7 +7894,7 @@
         <v>79</v>
       </c>
       <c r="K53" s="58" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="L53" s="47"/>
       <c r="M53" s="47" t="s">
@@ -7879,7 +7958,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D54" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7903,7 +7982,7 @@
         <v>79</v>
       </c>
       <c r="K54" s="58" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="L54" s="47"/>
       <c r="M54" s="47" t="s">
@@ -8843,7 +8922,7 @@
         <v>341</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G68" s="41" t="s">
         <v>439</v>
@@ -8932,7 +9011,7 @@
         <v>341</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G69" s="41" t="s">
         <v>440</v>
@@ -9026,7 +9105,7 @@
         <v>341</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G70" s="41" t="s">
         <v>441</v>
@@ -9113,7 +9192,7 @@
         <v>341</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G71" s="41" t="s">
         <v>439</v>
@@ -9202,7 +9281,7 @@
         <v>341</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G72" s="41" t="s">
         <v>440</v>
@@ -9296,7 +9375,7 @@
         <v>341</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G73" s="41" t="s">
         <v>441</v>
@@ -10690,7 +10769,7 @@
         <v>341</v>
       </c>
       <c r="F90" s="41" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G90" s="41" t="s">
         <v>186</v>
@@ -10707,7 +10786,7 @@
         <v>174</v>
       </c>
       <c r="K90" s="61" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="L90" s="51">
         <f>L78</f>
@@ -10788,7 +10867,7 @@
         <v>341</v>
       </c>
       <c r="F91" s="41" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G91" s="41" t="s">
         <v>331</v>
@@ -10801,7 +10880,7 @@
         <v>174</v>
       </c>
       <c r="K91" s="61" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="L91" s="51">
         <f>'Design Variables'!B43</f>
@@ -11366,7 +11445,7 @@
       </c>
       <c r="S98" s="69"/>
       <c r="T98" s="65" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="U98" s="80" t="s">
         <v>467</v>
@@ -11935,7 +12014,7 @@
         <v>3</v>
       </c>
       <c r="C105" s="58" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D105" s="41" t="str">
         <f t="shared" si="48"/>
@@ -11945,10 +12024,10 @@
         <v>341</v>
       </c>
       <c r="F105" s="41" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G105" s="41" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H105" s="45"/>
       <c r="I105" s="63">
@@ -11958,7 +12037,7 @@
         <v>174</v>
       </c>
       <c r="K105" s="61" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="L105" s="51"/>
       <c r="M105" s="51" t="s">
@@ -11972,16 +12051,16 @@
         <v>74</v>
       </c>
       <c r="Q105" s="61" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="R105" s="65" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="S105" s="87" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="T105" s="51" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="U105" s="80" t="s">
         <v>468</v>
@@ -12030,7 +12109,7 @@
         <v>3</v>
       </c>
       <c r="C106" s="58" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D106" s="41" t="str">
         <f t="shared" si="48"/>
@@ -12073,7 +12152,7 @@
         <v>4</v>
       </c>
       <c r="C107" s="58" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D107" s="41" t="str">
         <f t="shared" si="48"/>
@@ -12096,7 +12175,7 @@
         <v>174</v>
       </c>
       <c r="K107" s="61" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L107" s="51"/>
       <c r="M107" s="51" t="s">
@@ -12117,7 +12196,7 @@
       </c>
       <c r="S107" s="87"/>
       <c r="T107" s="106" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="U107" s="80" t="s">
         <v>467</v>
@@ -12166,7 +12245,7 @@
         <v>4</v>
       </c>
       <c r="C108" s="58" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D108" s="41" t="str">
         <f t="shared" si="48"/>
@@ -12190,7 +12269,7 @@
         <v>174</v>
       </c>
       <c r="K108" s="61" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L108" s="51">
         <v>387000</v>
@@ -15316,7 +15395,7 @@
         <v>2</v>
       </c>
       <c r="C152" s="58" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D152" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15339,7 +15418,7 @@
         <v>174</v>
       </c>
       <c r="K152" s="61" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="L152" s="51"/>
       <c r="M152" s="51" t="s">
@@ -15353,16 +15432,16 @@
         <v>74</v>
       </c>
       <c r="Q152" s="61" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="R152" s="65" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="S152" s="87" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="T152" s="51" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="U152" s="80" t="s">
         <v>468</v>
@@ -15430,14 +15509,14 @@
       <c r="O153" s="68"/>
       <c r="P153" s="51"/>
       <c r="Q153" s="61" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="R153" s="61" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="S153" s="51"/>
       <c r="T153" s="61" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="U153" s="80"/>
       <c r="V153" s="84"/>
@@ -15460,7 +15539,7 @@
         <v>2</v>
       </c>
       <c r="C154" s="58" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D154" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15479,14 +15558,14 @@
       <c r="O154" s="68"/>
       <c r="P154" s="51"/>
       <c r="Q154" s="106" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="R154" s="106" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="S154" s="51"/>
       <c r="T154" s="106" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="U154" s="80"/>
       <c r="V154" s="84"/>
@@ -15509,7 +15588,7 @@
         <v>2</v>
       </c>
       <c r="C155" s="58" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D155" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15552,7 +15631,7 @@
         <v>2</v>
       </c>
       <c r="C156" s="58" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D156" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15595,7 +15674,7 @@
         <v>2</v>
       </c>
       <c r="C157" s="58" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D157" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15638,7 +15717,7 @@
         <v>2</v>
       </c>
       <c r="C158" s="58" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D158" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15681,7 +15760,7 @@
         <v>2</v>
       </c>
       <c r="C159" s="58" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D159" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15753,7 +15832,7 @@
       <c r="R160" s="61"/>
       <c r="S160" s="51"/>
       <c r="T160" s="61" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="U160" s="80"/>
       <c r="V160" s="84"/>
@@ -16096,31 +16175,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132:P133">
-    <cfRule type="expression" dxfId="103" priority="177">
-      <formula>$B132=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="174">
+    <cfRule type="expression" dxfId="103" priority="174">
       <formula>$B132=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="175">
+    <cfRule type="expression" dxfId="102" priority="175">
       <formula>$B132=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="176">
+    <cfRule type="expression" dxfId="101" priority="176">
       <formula>$B132&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="177">
+      <formula>$B132=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:P143">
-    <cfRule type="expression" dxfId="99" priority="124">
+    <cfRule type="expression" dxfId="99" priority="122">
+      <formula>$B136=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="123">
+      <formula>$B136=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="124">
       <formula>$B136&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="125">
+    <cfRule type="expression" dxfId="96" priority="125">
       <formula>$B136=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="122">
-      <formula>$B136=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="123">
-      <formula>$B136=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A109:AE153 A154:P159 A160:AE164 U53:AE54 U108:AE108 Q154:AE154 S155:S159 U155:AE159">
@@ -16129,28 +16208,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="94" priority="233">
-      <formula>$B95=0</formula>
+    <cfRule type="expression" dxfId="94" priority="230">
+      <formula>$B95=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="93" priority="231">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="230">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="92" priority="232">
+      <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="232">
-      <formula>$B95&lt;2</formula>
+    <cfRule type="expression" dxfId="91" priority="233">
+      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
     <cfRule type="expression" dxfId="90" priority="13">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="15">
+    <cfRule type="expression" dxfId="89" priority="14">
+      <formula>$B74=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="15">
       <formula>$B74&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="14">
-      <formula>$B74=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
@@ -16221,17 +16300,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:R122 C123:P127">
-    <cfRule type="expression" dxfId="70" priority="52">
-      <formula>$B122=0</formula>
+    <cfRule type="expression" dxfId="70" priority="49">
+      <formula>$B122=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="51">
+    <cfRule type="expression" dxfId="69" priority="50">
+      <formula>$B122=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="51">
       <formula>$B122&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="50">
-      <formula>$B122=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="49">
-      <formula>$B122=3</formula>
+    <cfRule type="expression" dxfId="67" priority="52">
+      <formula>$B122=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
@@ -16280,31 +16359,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G54">
-    <cfRule type="expression" dxfId="65" priority="6">
+    <cfRule type="expression" dxfId="65" priority="5">
+      <formula>$B52=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="6">
       <formula>$B52=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="7">
+    <cfRule type="expression" dxfId="63" priority="7">
       <formula>$B52&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="8">
+    <cfRule type="expression" dxfId="62" priority="8">
       <formula>$B52=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="5">
-      <formula>$B52=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="61" priority="225">
-      <formula>$B96=0</formula>
+    <cfRule type="expression" dxfId="61" priority="222">
+      <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="224">
+    <cfRule type="expression" dxfId="60" priority="223">
+      <formula>$B96=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="224">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="222">
-      <formula>$B96=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="223">
-      <formula>$B96=2</formula>
+    <cfRule type="expression" dxfId="58" priority="225">
+      <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -16314,11 +16393,11 @@
     <cfRule type="expression" dxfId="56" priority="29">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="31">
+    <cfRule type="expression" dxfId="55" priority="30">
+      <formula>$B5&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="31">
       <formula>$B5=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="30">
-      <formula>$B5&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
@@ -16340,14 +16419,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="49" priority="76">
+    <cfRule type="expression" dxfId="49" priority="75">
+      <formula>$B69=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="76">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="77">
+    <cfRule type="expression" dxfId="47" priority="77">
       <formula>$B69&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="75">
-      <formula>$B69=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
@@ -16356,14 +16435,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="45" priority="87">
-      <formula>$B68&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="85">
+    <cfRule type="expression" dxfId="45" priority="85">
       <formula>$B68=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="86">
+    <cfRule type="expression" dxfId="44" priority="86">
       <formula>$B68=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="87">
+      <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
@@ -16372,28 +16451,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:J149">
-    <cfRule type="expression" dxfId="41" priority="109">
-      <formula>$B149=0</formula>
+    <cfRule type="expression" dxfId="41" priority="106">
+      <formula>$B149=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="108">
+    <cfRule type="expression" dxfId="40" priority="107">
+      <formula>$B149=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="108">
       <formula>$B149&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="107">
-      <formula>$B149=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="106">
-      <formula>$B149=3</formula>
+    <cfRule type="expression" dxfId="38" priority="109">
+      <formula>$B149=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I129:K130">
-    <cfRule type="expression" dxfId="37" priority="188">
-      <formula>$B129&lt;2</formula>
+    <cfRule type="expression" dxfId="37" priority="186">
+      <formula>$B129=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="187">
       <formula>$B129=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="186">
-      <formula>$B129=3</formula>
+    <cfRule type="expression" dxfId="35" priority="188">
+      <formula>$B129&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="189">
       <formula>$B129=0</formula>
@@ -16403,17 +16482,17 @@
     <cfRule type="expression" dxfId="33" priority="35">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="428">
-      <formula>#REF!=3</formula>
+    <cfRule type="expression" dxfId="32" priority="425">
+      <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="427">
+    <cfRule type="expression" dxfId="31" priority="426">
+      <formula>#REF!&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="427">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="426">
-      <formula>#REF!&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="425">
-      <formula>#REF!=2</formula>
+    <cfRule type="expression" dxfId="29" priority="428">
+      <formula>#REF!=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
@@ -16481,17 +16560,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:Q143">
-    <cfRule type="expression" dxfId="12" priority="168">
+    <cfRule type="expression" dxfId="12" priority="166">
+      <formula>$B142=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="167">
+      <formula>$B142=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="168">
       <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="169">
+    <cfRule type="expression" dxfId="9" priority="169">
       <formula>$B142=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="167">
-      <formula>$B142=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="166">
-      <formula>$B142=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
@@ -16517,14 +16596,14 @@
     <cfRule type="expression" dxfId="3" priority="251">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="253">
+    <cfRule type="expression" dxfId="2" priority="252">
+      <formula>$B95=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="253">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="254">
+    <cfRule type="expression" dxfId="0" priority="254">
       <formula>$B95=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="252">
-      <formula>$B95=2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
@@ -16592,6 +16671,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
   <legacyDrawing r:id="rId14"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3A5BD7CA-D901-4C35-8F1B-FB3DB8093CEC}">
+          <x14:formula1>
+            <xm:f>'Economics Parameters'!$A$9:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>U2:U164</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -16599,8 +16690,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAED81D3-2E1E-EB42-8F84-3B0F01FD7CDC}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="183" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A4" zoomScale="183" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -16772,6 +16866,10 @@
         <f>C16+C17+C18</f>
         <v>2004852</v>
       </c>
+      <c r="E15">
+        <f>C15/E19*AVERAGE('[1]Factory Fabricated Learning Rat'!$Q$3,'[1]Factory Fabricated Learning Rat'!$Q$4)+C19/E19*'[1]Factory Fabricated Learning Rat'!$Q$5+C25/E19*'[1]Factory Fabricated Learning Rat'!$Q$6</f>
+        <v>0.22343911000453887</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="31">
@@ -16784,7 +16882,7 @@
         <v>762382.4</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" s="31">
         <v>221.12</v>
       </c>
@@ -16795,7 +16893,7 @@
         <v>1201688.6000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="31">
         <v>221.13</v>
       </c>
@@ -16806,7 +16904,7 @@
         <v>40781</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" s="31">
         <v>221.2</v>
       </c>
@@ -16817,8 +16915,12 @@
         <f>C20</f>
         <v>2114223</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E19" s="8">
+        <f>C20+C25+C15</f>
+        <v>8937296.5999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
       <c r="A20" s="31">
         <v>221.21</v>
       </c>
@@ -16830,7 +16932,7 @@
         <v>2114223</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1">
       <c r="A21" s="10">
         <v>221.21100000000001</v>
       </c>
@@ -16842,7 +16944,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1">
       <c r="A22" s="10">
         <v>221.21199999999999</v>
       </c>
@@ -16853,7 +16955,7 @@
         <v>322663</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1">
       <c r="A23" s="10">
         <v>221.21299999999999</v>
       </c>
@@ -16864,7 +16966,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="10">
         <v>221.214</v>
       </c>
@@ -16872,7 +16974,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="31">
         <v>221.3</v>
       </c>
@@ -16884,7 +16986,7 @@
         <v>4818221.5999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="31">
         <v>221.31</v>
       </c>
@@ -16895,7 +16997,7 @@
         <v>4170231</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="33">
         <v>221.31100000000001</v>
       </c>
@@ -16906,7 +17008,7 @@
         <v>3200000</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="33">
         <v>221.31200000000001</v>
       </c>
@@ -16917,7 +17019,7 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" s="33">
         <v>221.31299999999999</v>
       </c>
@@ -16928,7 +17030,7 @@
         <v>120231</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" s="31">
         <v>221.32</v>
       </c>
@@ -16939,7 +17041,7 @@
         <v>647990.6</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="31">
         <v>221.33</v>
       </c>
@@ -16950,7 +17052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="31" t="s">
         <v>200</v>
       </c>
@@ -17508,6 +17610,7 @@
     <sheetView topLeftCell="A13" zoomScale="225" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
   <cols>
@@ -18197,9 +18300,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF46401-6828-1F49-B2C3-A6E5E28394B1}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A13" zoomScale="156" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
@@ -19319,27 +19423,37 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358A137-1626-9343-A399-452BA3D3C6F7}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="36" customFormat="1">
+    <row r="1" spans="1:5" s="36" customFormat="1">
       <c r="A1" s="36" t="s">
         <v>382</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" s="36" t="s">
+        <v>531</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>532</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>381</v>
       </c>
@@ -19347,7 +19461,7 @@
         <v>6.5389932052543287E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>391</v>
       </c>
@@ -19355,7 +19469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -19363,7 +19477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>393</v>
       </c>
@@ -19371,7 +19485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>394</v>
       </c>
@@ -19379,7 +19493,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>386</v>
       </c>
@@ -19387,7 +19501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>395</v>
       </c>
@@ -19395,72 +19509,94 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B9">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1">
+      <c r="C9" s="116" t="s">
+        <v>533</v>
+      </c>
+      <c r="D9" s="116" t="s">
+        <v>534</v>
+      </c>
+      <c r="E9" s="116" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>468</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="116" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" s="116"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="116"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
         <v>469</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11" s="116"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
         <v>472</v>
       </c>
       <c r="B12">
-        <v>0.6</v>
+        <v>0.22343911000453887</v>
       </c>
       <c r="C12" s="116"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="35" t="s">
-        <v>450</v>
-      </c>
-      <c r="B13">
-        <v>0.4</v>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B13" s="117">
+        <v>0.182369</v>
       </c>
       <c r="C13" s="116"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>467</v>
+        <v>535</v>
       </c>
       <c r="B14">
-        <v>0.3</v>
+        <v>0.63897814563472732</v>
       </c>
       <c r="C14" s="116"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>481</v>
+        <v>536</v>
       </c>
       <c r="B15">
-        <v>20</v>
-      </c>
+        <v>0.65783791594766872</v>
+      </c>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C10:C14"/>
+  <mergeCells count="3">
+    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="D9:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Learning Categories in Database; Add additional category for non-nuclear off-the-shelf components
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\mouse\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B4C26A-A334-40F9-B945-F62E3E33B9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3D4B0E-33CB-4DF8-8DE8-C62DAF5DD632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="877" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -2632,6 +2632,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2640,18 +2674,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2670,27 +2692,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2716,7 +2717,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2727,6 +2727,13 @@
   </cellStyles>
   <dxfs count="108">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2736,13 +2743,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2787,15 +2787,9 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2807,9 +2801,15 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2930,7 +2930,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2943,14 +2950,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2969,8 +2969,58 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -2988,6 +3038,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2996,31 +3053,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3034,40 +3068,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3105,10 +3105,45 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3118,11 +3153,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3152,22 +3186,18 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <i/>
       </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
+      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3181,17 +3211,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
       </fill>
     </dxf>
     <dxf>
@@ -3199,27 +3220,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3338,9 +3338,56 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3372,32 +3419,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3421,27 +3442,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3989,7 +3989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
   <dimension ref="A1:AH164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="T121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4227,7 +4227,7 @@
       <c r="R3" s="93" t="s">
         <v>445</v>
       </c>
-      <c r="S3" s="95" t="s">
+      <c r="S3" s="99" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4315,7 +4315,7 @@
         <v>57</v>
       </c>
       <c r="R4" s="93"/>
-      <c r="S4" s="95"/>
+      <c r="S4" s="99"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>468</v>
@@ -4397,7 +4397,7 @@
       <c r="R5" s="93" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="95" t="s">
+      <c r="S5" s="99" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4478,7 +4478,7 @@
         <v>58</v>
       </c>
       <c r="R6" s="93"/>
-      <c r="S6" s="95"/>
+      <c r="S6" s="99"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>468</v>
@@ -4790,7 +4790,7 @@
       <c r="R11" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="94" t="s">
+      <c r="S11" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -4883,7 +4883,7 @@
       </c>
       <c r="Q12" s="93"/>
       <c r="R12" s="93"/>
-      <c r="S12" s="95"/>
+      <c r="S12" s="99"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>471</v>
@@ -4967,7 +4967,7 @@
       </c>
       <c r="Q13" s="93"/>
       <c r="R13" s="93"/>
-      <c r="S13" s="95"/>
+      <c r="S13" s="99"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>471</v>
@@ -5098,7 +5098,7 @@
       <c r="R15" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="94" t="s">
+      <c r="S15" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5184,7 +5184,7 @@
       </c>
       <c r="Q16" s="93"/>
       <c r="R16" s="93"/>
-      <c r="S16" s="95"/>
+      <c r="S16" s="99"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>471</v>
@@ -5268,7 +5268,7 @@
       </c>
       <c r="Q17" s="93"/>
       <c r="R17" s="93"/>
-      <c r="S17" s="95"/>
+      <c r="S17" s="99"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>471</v>
@@ -5638,7 +5638,7 @@
       <c r="R22" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="94" t="s">
+      <c r="S22" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5724,7 +5724,7 @@
       </c>
       <c r="Q23" s="93"/>
       <c r="R23" s="93"/>
-      <c r="S23" s="95"/>
+      <c r="S23" s="99"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>471</v>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="Q24" s="93"/>
       <c r="R24" s="93"/>
-      <c r="S24" s="95"/>
+      <c r="S24" s="99"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>471</v>
@@ -5939,7 +5939,7 @@
       <c r="R26" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="94" t="s">
+      <c r="S26" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -6025,7 +6025,7 @@
       </c>
       <c r="Q27" s="93"/>
       <c r="R27" s="93"/>
-      <c r="S27" s="95"/>
+      <c r="S27" s="99"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>471</v>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="Q28" s="93"/>
       <c r="R28" s="93"/>
-      <c r="S28" s="95"/>
+      <c r="S28" s="99"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>471</v>
@@ -6244,7 +6244,7 @@
       <c r="R30" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="94" t="s">
+      <c r="S30" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6334,7 +6334,7 @@
       </c>
       <c r="Q31" s="93"/>
       <c r="R31" s="93"/>
-      <c r="S31" s="95"/>
+      <c r="S31" s="99"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>471</v>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="Q32" s="93"/>
       <c r="R32" s="93"/>
-      <c r="S32" s="95"/>
+      <c r="S32" s="99"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>471</v>
@@ -6737,7 +6737,7 @@
       <c r="R37" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="94" t="s">
+      <c r="S37" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -6823,7 +6823,7 @@
       </c>
       <c r="Q38" s="93"/>
       <c r="R38" s="93"/>
-      <c r="S38" s="95"/>
+      <c r="S38" s="99"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>471</v>
@@ -6907,7 +6907,7 @@
       </c>
       <c r="Q39" s="93"/>
       <c r="R39" s="93"/>
-      <c r="S39" s="95"/>
+      <c r="S39" s="99"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>471</v>
@@ -7038,7 +7038,7 @@
       <c r="R41" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="94" t="s">
+      <c r="S41" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7124,7 +7124,7 @@
       </c>
       <c r="Q42" s="93"/>
       <c r="R42" s="93"/>
-      <c r="S42" s="95"/>
+      <c r="S42" s="99"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>471</v>
@@ -7208,7 +7208,7 @@
       </c>
       <c r="Q43" s="93"/>
       <c r="R43" s="93"/>
-      <c r="S43" s="95"/>
+      <c r="S43" s="99"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>471</v>
@@ -7382,7 +7382,7 @@
       <c r="R46" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="94" t="s">
+      <c r="S46" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="Q47" s="93"/>
       <c r="R47" s="93"/>
-      <c r="S47" s="95"/>
+      <c r="S47" s="99"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
         <v>467</v>
@@ -7552,7 +7552,7 @@
       </c>
       <c r="Q48" s="93"/>
       <c r="R48" s="93"/>
-      <c r="S48" s="95"/>
+      <c r="S48" s="99"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
         <v>467</v>
@@ -7819,16 +7819,16 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="103" t="s">
+      <c r="Q52" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="R52" s="103" t="s">
+      <c r="R52" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="97" t="s">
+      <c r="S52" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="89" t="s">
+      <c r="T52" s="101" t="s">
         <v>504</v>
       </c>
       <c r="U52" s="80" t="s">
@@ -7915,10 +7915,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="104"/>
-      <c r="R53" s="104"/>
-      <c r="S53" s="98"/>
-      <c r="T53" s="90"/>
+      <c r="Q53" s="97"/>
+      <c r="R53" s="97"/>
+      <c r="S53" s="106"/>
+      <c r="T53" s="102"/>
       <c r="U53" s="80" t="s">
         <v>471</v>
       </c>
@@ -8003,10 +8003,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="105"/>
-      <c r="R54" s="105"/>
-      <c r="S54" s="99"/>
-      <c r="T54" s="91"/>
+      <c r="Q54" s="98"/>
+      <c r="R54" s="98"/>
+      <c r="S54" s="107"/>
+      <c r="T54" s="103"/>
       <c r="U54" s="80" t="s">
         <v>471</v>
       </c>
@@ -8179,7 +8179,7 @@
       <c r="R57" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="94" t="s">
+      <c r="S57" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8265,7 +8265,7 @@
       </c>
       <c r="Q58" s="93"/>
       <c r="R58" s="93"/>
-      <c r="S58" s="95"/>
+      <c r="S58" s="99"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>471</v>
@@ -8349,7 +8349,7 @@
       </c>
       <c r="Q59" s="93"/>
       <c r="R59" s="93"/>
-      <c r="S59" s="95"/>
+      <c r="S59" s="99"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>471</v>
@@ -8480,7 +8480,7 @@
       <c r="R61" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="94" t="s">
+      <c r="S61" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8566,7 +8566,7 @@
       </c>
       <c r="Q62" s="93"/>
       <c r="R62" s="93"/>
-      <c r="S62" s="95"/>
+      <c r="S62" s="99"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>471</v>
@@ -8650,7 +8650,7 @@
       </c>
       <c r="Q63" s="93"/>
       <c r="R63" s="93"/>
-      <c r="S63" s="95"/>
+      <c r="S63" s="99"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>471</v>
@@ -8957,7 +8957,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="92" t="s">
+      <c r="R68" s="94" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -9046,7 +9046,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="92"/>
+      <c r="R69" s="94"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9140,7 +9140,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="92"/>
+      <c r="R70" s="94"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9227,7 +9227,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="92"/>
+      <c r="R71" s="94"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9316,7 +9316,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="92"/>
+      <c r="R72" s="94"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9410,7 +9410,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="92"/>
+      <c r="R73" s="94"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9580,10 +9580,10 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="92" t="s">
+      <c r="R76" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="96" t="s">
+      <c r="S76" s="104" t="s">
         <v>447</v>
       </c>
       <c r="T76" s="61" t="s">
@@ -9670,8 +9670,8 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="92"/>
-      <c r="S77" s="96"/>
+      <c r="R77" s="94"/>
+      <c r="S77" s="104"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
         <v>450</v>
@@ -9765,8 +9765,8 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="92"/>
-      <c r="S78" s="96"/>
+      <c r="R78" s="94"/>
+      <c r="S78" s="104"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
         <v>450</v>
@@ -9859,8 +9859,8 @@
       <c r="Q79" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="R79" s="92"/>
-      <c r="S79" s="96"/>
+      <c r="R79" s="94"/>
+      <c r="S79" s="104"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
         <v>450</v>
@@ -9954,8 +9954,8 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="92"/>
-      <c r="S80" s="96"/>
+      <c r="R80" s="94"/>
+      <c r="S80" s="104"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
         <v>536</v>
@@ -10379,7 +10379,7 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="96" t="s">
+      <c r="S85" s="104" t="s">
         <v>447</v>
       </c>
       <c r="T85" s="51"/>
@@ -10485,7 +10485,7 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="96"/>
+      <c r="S86" s="104"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
         <v>467</v>
@@ -10581,7 +10581,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="96"/>
+      <c r="S87" s="104"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>467</v>
@@ -10675,7 +10675,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="96"/>
+      <c r="S88" s="104"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>467</v>
@@ -10744,7 +10744,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="96"/>
+      <c r="S89" s="104"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -10816,7 +10816,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="96"/>
+      <c r="S90" s="104"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>467</v>
@@ -10910,7 +10910,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="96"/>
+      <c r="S91" s="104"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>467</v>
@@ -11274,13 +11274,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="92" t="s">
+      <c r="R96" s="94" t="s">
         <v>448</v>
       </c>
-      <c r="S96" s="100" t="s">
+      <c r="S96" s="108" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="92"/>
+      <c r="T96" s="94"/>
       <c r="U96" s="80" t="s">
         <v>467</v>
       </c>
@@ -11367,9 +11367,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="92"/>
-      <c r="S97" s="101"/>
-      <c r="T97" s="92"/>
+      <c r="R97" s="94"/>
+      <c r="S97" s="109"/>
+      <c r="T97" s="94"/>
       <c r="U97" s="80" t="s">
         <v>467</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>360</v>
       </c>
       <c r="S107" s="87"/>
-      <c r="T107" s="106" t="s">
+      <c r="T107" s="90" t="s">
         <v>507</v>
       </c>
       <c r="U107" s="80" t="s">
@@ -12301,7 +12301,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="107"/>
+      <c r="T108" s="91"/>
       <c r="U108" s="80" t="s">
         <v>467</v>
       </c>
@@ -13302,10 +13302,10 @@
       <c r="P122" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q122" s="102" t="s">
+      <c r="Q122" s="95" t="s">
         <v>427</v>
       </c>
-      <c r="R122" s="102" t="s">
+      <c r="R122" s="95" t="s">
         <v>365</v>
       </c>
       <c r="S122" s="51"/>
@@ -13394,8 +13394,8 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="102"/>
-      <c r="R123" s="102"/>
+      <c r="Q123" s="95"/>
+      <c r="R123" s="95"/>
       <c r="S123" s="51"/>
       <c r="T123" s="51"/>
       <c r="U123" s="80" t="s">
@@ -13482,8 +13482,8 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="102"/>
-      <c r="R124" s="102"/>
+      <c r="Q124" s="95"/>
+      <c r="R124" s="95"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
@@ -13570,8 +13570,8 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="102"/>
-      <c r="R125" s="102"/>
+      <c r="Q125" s="95"/>
+      <c r="R125" s="95"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
@@ -13658,8 +13658,8 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="102"/>
-      <c r="R126" s="102"/>
+      <c r="Q126" s="95"/>
+      <c r="R126" s="95"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
@@ -13746,8 +13746,8 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="102"/>
-      <c r="R127" s="102"/>
+      <c r="Q127" s="95"/>
+      <c r="R127" s="95"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
@@ -13870,10 +13870,10 @@
       <c r="P129" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q129" s="92" t="s">
+      <c r="Q129" s="94" t="s">
         <v>369</v>
       </c>
-      <c r="R129" s="92" t="s">
+      <c r="R129" s="94" t="s">
         <v>370</v>
       </c>
       <c r="S129" s="51"/>
@@ -13955,8 +13955,8 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="92"/>
-      <c r="R130" s="92"/>
+      <c r="Q130" s="94"/>
+      <c r="R130" s="94"/>
       <c r="S130" s="51"/>
       <c r="T130" s="51"/>
       <c r="U130" s="80" t="s">
@@ -14038,8 +14038,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="92"/>
-      <c r="R131" s="92"/>
+      <c r="Q131" s="94"/>
+      <c r="R131" s="94"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14123,8 +14123,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="92"/>
-      <c r="R132" s="92"/>
+      <c r="Q132" s="94"/>
+      <c r="R132" s="94"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14215,8 +14215,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="92"/>
-      <c r="R133" s="92"/>
+      <c r="Q133" s="94"/>
+      <c r="R133" s="94"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -15565,14 +15565,14 @@
       <c r="N154" s="51"/>
       <c r="O154" s="68"/>
       <c r="P154" s="51"/>
-      <c r="Q154" s="106" t="s">
+      <c r="Q154" s="90" t="s">
         <v>501</v>
       </c>
-      <c r="R154" s="106" t="s">
+      <c r="R154" s="90" t="s">
         <v>501</v>
       </c>
       <c r="S154" s="51"/>
-      <c r="T154" s="106" t="s">
+      <c r="T154" s="90" t="s">
         <v>502</v>
       </c>
       <c r="U154" s="80"/>
@@ -15614,10 +15614,10 @@
       <c r="N155" s="51"/>
       <c r="O155" s="68"/>
       <c r="P155" s="51"/>
-      <c r="Q155" s="108"/>
-      <c r="R155" s="108"/>
+      <c r="Q155" s="92"/>
+      <c r="R155" s="92"/>
       <c r="S155" s="51"/>
-      <c r="T155" s="108"/>
+      <c r="T155" s="92"/>
       <c r="U155" s="80"/>
       <c r="V155" s="84"/>
       <c r="W155" s="84"/>
@@ -15657,10 +15657,10 @@
       <c r="N156" s="51"/>
       <c r="O156" s="68"/>
       <c r="P156" s="51"/>
-      <c r="Q156" s="108"/>
-      <c r="R156" s="108"/>
+      <c r="Q156" s="92"/>
+      <c r="R156" s="92"/>
       <c r="S156" s="51"/>
-      <c r="T156" s="108"/>
+      <c r="T156" s="92"/>
       <c r="U156" s="80"/>
       <c r="V156" s="84"/>
       <c r="W156" s="84"/>
@@ -15700,10 +15700,10 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="108"/>
-      <c r="R157" s="108"/>
+      <c r="Q157" s="92"/>
+      <c r="R157" s="92"/>
       <c r="S157" s="51"/>
-      <c r="T157" s="108"/>
+      <c r="T157" s="92"/>
       <c r="U157" s="80"/>
       <c r="V157" s="84"/>
       <c r="W157" s="84"/>
@@ -15743,10 +15743,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="108"/>
-      <c r="R158" s="108"/>
+      <c r="Q158" s="92"/>
+      <c r="R158" s="92"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="108"/>
+      <c r="T158" s="92"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -15786,10 +15786,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="107"/>
-      <c r="R159" s="107"/>
+      <c r="Q159" s="91"/>
+      <c r="R159" s="91"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="107"/>
+      <c r="T159" s="91"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -16111,11 +16111,39 @@
   </sheetData>
   <autoFilter ref="A1:Z164" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="54">
-    <mergeCell ref="T107:T108"/>
-    <mergeCell ref="R154:R159"/>
-    <mergeCell ref="Q154:Q159"/>
-    <mergeCell ref="T154:T159"/>
-    <mergeCell ref="Q138:Q141"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16132,39 +16160,11 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q129:Q133"/>
     <mergeCell ref="Q122:Q127"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
-    <mergeCell ref="S26:S28"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
+    <mergeCell ref="T107:T108"/>
+    <mergeCell ref="R154:R159"/>
+    <mergeCell ref="Q154:Q159"/>
+    <mergeCell ref="T154:T159"/>
+    <mergeCell ref="Q138:Q141"/>
   </mergeCells>
   <conditionalFormatting sqref="A96:F98 A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 A150:J152 S152:T152">
     <cfRule type="expression" dxfId="107" priority="226">
@@ -16183,31 +16183,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132:P133">
-    <cfRule type="expression" dxfId="103" priority="174">
+    <cfRule type="expression" dxfId="103" priority="177">
+      <formula>$B132=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="174">
       <formula>$B132=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="175">
+    <cfRule type="expression" dxfId="101" priority="175">
       <formula>$B132=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="176">
+    <cfRule type="expression" dxfId="100" priority="176">
       <formula>$B132&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="177">
-      <formula>$B132=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:P143">
-    <cfRule type="expression" dxfId="99" priority="122">
+    <cfRule type="expression" dxfId="99" priority="124">
+      <formula>$B136&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="125">
+      <formula>$B136=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="122">
       <formula>$B136=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="123">
+    <cfRule type="expression" dxfId="96" priority="123">
       <formula>$B136=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="124">
-      <formula>$B136&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="125">
-      <formula>$B136=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A109:AE153 A154:P159 A160:AE164 U53:AE54 U108:AE108 Q154:AE154 S155:S159 U155:AE159">
@@ -16216,28 +16216,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="94" priority="230">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="94" priority="233">
+      <formula>$B95=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="93" priority="231">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="232">
+    <cfRule type="expression" dxfId="92" priority="230">
+      <formula>$B95=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="232">
       <formula>$B95&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="233">
-      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
     <cfRule type="expression" dxfId="90" priority="13">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="14">
+    <cfRule type="expression" dxfId="89" priority="15">
+      <formula>$B74&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="14">
       <formula>$B74=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="15">
-      <formula>$B74&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
@@ -16308,17 +16308,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:R122 C123:P127">
-    <cfRule type="expression" dxfId="70" priority="49">
-      <formula>$B122=3</formula>
+    <cfRule type="expression" dxfId="70" priority="52">
+      <formula>$B122=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="50">
+    <cfRule type="expression" dxfId="69" priority="51">
+      <formula>$B122&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="50">
       <formula>$B122=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="51">
-      <formula>$B122&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="52">
-      <formula>$B122=0</formula>
+    <cfRule type="expression" dxfId="67" priority="49">
+      <formula>$B122=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
@@ -16367,31 +16367,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G54">
-    <cfRule type="expression" dxfId="65" priority="5">
-      <formula>$B52=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="6">
+    <cfRule type="expression" dxfId="65" priority="6">
       <formula>$B52=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="7">
+    <cfRule type="expression" dxfId="64" priority="7">
       <formula>$B52&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="8">
+    <cfRule type="expression" dxfId="63" priority="8">
       <formula>$B52=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="5">
+      <formula>$B52=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="61" priority="222">
+    <cfRule type="expression" dxfId="61" priority="225">
+      <formula>$B96=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="224">
+      <formula>$B96&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="222">
       <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="223">
+    <cfRule type="expression" dxfId="58" priority="223">
       <formula>$B96=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="224">
-      <formula>$B96&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="225">
-      <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -16401,11 +16401,11 @@
     <cfRule type="expression" dxfId="56" priority="29">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="30">
+    <cfRule type="expression" dxfId="55" priority="31">
+      <formula>$B5=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="30">
       <formula>$B5&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="31">
-      <formula>$B5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
@@ -16427,14 +16427,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="49" priority="75">
-      <formula>$B69=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="76">
+    <cfRule type="expression" dxfId="49" priority="76">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="77">
+    <cfRule type="expression" dxfId="48" priority="77">
       <formula>$B69&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="75">
+      <formula>$B69=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
@@ -16443,14 +16443,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="45" priority="85">
+    <cfRule type="expression" dxfId="45" priority="87">
+      <formula>$B68&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="85">
       <formula>$B68=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="86">
+    <cfRule type="expression" dxfId="43" priority="86">
       <formula>$B68=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="87">
-      <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
@@ -16459,28 +16459,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:J149">
-    <cfRule type="expression" dxfId="41" priority="106">
-      <formula>$B149=3</formula>
+    <cfRule type="expression" dxfId="41" priority="109">
+      <formula>$B149=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="107">
+    <cfRule type="expression" dxfId="40" priority="108">
+      <formula>$B149&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="107">
       <formula>$B149=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="108">
-      <formula>$B149&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="109">
-      <formula>$B149=0</formula>
+    <cfRule type="expression" dxfId="38" priority="106">
+      <formula>$B149=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I129:K130">
-    <cfRule type="expression" dxfId="37" priority="186">
-      <formula>$B129=3</formula>
+    <cfRule type="expression" dxfId="37" priority="188">
+      <formula>$B129&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="187">
       <formula>$B129=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="188">
-      <formula>$B129&lt;2</formula>
+    <cfRule type="expression" dxfId="35" priority="186">
+      <formula>$B129=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="189">
       <formula>$B129=0</formula>
@@ -16490,17 +16490,17 @@
     <cfRule type="expression" dxfId="33" priority="35">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="425">
-      <formula>#REF!=2</formula>
+    <cfRule type="expression" dxfId="32" priority="428">
+      <formula>#REF!=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="426">
+    <cfRule type="expression" dxfId="31" priority="427">
+      <formula>#REF!=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="426">
       <formula>#REF!&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="427">
-      <formula>#REF!=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="428">
-      <formula>#REF!=3</formula>
+    <cfRule type="expression" dxfId="29" priority="425">
+      <formula>#REF!=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
@@ -16568,17 +16568,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:Q143">
-    <cfRule type="expression" dxfId="12" priority="166">
-      <formula>$B142=3</formula>
+    <cfRule type="expression" dxfId="12" priority="168">
+      <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="167">
+    <cfRule type="expression" dxfId="11" priority="169">
+      <formula>$B142=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="167">
       <formula>$B142=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="168">
-      <formula>$B142&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="169">
-      <formula>$B142=0</formula>
+    <cfRule type="expression" dxfId="9" priority="166">
+      <formula>$B142=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
@@ -16604,14 +16604,14 @@
     <cfRule type="expression" dxfId="3" priority="251">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="252">
-      <formula>$B95=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="253">
+    <cfRule type="expression" dxfId="2" priority="253">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="254">
+    <cfRule type="expression" dxfId="1" priority="254">
       <formula>$B95=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="252">
+      <formula>$B95=2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
@@ -16711,20 +16711,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="110" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="C1" s="112" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="109"/>
-      <c r="B2" s="110"/>
-      <c r="C2" s="112"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="113"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="30">
@@ -17640,12 +17640,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="116"/>
     </row>
     <row r="3" spans="1:4" ht="13.5" thickBot="1">
       <c r="A3" s="22" t="s">
@@ -17702,12 +17702,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="114" t="s">
         <v>249</v>
       </c>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="115"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="116"/>
     </row>
     <row r="8" spans="1:4" ht="13.5" thickBot="1">
       <c r="A8" s="22" t="s">
@@ -17766,12 +17766,12 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A12" s="113" t="s">
+      <c r="A12" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="115"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="116"/>
     </row>
     <row r="13" spans="1:4" ht="13.5" thickBot="1">
       <c r="A13" s="22" t="s">
@@ -17870,12 +17870,12 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="114" t="s">
         <v>272</v>
       </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="115"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="115"/>
+      <c r="D20" s="116"/>
     </row>
     <row r="21" spans="1:4" ht="13.5" thickBot="1">
       <c r="A21" s="22" t="s">
@@ -18004,12 +18004,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A30" s="113" t="s">
+      <c r="A30" s="114" t="s">
         <v>285</v>
       </c>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="115"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="115"/>
+      <c r="D30" s="116"/>
     </row>
     <row r="31" spans="1:4" ht="13.5" thickBot="1">
       <c r="A31" s="22" t="s">
@@ -18084,12 +18084,12 @@
       <c r="D36" s="28"/>
     </row>
     <row r="37" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A37" s="113" t="s">
+      <c r="A37" s="114" t="s">
         <v>292</v>
       </c>
-      <c r="B37" s="114"/>
-      <c r="C37" s="114"/>
-      <c r="D37" s="115"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="116"/>
     </row>
     <row r="38" spans="1:4" ht="13.5" thickBot="1">
       <c r="A38" s="22" t="s">
@@ -18176,12 +18176,12 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A44" s="113" t="s">
+      <c r="A44" s="114" t="s">
         <v>305</v>
       </c>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="115"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="116"/>
     </row>
     <row r="45" spans="1:4" ht="13.5" thickBot="1">
       <c r="A45" s="22" t="s">
@@ -18198,12 +18198,12 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A46" s="113" t="s">
+      <c r="A46" s="114" t="s">
         <v>308</v>
       </c>
-      <c r="B46" s="114"/>
-      <c r="C46" s="114"/>
-      <c r="D46" s="115"/>
+      <c r="B46" s="115"/>
+      <c r="C46" s="115"/>
+      <c r="D46" s="116"/>
     </row>
     <row r="47" spans="1:4" ht="13.5" thickBot="1">
       <c r="A47" s="22" t="s">
@@ -18248,12 +18248,12 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A50" s="113" t="s">
+      <c r="A50" s="114" t="s">
         <v>315</v>
       </c>
-      <c r="B50" s="114"/>
-      <c r="C50" s="114"/>
-      <c r="D50" s="115"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="115"/>
+      <c r="D50" s="116"/>
     </row>
     <row r="51" spans="1:4" ht="13.5" thickBot="1">
       <c r="A51" s="22" t="s">
@@ -19428,8 +19428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358A137-1626-9343-A399-452BA3D3C6F7}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="164" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -19518,13 +19518,13 @@
       <c r="B9">
         <v>0.08</v>
       </c>
-      <c r="C9" s="116" t="s">
+      <c r="C9" s="117" t="s">
         <v>533</v>
       </c>
-      <c r="D9" s="116" t="s">
+      <c r="D9" s="117" t="s">
         <v>534</v>
       </c>
-      <c r="E9" s="116" t="s">
+      <c r="E9" s="117" t="s">
         <v>537</v>
       </c>
     </row>
@@ -19535,9 +19535,9 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
+      <c r="C10" s="117"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="117"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
@@ -19546,9 +19546,9 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
@@ -19557,20 +19557,20 @@
       <c r="B12">
         <v>0.22343911000453887</v>
       </c>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="B13" s="117">
+      <c r="B13" s="89">
         <v>0.182369</v>
       </c>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
@@ -19579,9 +19579,9 @@
       <c r="B14">
         <v>0.63897814563472732</v>
       </c>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="116"/>
+      <c r="C14" s="117"/>
+      <c r="D14" s="117"/>
+      <c r="E14" s="117"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
@@ -19590,9 +19590,9 @@
       <c r="B15">
         <v>0.65783791594766872</v>
       </c>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
+      <c r="E15" s="117"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
@@ -19601,7 +19601,7 @@
       <c r="B16">
         <v>0.05</v>
       </c>
-      <c r="C16" s="116"/>
+      <c r="C16" s="117"/>
       <c r="D16" t="s">
         <v>538</v>
       </c>

</xml_diff>

<commit_message>
Fix A751 replacement period ; Separate A751 to RPV and Core Barrel.
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\mouse\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77BEB7A-F0FA-444D-83F2-92C33FE03E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420E76B7-1038-4A67-8FE9-B04B26A2BCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Database'!$A$1:$Z$164</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Database'!$A$1:$Z$165</definedName>
     <definedName name="CRF">#REF!</definedName>
     <definedName name="DiscountRate">#REF!</definedName>
     <definedName name="FacilityLifetime">#REF!</definedName>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="541">
   <si>
     <t>Account</t>
   </si>
@@ -1898,9 +1898,6 @@
     <t>Integrated Heat Transfer Vessel Mass</t>
   </si>
   <si>
-    <t>Annualized Vessel Replacements</t>
-  </si>
-  <si>
     <t>Annualized Moderator Replacements</t>
   </si>
   <si>
@@ -1994,6 +1991,12 @@
   </si>
   <si>
     <t>Non-nuclear off-the-shelf</t>
+  </si>
+  <si>
+    <t>Annualized Core Barrel Replacements</t>
+  </si>
+  <si>
+    <t>Annualized RPV Replacements</t>
   </si>
 </sst>
 </file>
@@ -2631,39 +2634,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2671,6 +2641,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2689,6 +2671,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2724,13 +2727,6 @@
   </cellStyles>
   <dxfs count="108">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2740,6 +2736,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2784,9 +2787,15 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2798,15 +2807,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2927,14 +2930,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2947,7 +2943,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2966,58 +2969,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3035,13 +2988,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3050,8 +2996,31 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3065,6 +3034,40 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3102,13 +3105,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3117,14 +3113,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3134,26 +3123,6 @@
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3183,18 +3152,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
-        <i/>
+        <i val="0"/>
       </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3208,8 +3181,17 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
       </fill>
     </dxf>
     <dxf>
@@ -3217,6 +3199,27 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3335,56 +3338,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3416,6 +3372,32 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3439,6 +3421,27 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3598,16 +3601,16 @@
       <sheetName val="Factory Fabricated Learning Rat"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
       <sheetData sheetId="10">
         <row r="3">
           <cell r="Q3">
@@ -3984,13 +3987,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
-  <dimension ref="A1:AH164"/>
+  <dimension ref="A1:AH165"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="T71" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H148" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U85" sqref="U85:U86"/>
+      <selection pane="bottomRight" activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -4221,10 +4224,10 @@
       <c r="Q3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="93" t="s">
+      <c r="R3" s="94" t="s">
         <v>445</v>
       </c>
-      <c r="S3" s="99" t="s">
+      <c r="S3" s="96" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4311,8 +4314,8 @@
       <c r="Q4" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="93"/>
-      <c r="S4" s="99"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="96"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>467</v>
@@ -4391,10 +4394,10 @@
       <c r="Q5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="93" t="s">
+      <c r="R5" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="99" t="s">
+      <c r="S5" s="96" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4474,8 +4477,8 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="93"/>
-      <c r="S6" s="99"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="96"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>467</v>
@@ -4781,13 +4784,13 @@
       <c r="P11" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="93" t="s">
+      <c r="Q11" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="93" t="s">
+      <c r="R11" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="100" t="s">
+      <c r="S11" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -4878,9 +4881,9 @@
       <c r="P12" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="93"/>
-      <c r="S12" s="99"/>
+      <c r="Q12" s="94"/>
+      <c r="R12" s="94"/>
+      <c r="S12" s="96"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>470</v>
@@ -4962,9 +4965,9 @@
       <c r="P13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="99"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="94"/>
+      <c r="S13" s="96"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>470</v>
@@ -5089,13 +5092,13 @@
       <c r="P15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="93" t="s">
+      <c r="Q15" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="93" t="s">
+      <c r="R15" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="100" t="s">
+      <c r="S15" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5179,9 +5182,9 @@
       <c r="P16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="99"/>
+      <c r="Q16" s="94"/>
+      <c r="R16" s="94"/>
+      <c r="S16" s="96"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>470</v>
@@ -5263,9 +5266,9 @@
       <c r="P17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="93"/>
-      <c r="R17" s="93"/>
-      <c r="S17" s="99"/>
+      <c r="Q17" s="94"/>
+      <c r="R17" s="94"/>
+      <c r="S17" s="96"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>470</v>
@@ -5314,7 +5317,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D18" s="41" t="str">
         <f>REPT("   ", B18*2) &amp; C18</f>
@@ -5335,16 +5338,16 @@
         <v>6491.9267043635973</v>
       </c>
       <c r="J18" s="47" t="s">
+        <v>517</v>
+      </c>
+      <c r="K18" s="49" t="s">
         <v>518</v>
-      </c>
-      <c r="K18" s="49" t="s">
-        <v>519</v>
       </c>
       <c r="L18" s="48">
         <v>9373</v>
       </c>
       <c r="M18" s="47" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N18" s="48">
         <v>1</v>
@@ -5356,13 +5359,13 @@
         <v>77</v>
       </c>
       <c r="Q18" s="49" t="s">
+        <v>514</v>
+      </c>
+      <c r="R18" s="49" t="s">
+        <v>514</v>
+      </c>
+      <c r="S18" s="88" t="s">
         <v>515</v>
-      </c>
-      <c r="R18" s="49" t="s">
-        <v>515</v>
-      </c>
-      <c r="S18" s="88" t="s">
-        <v>516</v>
       </c>
       <c r="T18" s="51"/>
       <c r="U18" s="80" t="s">
@@ -5412,7 +5415,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D19" s="41" t="str">
         <f>REPT("   ", B19*2) &amp; C19</f>
@@ -5454,13 +5457,13 @@
         <v>77</v>
       </c>
       <c r="Q19" s="49" t="s">
+        <v>514</v>
+      </c>
+      <c r="R19" s="49" t="s">
+        <v>514</v>
+      </c>
+      <c r="S19" s="88" t="s">
         <v>515</v>
-      </c>
-      <c r="R19" s="49" t="s">
-        <v>515</v>
-      </c>
-      <c r="S19" s="88" t="s">
-        <v>516</v>
       </c>
       <c r="T19" s="51"/>
       <c r="U19" s="80" t="s">
@@ -5629,13 +5632,13 @@
       <c r="P22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="93" t="s">
+      <c r="Q22" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="93" t="s">
+      <c r="R22" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="100" t="s">
+      <c r="S22" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5719,9 +5722,9 @@
       <c r="P23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="99"/>
+      <c r="Q23" s="94"/>
+      <c r="R23" s="94"/>
+      <c r="S23" s="96"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>470</v>
@@ -5803,9 +5806,9 @@
       <c r="P24" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="99"/>
+      <c r="Q24" s="94"/>
+      <c r="R24" s="94"/>
+      <c r="S24" s="96"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>470</v>
@@ -5930,13 +5933,13 @@
       <c r="P26" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="93" t="s">
+      <c r="Q26" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R26" s="93" t="s">
+      <c r="R26" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="100" t="s">
+      <c r="S26" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -6020,9 +6023,9 @@
       <c r="P27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="93"/>
-      <c r="S27" s="99"/>
+      <c r="Q27" s="94"/>
+      <c r="R27" s="94"/>
+      <c r="S27" s="96"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>470</v>
@@ -6104,9 +6107,9 @@
       <c r="P28" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="93"/>
-      <c r="S28" s="99"/>
+      <c r="Q28" s="94"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="96"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>470</v>
@@ -6155,7 +6158,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D29" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6198,7 +6201,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D30" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6222,7 +6225,7 @@
         <v>79</v>
       </c>
       <c r="K30" s="49" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L30" s="48"/>
       <c r="M30" s="47" t="s">
@@ -6235,13 +6238,13 @@
       <c r="P30" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="93" t="s">
+      <c r="Q30" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="93" t="s">
+      <c r="R30" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="100" t="s">
+      <c r="S30" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6292,7 +6295,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D31" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6316,7 +6319,7 @@
         <v>79</v>
       </c>
       <c r="K31" s="49" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L31" s="48"/>
       <c r="M31" s="47" t="s">
@@ -6329,9 +6332,9 @@
       <c r="P31" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="99"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="96"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>470</v>
@@ -6380,7 +6383,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D32" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6404,7 +6407,7 @@
         <v>79</v>
       </c>
       <c r="K32" s="49" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L32" s="48"/>
       <c r="M32" s="47" t="s">
@@ -6417,9 +6420,9 @@
       <c r="P32" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="93"/>
-      <c r="S32" s="99"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="96"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>470</v>
@@ -6468,7 +6471,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D33" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6489,16 +6492,16 @@
         <v>6491.9267043635973</v>
       </c>
       <c r="J33" s="47" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K33" s="49" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L33" s="48">
         <v>9373</v>
       </c>
       <c r="M33" s="47" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N33" s="48">
         <v>1</v>
@@ -6510,13 +6513,13 @@
         <v>77</v>
       </c>
       <c r="Q33" s="49" t="s">
+        <v>514</v>
+      </c>
+      <c r="R33" s="49" t="s">
+        <v>514</v>
+      </c>
+      <c r="S33" s="88" t="s">
         <v>515</v>
-      </c>
-      <c r="R33" s="49" t="s">
-        <v>515</v>
-      </c>
-      <c r="S33" s="88" t="s">
-        <v>516</v>
       </c>
       <c r="T33" s="51"/>
       <c r="U33" s="80" t="s">
@@ -6728,13 +6731,13 @@
       <c r="P37" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q37" s="93" t="s">
+      <c r="Q37" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R37" s="93" t="s">
+      <c r="R37" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="100" t="s">
+      <c r="S37" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -6818,9 +6821,9 @@
       <c r="P38" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="93"/>
-      <c r="R38" s="93"/>
-      <c r="S38" s="99"/>
+      <c r="Q38" s="94"/>
+      <c r="R38" s="94"/>
+      <c r="S38" s="96"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>470</v>
@@ -6902,9 +6905,9 @@
       <c r="P39" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="93"/>
-      <c r="R39" s="93"/>
-      <c r="S39" s="99"/>
+      <c r="Q39" s="94"/>
+      <c r="R39" s="94"/>
+      <c r="S39" s="96"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>470</v>
@@ -7029,13 +7032,13 @@
       <c r="P41" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="93" t="s">
+      <c r="Q41" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="93" t="s">
+      <c r="R41" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="100" t="s">
+      <c r="S41" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7119,9 +7122,9 @@
       <c r="P42" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="93"/>
-      <c r="R42" s="93"/>
-      <c r="S42" s="99"/>
+      <c r="Q42" s="94"/>
+      <c r="R42" s="94"/>
+      <c r="S42" s="96"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>470</v>
@@ -7203,9 +7206,9 @@
       <c r="P43" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q43" s="93"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="99"/>
+      <c r="Q43" s="94"/>
+      <c r="R43" s="94"/>
+      <c r="S43" s="96"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>470</v>
@@ -7373,13 +7376,13 @@
       <c r="P46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="93" t="s">
+      <c r="Q46" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R46" s="93" t="s">
+      <c r="R46" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="100" t="s">
+      <c r="S46" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
@@ -7463,9 +7466,9 @@
       <c r="P47" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="93"/>
-      <c r="R47" s="93"/>
-      <c r="S47" s="99"/>
+      <c r="Q47" s="94"/>
+      <c r="R47" s="94"/>
+      <c r="S47" s="96"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
         <v>466</v>
@@ -7547,9 +7550,9 @@
       <c r="P48" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q48" s="93"/>
-      <c r="R48" s="93"/>
-      <c r="S48" s="99"/>
+      <c r="Q48" s="94"/>
+      <c r="R48" s="94"/>
+      <c r="S48" s="96"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
         <v>466</v>
@@ -7816,16 +7819,16 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="96" t="s">
+      <c r="Q52" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="R52" s="96" t="s">
+      <c r="R52" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="105" t="s">
+      <c r="S52" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="101" t="s">
+      <c r="T52" s="90" t="s">
         <v>503</v>
       </c>
       <c r="U52" s="80" t="s">
@@ -7912,10 +7915,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="97"/>
-      <c r="R53" s="97"/>
-      <c r="S53" s="106"/>
-      <c r="T53" s="102"/>
+      <c r="Q53" s="105"/>
+      <c r="R53" s="105"/>
+      <c r="S53" s="99"/>
+      <c r="T53" s="91"/>
       <c r="U53" s="80" t="s">
         <v>470</v>
       </c>
@@ -8000,10 +8003,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="98"/>
-      <c r="R54" s="98"/>
-      <c r="S54" s="107"/>
-      <c r="T54" s="103"/>
+      <c r="Q54" s="106"/>
+      <c r="R54" s="106"/>
+      <c r="S54" s="100"/>
+      <c r="T54" s="92"/>
       <c r="U54" s="80" t="s">
         <v>470</v>
       </c>
@@ -8170,13 +8173,13 @@
       <c r="P57" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q57" s="93" t="s">
+      <c r="Q57" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R57" s="93" t="s">
+      <c r="R57" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="100" t="s">
+      <c r="S57" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8260,9 +8263,9 @@
       <c r="P58" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q58" s="93"/>
-      <c r="R58" s="93"/>
-      <c r="S58" s="99"/>
+      <c r="Q58" s="94"/>
+      <c r="R58" s="94"/>
+      <c r="S58" s="96"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>470</v>
@@ -8344,9 +8347,9 @@
       <c r="P59" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q59" s="93"/>
-      <c r="R59" s="93"/>
-      <c r="S59" s="99"/>
+      <c r="Q59" s="94"/>
+      <c r="R59" s="94"/>
+      <c r="S59" s="96"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>470</v>
@@ -8471,13 +8474,13 @@
       <c r="P61" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q61" s="93" t="s">
+      <c r="Q61" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R61" s="93" t="s">
+      <c r="R61" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="100" t="s">
+      <c r="S61" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8561,9 +8564,9 @@
       <c r="P62" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="99"/>
+      <c r="Q62" s="94"/>
+      <c r="R62" s="94"/>
+      <c r="S62" s="96"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>470</v>
@@ -8645,9 +8648,9 @@
       <c r="P63" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q63" s="93"/>
-      <c r="R63" s="93"/>
-      <c r="S63" s="99"/>
+      <c r="Q63" s="94"/>
+      <c r="R63" s="94"/>
+      <c r="S63" s="96"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>470</v>
@@ -8954,7 +8957,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="94" t="s">
+      <c r="R68" s="93" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -9043,7 +9046,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="94"/>
+      <c r="R69" s="93"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9137,7 +9140,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="94"/>
+      <c r="R70" s="93"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9224,7 +9227,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="94"/>
+      <c r="R71" s="93"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9313,7 +9316,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="94"/>
+      <c r="R72" s="93"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9407,7 +9410,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="94"/>
+      <c r="R73" s="93"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9577,10 +9580,10 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="94" t="s">
+      <c r="R76" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="104" t="s">
+      <c r="S76" s="97" t="s">
         <v>447</v>
       </c>
       <c r="T76" s="61" t="s">
@@ -9667,8 +9670,8 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="94"/>
-      <c r="S77" s="104"/>
+      <c r="R77" s="93"/>
+      <c r="S77" s="97"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
         <v>466</v>
@@ -9762,8 +9765,8 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="94"/>
-      <c r="S78" s="104"/>
+      <c r="R78" s="93"/>
+      <c r="S78" s="97"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
         <v>466</v>
@@ -9856,8 +9859,8 @@
       <c r="Q79" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="R79" s="94"/>
-      <c r="S79" s="104"/>
+      <c r="R79" s="93"/>
+      <c r="S79" s="97"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
         <v>466</v>
@@ -9951,11 +9954,11 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="94"/>
-      <c r="S80" s="104"/>
+      <c r="R80" s="93"/>
+      <c r="S80" s="97"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="V80" s="84">
         <f t="shared" ref="V80:V143" si="25">0.9*$H80</f>
@@ -10050,7 +10053,7 @@
       <c r="S81" s="67"/>
       <c r="T81" s="51"/>
       <c r="U81" s="80" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="V81" s="84">
         <f t="shared" si="25"/>
@@ -10376,12 +10379,12 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="104" t="s">
+      <c r="S85" s="97" t="s">
         <v>447</v>
       </c>
       <c r="T85" s="51"/>
       <c r="U85" s="80" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="V85" s="84">
         <f t="shared" si="25"/>
@@ -10482,10 +10485,10 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="104"/>
+      <c r="S86" s="97"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="V86" s="84">
         <f t="shared" si="25"/>
@@ -10578,7 +10581,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="104"/>
+      <c r="S87" s="97"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>466</v>
@@ -10672,7 +10675,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="104"/>
+      <c r="S88" s="97"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>466</v>
@@ -10741,7 +10744,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="104"/>
+      <c r="S89" s="97"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -10813,7 +10816,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="104"/>
+      <c r="S90" s="97"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>466</v>
@@ -10907,7 +10910,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="104"/>
+      <c r="S91" s="97"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>466</v>
@@ -11271,13 +11274,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="94" t="s">
+      <c r="R96" s="93" t="s">
         <v>448</v>
       </c>
-      <c r="S96" s="108" t="s">
+      <c r="S96" s="101" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="94"/>
+      <c r="T96" s="93"/>
       <c r="U96" s="80" t="s">
         <v>466</v>
       </c>
@@ -11364,9 +11367,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="94"/>
-      <c r="S97" s="109"/>
-      <c r="T97" s="94"/>
+      <c r="R97" s="93"/>
+      <c r="S97" s="102"/>
+      <c r="T97" s="93"/>
       <c r="U97" s="80" t="s">
         <v>466</v>
       </c>
@@ -12200,7 +12203,7 @@
         <v>360</v>
       </c>
       <c r="S107" s="87"/>
-      <c r="T107" s="90" t="s">
+      <c r="T107" s="107" t="s">
         <v>506</v>
       </c>
       <c r="U107" s="80" t="s">
@@ -12298,7 +12301,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="91"/>
+      <c r="T108" s="108"/>
       <c r="U108" s="80" t="s">
         <v>466</v>
       </c>
@@ -12783,7 +12786,7 @@
         <v>227</v>
       </c>
       <c r="B115" s="40">
-        <f t="shared" ref="B115:B164" si="53">IF(ISNUMBER(A115),
+        <f t="shared" ref="B115:B165" si="53">IF(ISNUMBER(A115),
     IF(AND(A115=INT(A115), MOD(A115, 10) = 0), 0,
         IF(AND(A115=INT(A115), LEN(A115)=2), 1,
             IF(AND(A115=INT(A115), LEN(A115)=3), 2,
@@ -12797,7 +12800,7 @@
         <v>20</v>
       </c>
       <c r="D115" s="41" t="str">
-        <f t="shared" ref="D115:D164" si="54">REPT("   ", B115*2) &amp; C115</f>
+        <f t="shared" ref="D115:D165" si="54">REPT("   ", B115*2) &amp; C115</f>
         <v xml:space="preserve">            Reactor Instrumentation and Control (I&amp;C)</v>
       </c>
       <c r="E115" s="41" t="s">
@@ -13090,7 +13093,7 @@
       </c>
       <c r="T119" s="51"/>
       <c r="U119" s="80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V119" s="84">
         <f t="shared" si="25"/>
@@ -13299,16 +13302,16 @@
       <c r="P122" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q122" s="95" t="s">
+      <c r="Q122" s="103" t="s">
         <v>427</v>
       </c>
-      <c r="R122" s="95" t="s">
+      <c r="R122" s="103" t="s">
         <v>365</v>
       </c>
       <c r="S122" s="51"/>
       <c r="T122" s="51"/>
       <c r="U122" s="80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V122" s="84">
         <f t="shared" si="25"/>
@@ -13391,12 +13394,12 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="95"/>
-      <c r="R123" s="95"/>
+      <c r="Q123" s="103"/>
+      <c r="R123" s="103"/>
       <c r="S123" s="51"/>
       <c r="T123" s="51"/>
       <c r="U123" s="80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V123" s="84">
         <f t="shared" si="25"/>
@@ -13479,12 +13482,12 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="95"/>
-      <c r="R124" s="95"/>
+      <c r="Q124" s="103"/>
+      <c r="R124" s="103"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V124" s="84">
         <f t="shared" si="25"/>
@@ -13567,12 +13570,12 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="95"/>
-      <c r="R125" s="95"/>
+      <c r="Q125" s="103"/>
+      <c r="R125" s="103"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V125" s="84">
         <f t="shared" si="25"/>
@@ -13655,12 +13658,12 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="95"/>
-      <c r="R126" s="95"/>
+      <c r="Q126" s="103"/>
+      <c r="R126" s="103"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V126" s="84">
         <f t="shared" si="25"/>
@@ -13743,12 +13746,12 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="95"/>
-      <c r="R127" s="95"/>
+      <c r="Q127" s="103"/>
+      <c r="R127" s="103"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V127" s="84">
         <f t="shared" si="25"/>
@@ -13867,10 +13870,10 @@
       <c r="P129" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q129" s="94" t="s">
+      <c r="Q129" s="93" t="s">
         <v>369</v>
       </c>
-      <c r="R129" s="94" t="s">
+      <c r="R129" s="93" t="s">
         <v>370</v>
       </c>
       <c r="S129" s="51"/>
@@ -13952,8 +13955,8 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="94"/>
-      <c r="R130" s="94"/>
+      <c r="Q130" s="93"/>
+      <c r="R130" s="93"/>
       <c r="S130" s="51"/>
       <c r="T130" s="51"/>
       <c r="U130" s="80" t="s">
@@ -14035,8 +14038,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="94"/>
-      <c r="R131" s="94"/>
+      <c r="Q131" s="93"/>
+      <c r="R131" s="93"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14120,8 +14123,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="94"/>
-      <c r="R132" s="94"/>
+      <c r="Q132" s="93"/>
+      <c r="R132" s="93"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14212,8 +14215,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="94"/>
-      <c r="R133" s="94"/>
+      <c r="Q133" s="93"/>
+      <c r="R133" s="93"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -14505,7 +14508,7 @@
       <c r="P138" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q138" s="93" t="s">
+      <c r="Q138" s="94" t="s">
         <v>364</v>
       </c>
       <c r="R138" s="48"/>
@@ -14585,7 +14588,7 @@
       <c r="P139" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q139" s="93"/>
+      <c r="Q139" s="94"/>
       <c r="R139" s="48"/>
       <c r="S139" s="48"/>
       <c r="T139" s="48"/>
@@ -14663,7 +14666,7 @@
       <c r="P140" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q140" s="93"/>
+      <c r="Q140" s="94"/>
       <c r="R140" s="51"/>
       <c r="S140" s="51"/>
       <c r="T140" s="51"/>
@@ -14741,7 +14744,7 @@
       <c r="P141" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q141" s="93"/>
+      <c r="Q141" s="94"/>
       <c r="R141" s="51"/>
       <c r="S141" s="51"/>
       <c r="T141" s="51"/>
@@ -15130,22 +15133,22 @@
         <v>467</v>
       </c>
       <c r="V148" s="84">
-        <f t="shared" ref="V148:V164" si="57">0.9*$H148</f>
+        <f t="shared" ref="V148:V165" si="57">0.9*$H148</f>
         <v>0</v>
       </c>
       <c r="W148" s="84">
-        <f t="shared" ref="W148:W164" si="58">1.5*H148</f>
+        <f t="shared" ref="W148:W165" si="58">1.5*H148</f>
         <v>0</v>
       </c>
       <c r="X148" s="80" t="s">
         <v>450</v>
       </c>
       <c r="Y148" s="83">
-        <f t="shared" ref="Y148:Y164" si="59">0.9*I148</f>
+        <f t="shared" ref="Y148:Y165" si="59">0.9*I148</f>
         <v>160650</v>
       </c>
       <c r="Z148" s="83">
-        <f t="shared" ref="Z148:Z164" si="60">1.3*I148</f>
+        <f t="shared" ref="Z148:Z165" si="60">1.3*I148</f>
         <v>232050</v>
       </c>
       <c r="AA148" s="80" t="s">
@@ -15544,11 +15547,11 @@
         <v>2</v>
       </c>
       <c r="C154" s="58" t="s">
-        <v>508</v>
+        <v>540</v>
       </c>
       <c r="D154" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Vessel Replacements</v>
+        <v xml:space="preserve">            Annualized RPV Replacements</v>
       </c>
       <c r="E154" s="41"/>
       <c r="F154" s="41"/>
@@ -15562,14 +15565,14 @@
       <c r="N154" s="51"/>
       <c r="O154" s="68"/>
       <c r="P154" s="51"/>
-      <c r="Q154" s="90" t="s">
+      <c r="Q154" s="107" t="s">
         <v>500</v>
       </c>
-      <c r="R154" s="90" t="s">
+      <c r="R154" s="107" t="s">
         <v>500</v>
       </c>
       <c r="S154" s="51"/>
-      <c r="T154" s="90" t="s">
+      <c r="T154" s="107" t="s">
         <v>501</v>
       </c>
       <c r="U154" s="80"/>
@@ -15584,7 +15587,7 @@
       <c r="AD154" s="83"/>
       <c r="AE154" s="80"/>
     </row>
-    <row r="155" spans="1:31" ht="25.5">
+    <row r="155" spans="1:31" ht="12.75" customHeight="1">
       <c r="A155" s="39">
         <v>752</v>
       </c>
@@ -15593,11 +15596,11 @@
         <v>2</v>
       </c>
       <c r="C155" s="58" t="s">
-        <v>509</v>
+        <v>539</v>
       </c>
       <c r="D155" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Moderator Replacements</v>
+        <v xml:space="preserve">            Annualized Core Barrel Replacements</v>
       </c>
       <c r="E155" s="41"/>
       <c r="F155" s="41"/>
@@ -15611,10 +15614,10 @@
       <c r="N155" s="51"/>
       <c r="O155" s="68"/>
       <c r="P155" s="51"/>
-      <c r="Q155" s="92"/>
-      <c r="R155" s="92"/>
+      <c r="Q155" s="109"/>
+      <c r="R155" s="109"/>
       <c r="S155" s="51"/>
-      <c r="T155" s="92"/>
+      <c r="T155" s="109"/>
       <c r="U155" s="80"/>
       <c r="V155" s="84"/>
       <c r="W155" s="84"/>
@@ -15627,7 +15630,7 @@
       <c r="AD155" s="83"/>
       <c r="AE155" s="80"/>
     </row>
-    <row r="156" spans="1:31">
+    <row r="156" spans="1:31" ht="25.5">
       <c r="A156" s="39">
         <v>753</v>
       </c>
@@ -15636,11 +15639,11 @@
         <v>2</v>
       </c>
       <c r="C156" s="58" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D156" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Reflector Replacements</v>
+        <v xml:space="preserve">            Annualized Moderator Replacements</v>
       </c>
       <c r="E156" s="41"/>
       <c r="F156" s="41"/>
@@ -15654,10 +15657,10 @@
       <c r="N156" s="51"/>
       <c r="O156" s="68"/>
       <c r="P156" s="51"/>
-      <c r="Q156" s="92"/>
-      <c r="R156" s="92"/>
+      <c r="Q156" s="109"/>
+      <c r="R156" s="109"/>
       <c r="S156" s="51"/>
-      <c r="T156" s="92"/>
+      <c r="T156" s="109"/>
       <c r="U156" s="80"/>
       <c r="V156" s="84"/>
       <c r="W156" s="84"/>
@@ -15670,7 +15673,7 @@
       <c r="AD156" s="83"/>
       <c r="AE156" s="80"/>
     </row>
-    <row r="157" spans="1:31" ht="25.5">
+    <row r="157" spans="1:31">
       <c r="A157" s="39">
         <v>754</v>
       </c>
@@ -15679,11 +15682,11 @@
         <v>2</v>
       </c>
       <c r="C157" s="58" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D157" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Reactivity Control Replacements</v>
+        <v xml:space="preserve">            Annualized Reflector Replacements</v>
       </c>
       <c r="E157" s="41"/>
       <c r="F157" s="41"/>
@@ -15697,10 +15700,10 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="92"/>
-      <c r="R157" s="92"/>
+      <c r="Q157" s="109"/>
+      <c r="R157" s="109"/>
       <c r="S157" s="51"/>
-      <c r="T157" s="92"/>
+      <c r="T157" s="109"/>
       <c r="U157" s="80"/>
       <c r="V157" s="84"/>
       <c r="W157" s="84"/>
@@ -15722,11 +15725,11 @@
         <v>2</v>
       </c>
       <c r="C158" s="58" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D158" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Integrated Heat Transfer System Replacements</v>
+        <v xml:space="preserve">            Annualized Reactivity Control Replacements</v>
       </c>
       <c r="E158" s="41"/>
       <c r="F158" s="41"/>
@@ -15740,10 +15743,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="92"/>
-      <c r="R158" s="92"/>
+      <c r="Q158" s="109"/>
+      <c r="R158" s="109"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="92"/>
+      <c r="T158" s="109"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -15756,20 +15759,20 @@
       <c r="AD158" s="83"/>
       <c r="AE158" s="80"/>
     </row>
-    <row r="159" spans="1:31" ht="25.5" customHeight="1">
+    <row r="159" spans="1:31" ht="25.5">
       <c r="A159" s="39">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B159" s="40">
         <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="C159" s="58" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D159" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Misc. Replacements</v>
+        <v xml:space="preserve">            Annualized Integrated Heat Transfer System Replacements</v>
       </c>
       <c r="E159" s="41"/>
       <c r="F159" s="41"/>
@@ -15783,10 +15786,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="91"/>
-      <c r="R159" s="91"/>
+      <c r="Q159" s="109"/>
+      <c r="R159" s="109"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="91"/>
+      <c r="T159" s="109"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -15799,46 +15802,37 @@
       <c r="AD159" s="83"/>
       <c r="AE159" s="80"/>
     </row>
-    <row r="160" spans="1:31" ht="30" customHeight="1">
+    <row r="160" spans="1:31" ht="25.5" customHeight="1">
       <c r="A160" s="39">
-        <v>78</v>
+        <v>759</v>
       </c>
       <c r="B160" s="40">
-        <f t="shared" ref="B160" si="65">IF(ISNUMBER(A160),
-    IF(AND(A160=INT(A160), MOD(A160, 10) = 0), 0,
-        IF(AND(A160=INT(A160), LEN(A160)=2), 1,
-            IF(AND(A160=INT(A160), LEN(A160)=3), 2,
-                LEN(A160) - FIND(".", A160) + 2)
-        )
-    ),
-"")</f>
-        <v>1</v>
+        <f t="shared" si="53"/>
+        <v>2</v>
       </c>
       <c r="C160" s="58" t="s">
-        <v>42</v>
+        <v>512</v>
       </c>
       <c r="D160" s="41" t="str">
-        <f t="shared" ref="D160" si="66">REPT("   ", B160*2) &amp; C160</f>
-        <v xml:space="preserve">      Annualized Decommissioning Cost</v>
+        <f t="shared" si="54"/>
+        <v xml:space="preserve">            Annualized Misc. Replacements</v>
       </c>
       <c r="E160" s="41"/>
       <c r="F160" s="41"/>
       <c r="G160" s="41"/>
       <c r="H160" s="45"/>
-      <c r="I160" s="75"/>
+      <c r="I160" s="63"/>
       <c r="J160" s="51"/>
-      <c r="K160" s="47"/>
+      <c r="K160" s="61"/>
       <c r="L160" s="51"/>
       <c r="M160" s="51"/>
       <c r="N160" s="51"/>
       <c r="O160" s="68"/>
-      <c r="P160" s="76"/>
-      <c r="Q160" s="61"/>
-      <c r="R160" s="61"/>
+      <c r="P160" s="51"/>
+      <c r="Q160" s="108"/>
+      <c r="R160" s="108"/>
       <c r="S160" s="51"/>
-      <c r="T160" s="61" t="s">
-        <v>499</v>
-      </c>
+      <c r="T160" s="108"/>
       <c r="U160" s="80"/>
       <c r="V160" s="84"/>
       <c r="W160" s="84"/>
@@ -15851,37 +15845,46 @@
       <c r="AD160" s="83"/>
       <c r="AE160" s="80"/>
     </row>
-    <row r="161" spans="1:31">
+    <row r="161" spans="1:31" ht="30" customHeight="1">
       <c r="A161" s="39">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B161" s="40">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="C161" s="74" t="s">
-        <v>43</v>
+        <f t="shared" ref="B161" si="65">IF(ISNUMBER(A161),
+    IF(AND(A161=INT(A161), MOD(A161, 10) = 0), 0,
+        IF(AND(A161=INT(A161), LEN(A161)=2), 1,
+            IF(AND(A161=INT(A161), LEN(A161)=3), 2,
+                LEN(A161) - FIND(".", A161) + 2)
+        )
+    ),
+"")</f>
+        <v>1</v>
+      </c>
+      <c r="C161" s="58" t="s">
+        <v>42</v>
       </c>
       <c r="D161" s="41" t="str">
-        <f t="shared" si="54"/>
-        <v>Annualized Fuel Cost</v>
+        <f t="shared" ref="D161" si="66">REPT("   ", B161*2) &amp; C161</f>
+        <v xml:space="preserve">      Annualized Decommissioning Cost</v>
       </c>
       <c r="E161" s="41"/>
       <c r="F161" s="41"/>
       <c r="G161" s="41"/>
-      <c r="H161" s="42"/>
-      <c r="I161" s="42"/>
-      <c r="J161" s="40"/>
-      <c r="K161" s="43"/>
-      <c r="L161" s="40"/>
-      <c r="M161" s="40"/>
-      <c r="N161" s="40"/>
-      <c r="O161" s="42"/>
-      <c r="P161" s="40"/>
-      <c r="Q161" s="43"/>
-      <c r="R161" s="40"/>
-      <c r="S161" s="40"/>
-      <c r="T161" s="40"/>
+      <c r="H161" s="45"/>
+      <c r="I161" s="75"/>
+      <c r="J161" s="51"/>
+      <c r="K161" s="47"/>
+      <c r="L161" s="51"/>
+      <c r="M161" s="51"/>
+      <c r="N161" s="51"/>
+      <c r="O161" s="68"/>
+      <c r="P161" s="76"/>
+      <c r="Q161" s="61"/>
+      <c r="R161" s="61"/>
+      <c r="S161" s="51"/>
+      <c r="T161" s="61" t="s">
+        <v>499</v>
+      </c>
       <c r="U161" s="80"/>
       <c r="V161" s="84"/>
       <c r="W161" s="84"/>
@@ -15894,253 +15897,268 @@
       <c r="AD161" s="83"/>
       <c r="AE161" s="80"/>
     </row>
-    <row r="162" spans="1:31" ht="89.25">
+    <row r="162" spans="1:31">
       <c r="A162" s="39">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B162" s="40">
         <f t="shared" si="53"/>
-        <v>1</v>
-      </c>
-      <c r="C162" s="58" t="s">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="C162" s="74" t="s">
+        <v>43</v>
       </c>
       <c r="D162" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">      Refueling Operations</v>
-      </c>
-      <c r="E162" s="41" t="s">
-        <v>342</v>
-      </c>
+        <v>Annualized Fuel Cost</v>
+      </c>
+      <c r="E162" s="41"/>
       <c r="F162" s="41"/>
       <c r="G162" s="41"/>
-      <c r="H162" s="45"/>
-      <c r="I162" s="63">
-        <v>178500</v>
-      </c>
-      <c r="J162" s="51" t="s">
-        <v>383</v>
-      </c>
-      <c r="K162" s="61" t="s">
-        <v>384</v>
-      </c>
-      <c r="L162" s="51"/>
-      <c r="M162" s="51"/>
-      <c r="N162" s="51">
-        <v>1</v>
-      </c>
-      <c r="O162" s="68">
-        <v>2024</v>
-      </c>
-      <c r="P162" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q162" s="61"/>
-      <c r="R162" s="61" t="s">
-        <v>385</v>
-      </c>
-      <c r="S162" s="51"/>
-      <c r="T162" s="51"/>
-      <c r="U162" s="80" t="s">
-        <v>467</v>
-      </c>
-      <c r="V162" s="84">
-        <f t="shared" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="W162" s="84">
-        <f t="shared" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="X162" s="80" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y162" s="83">
-        <f t="shared" si="59"/>
-        <v>160650</v>
-      </c>
-      <c r="Z162" s="83">
-        <f t="shared" si="60"/>
-        <v>232050</v>
-      </c>
-      <c r="AA162" s="80" t="s">
-        <v>450</v>
-      </c>
-      <c r="AB162" s="83" t="s">
-        <v>474</v>
-      </c>
-      <c r="AC162" s="83" t="s">
-        <v>475</v>
-      </c>
-      <c r="AD162" s="83" t="s">
-        <v>476</v>
-      </c>
-      <c r="AE162" s="80" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="163" spans="1:31">
+      <c r="H162" s="42"/>
+      <c r="I162" s="42"/>
+      <c r="J162" s="40"/>
+      <c r="K162" s="43"/>
+      <c r="L162" s="40"/>
+      <c r="M162" s="40"/>
+      <c r="N162" s="40"/>
+      <c r="O162" s="42"/>
+      <c r="P162" s="40"/>
+      <c r="Q162" s="43"/>
+      <c r="R162" s="40"/>
+      <c r="S162" s="40"/>
+      <c r="T162" s="40"/>
+      <c r="U162" s="80"/>
+      <c r="V162" s="84"/>
+      <c r="W162" s="84"/>
+      <c r="X162" s="80"/>
+      <c r="Y162" s="83"/>
+      <c r="Z162" s="83"/>
+      <c r="AA162" s="80"/>
+      <c r="AB162" s="83"/>
+      <c r="AC162" s="83"/>
+      <c r="AD162" s="83"/>
+      <c r="AE162" s="80"/>
+    </row>
+    <row r="163" spans="1:31" ht="89.25">
       <c r="A163" s="39">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B163" s="40">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="C163" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D163" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">      Additional Nuclear Fuel</v>
-      </c>
-      <c r="E163" s="41"/>
+        <v xml:space="preserve">      Refueling Operations</v>
+      </c>
+      <c r="E163" s="41" t="s">
+        <v>342</v>
+      </c>
       <c r="F163" s="41"/>
       <c r="G163" s="41"/>
       <c r="H163" s="45"/>
-      <c r="I163" s="63"/>
-      <c r="J163" s="51"/>
-      <c r="K163" s="61"/>
+      <c r="I163" s="63">
+        <v>178500</v>
+      </c>
+      <c r="J163" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="K163" s="61" t="s">
+        <v>384</v>
+      </c>
       <c r="L163" s="51"/>
       <c r="M163" s="51"/>
-      <c r="N163" s="51"/>
-      <c r="O163" s="68"/>
-      <c r="P163" s="51"/>
+      <c r="N163" s="51">
+        <v>1</v>
+      </c>
+      <c r="O163" s="68">
+        <v>2024</v>
+      </c>
+      <c r="P163" s="76" t="s">
+        <v>72</v>
+      </c>
       <c r="Q163" s="61"/>
-      <c r="R163" s="51"/>
+      <c r="R163" s="61" t="s">
+        <v>385</v>
+      </c>
       <c r="S163" s="51"/>
       <c r="T163" s="51"/>
-      <c r="U163" s="80"/>
-      <c r="V163" s="84"/>
-      <c r="W163" s="84"/>
-      <c r="X163" s="80"/>
-      <c r="Y163" s="83"/>
-      <c r="Z163" s="83"/>
-      <c r="AA163" s="80"/>
-      <c r="AB163" s="83"/>
-      <c r="AC163" s="83"/>
-      <c r="AD163" s="83"/>
-      <c r="AE163" s="80"/>
-    </row>
-    <row r="164" spans="1:31" ht="25.5">
+      <c r="U163" s="80" t="s">
+        <v>467</v>
+      </c>
+      <c r="V163" s="84">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="W163" s="84">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="X163" s="80" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y163" s="83">
+        <f t="shared" si="59"/>
+        <v>160650</v>
+      </c>
+      <c r="Z163" s="83">
+        <f t="shared" si="60"/>
+        <v>232050</v>
+      </c>
+      <c r="AA163" s="80" t="s">
+        <v>450</v>
+      </c>
+      <c r="AB163" s="83" t="s">
+        <v>474</v>
+      </c>
+      <c r="AC163" s="83" t="s">
+        <v>475</v>
+      </c>
+      <c r="AD163" s="83" t="s">
+        <v>476</v>
+      </c>
+      <c r="AE163" s="80" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="164" spans="1:31">
       <c r="A164" s="39">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B164" s="40">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="C164" s="58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D164" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">      Spent Fuel Management</v>
-      </c>
-      <c r="E164" s="41" t="s">
-        <v>341</v>
-      </c>
+        <v xml:space="preserve">      Additional Nuclear Fuel</v>
+      </c>
+      <c r="E164" s="41"/>
       <c r="F164" s="41"/>
       <c r="G164" s="41"/>
       <c r="H164" s="45"/>
-      <c r="I164" s="63">
-        <v>1</v>
-      </c>
-      <c r="J164" s="51" t="s">
-        <v>396</v>
-      </c>
-      <c r="K164" s="61" t="s">
-        <v>397</v>
-      </c>
+      <c r="I164" s="63"/>
+      <c r="J164" s="51"/>
+      <c r="K164" s="61"/>
       <c r="L164" s="51"/>
       <c r="M164" s="51"/>
-      <c r="N164" s="51">
-        <v>1</v>
-      </c>
-      <c r="O164" s="68">
-        <v>2024</v>
-      </c>
-      <c r="P164" s="51" t="s">
-        <v>77</v>
-      </c>
+      <c r="N164" s="51"/>
+      <c r="O164" s="68"/>
+      <c r="P164" s="51"/>
       <c r="Q164" s="61"/>
       <c r="R164" s="51"/>
       <c r="S164" s="51"/>
       <c r="T164" s="51"/>
-      <c r="U164" s="80" t="s">
+      <c r="U164" s="80"/>
+      <c r="V164" s="84"/>
+      <c r="W164" s="84"/>
+      <c r="X164" s="80"/>
+      <c r="Y164" s="83"/>
+      <c r="Z164" s="83"/>
+      <c r="AA164" s="80"/>
+      <c r="AB164" s="83"/>
+      <c r="AC164" s="83"/>
+      <c r="AD164" s="83"/>
+      <c r="AE164" s="80"/>
+    </row>
+    <row r="165" spans="1:31" ht="25.5">
+      <c r="A165" s="39">
+        <v>83</v>
+      </c>
+      <c r="B165" s="40">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="C165" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="D165" s="41" t="str">
+        <f t="shared" si="54"/>
+        <v xml:space="preserve">      Spent Fuel Management</v>
+      </c>
+      <c r="E165" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="F165" s="41"/>
+      <c r="G165" s="41"/>
+      <c r="H165" s="45"/>
+      <c r="I165" s="63">
+        <v>1</v>
+      </c>
+      <c r="J165" s="51" t="s">
+        <v>396</v>
+      </c>
+      <c r="K165" s="61" t="s">
+        <v>397</v>
+      </c>
+      <c r="L165" s="51"/>
+      <c r="M165" s="51"/>
+      <c r="N165" s="51">
+        <v>1</v>
+      </c>
+      <c r="O165" s="68">
+        <v>2024</v>
+      </c>
+      <c r="P165" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q165" s="61"/>
+      <c r="R165" s="51"/>
+      <c r="S165" s="51"/>
+      <c r="T165" s="51"/>
+      <c r="U165" s="80" t="s">
         <v>467</v>
       </c>
-      <c r="V164" s="84">
+      <c r="V165" s="84">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="W164" s="84">
+      <c r="W165" s="84">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="X164" s="80" t="s">
+      <c r="X165" s="80" t="s">
         <v>450</v>
       </c>
-      <c r="Y164" s="83">
+      <c r="Y165" s="83">
         <f t="shared" si="59"/>
         <v>0.9</v>
       </c>
-      <c r="Z164" s="83">
+      <c r="Z165" s="83">
         <f t="shared" si="60"/>
         <v>1.3</v>
       </c>
-      <c r="AA164" s="80" t="s">
+      <c r="AA165" s="80" t="s">
         <v>450</v>
       </c>
-      <c r="AB164" s="83" t="s">
+      <c r="AB165" s="83" t="s">
         <v>474</v>
       </c>
-      <c r="AC164" s="83" t="s">
+      <c r="AC165" s="83" t="s">
         <v>475</v>
       </c>
-      <c r="AD164" s="83" t="s">
+      <c r="AD165" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="AE164" s="80" t="s">
+      <c r="AE165" s="80" t="s">
         <v>451</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z164" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
+  <autoFilter ref="A1:Z165" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="54">
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="S26:S28"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="T107:T108"/>
+    <mergeCell ref="R154:R160"/>
+    <mergeCell ref="Q154:Q160"/>
+    <mergeCell ref="T154:T160"/>
+    <mergeCell ref="Q138:Q141"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16157,11 +16175,39 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q129:Q133"/>
     <mergeCell ref="Q122:Q127"/>
-    <mergeCell ref="T107:T108"/>
-    <mergeCell ref="R154:R159"/>
-    <mergeCell ref="Q154:Q159"/>
-    <mergeCell ref="T154:T159"/>
-    <mergeCell ref="Q138:Q141"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
   </mergeCells>
   <conditionalFormatting sqref="A96:F98 A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 A150:J152 S152:T152">
     <cfRule type="expression" dxfId="107" priority="226">
@@ -16180,61 +16226,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132:P133">
-    <cfRule type="expression" dxfId="103" priority="177">
-      <formula>$B132=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="174">
+    <cfRule type="expression" dxfId="103" priority="174">
       <formula>$B132=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="175">
+    <cfRule type="expression" dxfId="102" priority="175">
       <formula>$B132=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="176">
+    <cfRule type="expression" dxfId="101" priority="176">
       <formula>$B132&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="177">
+      <formula>$B132=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:P143">
-    <cfRule type="expression" dxfId="99" priority="124">
+    <cfRule type="expression" dxfId="99" priority="122">
+      <formula>$B136=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="123">
+      <formula>$B136=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="124">
       <formula>$B136&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="125">
+    <cfRule type="expression" dxfId="96" priority="125">
       <formula>$B136=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="122">
-      <formula>$B136=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="123">
-      <formula>$B136=2</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A109:AE153 A154:P159 A160:AE164 U53:AE54 U108:AE108 Q154:AE154 S155:S159 U155:AE159">
+  <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A109:AE153 A161:AE165 U53:AE54 U108:AE108 Q154:AE155 S156:S160 U156:AE160 A154:P160">
     <cfRule type="expression" dxfId="95" priority="193">
       <formula>$B53=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="94" priority="233">
-      <formula>$B95=0</formula>
+    <cfRule type="expression" dxfId="94" priority="230">
+      <formula>$B95=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="93" priority="231">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="230">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="92" priority="232">
+      <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="232">
-      <formula>$B95&lt;2</formula>
+    <cfRule type="expression" dxfId="91" priority="233">
+      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
     <cfRule type="expression" dxfId="90" priority="13">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="15">
+    <cfRule type="expression" dxfId="89" priority="14">
+      <formula>$B74=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="15">
       <formula>$B74&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="14">
-      <formula>$B74=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
@@ -16277,21 +16323,21 @@
       <formula>$B135=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A161:T164">
+  <conditionalFormatting sqref="A162:T165">
     <cfRule type="expression" dxfId="77" priority="90">
-      <formula>$B161=3</formula>
+      <formula>$B162=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="76" priority="91">
-      <formula>$B161=2</formula>
+      <formula>$B162=2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="75" priority="92">
-      <formula>$B161&lt;2</formula>
+      <formula>$B162&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="74" priority="93">
-      <formula>$B161=0</formula>
+      <formula>$B162=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE52 A53:S54 U53:AE54 A55:AE107 A108:S108 U108:AE108 A109:AE153 Q154:AE154 A154:P159 S155:S159 U155:AE159 A160:AE164">
+  <conditionalFormatting sqref="A1:AE52 A53:S54 U53:AE54 A55:AE107 A108:S108 U108:AE108 A109:AE153 Q154:AE155 S156:S160 U156:AE160 A161:AE165 A154:P160">
     <cfRule type="expression" dxfId="73" priority="191">
       <formula>$B1=2</formula>
     </cfRule>
@@ -16299,23 +16345,23 @@
       <formula>$B1&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A109:AE153 A160:AE164 A55:AE107 A1:AE52 A53:S54 U53:AE54 A108:S108 U108:AE108 Q154:AE154 A154:P159 S155:S159 U155:AE159">
+  <conditionalFormatting sqref="A109:AE153 A161:AE165 A55:AE107 A1:AE52 A53:S54 U53:AE54 A108:S108 U108:AE108 Q154:AE155 S156:S160 U156:AE160 A154:P160">
     <cfRule type="expression" dxfId="71" priority="190">
       <formula>$B1=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:R122 C123:P127">
-    <cfRule type="expression" dxfId="70" priority="52">
-      <formula>$B122=0</formula>
+    <cfRule type="expression" dxfId="70" priority="49">
+      <formula>$B122=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="51">
+    <cfRule type="expression" dxfId="69" priority="50">
+      <formula>$B122=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="51">
       <formula>$B122&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="50">
-      <formula>$B122=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="49">
-      <formula>$B122=3</formula>
+    <cfRule type="expression" dxfId="67" priority="52">
+      <formula>$B122=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
@@ -16348,7 +16394,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D128:D164 D2:D80 D82 D84:D121">
+  <conditionalFormatting sqref="D128:D165 D2:D80 D82 D84:D121">
     <cfRule type="colorScale" priority="478">
       <colorScale>
         <cfvo type="min"/>
@@ -16364,31 +16410,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G54">
-    <cfRule type="expression" dxfId="65" priority="6">
+    <cfRule type="expression" dxfId="65" priority="5">
+      <formula>$B52=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="6">
       <formula>$B52=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="7">
+    <cfRule type="expression" dxfId="63" priority="7">
       <formula>$B52&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="8">
+    <cfRule type="expression" dxfId="62" priority="8">
       <formula>$B52=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="5">
-      <formula>$B52=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="61" priority="225">
-      <formula>$B96=0</formula>
+    <cfRule type="expression" dxfId="61" priority="222">
+      <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="224">
+    <cfRule type="expression" dxfId="60" priority="223">
+      <formula>$B96=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="224">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="222">
-      <formula>$B96=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="223">
-      <formula>$B96=2</formula>
+    <cfRule type="expression" dxfId="58" priority="225">
+      <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -16398,11 +16444,11 @@
     <cfRule type="expression" dxfId="56" priority="29">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="31">
+    <cfRule type="expression" dxfId="55" priority="30">
+      <formula>$B5&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="31">
       <formula>$B5=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="30">
-      <formula>$B5&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
@@ -16424,14 +16470,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="49" priority="76">
+    <cfRule type="expression" dxfId="49" priority="75">
+      <formula>$B69=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="76">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="77">
+    <cfRule type="expression" dxfId="47" priority="77">
       <formula>$B69&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="75">
-      <formula>$B69=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
@@ -16440,14 +16486,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="45" priority="87">
-      <formula>$B68&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="85">
+    <cfRule type="expression" dxfId="45" priority="85">
       <formula>$B68=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="86">
+    <cfRule type="expression" dxfId="44" priority="86">
       <formula>$B68=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="87">
+      <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
@@ -16456,28 +16502,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:J149">
-    <cfRule type="expression" dxfId="41" priority="109">
-      <formula>$B149=0</formula>
+    <cfRule type="expression" dxfId="41" priority="106">
+      <formula>$B149=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="108">
+    <cfRule type="expression" dxfId="40" priority="107">
+      <formula>$B149=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="108">
       <formula>$B149&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="107">
-      <formula>$B149=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="106">
-      <formula>$B149=3</formula>
+    <cfRule type="expression" dxfId="38" priority="109">
+      <formula>$B149=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I129:K130">
-    <cfRule type="expression" dxfId="37" priority="188">
-      <formula>$B129&lt;2</formula>
+    <cfRule type="expression" dxfId="37" priority="186">
+      <formula>$B129=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="187">
       <formula>$B129=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="186">
-      <formula>$B129=3</formula>
+    <cfRule type="expression" dxfId="35" priority="188">
+      <formula>$B129&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="189">
       <formula>$B129=0</formula>
@@ -16487,17 +16533,17 @@
     <cfRule type="expression" dxfId="33" priority="35">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="428">
-      <formula>#REF!=3</formula>
+    <cfRule type="expression" dxfId="32" priority="425">
+      <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="427">
+    <cfRule type="expression" dxfId="31" priority="426">
+      <formula>#REF!&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="427">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="426">
-      <formula>#REF!&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="425">
-      <formula>#REF!=2</formula>
+    <cfRule type="expression" dxfId="29" priority="428">
+      <formula>#REF!=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
@@ -16565,17 +16611,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:Q143">
-    <cfRule type="expression" dxfId="12" priority="168">
+    <cfRule type="expression" dxfId="12" priority="166">
+      <formula>$B142=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="167">
+      <formula>$B142=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="168">
       <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="169">
+    <cfRule type="expression" dxfId="9" priority="169">
       <formula>$B142=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="167">
-      <formula>$B142=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="166">
-      <formula>$B142=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
@@ -16601,42 +16647,42 @@
     <cfRule type="expression" dxfId="3" priority="251">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="253">
+    <cfRule type="expression" dxfId="2" priority="252">
+      <formula>$B95=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="253">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="254">
+    <cfRule type="expression" dxfId="0" priority="254">
       <formula>$B95=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="252">
-      <formula>$B95=2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O165:P172 O137:O164 O2:O135" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O166:P173 O137:O165 O2:O135" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
       <formula1>1950</formula1>
       <formula2>2025</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9 I57:I59 I61:I63 I84 L85:L93 I89:I94 H117:H118 H121:H128 I67:I79 L71:L83 I52:I54 I135:I164 H132:H164 I96:I133 L95:L1048576 H2:H114 L1:L67 I11:I48" xr:uid="{66ABF627-CC97-3E44-B6AC-09E441BED0CD}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9 I57:I59 I61:I63 I84 L85:L93 I89:I94 H117:H118 H121:H128 I67:I79 L71:L83 I52:I54 I135:I165 H132:H165 I96:I133 L95:L1048576 H2:H114 L1:L67 I11:I48" xr:uid="{66ABF627-CC97-3E44-B6AC-09E441BED0CD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K339:K349" xr:uid="{9E6037A9-5EC7-2945-A2FE-1723BA7DEE83}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K340:K350" xr:uid="{9E6037A9-5EC7-2945-A2FE-1723BA7DEE83}">
       <formula1>"Land Area, Power MWe, Excavation Volume,  Reactor Building Slab Roof Volume,	Reactor Building  Basement Volume, Reactor Building  Exterior Walls Volume,		Turbine Building Slab Roof Volume,	Turbine Building  Basement Volume,	Turbine Building  Exterior Wall"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J165:J1048576" xr:uid="{EEDF1E2A-32DC-6242-8EBD-BD01BBD19C77}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J166:J1048576" xr:uid="{EEDF1E2A-32DC-6242-8EBD-BD01BBD19C77}">
       <formula1>"$/acres, $/MWe, $/m^3, $/MWt"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N165:N318" xr:uid="{6D536505-A5B6-E145-A4B9-9C3C8E6B8527}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N166:N319" xr:uid="{6D536505-A5B6-E145-A4B9-9C3C8E6B8527}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N128:N164 N82:N121 N2:N80" xr:uid="{1C0096F5-23AB-5A48-8F14-E27BC72A38A6}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N128:N165 N82:N121 N2:N80" xr:uid="{1C0096F5-23AB-5A48-8F14-E27BC72A38A6}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M121 M128:M164 M82:M118 M2:M80" xr:uid="{127B7473-9D01-354E-A3BD-12180E660A5C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M121 M128:M165 M82:M118 M2:M80" xr:uid="{127B7473-9D01-354E-A3BD-12180E660A5C}">
       <formula1>"acres, MWe, m^3, MWt, Kg, Drums, kW, $, m^2, kg/s"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J128:J164 J82:J121 J2:J80" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J128:J165 J82:J121 J2:J80" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
       <formula1>"$/m^2,$/MWeHour,$/FTE, $/acres, $/MWe, $/m^3, $/MWt, $/Kg, $/Drum, $/(kg.sec), $/SWU, unitless, $/kWe"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M119:M120" xr:uid="{3DD8CB7E-F66A-4C30-8943-BB08D88ABA07}">
@@ -16652,10 +16698,10 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E164" xr:uid="{E571E7A1-C2F9-2E4D-99A9-8FA0C5D45C39}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E165" xr:uid="{E571E7A1-C2F9-2E4D-99A9-8FA0C5D45C39}">
       <formula1>"standard, nonstandard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P164" xr:uid="{17DDFD40-D97D-B64B-BD3B-AEAF52F6302C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P165" xr:uid="{17DDFD40-D97D-B64B-BD3B-AEAF52F6302C}">
       <formula1>"NA, General, Labor, Material, Equipment,Lab and Mat and Equip, 'Lab and Equip"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16683,7 +16729,7 @@
           <x14:formula1>
             <xm:f>'Economics Parameters'!$A$9:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U164</xm:sqref>
+          <xm:sqref>U2:U165</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19425,7 +19471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358A137-1626-9343-A399-452BA3D3C6F7}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="164" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="164" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -19443,10 +19489,10 @@
         <v>238</v>
       </c>
       <c r="C1" s="36" t="s">
+        <v>529</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>530</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>531</v>
       </c>
       <c r="E1" s="36" t="s">
         <v>62</v>
@@ -19516,13 +19562,13 @@
         <v>0.08</v>
       </c>
       <c r="C9" s="117" t="s">
+        <v>531</v>
+      </c>
+      <c r="D9" s="117" t="s">
         <v>532</v>
       </c>
-      <c r="D9" s="117" t="s">
-        <v>533</v>
-      </c>
       <c r="E9" s="117" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
@@ -19571,7 +19617,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B14">
         <v>0.41505377678599265</v>
@@ -19582,7 +19628,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B15">
         <v>0.39914905811401724</v>
@@ -19593,17 +19639,17 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B16">
         <v>0.05</v>
       </c>
       <c r="C16" s="117"/>
       <c r="D16" t="s">
+        <v>536</v>
+      </c>
+      <c r="E16" t="s">
         <v>537</v>
-      </c>
-      <c r="E16" t="s">
-        <v>538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update NOAK cost multipliers based on Factory Fabrications paper
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\mouse\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77BEB7A-F0FA-444D-83F2-92C33FE03E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1562A68-B21C-4A00-9A1D-53302E3A0D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="877" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="541">
   <si>
     <t>Account</t>
   </si>
@@ -1994,6 +1994,9 @@
   </si>
   <si>
     <t>Non-nuclear off-the-shelf</t>
+  </si>
+  <si>
+    <t>Factory Drums</t>
   </si>
 </sst>
 </file>
@@ -2631,39 +2634,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2671,6 +2641,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2689,6 +2671,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2724,13 +2727,6 @@
   </cellStyles>
   <dxfs count="108">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2740,6 +2736,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2784,9 +2787,15 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2798,15 +2807,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2927,14 +2930,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2947,7 +2943,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2966,58 +2969,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3035,13 +2988,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3050,8 +2996,31 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3065,6 +3034,40 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3102,13 +3105,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3117,14 +3113,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3134,26 +3123,6 @@
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3183,18 +3152,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
-        <i/>
+        <i val="0"/>
       </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3208,8 +3181,17 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
       </fill>
     </dxf>
     <dxf>
@@ -3217,6 +3199,27 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3335,56 +3338,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3416,6 +3372,32 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3439,6 +3421,27 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4221,10 +4224,10 @@
       <c r="Q3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="93" t="s">
+      <c r="R3" s="94" t="s">
         <v>445</v>
       </c>
-      <c r="S3" s="99" t="s">
+      <c r="S3" s="96" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4311,8 +4314,8 @@
       <c r="Q4" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="93"/>
-      <c r="S4" s="99"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="96"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>467</v>
@@ -4391,10 +4394,10 @@
       <c r="Q5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="93" t="s">
+      <c r="R5" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="99" t="s">
+      <c r="S5" s="96" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4474,8 +4477,8 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="93"/>
-      <c r="S6" s="99"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="96"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>467</v>
@@ -4781,13 +4784,13 @@
       <c r="P11" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="93" t="s">
+      <c r="Q11" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="93" t="s">
+      <c r="R11" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="100" t="s">
+      <c r="S11" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -4878,9 +4881,9 @@
       <c r="P12" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="93"/>
-      <c r="S12" s="99"/>
+      <c r="Q12" s="94"/>
+      <c r="R12" s="94"/>
+      <c r="S12" s="96"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>470</v>
@@ -4962,9 +4965,9 @@
       <c r="P13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="99"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="94"/>
+      <c r="S13" s="96"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>470</v>
@@ -5089,13 +5092,13 @@
       <c r="P15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="93" t="s">
+      <c r="Q15" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="93" t="s">
+      <c r="R15" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="100" t="s">
+      <c r="S15" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5179,9 +5182,9 @@
       <c r="P16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="99"/>
+      <c r="Q16" s="94"/>
+      <c r="R16" s="94"/>
+      <c r="S16" s="96"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>470</v>
@@ -5263,9 +5266,9 @@
       <c r="P17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="93"/>
-      <c r="R17" s="93"/>
-      <c r="S17" s="99"/>
+      <c r="Q17" s="94"/>
+      <c r="R17" s="94"/>
+      <c r="S17" s="96"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>470</v>
@@ -5629,13 +5632,13 @@
       <c r="P22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="93" t="s">
+      <c r="Q22" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="93" t="s">
+      <c r="R22" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="100" t="s">
+      <c r="S22" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5719,9 +5722,9 @@
       <c r="P23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="99"/>
+      <c r="Q23" s="94"/>
+      <c r="R23" s="94"/>
+      <c r="S23" s="96"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>470</v>
@@ -5803,9 +5806,9 @@
       <c r="P24" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="99"/>
+      <c r="Q24" s="94"/>
+      <c r="R24" s="94"/>
+      <c r="S24" s="96"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>470</v>
@@ -5930,13 +5933,13 @@
       <c r="P26" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="93" t="s">
+      <c r="Q26" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R26" s="93" t="s">
+      <c r="R26" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="100" t="s">
+      <c r="S26" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -6020,9 +6023,9 @@
       <c r="P27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="93"/>
-      <c r="S27" s="99"/>
+      <c r="Q27" s="94"/>
+      <c r="R27" s="94"/>
+      <c r="S27" s="96"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>470</v>
@@ -6104,9 +6107,9 @@
       <c r="P28" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="93"/>
-      <c r="S28" s="99"/>
+      <c r="Q28" s="94"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="96"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>470</v>
@@ -6235,13 +6238,13 @@
       <c r="P30" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="93" t="s">
+      <c r="Q30" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="93" t="s">
+      <c r="R30" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="100" t="s">
+      <c r="S30" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6329,9 +6332,9 @@
       <c r="P31" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="99"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="96"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>470</v>
@@ -6417,9 +6420,9 @@
       <c r="P32" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="93"/>
-      <c r="S32" s="99"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="96"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>470</v>
@@ -6728,13 +6731,13 @@
       <c r="P37" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q37" s="93" t="s">
+      <c r="Q37" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R37" s="93" t="s">
+      <c r="R37" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="100" t="s">
+      <c r="S37" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -6818,9 +6821,9 @@
       <c r="P38" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="93"/>
-      <c r="R38" s="93"/>
-      <c r="S38" s="99"/>
+      <c r="Q38" s="94"/>
+      <c r="R38" s="94"/>
+      <c r="S38" s="96"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>470</v>
@@ -6902,9 +6905,9 @@
       <c r="P39" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="93"/>
-      <c r="R39" s="93"/>
-      <c r="S39" s="99"/>
+      <c r="Q39" s="94"/>
+      <c r="R39" s="94"/>
+      <c r="S39" s="96"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>470</v>
@@ -7029,13 +7032,13 @@
       <c r="P41" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="93" t="s">
+      <c r="Q41" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="93" t="s">
+      <c r="R41" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="100" t="s">
+      <c r="S41" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7119,9 +7122,9 @@
       <c r="P42" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="93"/>
-      <c r="R42" s="93"/>
-      <c r="S42" s="99"/>
+      <c r="Q42" s="94"/>
+      <c r="R42" s="94"/>
+      <c r="S42" s="96"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>470</v>
@@ -7203,9 +7206,9 @@
       <c r="P43" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q43" s="93"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="99"/>
+      <c r="Q43" s="94"/>
+      <c r="R43" s="94"/>
+      <c r="S43" s="96"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>470</v>
@@ -7373,13 +7376,13 @@
       <c r="P46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="93" t="s">
+      <c r="Q46" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R46" s="93" t="s">
+      <c r="R46" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="100" t="s">
+      <c r="S46" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
@@ -7463,9 +7466,9 @@
       <c r="P47" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="93"/>
-      <c r="R47" s="93"/>
-      <c r="S47" s="99"/>
+      <c r="Q47" s="94"/>
+      <c r="R47" s="94"/>
+      <c r="S47" s="96"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
         <v>466</v>
@@ -7547,9 +7550,9 @@
       <c r="P48" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q48" s="93"/>
-      <c r="R48" s="93"/>
-      <c r="S48" s="99"/>
+      <c r="Q48" s="94"/>
+      <c r="R48" s="94"/>
+      <c r="S48" s="96"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
         <v>466</v>
@@ -7816,16 +7819,16 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="96" t="s">
+      <c r="Q52" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="R52" s="96" t="s">
+      <c r="R52" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="105" t="s">
+      <c r="S52" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="101" t="s">
+      <c r="T52" s="90" t="s">
         <v>503</v>
       </c>
       <c r="U52" s="80" t="s">
@@ -7912,10 +7915,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="97"/>
-      <c r="R53" s="97"/>
-      <c r="S53" s="106"/>
-      <c r="T53" s="102"/>
+      <c r="Q53" s="105"/>
+      <c r="R53" s="105"/>
+      <c r="S53" s="99"/>
+      <c r="T53" s="91"/>
       <c r="U53" s="80" t="s">
         <v>470</v>
       </c>
@@ -8000,10 +8003,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="98"/>
-      <c r="R54" s="98"/>
-      <c r="S54" s="107"/>
-      <c r="T54" s="103"/>
+      <c r="Q54" s="106"/>
+      <c r="R54" s="106"/>
+      <c r="S54" s="100"/>
+      <c r="T54" s="92"/>
       <c r="U54" s="80" t="s">
         <v>470</v>
       </c>
@@ -8170,13 +8173,13 @@
       <c r="P57" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q57" s="93" t="s">
+      <c r="Q57" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R57" s="93" t="s">
+      <c r="R57" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="100" t="s">
+      <c r="S57" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8260,9 +8263,9 @@
       <c r="P58" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q58" s="93"/>
-      <c r="R58" s="93"/>
-      <c r="S58" s="99"/>
+      <c r="Q58" s="94"/>
+      <c r="R58" s="94"/>
+      <c r="S58" s="96"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>470</v>
@@ -8344,9 +8347,9 @@
       <c r="P59" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q59" s="93"/>
-      <c r="R59" s="93"/>
-      <c r="S59" s="99"/>
+      <c r="Q59" s="94"/>
+      <c r="R59" s="94"/>
+      <c r="S59" s="96"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>470</v>
@@ -8471,13 +8474,13 @@
       <c r="P61" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q61" s="93" t="s">
+      <c r="Q61" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R61" s="93" t="s">
+      <c r="R61" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="100" t="s">
+      <c r="S61" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8561,9 +8564,9 @@
       <c r="P62" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="99"/>
+      <c r="Q62" s="94"/>
+      <c r="R62" s="94"/>
+      <c r="S62" s="96"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>470</v>
@@ -8645,9 +8648,9 @@
       <c r="P63" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q63" s="93"/>
-      <c r="R63" s="93"/>
-      <c r="S63" s="99"/>
+      <c r="Q63" s="94"/>
+      <c r="R63" s="94"/>
+      <c r="S63" s="96"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>470</v>
@@ -8954,7 +8957,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="94" t="s">
+      <c r="R68" s="93" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -9043,7 +9046,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="94"/>
+      <c r="R69" s="93"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9137,7 +9140,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="94"/>
+      <c r="R70" s="93"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9224,7 +9227,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="94"/>
+      <c r="R71" s="93"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9313,7 +9316,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="94"/>
+      <c r="R72" s="93"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9407,7 +9410,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="94"/>
+      <c r="R73" s="93"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9577,10 +9580,10 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="94" t="s">
+      <c r="R76" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="104" t="s">
+      <c r="S76" s="97" t="s">
         <v>447</v>
       </c>
       <c r="T76" s="61" t="s">
@@ -9667,8 +9670,8 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="94"/>
-      <c r="S77" s="104"/>
+      <c r="R77" s="93"/>
+      <c r="S77" s="97"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
         <v>466</v>
@@ -9762,8 +9765,8 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="94"/>
-      <c r="S78" s="104"/>
+      <c r="R78" s="93"/>
+      <c r="S78" s="97"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
         <v>466</v>
@@ -9856,8 +9859,8 @@
       <c r="Q79" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="R79" s="94"/>
-      <c r="S79" s="104"/>
+      <c r="R79" s="93"/>
+      <c r="S79" s="97"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
         <v>466</v>
@@ -9951,8 +9954,8 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="94"/>
-      <c r="S80" s="104"/>
+      <c r="R80" s="93"/>
+      <c r="S80" s="97"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
         <v>535</v>
@@ -10376,7 +10379,7 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="104" t="s">
+      <c r="S85" s="97" t="s">
         <v>447</v>
       </c>
       <c r="T85" s="51"/>
@@ -10482,7 +10485,7 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="104"/>
+      <c r="S86" s="97"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
         <v>534</v>
@@ -10578,7 +10581,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="104"/>
+      <c r="S87" s="97"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>466</v>
@@ -10672,7 +10675,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="104"/>
+      <c r="S88" s="97"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>466</v>
@@ -10741,7 +10744,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="104"/>
+      <c r="S89" s="97"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -10813,7 +10816,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="104"/>
+      <c r="S90" s="97"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>466</v>
@@ -10907,7 +10910,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="104"/>
+      <c r="S91" s="97"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>466</v>
@@ -11271,13 +11274,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="94" t="s">
+      <c r="R96" s="93" t="s">
         <v>448</v>
       </c>
-      <c r="S96" s="108" t="s">
+      <c r="S96" s="101" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="94"/>
+      <c r="T96" s="93"/>
       <c r="U96" s="80" t="s">
         <v>466</v>
       </c>
@@ -11364,9 +11367,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="94"/>
-      <c r="S97" s="109"/>
-      <c r="T97" s="94"/>
+      <c r="R97" s="93"/>
+      <c r="S97" s="102"/>
+      <c r="T97" s="93"/>
       <c r="U97" s="80" t="s">
         <v>466</v>
       </c>
@@ -12200,7 +12203,7 @@
         <v>360</v>
       </c>
       <c r="S107" s="87"/>
-      <c r="T107" s="90" t="s">
+      <c r="T107" s="107" t="s">
         <v>506</v>
       </c>
       <c r="U107" s="80" t="s">
@@ -12298,7 +12301,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="91"/>
+      <c r="T108" s="108"/>
       <c r="U108" s="80" t="s">
         <v>466</v>
       </c>
@@ -13299,10 +13302,10 @@
       <c r="P122" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q122" s="95" t="s">
+      <c r="Q122" s="103" t="s">
         <v>427</v>
       </c>
-      <c r="R122" s="95" t="s">
+      <c r="R122" s="103" t="s">
         <v>365</v>
       </c>
       <c r="S122" s="51"/>
@@ -13391,8 +13394,8 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="95"/>
-      <c r="R123" s="95"/>
+      <c r="Q123" s="103"/>
+      <c r="R123" s="103"/>
       <c r="S123" s="51"/>
       <c r="T123" s="51"/>
       <c r="U123" s="80" t="s">
@@ -13479,8 +13482,8 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="95"/>
-      <c r="R124" s="95"/>
+      <c r="Q124" s="103"/>
+      <c r="R124" s="103"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
@@ -13567,8 +13570,8 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="95"/>
-      <c r="R125" s="95"/>
+      <c r="Q125" s="103"/>
+      <c r="R125" s="103"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
@@ -13655,8 +13658,8 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="95"/>
-      <c r="R126" s="95"/>
+      <c r="Q126" s="103"/>
+      <c r="R126" s="103"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
@@ -13743,8 +13746,8 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="95"/>
-      <c r="R127" s="95"/>
+      <c r="Q127" s="103"/>
+      <c r="R127" s="103"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
@@ -13867,10 +13870,10 @@
       <c r="P129" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q129" s="94" t="s">
+      <c r="Q129" s="93" t="s">
         <v>369</v>
       </c>
-      <c r="R129" s="94" t="s">
+      <c r="R129" s="93" t="s">
         <v>370</v>
       </c>
       <c r="S129" s="51"/>
@@ -13952,8 +13955,8 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="94"/>
-      <c r="R130" s="94"/>
+      <c r="Q130" s="93"/>
+      <c r="R130" s="93"/>
       <c r="S130" s="51"/>
       <c r="T130" s="51"/>
       <c r="U130" s="80" t="s">
@@ -14035,8 +14038,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="94"/>
-      <c r="R131" s="94"/>
+      <c r="Q131" s="93"/>
+      <c r="R131" s="93"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14120,8 +14123,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="94"/>
-      <c r="R132" s="94"/>
+      <c r="Q132" s="93"/>
+      <c r="R132" s="93"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14212,8 +14215,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="94"/>
-      <c r="R133" s="94"/>
+      <c r="Q133" s="93"/>
+      <c r="R133" s="93"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -14505,7 +14508,7 @@
       <c r="P138" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q138" s="93" t="s">
+      <c r="Q138" s="94" t="s">
         <v>364</v>
       </c>
       <c r="R138" s="48"/>
@@ -14585,7 +14588,7 @@
       <c r="P139" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q139" s="93"/>
+      <c r="Q139" s="94"/>
       <c r="R139" s="48"/>
       <c r="S139" s="48"/>
       <c r="T139" s="48"/>
@@ -14663,7 +14666,7 @@
       <c r="P140" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q140" s="93"/>
+      <c r="Q140" s="94"/>
       <c r="R140" s="51"/>
       <c r="S140" s="51"/>
       <c r="T140" s="51"/>
@@ -14741,7 +14744,7 @@
       <c r="P141" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q141" s="93"/>
+      <c r="Q141" s="94"/>
       <c r="R141" s="51"/>
       <c r="S141" s="51"/>
       <c r="T141" s="51"/>
@@ -15562,14 +15565,14 @@
       <c r="N154" s="51"/>
       <c r="O154" s="68"/>
       <c r="P154" s="51"/>
-      <c r="Q154" s="90" t="s">
+      <c r="Q154" s="107" t="s">
         <v>500</v>
       </c>
-      <c r="R154" s="90" t="s">
+      <c r="R154" s="107" t="s">
         <v>500</v>
       </c>
       <c r="S154" s="51"/>
-      <c r="T154" s="90" t="s">
+      <c r="T154" s="107" t="s">
         <v>501</v>
       </c>
       <c r="U154" s="80"/>
@@ -15611,10 +15614,10 @@
       <c r="N155" s="51"/>
       <c r="O155" s="68"/>
       <c r="P155" s="51"/>
-      <c r="Q155" s="92"/>
-      <c r="R155" s="92"/>
+      <c r="Q155" s="109"/>
+      <c r="R155" s="109"/>
       <c r="S155" s="51"/>
-      <c r="T155" s="92"/>
+      <c r="T155" s="109"/>
       <c r="U155" s="80"/>
       <c r="V155" s="84"/>
       <c r="W155" s="84"/>
@@ -15654,10 +15657,10 @@
       <c r="N156" s="51"/>
       <c r="O156" s="68"/>
       <c r="P156" s="51"/>
-      <c r="Q156" s="92"/>
-      <c r="R156" s="92"/>
+      <c r="Q156" s="109"/>
+      <c r="R156" s="109"/>
       <c r="S156" s="51"/>
-      <c r="T156" s="92"/>
+      <c r="T156" s="109"/>
       <c r="U156" s="80"/>
       <c r="V156" s="84"/>
       <c r="W156" s="84"/>
@@ -15697,10 +15700,10 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="92"/>
-      <c r="R157" s="92"/>
+      <c r="Q157" s="109"/>
+      <c r="R157" s="109"/>
       <c r="S157" s="51"/>
-      <c r="T157" s="92"/>
+      <c r="T157" s="109"/>
       <c r="U157" s="80"/>
       <c r="V157" s="84"/>
       <c r="W157" s="84"/>
@@ -15740,10 +15743,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="92"/>
-      <c r="R158" s="92"/>
+      <c r="Q158" s="109"/>
+      <c r="R158" s="109"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="92"/>
+      <c r="T158" s="109"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -15783,10 +15786,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="91"/>
-      <c r="R159" s="91"/>
+      <c r="Q159" s="108"/>
+      <c r="R159" s="108"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="91"/>
+      <c r="T159" s="108"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -16108,39 +16111,11 @@
   </sheetData>
   <autoFilter ref="A1:Z164" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="54">
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="S26:S28"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="T107:T108"/>
+    <mergeCell ref="R154:R159"/>
+    <mergeCell ref="Q154:Q159"/>
+    <mergeCell ref="T154:T159"/>
+    <mergeCell ref="Q138:Q141"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16157,11 +16132,39 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q129:Q133"/>
     <mergeCell ref="Q122:Q127"/>
-    <mergeCell ref="T107:T108"/>
-    <mergeCell ref="R154:R159"/>
-    <mergeCell ref="Q154:Q159"/>
-    <mergeCell ref="T154:T159"/>
-    <mergeCell ref="Q138:Q141"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
   </mergeCells>
   <conditionalFormatting sqref="A96:F98 A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 A150:J152 S152:T152">
     <cfRule type="expression" dxfId="107" priority="226">
@@ -16180,31 +16183,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132:P133">
-    <cfRule type="expression" dxfId="103" priority="177">
-      <formula>$B132=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="174">
+    <cfRule type="expression" dxfId="103" priority="174">
       <formula>$B132=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="175">
+    <cfRule type="expression" dxfId="102" priority="175">
       <formula>$B132=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="176">
+    <cfRule type="expression" dxfId="101" priority="176">
       <formula>$B132&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="177">
+      <formula>$B132=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:P143">
-    <cfRule type="expression" dxfId="99" priority="124">
+    <cfRule type="expression" dxfId="99" priority="122">
+      <formula>$B136=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="123">
+      <formula>$B136=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="124">
       <formula>$B136&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="125">
+    <cfRule type="expression" dxfId="96" priority="125">
       <formula>$B136=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="122">
-      <formula>$B136=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="123">
-      <formula>$B136=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A109:AE153 A154:P159 A160:AE164 U53:AE54 U108:AE108 Q154:AE154 S155:S159 U155:AE159">
@@ -16213,28 +16216,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="94" priority="233">
-      <formula>$B95=0</formula>
+    <cfRule type="expression" dxfId="94" priority="230">
+      <formula>$B95=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="93" priority="231">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="230">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="92" priority="232">
+      <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="232">
-      <formula>$B95&lt;2</formula>
+    <cfRule type="expression" dxfId="91" priority="233">
+      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
     <cfRule type="expression" dxfId="90" priority="13">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="15">
+    <cfRule type="expression" dxfId="89" priority="14">
+      <formula>$B74=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="15">
       <formula>$B74&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="14">
-      <formula>$B74=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
@@ -16305,17 +16308,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:R122 C123:P127">
-    <cfRule type="expression" dxfId="70" priority="52">
-      <formula>$B122=0</formula>
+    <cfRule type="expression" dxfId="70" priority="49">
+      <formula>$B122=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="51">
+    <cfRule type="expression" dxfId="69" priority="50">
+      <formula>$B122=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="51">
       <formula>$B122&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="50">
-      <formula>$B122=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="49">
-      <formula>$B122=3</formula>
+    <cfRule type="expression" dxfId="67" priority="52">
+      <formula>$B122=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
@@ -16364,31 +16367,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G54">
-    <cfRule type="expression" dxfId="65" priority="6">
+    <cfRule type="expression" dxfId="65" priority="5">
+      <formula>$B52=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="6">
       <formula>$B52=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="7">
+    <cfRule type="expression" dxfId="63" priority="7">
       <formula>$B52&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="8">
+    <cfRule type="expression" dxfId="62" priority="8">
       <formula>$B52=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="5">
-      <formula>$B52=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="61" priority="225">
-      <formula>$B96=0</formula>
+    <cfRule type="expression" dxfId="61" priority="222">
+      <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="224">
+    <cfRule type="expression" dxfId="60" priority="223">
+      <formula>$B96=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="224">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="222">
-      <formula>$B96=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="223">
-      <formula>$B96=2</formula>
+    <cfRule type="expression" dxfId="58" priority="225">
+      <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -16398,11 +16401,11 @@
     <cfRule type="expression" dxfId="56" priority="29">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="31">
+    <cfRule type="expression" dxfId="55" priority="30">
+      <formula>$B5&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="31">
       <formula>$B5=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="30">
-      <formula>$B5&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
@@ -16424,14 +16427,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="49" priority="76">
+    <cfRule type="expression" dxfId="49" priority="75">
+      <formula>$B69=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="76">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="77">
+    <cfRule type="expression" dxfId="47" priority="77">
       <formula>$B69&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="75">
-      <formula>$B69=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
@@ -16440,14 +16443,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="45" priority="87">
-      <formula>$B68&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="85">
+    <cfRule type="expression" dxfId="45" priority="85">
       <formula>$B68=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="86">
+    <cfRule type="expression" dxfId="44" priority="86">
       <formula>$B68=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="87">
+      <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
@@ -16456,28 +16459,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:J149">
-    <cfRule type="expression" dxfId="41" priority="109">
-      <formula>$B149=0</formula>
+    <cfRule type="expression" dxfId="41" priority="106">
+      <formula>$B149=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="108">
+    <cfRule type="expression" dxfId="40" priority="107">
+      <formula>$B149=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="108">
       <formula>$B149&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="107">
-      <formula>$B149=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="106">
-      <formula>$B149=3</formula>
+    <cfRule type="expression" dxfId="38" priority="109">
+      <formula>$B149=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I129:K130">
-    <cfRule type="expression" dxfId="37" priority="188">
-      <formula>$B129&lt;2</formula>
+    <cfRule type="expression" dxfId="37" priority="186">
+      <formula>$B129=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="187">
       <formula>$B129=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="186">
-      <formula>$B129=3</formula>
+    <cfRule type="expression" dxfId="35" priority="188">
+      <formula>$B129&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="189">
       <formula>$B129=0</formula>
@@ -16487,17 +16490,17 @@
     <cfRule type="expression" dxfId="33" priority="35">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="428">
-      <formula>#REF!=3</formula>
+    <cfRule type="expression" dxfId="32" priority="425">
+      <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="427">
+    <cfRule type="expression" dxfId="31" priority="426">
+      <formula>#REF!&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="427">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="426">
-      <formula>#REF!&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="425">
-      <formula>#REF!=2</formula>
+    <cfRule type="expression" dxfId="29" priority="428">
+      <formula>#REF!=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
@@ -16565,17 +16568,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:Q143">
-    <cfRule type="expression" dxfId="12" priority="168">
+    <cfRule type="expression" dxfId="12" priority="166">
+      <formula>$B142=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="167">
+      <formula>$B142=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="168">
       <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="169">
+    <cfRule type="expression" dxfId="9" priority="169">
       <formula>$B142=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="167">
-      <formula>$B142=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="166">
-      <formula>$B142=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
@@ -16601,14 +16604,14 @@
     <cfRule type="expression" dxfId="3" priority="251">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="253">
+    <cfRule type="expression" dxfId="2" priority="252">
+      <formula>$B95=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="253">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="254">
+    <cfRule type="expression" dxfId="0" priority="254">
       <formula>$B95=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="252">
-      <formula>$B95=2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
@@ -16681,7 +16684,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3A5BD7CA-D901-4C35-8F1B-FB3DB8093CEC}">
           <x14:formula1>
-            <xm:f>'Economics Parameters'!$A$9:$A$16</xm:f>
+            <xm:f>'Economics Parameters'!$A$9:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>U2:U164</xm:sqref>
         </x14:dataValidation>
@@ -19423,10 +19426,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358A137-1626-9343-A399-452BA3D3C6F7}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="164" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -19552,7 +19555,7 @@
         <v>471</v>
       </c>
       <c r="B12">
-        <v>0.22343911000453887</v>
+        <v>0.18443169820109745</v>
       </c>
       <c r="C12" s="117"/>
       <c r="D12" s="117"/>
@@ -19560,10 +19563,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="B13" s="89">
-        <v>0.182369</v>
+        <v>540</v>
+      </c>
+      <c r="B13">
+        <v>0.24138000000000001</v>
       </c>
       <c r="C13" s="117"/>
       <c r="D13" s="117"/>
@@ -19571,10 +19574,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="B14">
-        <v>0.41505377678599265</v>
+        <v>466</v>
+      </c>
+      <c r="B14" s="89">
+        <v>0.22962848022115534</v>
       </c>
       <c r="C14" s="117"/>
       <c r="D14" s="117"/>
@@ -19582,10 +19585,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B15">
-        <v>0.39914905811401724</v>
+        <v>0.41505377678599265</v>
       </c>
       <c r="C15" s="117"/>
       <c r="D15" s="117"/>
@@ -19593,24 +19596,35 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="B16">
+        <v>0.39914905811401724</v>
+      </c>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>0.05</v>
       </c>
-      <c r="C16" s="117"/>
-      <c r="D16" t="s">
+      <c r="C17" s="117"/>
+      <c r="D17" t="s">
         <v>537</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>538</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E9:E15"/>
-    <mergeCell ref="C9:C16"/>
-    <mergeCell ref="D9:D15"/>
+    <mergeCell ref="E9:E16"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="D9:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add missing Drum Cost Multiplier for NOAK
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\mouse\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1562A68-B21C-4A00-9A1D-53302E3A0D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0862F8A5-41EC-49D3-AE4A-4EC17C88E3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="877" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="16530" tabRatio="877" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -2634,6 +2634,39 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2641,18 +2674,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2671,27 +2692,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2727,6 +2727,13 @@
   </cellStyles>
   <dxfs count="108">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2736,13 +2743,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2787,15 +2787,9 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2807,9 +2801,15 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2930,7 +2930,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2943,14 +2950,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2969,8 +2969,58 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -2988,6 +3038,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2996,31 +3053,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
@@ -3034,40 +3068,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3105,10 +3105,45 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3118,11 +3153,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3152,22 +3186,18 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <i/>
       </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
+      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3181,17 +3211,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
       </fill>
     </dxf>
     <dxf>
@@ -3199,27 +3220,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3338,9 +3338,56 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3372,32 +3419,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3421,27 +3442,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4224,10 +4224,10 @@
       <c r="Q3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="94" t="s">
+      <c r="R3" s="93" t="s">
         <v>445</v>
       </c>
-      <c r="S3" s="96" t="s">
+      <c r="S3" s="99" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4314,8 +4314,8 @@
       <c r="Q4" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="94"/>
-      <c r="S4" s="96"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="99"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>467</v>
@@ -4394,10 +4394,10 @@
       <c r="Q5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="94" t="s">
+      <c r="R5" s="93" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="96" t="s">
+      <c r="S5" s="99" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4477,8 +4477,8 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="94"/>
-      <c r="S6" s="96"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="99"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>467</v>
@@ -4784,13 +4784,13 @@
       <c r="P11" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="94" t="s">
+      <c r="Q11" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="94" t="s">
+      <c r="R11" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="95" t="s">
+      <c r="S11" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -4881,9 +4881,9 @@
       <c r="P12" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="94"/>
-      <c r="R12" s="94"/>
-      <c r="S12" s="96"/>
+      <c r="Q12" s="93"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="99"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>470</v>
@@ -4965,9 +4965,9 @@
       <c r="P13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="94"/>
-      <c r="S13" s="96"/>
+      <c r="Q13" s="93"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="99"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>470</v>
@@ -5092,13 +5092,13 @@
       <c r="P15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="94" t="s">
+      <c r="Q15" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="94" t="s">
+      <c r="R15" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="95" t="s">
+      <c r="S15" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5182,9 +5182,9 @@
       <c r="P16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="94"/>
-      <c r="R16" s="94"/>
-      <c r="S16" s="96"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="99"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>470</v>
@@ -5266,9 +5266,9 @@
       <c r="P17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="94"/>
-      <c r="R17" s="94"/>
-      <c r="S17" s="96"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="93"/>
+      <c r="S17" s="99"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>470</v>
@@ -5632,13 +5632,13 @@
       <c r="P22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="94" t="s">
+      <c r="Q22" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="94" t="s">
+      <c r="R22" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="95" t="s">
+      <c r="S22" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5722,9 +5722,9 @@
       <c r="P23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q23" s="94"/>
-      <c r="R23" s="94"/>
-      <c r="S23" s="96"/>
+      <c r="Q23" s="93"/>
+      <c r="R23" s="93"/>
+      <c r="S23" s="99"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>470</v>
@@ -5806,9 +5806,9 @@
       <c r="P24" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="94"/>
-      <c r="R24" s="94"/>
-      <c r="S24" s="96"/>
+      <c r="Q24" s="93"/>
+      <c r="R24" s="93"/>
+      <c r="S24" s="99"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>470</v>
@@ -5933,13 +5933,13 @@
       <c r="P26" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="94" t="s">
+      <c r="Q26" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R26" s="94" t="s">
+      <c r="R26" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="95" t="s">
+      <c r="S26" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -6023,9 +6023,9 @@
       <c r="P27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" s="94"/>
-      <c r="R27" s="94"/>
-      <c r="S27" s="96"/>
+      <c r="Q27" s="93"/>
+      <c r="R27" s="93"/>
+      <c r="S27" s="99"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>470</v>
@@ -6107,9 +6107,9 @@
       <c r="P28" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="94"/>
-      <c r="R28" s="94"/>
-      <c r="S28" s="96"/>
+      <c r="Q28" s="93"/>
+      <c r="R28" s="93"/>
+      <c r="S28" s="99"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>470</v>
@@ -6238,13 +6238,13 @@
       <c r="P30" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="94" t="s">
+      <c r="Q30" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="94" t="s">
+      <c r="R30" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="95" t="s">
+      <c r="S30" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6332,9 +6332,9 @@
       <c r="P31" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="94"/>
-      <c r="R31" s="94"/>
-      <c r="S31" s="96"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="99"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>470</v>
@@ -6420,9 +6420,9 @@
       <c r="P32" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="94"/>
-      <c r="R32" s="94"/>
-      <c r="S32" s="96"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="93"/>
+      <c r="S32" s="99"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>470</v>
@@ -6731,13 +6731,13 @@
       <c r="P37" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q37" s="94" t="s">
+      <c r="Q37" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R37" s="94" t="s">
+      <c r="R37" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="95" t="s">
+      <c r="S37" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -6821,9 +6821,9 @@
       <c r="P38" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="94"/>
-      <c r="R38" s="94"/>
-      <c r="S38" s="96"/>
+      <c r="Q38" s="93"/>
+      <c r="R38" s="93"/>
+      <c r="S38" s="99"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>470</v>
@@ -6905,9 +6905,9 @@
       <c r="P39" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="94"/>
-      <c r="R39" s="94"/>
-      <c r="S39" s="96"/>
+      <c r="Q39" s="93"/>
+      <c r="R39" s="93"/>
+      <c r="S39" s="99"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>470</v>
@@ -7032,13 +7032,13 @@
       <c r="P41" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="94" t="s">
+      <c r="Q41" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="94" t="s">
+      <c r="R41" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="95" t="s">
+      <c r="S41" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7122,9 +7122,9 @@
       <c r="P42" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="94"/>
-      <c r="R42" s="94"/>
-      <c r="S42" s="96"/>
+      <c r="Q42" s="93"/>
+      <c r="R42" s="93"/>
+      <c r="S42" s="99"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>470</v>
@@ -7206,9 +7206,9 @@
       <c r="P43" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q43" s="94"/>
-      <c r="R43" s="94"/>
-      <c r="S43" s="96"/>
+      <c r="Q43" s="93"/>
+      <c r="R43" s="93"/>
+      <c r="S43" s="99"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>470</v>
@@ -7376,18 +7376,18 @@
       <c r="P46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="94" t="s">
+      <c r="Q46" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R46" s="94" t="s">
+      <c r="R46" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="95" t="s">
+      <c r="S46" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
       <c r="U46" s="80" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="V46" s="84">
         <f t="shared" si="4"/>
@@ -7466,12 +7466,12 @@
       <c r="P47" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="94"/>
-      <c r="R47" s="94"/>
-      <c r="S47" s="96"/>
+      <c r="Q47" s="93"/>
+      <c r="R47" s="93"/>
+      <c r="S47" s="99"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="V47" s="84">
         <f t="shared" si="4"/>
@@ -7550,12 +7550,12 @@
       <c r="P48" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q48" s="94"/>
-      <c r="R48" s="94"/>
-      <c r="S48" s="96"/>
+      <c r="Q48" s="93"/>
+      <c r="R48" s="93"/>
+      <c r="S48" s="99"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="V48" s="84">
         <f t="shared" si="4"/>
@@ -7819,16 +7819,16 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="104" t="s">
+      <c r="Q52" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="R52" s="104" t="s">
+      <c r="R52" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="98" t="s">
+      <c r="S52" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="90" t="s">
+      <c r="T52" s="101" t="s">
         <v>503</v>
       </c>
       <c r="U52" s="80" t="s">
@@ -7915,10 +7915,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="105"/>
-      <c r="R53" s="105"/>
-      <c r="S53" s="99"/>
-      <c r="T53" s="91"/>
+      <c r="Q53" s="97"/>
+      <c r="R53" s="97"/>
+      <c r="S53" s="106"/>
+      <c r="T53" s="102"/>
       <c r="U53" s="80" t="s">
         <v>470</v>
       </c>
@@ -8003,10 +8003,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="106"/>
-      <c r="R54" s="106"/>
-      <c r="S54" s="100"/>
-      <c r="T54" s="92"/>
+      <c r="Q54" s="98"/>
+      <c r="R54" s="98"/>
+      <c r="S54" s="107"/>
+      <c r="T54" s="103"/>
       <c r="U54" s="80" t="s">
         <v>470</v>
       </c>
@@ -8173,13 +8173,13 @@
       <c r="P57" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q57" s="94" t="s">
+      <c r="Q57" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R57" s="94" t="s">
+      <c r="R57" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="95" t="s">
+      <c r="S57" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8263,9 +8263,9 @@
       <c r="P58" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q58" s="94"/>
-      <c r="R58" s="94"/>
-      <c r="S58" s="96"/>
+      <c r="Q58" s="93"/>
+      <c r="R58" s="93"/>
+      <c r="S58" s="99"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>470</v>
@@ -8347,9 +8347,9 @@
       <c r="P59" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q59" s="94"/>
-      <c r="R59" s="94"/>
-      <c r="S59" s="96"/>
+      <c r="Q59" s="93"/>
+      <c r="R59" s="93"/>
+      <c r="S59" s="99"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>470</v>
@@ -8474,13 +8474,13 @@
       <c r="P61" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q61" s="94" t="s">
+      <c r="Q61" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R61" s="94" t="s">
+      <c r="R61" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="95" t="s">
+      <c r="S61" s="100" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8564,9 +8564,9 @@
       <c r="P62" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q62" s="94"/>
-      <c r="R62" s="94"/>
-      <c r="S62" s="96"/>
+      <c r="Q62" s="93"/>
+      <c r="R62" s="93"/>
+      <c r="S62" s="99"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>470</v>
@@ -8648,9 +8648,9 @@
       <c r="P63" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q63" s="94"/>
-      <c r="R63" s="94"/>
-      <c r="S63" s="96"/>
+      <c r="Q63" s="93"/>
+      <c r="R63" s="93"/>
+      <c r="S63" s="99"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>470</v>
@@ -8957,7 +8957,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="93" t="s">
+      <c r="R68" s="94" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -9046,7 +9046,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="93"/>
+      <c r="R69" s="94"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9140,7 +9140,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="93"/>
+      <c r="R70" s="94"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9227,7 +9227,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="93"/>
+      <c r="R71" s="94"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9316,7 +9316,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="93"/>
+      <c r="R72" s="94"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9410,7 +9410,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="93"/>
+      <c r="R73" s="94"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9580,17 +9580,17 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="93" t="s">
+      <c r="R76" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="97" t="s">
+      <c r="S76" s="104" t="s">
         <v>447</v>
       </c>
       <c r="T76" s="61" t="s">
         <v>184</v>
       </c>
       <c r="U76" s="80" t="s">
-        <v>466</v>
+        <v>540</v>
       </c>
       <c r="V76" s="84">
         <f t="shared" si="4"/>
@@ -9670,11 +9670,11 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="93"/>
-      <c r="S77" s="97"/>
+      <c r="R77" s="94"/>
+      <c r="S77" s="104"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
-        <v>466</v>
+        <v>540</v>
       </c>
       <c r="V77" s="84">
         <f t="shared" si="4"/>
@@ -9765,8 +9765,8 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="93"/>
-      <c r="S78" s="97"/>
+      <c r="R78" s="94"/>
+      <c r="S78" s="104"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
         <v>466</v>
@@ -9859,8 +9859,8 @@
       <c r="Q79" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="R79" s="93"/>
-      <c r="S79" s="97"/>
+      <c r="R79" s="94"/>
+      <c r="S79" s="104"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
         <v>466</v>
@@ -9954,8 +9954,8 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="93"/>
-      <c r="S80" s="97"/>
+      <c r="R80" s="94"/>
+      <c r="S80" s="104"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
         <v>535</v>
@@ -10237,7 +10237,7 @@
         <v>402</v>
       </c>
       <c r="U83" s="80" t="s">
-        <v>466</v>
+        <v>540</v>
       </c>
       <c r="V83" s="84">
         <f t="shared" si="25"/>
@@ -10379,7 +10379,7 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="97" t="s">
+      <c r="S85" s="104" t="s">
         <v>447</v>
       </c>
       <c r="T85" s="51"/>
@@ -10485,7 +10485,7 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="97"/>
+      <c r="S86" s="104"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
         <v>534</v>
@@ -10581,7 +10581,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="97"/>
+      <c r="S87" s="104"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>466</v>
@@ -10675,7 +10675,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="97"/>
+      <c r="S88" s="104"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>466</v>
@@ -10744,7 +10744,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="97"/>
+      <c r="S89" s="104"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -10816,7 +10816,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="97"/>
+      <c r="S90" s="104"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>466</v>
@@ -10910,7 +10910,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="97"/>
+      <c r="S91" s="104"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>466</v>
@@ -11274,13 +11274,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="93" t="s">
+      <c r="R96" s="94" t="s">
         <v>448</v>
       </c>
-      <c r="S96" s="101" t="s">
+      <c r="S96" s="108" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="93"/>
+      <c r="T96" s="94"/>
       <c r="U96" s="80" t="s">
         <v>466</v>
       </c>
@@ -11367,9 +11367,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="93"/>
-      <c r="S97" s="102"/>
-      <c r="T97" s="93"/>
+      <c r="R97" s="94"/>
+      <c r="S97" s="109"/>
+      <c r="T97" s="94"/>
       <c r="U97" s="80" t="s">
         <v>466</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>360</v>
       </c>
       <c r="S107" s="87"/>
-      <c r="T107" s="107" t="s">
+      <c r="T107" s="90" t="s">
         <v>506</v>
       </c>
       <c r="U107" s="80" t="s">
@@ -12301,7 +12301,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="108"/>
+      <c r="T108" s="91"/>
       <c r="U108" s="80" t="s">
         <v>466</v>
       </c>
@@ -13302,10 +13302,10 @@
       <c r="P122" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q122" s="103" t="s">
+      <c r="Q122" s="95" t="s">
         <v>427</v>
       </c>
-      <c r="R122" s="103" t="s">
+      <c r="R122" s="95" t="s">
         <v>365</v>
       </c>
       <c r="S122" s="51"/>
@@ -13394,8 +13394,8 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="103"/>
-      <c r="R123" s="103"/>
+      <c r="Q123" s="95"/>
+      <c r="R123" s="95"/>
       <c r="S123" s="51"/>
       <c r="T123" s="51"/>
       <c r="U123" s="80" t="s">
@@ -13482,8 +13482,8 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="103"/>
-      <c r="R124" s="103"/>
+      <c r="Q124" s="95"/>
+      <c r="R124" s="95"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
@@ -13570,8 +13570,8 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="103"/>
-      <c r="R125" s="103"/>
+      <c r="Q125" s="95"/>
+      <c r="R125" s="95"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
@@ -13658,8 +13658,8 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="103"/>
-      <c r="R126" s="103"/>
+      <c r="Q126" s="95"/>
+      <c r="R126" s="95"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
@@ -13746,8 +13746,8 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="103"/>
-      <c r="R127" s="103"/>
+      <c r="Q127" s="95"/>
+      <c r="R127" s="95"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
@@ -13870,10 +13870,10 @@
       <c r="P129" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q129" s="93" t="s">
+      <c r="Q129" s="94" t="s">
         <v>369</v>
       </c>
-      <c r="R129" s="93" t="s">
+      <c r="R129" s="94" t="s">
         <v>370</v>
       </c>
       <c r="S129" s="51"/>
@@ -13955,8 +13955,8 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="93"/>
-      <c r="R130" s="93"/>
+      <c r="Q130" s="94"/>
+      <c r="R130" s="94"/>
       <c r="S130" s="51"/>
       <c r="T130" s="51"/>
       <c r="U130" s="80" t="s">
@@ -14038,8 +14038,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="93"/>
-      <c r="R131" s="93"/>
+      <c r="Q131" s="94"/>
+      <c r="R131" s="94"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14123,8 +14123,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="93"/>
-      <c r="R132" s="93"/>
+      <c r="Q132" s="94"/>
+      <c r="R132" s="94"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14215,8 +14215,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="93"/>
-      <c r="R133" s="93"/>
+      <c r="Q133" s="94"/>
+      <c r="R133" s="94"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -14508,7 +14508,7 @@
       <c r="P138" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q138" s="94" t="s">
+      <c r="Q138" s="93" t="s">
         <v>364</v>
       </c>
       <c r="R138" s="48"/>
@@ -14588,7 +14588,7 @@
       <c r="P139" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q139" s="94"/>
+      <c r="Q139" s="93"/>
       <c r="R139" s="48"/>
       <c r="S139" s="48"/>
       <c r="T139" s="48"/>
@@ -14666,7 +14666,7 @@
       <c r="P140" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q140" s="94"/>
+      <c r="Q140" s="93"/>
       <c r="R140" s="51"/>
       <c r="S140" s="51"/>
       <c r="T140" s="51"/>
@@ -14744,7 +14744,7 @@
       <c r="P141" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q141" s="94"/>
+      <c r="Q141" s="93"/>
       <c r="R141" s="51"/>
       <c r="S141" s="51"/>
       <c r="T141" s="51"/>
@@ -15565,14 +15565,14 @@
       <c r="N154" s="51"/>
       <c r="O154" s="68"/>
       <c r="P154" s="51"/>
-      <c r="Q154" s="107" t="s">
+      <c r="Q154" s="90" t="s">
         <v>500</v>
       </c>
-      <c r="R154" s="107" t="s">
+      <c r="R154" s="90" t="s">
         <v>500</v>
       </c>
       <c r="S154" s="51"/>
-      <c r="T154" s="107" t="s">
+      <c r="T154" s="90" t="s">
         <v>501</v>
       </c>
       <c r="U154" s="80"/>
@@ -15614,10 +15614,10 @@
       <c r="N155" s="51"/>
       <c r="O155" s="68"/>
       <c r="P155" s="51"/>
-      <c r="Q155" s="109"/>
-      <c r="R155" s="109"/>
+      <c r="Q155" s="92"/>
+      <c r="R155" s="92"/>
       <c r="S155" s="51"/>
-      <c r="T155" s="109"/>
+      <c r="T155" s="92"/>
       <c r="U155" s="80"/>
       <c r="V155" s="84"/>
       <c r="W155" s="84"/>
@@ -15657,10 +15657,10 @@
       <c r="N156" s="51"/>
       <c r="O156" s="68"/>
       <c r="P156" s="51"/>
-      <c r="Q156" s="109"/>
-      <c r="R156" s="109"/>
+      <c r="Q156" s="92"/>
+      <c r="R156" s="92"/>
       <c r="S156" s="51"/>
-      <c r="T156" s="109"/>
+      <c r="T156" s="92"/>
       <c r="U156" s="80"/>
       <c r="V156" s="84"/>
       <c r="W156" s="84"/>
@@ -15700,10 +15700,10 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="109"/>
-      <c r="R157" s="109"/>
+      <c r="Q157" s="92"/>
+      <c r="R157" s="92"/>
       <c r="S157" s="51"/>
-      <c r="T157" s="109"/>
+      <c r="T157" s="92"/>
       <c r="U157" s="80"/>
       <c r="V157" s="84"/>
       <c r="W157" s="84"/>
@@ -15743,10 +15743,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="109"/>
-      <c r="R158" s="109"/>
+      <c r="Q158" s="92"/>
+      <c r="R158" s="92"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="109"/>
+      <c r="T158" s="92"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -15786,10 +15786,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="108"/>
-      <c r="R159" s="108"/>
+      <c r="Q159" s="91"/>
+      <c r="R159" s="91"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="108"/>
+      <c r="T159" s="91"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -16111,11 +16111,39 @@
   </sheetData>
   <autoFilter ref="A1:Z164" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="54">
-    <mergeCell ref="T107:T108"/>
-    <mergeCell ref="R154:R159"/>
-    <mergeCell ref="Q154:Q159"/>
-    <mergeCell ref="T154:T159"/>
-    <mergeCell ref="Q138:Q141"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16132,39 +16160,11 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q129:Q133"/>
     <mergeCell ref="Q122:Q127"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
-    <mergeCell ref="S26:S28"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
+    <mergeCell ref="T107:T108"/>
+    <mergeCell ref="R154:R159"/>
+    <mergeCell ref="Q154:Q159"/>
+    <mergeCell ref="T154:T159"/>
+    <mergeCell ref="Q138:Q141"/>
   </mergeCells>
   <conditionalFormatting sqref="A96:F98 A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 A150:J152 S152:T152">
     <cfRule type="expression" dxfId="107" priority="226">
@@ -16177,67 +16177,67 @@
       <formula>$B96&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81:K81 A1:AE52 A111:Q112 S111:T112 A150:J152 S152:T152">
+  <conditionalFormatting sqref="A81:K81 A111:Q112 S111:T112 A150:J152 S152:T152 A1:AE52">
     <cfRule type="expression" dxfId="104" priority="22">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132:P133">
-    <cfRule type="expression" dxfId="103" priority="174">
+    <cfRule type="expression" dxfId="103" priority="177">
+      <formula>$B132=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="174">
       <formula>$B132=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="175">
+    <cfRule type="expression" dxfId="101" priority="175">
       <formula>$B132=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="176">
+    <cfRule type="expression" dxfId="100" priority="176">
       <formula>$B132&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="177">
-      <formula>$B132=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:P143">
-    <cfRule type="expression" dxfId="99" priority="122">
+    <cfRule type="expression" dxfId="99" priority="124">
+      <formula>$B136&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="125">
+      <formula>$B136=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="122">
       <formula>$B136=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="123">
+    <cfRule type="expression" dxfId="96" priority="123">
       <formula>$B136=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="124">
-      <formula>$B136&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="125">
-      <formula>$B136=0</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A109:AE153 A154:P159 A160:AE164 U53:AE54 U108:AE108 Q154:AE154 S155:S159 U155:AE159">
+  <conditionalFormatting sqref="A53:S54 A108:S108 A109:AE153 A154:P159 A160:AE164 U53:AE54 U108:AE108 Q154:AE154 S155:S159 U155:AE159 A55:AE107">
     <cfRule type="expression" dxfId="95" priority="193">
       <formula>$B53=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="94" priority="230">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="94" priority="233">
+      <formula>$B95=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="93" priority="231">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="232">
+    <cfRule type="expression" dxfId="92" priority="230">
+      <formula>$B95=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="232">
       <formula>$B95&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="233">
-      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
     <cfRule type="expression" dxfId="90" priority="13">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="14">
+    <cfRule type="expression" dxfId="89" priority="15">
+      <formula>$B74&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="14">
       <formula>$B74=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="15">
-      <formula>$B74&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
@@ -16294,7 +16294,7 @@
       <formula>$B161=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE52 A53:S54 U53:AE54 A55:AE107 A108:S108 U108:AE108 A109:AE153 Q154:AE154 A154:P159 S155:S159 U155:AE159 A160:AE164">
+  <conditionalFormatting sqref="A53:S54 U53:AE54 A108:S108 U108:AE108 A109:AE153 Q154:AE154 A154:P159 S155:S159 U155:AE159 A160:AE164 A1:AE52 A55:AE107">
     <cfRule type="expression" dxfId="73" priority="191">
       <formula>$B1=2</formula>
     </cfRule>
@@ -16302,23 +16302,23 @@
       <formula>$B1&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A109:AE153 A160:AE164 A55:AE107 A1:AE52 A53:S54 U53:AE54 A108:S108 U108:AE108 Q154:AE154 A154:P159 S155:S159 U155:AE159">
+  <conditionalFormatting sqref="A109:AE153 A160:AE164 A53:S54 U53:AE54 A108:S108 U108:AE108 Q154:AE154 A154:P159 S155:S159 U155:AE159 A1:AE52 A55:AE107">
     <cfRule type="expression" dxfId="71" priority="190">
       <formula>$B1=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:R122 C123:P127">
-    <cfRule type="expression" dxfId="70" priority="49">
-      <formula>$B122=3</formula>
+    <cfRule type="expression" dxfId="70" priority="52">
+      <formula>$B122=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="50">
+    <cfRule type="expression" dxfId="69" priority="51">
+      <formula>$B122&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="50">
       <formula>$B122=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="51">
-      <formula>$B122&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="52">
-      <formula>$B122=0</formula>
+    <cfRule type="expression" dxfId="67" priority="49">
+      <formula>$B122=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
@@ -16367,31 +16367,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G54">
-    <cfRule type="expression" dxfId="65" priority="5">
-      <formula>$B52=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="6">
+    <cfRule type="expression" dxfId="65" priority="6">
       <formula>$B52=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="7">
+    <cfRule type="expression" dxfId="64" priority="7">
       <formula>$B52&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="8">
+    <cfRule type="expression" dxfId="63" priority="8">
       <formula>$B52=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="5">
+      <formula>$B52=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="61" priority="222">
+    <cfRule type="expression" dxfId="61" priority="225">
+      <formula>$B96=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="224">
+      <formula>$B96&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="222">
       <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="223">
+    <cfRule type="expression" dxfId="58" priority="223">
       <formula>$B96=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="224">
-      <formula>$B96&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="225">
-      <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -16401,11 +16401,11 @@
     <cfRule type="expression" dxfId="56" priority="29">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="30">
+    <cfRule type="expression" dxfId="55" priority="31">
+      <formula>$B5=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="30">
       <formula>$B5&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="31">
-      <formula>$B5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
@@ -16427,14 +16427,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="49" priority="75">
-      <formula>$B69=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="76">
+    <cfRule type="expression" dxfId="49" priority="76">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="77">
+    <cfRule type="expression" dxfId="48" priority="77">
       <formula>$B69&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="75">
+      <formula>$B69=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
@@ -16443,14 +16443,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="45" priority="85">
+    <cfRule type="expression" dxfId="45" priority="87">
+      <formula>$B68&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="85">
       <formula>$B68=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="86">
+    <cfRule type="expression" dxfId="43" priority="86">
       <formula>$B68=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="87">
-      <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
@@ -16459,28 +16459,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:J149">
-    <cfRule type="expression" dxfId="41" priority="106">
-      <formula>$B149=3</formula>
+    <cfRule type="expression" dxfId="41" priority="109">
+      <formula>$B149=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="107">
+    <cfRule type="expression" dxfId="40" priority="108">
+      <formula>$B149&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="107">
       <formula>$B149=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="108">
-      <formula>$B149&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="109">
-      <formula>$B149=0</formula>
+    <cfRule type="expression" dxfId="38" priority="106">
+      <formula>$B149=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I129:K130">
-    <cfRule type="expression" dxfId="37" priority="186">
-      <formula>$B129=3</formula>
+    <cfRule type="expression" dxfId="37" priority="188">
+      <formula>$B129&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="187">
       <formula>$B129=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="188">
-      <formula>$B129&lt;2</formula>
+    <cfRule type="expression" dxfId="35" priority="186">
+      <formula>$B129=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="189">
       <formula>$B129=0</formula>
@@ -16490,17 +16490,17 @@
     <cfRule type="expression" dxfId="33" priority="35">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="425">
-      <formula>#REF!=2</formula>
+    <cfRule type="expression" dxfId="32" priority="428">
+      <formula>#REF!=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="426">
+    <cfRule type="expression" dxfId="31" priority="427">
+      <formula>#REF!=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="426">
       <formula>#REF!&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="427">
-      <formula>#REF!=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="428">
-      <formula>#REF!=3</formula>
+    <cfRule type="expression" dxfId="29" priority="425">
+      <formula>#REF!=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
@@ -16568,17 +16568,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:Q143">
-    <cfRule type="expression" dxfId="12" priority="166">
-      <formula>$B142=3</formula>
+    <cfRule type="expression" dxfId="12" priority="168">
+      <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="167">
+    <cfRule type="expression" dxfId="11" priority="169">
+      <formula>$B142=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="167">
       <formula>$B142=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="168">
-      <formula>$B142&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="169">
-      <formula>$B142=0</formula>
+    <cfRule type="expression" dxfId="9" priority="166">
+      <formula>$B142=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
@@ -16604,14 +16604,14 @@
     <cfRule type="expression" dxfId="3" priority="251">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="252">
-      <formula>$B95=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="253">
+    <cfRule type="expression" dxfId="2" priority="253">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="254">
+    <cfRule type="expression" dxfId="1" priority="254">
       <formula>$B95=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="252">
+      <formula>$B95=2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
@@ -19429,7 +19429,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="164" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fix the LTMR results after changing the GCMR
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannbn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2728A36D-1E14-0049-9F8D-A70CB348B083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDC7B5E-1732-D844-82E6-3FDCF9732E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="21100" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Economics Parameters" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Database'!$A$1:$Z$164</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cost Database'!$A$1:$Z$165</definedName>
     <definedName name="CRF">#REF!</definedName>
     <definedName name="DiscountRate">#REF!</definedName>
     <definedName name="FacilityLifetime">#REF!</definedName>
@@ -167,7 +167,7 @@
     For the GCMR, likley includes replacement coolant, CO2 refill, etc.</t>
       </text>
     </comment>
-    <comment ref="C153" authorId="11" shapeId="0" xr:uid="{335259DE-3294-4740-8C40-6B23AE73FFDB}">
+    <comment ref="C154" authorId="11" shapeId="0" xr:uid="{335259DE-3294-4740-8C40-6B23AE73FFDB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="537">
   <si>
     <t>Account</t>
   </si>
@@ -1971,6 +1971,15 @@
   </si>
   <si>
     <t>Integrated Heat Exchanger Building Superstructure Area</t>
+  </si>
+  <si>
+    <t>NaK</t>
+  </si>
+  <si>
+    <t>MARVEL Project (communication with MARVEL Team)</t>
+  </si>
+  <si>
+    <t>Vendor Quotes</t>
   </si>
 </sst>
 </file>
@@ -2607,6 +2616,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2614,18 +2656,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2644,27 +2674,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2698,7 +2707,73 @@
     <cellStyle name="Normal 2" xfId="4" xr:uid="{E15291B7-9068-3147-AE9D-D55638463741}"/>
     <cellStyle name="Normal 2 5" xfId="3" xr:uid="{D5427F60-54E8-014E-9224-5454BAE094F2}"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="110">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2760,9 +2835,15 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2776,7 +2857,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2789,7 +2870,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2803,15 +2884,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2882,7 +2957,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2896,7 +2971,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2934,11 +3009,10 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2948,10 +3022,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3006,22 +3081,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3029,53 +3091,6 @@
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -3105,9 +3120,48 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray125"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3117,19 +3171,6 @@
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3159,32 +3200,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3193,13 +3211,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3218,7 +3229,43 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3231,7 +3278,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3239,6 +3286,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3311,28 +3365,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3346,48 +3379,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -3405,14 +3399,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3421,6 +3415,13 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3437,9 +3438,29 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3892,10 +3913,10 @@
   <threadedComment ref="C151" dT="2025-06-20T19:14:14.35" personId="{3B5B98F4-A9DA-4CFD-B3D9-F7907C025518}" id="{60EA5C16-5BC5-40F2-AD75-9609617C429D}" parentId="{8C62D7C0-F520-42A3-9908-A880BA4D938B}">
     <text>For the GCMR, likley includes replacement coolant, CO2 refill, etc.</text>
   </threadedComment>
-  <threadedComment ref="C153" dT="2025-06-20T19:15:18.25" personId="{3B5B98F4-A9DA-4CFD-B3D9-F7907C025518}" id="{335259DE-3294-4740-8C40-6B23AE73FFDB}">
+  <threadedComment ref="C154" dT="2025-06-20T19:15:18.25" personId="{3B5B98F4-A9DA-4CFD-B3D9-F7907C025518}" id="{335259DE-3294-4740-8C40-6B23AE73FFDB}">
     <text xml:space="preserve">Upgrades to maintain or improve plant capacity, meet future regulatory requirements, or plant life extensions. These costs are considered "sustaining capital" for continued plant operation and performance. </text>
   </threadedComment>
-  <threadedComment ref="C153" dT="2025-06-20T19:15:33.63" personId="{3B5B98F4-A9DA-4CFD-B3D9-F7907C025518}" id="{BCE40344-6953-455E-AB5E-F11B66204C5B}" parentId="{335259DE-3294-4740-8C40-6B23AE73FFDB}">
+  <threadedComment ref="C154" dT="2025-06-20T19:15:33.63" personId="{3B5B98F4-A9DA-4CFD-B3D9-F7907C025518}" id="{BCE40344-6953-455E-AB5E-F11B66204C5B}" parentId="{335259DE-3294-4740-8C40-6B23AE73FFDB}">
     <text>Will allocate vessel, internals, IHX replacement, etc.</text>
   </threadedComment>
 </ThreadedComments>
@@ -3903,10 +3924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
-  <dimension ref="A1:AH164"/>
+  <dimension ref="A1:AH165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -4137,10 +4158,10 @@
       <c r="Q3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="93" t="s">
+      <c r="R3" s="92" t="s">
         <v>445</v>
       </c>
-      <c r="S3" s="95" t="s">
+      <c r="S3" s="98" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4227,8 +4248,8 @@
       <c r="Q4" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="93"/>
-      <c r="S4" s="95"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="98"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>468</v>
@@ -4307,10 +4328,10 @@
       <c r="Q5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="93" t="s">
+      <c r="R5" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="95" t="s">
+      <c r="S5" s="98" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4390,8 +4411,8 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="93"/>
-      <c r="S6" s="95"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="98"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>468</v>
@@ -4697,13 +4718,13 @@
       <c r="P11" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="93" t="s">
+      <c r="Q11" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="93" t="s">
+      <c r="R11" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="94" t="s">
+      <c r="S11" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -4794,9 +4815,9 @@
       <c r="P12" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="93"/>
-      <c r="S12" s="95"/>
+      <c r="Q12" s="92"/>
+      <c r="R12" s="92"/>
+      <c r="S12" s="98"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>471</v>
@@ -4878,9 +4899,9 @@
       <c r="P13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="95"/>
+      <c r="Q13" s="92"/>
+      <c r="R13" s="92"/>
+      <c r="S13" s="98"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>471</v>
@@ -5005,13 +5026,13 @@
       <c r="P15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="93" t="s">
+      <c r="Q15" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="93" t="s">
+      <c r="R15" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="94" t="s">
+      <c r="S15" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5095,9 +5116,9 @@
       <c r="P16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="95"/>
+      <c r="Q16" s="92"/>
+      <c r="R16" s="92"/>
+      <c r="S16" s="98"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>471</v>
@@ -5179,9 +5200,9 @@
       <c r="P17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="93"/>
-      <c r="R17" s="93"/>
-      <c r="S17" s="95"/>
+      <c r="Q17" s="92"/>
+      <c r="R17" s="92"/>
+      <c r="S17" s="98"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>471</v>
@@ -5545,13 +5566,13 @@
       <c r="P22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="93" t="s">
+      <c r="Q22" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="93" t="s">
+      <c r="R22" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="94" t="s">
+      <c r="S22" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5635,9 +5656,9 @@
       <c r="P23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="95"/>
+      <c r="Q23" s="92"/>
+      <c r="R23" s="92"/>
+      <c r="S23" s="98"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>471</v>
@@ -5719,9 +5740,9 @@
       <c r="P24" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="95"/>
+      <c r="Q24" s="92"/>
+      <c r="R24" s="92"/>
+      <c r="S24" s="98"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>471</v>
@@ -5846,13 +5867,13 @@
       <c r="P26" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="93" t="s">
+      <c r="Q26" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R26" s="93" t="s">
+      <c r="R26" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="94" t="s">
+      <c r="S26" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -5936,9 +5957,9 @@
       <c r="P27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="93"/>
-      <c r="S27" s="95"/>
+      <c r="Q27" s="92"/>
+      <c r="R27" s="92"/>
+      <c r="S27" s="98"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>471</v>
@@ -6020,9 +6041,9 @@
       <c r="P28" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="93"/>
-      <c r="S28" s="95"/>
+      <c r="Q28" s="92"/>
+      <c r="R28" s="92"/>
+      <c r="S28" s="98"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>471</v>
@@ -6078,8 +6099,12 @@
         <v xml:space="preserve">                  Integrated Heat Exchanger Building</v>
       </c>
       <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
+      <c r="F29" s="41" t="s">
+        <v>351</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>354</v>
+      </c>
       <c r="H29" s="45"/>
       <c r="I29" s="46"/>
       <c r="J29" s="47"/>
@@ -6151,13 +6176,13 @@
       <c r="P30" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="93" t="s">
+      <c r="Q30" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="93" t="s">
+      <c r="R30" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="94" t="s">
+      <c r="S30" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6245,9 +6270,9 @@
       <c r="P31" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="95"/>
+      <c r="Q31" s="92"/>
+      <c r="R31" s="92"/>
+      <c r="S31" s="98"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>471</v>
@@ -6333,9 +6358,9 @@
       <c r="P32" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="93"/>
-      <c r="S32" s="95"/>
+      <c r="Q32" s="92"/>
+      <c r="R32" s="92"/>
+      <c r="S32" s="98"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>471</v>
@@ -6644,13 +6669,13 @@
       <c r="P37" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q37" s="93" t="s">
+      <c r="Q37" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R37" s="93" t="s">
+      <c r="R37" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="94" t="s">
+      <c r="S37" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -6734,9 +6759,9 @@
       <c r="P38" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="93"/>
-      <c r="R38" s="93"/>
-      <c r="S38" s="95"/>
+      <c r="Q38" s="92"/>
+      <c r="R38" s="92"/>
+      <c r="S38" s="98"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>471</v>
@@ -6818,9 +6843,9 @@
       <c r="P39" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="93"/>
-      <c r="R39" s="93"/>
-      <c r="S39" s="95"/>
+      <c r="Q39" s="92"/>
+      <c r="R39" s="92"/>
+      <c r="S39" s="98"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>471</v>
@@ -6945,13 +6970,13 @@
       <c r="P41" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="93" t="s">
+      <c r="Q41" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="93" t="s">
+      <c r="R41" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="94" t="s">
+      <c r="S41" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7035,9 +7060,9 @@
       <c r="P42" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="93"/>
-      <c r="R42" s="93"/>
-      <c r="S42" s="95"/>
+      <c r="Q42" s="92"/>
+      <c r="R42" s="92"/>
+      <c r="S42" s="98"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>471</v>
@@ -7119,9 +7144,9 @@
       <c r="P43" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q43" s="93"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="95"/>
+      <c r="Q43" s="92"/>
+      <c r="R43" s="92"/>
+      <c r="S43" s="98"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>471</v>
@@ -7289,13 +7314,13 @@
       <c r="P46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="93" t="s">
+      <c r="Q46" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R46" s="93" t="s">
+      <c r="R46" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="94" t="s">
+      <c r="S46" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
@@ -7379,9 +7404,9 @@
       <c r="P47" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="93"/>
-      <c r="R47" s="93"/>
-      <c r="S47" s="95"/>
+      <c r="Q47" s="92"/>
+      <c r="R47" s="92"/>
+      <c r="S47" s="98"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
         <v>467</v>
@@ -7463,9 +7488,9 @@
       <c r="P48" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q48" s="93"/>
-      <c r="R48" s="93"/>
-      <c r="S48" s="95"/>
+      <c r="Q48" s="92"/>
+      <c r="R48" s="92"/>
+      <c r="S48" s="98"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
         <v>467</v>
@@ -7660,7 +7685,7 @@
       </c>
       <c r="E51" s="41"/>
       <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
+      <c r="G51" s="47"/>
       <c r="H51" s="45"/>
       <c r="I51" s="59"/>
       <c r="J51" s="47"/>
@@ -7701,15 +7726,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">                              Manipulator Building Slab Roof</v>
       </c>
-      <c r="E52" s="41" t="s">
-        <v>341</v>
-      </c>
-      <c r="F52" s="41" t="s">
-        <v>351</v>
-      </c>
-      <c r="G52" s="47" t="s">
-        <v>354</v>
-      </c>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="47"/>
       <c r="H52" s="45"/>
       <c r="I52" s="46">
         <f>1200 *1.53</f>
@@ -7732,16 +7751,16 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="103" t="s">
+      <c r="Q52" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="R52" s="103" t="s">
+      <c r="R52" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="97" t="s">
+      <c r="S52" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="89" t="s">
+      <c r="T52" s="100" t="s">
         <v>507</v>
       </c>
       <c r="U52" s="80" t="s">
@@ -7797,15 +7816,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">                              ManipulatorBuilding Basement</v>
       </c>
-      <c r="E53" s="41" t="s">
-        <v>341</v>
-      </c>
-      <c r="F53" s="41" t="s">
-        <v>351</v>
-      </c>
-      <c r="G53" s="47" t="s">
-        <v>354</v>
-      </c>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="47"/>
       <c r="H53" s="45"/>
       <c r="I53" s="46">
         <f>943.9*1.53</f>
@@ -7828,10 +7841,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="104"/>
-      <c r="R53" s="104"/>
-      <c r="S53" s="98"/>
-      <c r="T53" s="90"/>
+      <c r="Q53" s="96"/>
+      <c r="R53" s="96"/>
+      <c r="S53" s="105"/>
+      <c r="T53" s="101"/>
       <c r="U53" s="80" t="s">
         <v>471</v>
       </c>
@@ -7885,15 +7898,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">                              Manipulator Building Exterior Walls</v>
       </c>
-      <c r="E54" s="41" t="s">
-        <v>341</v>
-      </c>
-      <c r="F54" s="41" t="s">
-        <v>351</v>
-      </c>
-      <c r="G54" s="47" t="s">
-        <v>354</v>
-      </c>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="47"/>
       <c r="H54" s="45"/>
       <c r="I54" s="46">
         <f>721.21*1.53</f>
@@ -7916,10 +7923,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="105"/>
-      <c r="R54" s="105"/>
-      <c r="S54" s="99"/>
-      <c r="T54" s="91"/>
+      <c r="Q54" s="97"/>
+      <c r="R54" s="97"/>
+      <c r="S54" s="106"/>
+      <c r="T54" s="102"/>
       <c r="U54" s="80" t="s">
         <v>471</v>
       </c>
@@ -8086,13 +8093,13 @@
       <c r="P57" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q57" s="93" t="s">
+      <c r="Q57" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R57" s="93" t="s">
+      <c r="R57" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="94" t="s">
+      <c r="S57" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8176,9 +8183,9 @@
       <c r="P58" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q58" s="93"/>
-      <c r="R58" s="93"/>
-      <c r="S58" s="95"/>
+      <c r="Q58" s="92"/>
+      <c r="R58" s="92"/>
+      <c r="S58" s="98"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>471</v>
@@ -8260,9 +8267,9 @@
       <c r="P59" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q59" s="93"/>
-      <c r="R59" s="93"/>
-      <c r="S59" s="95"/>
+      <c r="Q59" s="92"/>
+      <c r="R59" s="92"/>
+      <c r="S59" s="98"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>471</v>
@@ -8387,13 +8394,13 @@
       <c r="P61" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q61" s="93" t="s">
+      <c r="Q61" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="R61" s="93" t="s">
+      <c r="R61" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="94" t="s">
+      <c r="S61" s="99" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8477,9 +8484,9 @@
       <c r="P62" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="95"/>
+      <c r="Q62" s="92"/>
+      <c r="R62" s="92"/>
+      <c r="S62" s="98"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>471</v>
@@ -8561,9 +8568,9 @@
       <c r="P63" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q63" s="93"/>
-      <c r="R63" s="93"/>
-      <c r="S63" s="95"/>
+      <c r="Q63" s="92"/>
+      <c r="R63" s="92"/>
+      <c r="S63" s="98"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>471</v>
@@ -8870,7 +8877,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="92" t="s">
+      <c r="R68" s="93" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -8959,7 +8966,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="92"/>
+      <c r="R69" s="93"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9053,7 +9060,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="92"/>
+      <c r="R70" s="93"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9140,7 +9147,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="92"/>
+      <c r="R71" s="93"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9229,7 +9236,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="92"/>
+      <c r="R72" s="93"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9323,7 +9330,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="92"/>
+      <c r="R73" s="93"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9493,10 +9500,10 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="92" t="s">
+      <c r="R76" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="96" t="s">
+      <c r="S76" s="103" t="s">
         <v>447</v>
       </c>
       <c r="T76" s="61" t="s">
@@ -9583,8 +9590,8 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="92"/>
-      <c r="S77" s="96"/>
+      <c r="R77" s="93"/>
+      <c r="S77" s="103"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
         <v>450</v>
@@ -9678,8 +9685,8 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="92"/>
-      <c r="S78" s="96"/>
+      <c r="R78" s="93"/>
+      <c r="S78" s="103"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
         <v>450</v>
@@ -9772,8 +9779,8 @@
       <c r="Q79" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="R79" s="92"/>
-      <c r="S79" s="96"/>
+      <c r="R79" s="93"/>
+      <c r="S79" s="103"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
         <v>450</v>
@@ -9867,8 +9874,8 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="92"/>
-      <c r="S80" s="96"/>
+      <c r="R80" s="93"/>
+      <c r="S80" s="103"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
         <v>450</v>
@@ -10292,7 +10299,7 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="96" t="s">
+      <c r="S85" s="103" t="s">
         <v>447</v>
       </c>
       <c r="T85" s="51"/>
@@ -10398,7 +10405,7 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="96"/>
+      <c r="S86" s="103"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
         <v>467</v>
@@ -10494,7 +10501,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="96"/>
+      <c r="S87" s="103"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>467</v>
@@ -10588,7 +10595,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="96"/>
+      <c r="S88" s="103"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>467</v>
@@ -10657,7 +10664,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="96"/>
+      <c r="S89" s="103"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -10729,7 +10736,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="96"/>
+      <c r="S90" s="103"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>467</v>
@@ -10823,7 +10830,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="96"/>
+      <c r="S91" s="103"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>467</v>
@@ -11187,13 +11194,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="92" t="s">
+      <c r="R96" s="93" t="s">
         <v>448</v>
       </c>
-      <c r="S96" s="100" t="s">
+      <c r="S96" s="107" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="92"/>
+      <c r="T96" s="93"/>
       <c r="U96" s="80" t="s">
         <v>467</v>
       </c>
@@ -11280,9 +11287,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="92"/>
-      <c r="S97" s="101"/>
-      <c r="T97" s="92"/>
+      <c r="R97" s="93"/>
+      <c r="S97" s="108"/>
+      <c r="T97" s="93"/>
       <c r="U97" s="80" t="s">
         <v>467</v>
       </c>
@@ -12041,8 +12048,12 @@
         <v xml:space="preserve">                  Integrated Heat Transfer Vessel</v>
       </c>
       <c r="E106" s="41"/>
-      <c r="F106" s="41"/>
-      <c r="G106" s="41"/>
+      <c r="F106" s="41" t="s">
+        <v>351</v>
+      </c>
+      <c r="G106" s="41" t="s">
+        <v>354</v>
+      </c>
       <c r="H106" s="45"/>
       <c r="I106" s="63"/>
       <c r="J106" s="51"/>
@@ -12120,7 +12131,7 @@
         <v>360</v>
       </c>
       <c r="S107" s="87"/>
-      <c r="T107" s="106" t="s">
+      <c r="T107" s="89" t="s">
         <v>510</v>
       </c>
       <c r="U107" s="80" t="s">
@@ -12218,7 +12229,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="107"/>
+      <c r="T108" s="90"/>
       <c r="U108" s="80" t="s">
         <v>467</v>
       </c>
@@ -12703,7 +12714,7 @@
         <v>227</v>
       </c>
       <c r="B115" s="40">
-        <f t="shared" ref="B115:B164" si="53">IF(ISNUMBER(A115),
+        <f t="shared" ref="B115:B165" si="53">IF(ISNUMBER(A115),
     IF(AND(A115=INT(A115), MOD(A115, 10) = 0), 0,
         IF(AND(A115=INT(A115), LEN(A115)=2), 1,
             IF(AND(A115=INT(A115), LEN(A115)=3), 2,
@@ -12717,7 +12728,7 @@
         <v>20</v>
       </c>
       <c r="D115" s="41" t="str">
-        <f t="shared" ref="D115:D164" si="54">REPT("   ", B115*2) &amp; C115</f>
+        <f t="shared" ref="D115:D165" si="54">REPT("   ", B115*2) &amp; C115</f>
         <v xml:space="preserve">            Reactor Instrumentation and Control (I&amp;C)</v>
       </c>
       <c r="E115" s="41" t="s">
@@ -13219,10 +13230,10 @@
       <c r="P122" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q122" s="102" t="s">
+      <c r="Q122" s="94" t="s">
         <v>427</v>
       </c>
-      <c r="R122" s="102" t="s">
+      <c r="R122" s="94" t="s">
         <v>365</v>
       </c>
       <c r="S122" s="51"/>
@@ -13311,8 +13322,8 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="102"/>
-      <c r="R123" s="102"/>
+      <c r="Q123" s="94"/>
+      <c r="R123" s="94"/>
       <c r="S123" s="51"/>
       <c r="T123" s="51"/>
       <c r="U123" s="80" t="s">
@@ -13399,8 +13410,8 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="102"/>
-      <c r="R124" s="102"/>
+      <c r="Q124" s="94"/>
+      <c r="R124" s="94"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
@@ -13487,8 +13498,8 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="102"/>
-      <c r="R125" s="102"/>
+      <c r="Q125" s="94"/>
+      <c r="R125" s="94"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
@@ -13575,8 +13586,8 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="102"/>
-      <c r="R126" s="102"/>
+      <c r="Q126" s="94"/>
+      <c r="R126" s="94"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
@@ -13619,7 +13630,7 @@
     </row>
     <row r="127" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="39">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B127" s="40">
         <f t="shared" si="53"/>
@@ -13663,8 +13674,8 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="102"/>
-      <c r="R127" s="102"/>
+      <c r="Q127" s="94"/>
+      <c r="R127" s="94"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
@@ -13787,10 +13798,10 @@
       <c r="P129" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q129" s="92" t="s">
+      <c r="Q129" s="93" t="s">
         <v>369</v>
       </c>
-      <c r="R129" s="92" t="s">
+      <c r="R129" s="93" t="s">
         <v>370</v>
       </c>
       <c r="S129" s="51"/>
@@ -13872,8 +13883,8 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="92"/>
-      <c r="R130" s="92"/>
+      <c r="Q130" s="93"/>
+      <c r="R130" s="93"/>
       <c r="S130" s="51"/>
       <c r="T130" s="51"/>
       <c r="U130" s="80" t="s">
@@ -13955,8 +13966,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="92"/>
-      <c r="R131" s="92"/>
+      <c r="Q131" s="93"/>
+      <c r="R131" s="93"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14040,8 +14051,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="92"/>
-      <c r="R132" s="92"/>
+      <c r="Q132" s="93"/>
+      <c r="R132" s="93"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14132,8 +14143,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="92"/>
-      <c r="R133" s="92"/>
+      <c r="Q133" s="93"/>
+      <c r="R133" s="93"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -14425,7 +14436,7 @@
       <c r="P138" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q138" s="93" t="s">
+      <c r="Q138" s="92" t="s">
         <v>364</v>
       </c>
       <c r="R138" s="48"/>
@@ -14505,7 +14516,7 @@
       <c r="P139" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q139" s="93"/>
+      <c r="Q139" s="92"/>
       <c r="R139" s="48"/>
       <c r="S139" s="48"/>
       <c r="T139" s="48"/>
@@ -14583,7 +14594,7 @@
       <c r="P140" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q140" s="93"/>
+      <c r="Q140" s="92"/>
       <c r="R140" s="51"/>
       <c r="S140" s="51"/>
       <c r="T140" s="51"/>
@@ -14661,7 +14672,7 @@
       <c r="P141" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q141" s="93"/>
+      <c r="Q141" s="92"/>
       <c r="R141" s="51"/>
       <c r="S141" s="51"/>
       <c r="T141" s="51"/>
@@ -15050,22 +15061,22 @@
         <v>468</v>
       </c>
       <c r="V148" s="84">
-        <f t="shared" ref="V148:V164" si="57">0.9*$H148</f>
+        <f t="shared" ref="V148:V165" si="57">0.9*$H148</f>
         <v>0</v>
       </c>
       <c r="W148" s="84">
-        <f t="shared" ref="W148:W164" si="58">1.5*H148</f>
+        <f t="shared" ref="W148:W165" si="58">1.5*H148</f>
         <v>0</v>
       </c>
       <c r="X148" s="80" t="s">
         <v>451</v>
       </c>
       <c r="Y148" s="83">
-        <f t="shared" ref="Y148:Y164" si="59">0.9*I148</f>
+        <f t="shared" ref="Y148:Y165" si="59">0.9*I148</f>
         <v>160650</v>
       </c>
       <c r="Z148" s="83">
-        <f t="shared" ref="Z148:Z164" si="60">1.3*I148</f>
+        <f t="shared" ref="Z148:Z165" si="60">1.3*I148</f>
         <v>232050</v>
       </c>
       <c r="AA148" s="80" t="s">
@@ -15330,10 +15341,10 @@
         <v>342</v>
       </c>
       <c r="F152" s="41" t="s">
-        <v>351</v>
+        <v>495</v>
       </c>
       <c r="G152" s="41" t="s">
-        <v>354</v>
+        <v>496</v>
       </c>
       <c r="H152" s="45"/>
       <c r="I152" s="63">
@@ -15354,7 +15365,7 @@
         <v>2024</v>
       </c>
       <c r="P152" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q152" s="61" t="s">
         <v>498</v>
@@ -15372,7 +15383,7 @@
         <v>468</v>
       </c>
       <c r="V152" s="84">
-        <f t="shared" ref="V152" si="61">0.9*$H152</f>
+        <f t="shared" ref="V152:V153" si="61">0.9*$H152</f>
         <v>0</v>
       </c>
       <c r="W152" s="84">
@@ -15383,11 +15394,11 @@
         <v>451</v>
       </c>
       <c r="Y152" s="83">
-        <f t="shared" ref="Y152" si="63">0.9*I152</f>
+        <f>0.9*I152</f>
         <v>153</v>
       </c>
       <c r="Z152" s="83">
-        <f t="shared" ref="Z152" si="64">1.3*I152</f>
+        <f t="shared" ref="Z152" si="63">1.3*I152</f>
         <v>221</v>
       </c>
       <c r="AA152" s="80" t="s">
@@ -15406,69 +15417,118 @@
         <v>452</v>
       </c>
     </row>
-    <row r="153" spans="1:31" ht="127" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:31" ht="29" x14ac:dyDescent="0.2">
       <c r="A153" s="39">
+        <v>721</v>
+      </c>
+      <c r="B153" s="40">
+        <f t="shared" ref="B153" si="64">IF(ISNUMBER(A153),
+    IF(AND(A153=INT(A153), MOD(A153, 10) = 0), 0,
+        IF(AND(A153=INT(A153), LEN(A153)=2), 1,
+            IF(AND(A153=INT(A153), LEN(A153)=3), 2,
+                LEN(A153) - FIND(".", A153) + 2)
+        )
+    ),
+"")</f>
+        <v>2</v>
+      </c>
+      <c r="C153" s="58" t="s">
+        <v>495</v>
+      </c>
+      <c r="D153" s="41" t="str">
+        <f t="shared" ref="D153" si="65">REPT("   ", B153*2) &amp; C153</f>
+        <v xml:space="preserve">            Coolant</v>
+      </c>
+      <c r="E153" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="F153" s="41" t="s">
+        <v>495</v>
+      </c>
+      <c r="G153" s="41" t="s">
+        <v>534</v>
+      </c>
+      <c r="H153" s="45"/>
+      <c r="I153" s="63">
+        <v>118</v>
+      </c>
+      <c r="J153" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="K153" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="L153" s="51"/>
+      <c r="M153" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="N153" s="51"/>
+      <c r="O153" s="68">
+        <v>2023</v>
+      </c>
+      <c r="P153" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q153" s="61" t="s">
+        <v>535</v>
+      </c>
+      <c r="R153" s="65"/>
+      <c r="S153" s="87"/>
+      <c r="T153" s="51" t="s">
+        <v>536</v>
+      </c>
+      <c r="U153" s="80" t="s">
+        <v>468</v>
+      </c>
+      <c r="V153" s="84">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="W153" s="84">
+        <f t="shared" ref="W153" si="66">1.5*H153</f>
+        <v>0</v>
+      </c>
+      <c r="X153" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y153" s="83">
+        <f t="shared" ref="Y153" si="67">0.9*I153</f>
+        <v>106.2</v>
+      </c>
+      <c r="Z153" s="83">
+        <f t="shared" ref="Z153" si="68">1.3*I153</f>
+        <v>153.4</v>
+      </c>
+      <c r="AA153" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="AB153" s="83" t="s">
+        <v>475</v>
+      </c>
+      <c r="AC153" s="83" t="s">
+        <v>476</v>
+      </c>
+      <c r="AD153" s="83" t="s">
+        <v>477</v>
+      </c>
+      <c r="AE153" s="80" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="154" spans="1:31" ht="127" x14ac:dyDescent="0.2">
+      <c r="A154" s="39">
         <v>75</v>
       </c>
-      <c r="B153" s="40">
+      <c r="B154" s="40">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
-      <c r="C153" s="58" t="s">
+      <c r="C154" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D153" s="41" t="str">
+      <c r="D154" s="41" t="str">
         <f t="shared" si="54"/>
         <v xml:space="preserve">      Capital Plant Expenditures</v>
-      </c>
-      <c r="E153" s="41"/>
-      <c r="F153" s="41"/>
-      <c r="G153" s="41"/>
-      <c r="H153" s="45"/>
-      <c r="I153" s="63"/>
-      <c r="J153" s="51"/>
-      <c r="K153" s="61"/>
-      <c r="L153" s="51"/>
-      <c r="M153" s="51"/>
-      <c r="N153" s="51"/>
-      <c r="O153" s="68"/>
-      <c r="P153" s="51"/>
-      <c r="Q153" s="61" t="s">
-        <v>504</v>
-      </c>
-      <c r="R153" s="61" t="s">
-        <v>504</v>
-      </c>
-      <c r="S153" s="51"/>
-      <c r="T153" s="61" t="s">
-        <v>505</v>
-      </c>
-      <c r="U153" s="80"/>
-      <c r="V153" s="84"/>
-      <c r="W153" s="84"/>
-      <c r="X153" s="80"/>
-      <c r="Y153" s="83"/>
-      <c r="Z153" s="83"/>
-      <c r="AA153" s="80"/>
-      <c r="AB153" s="83"/>
-      <c r="AC153" s="83"/>
-      <c r="AD153" s="83"/>
-      <c r="AE153" s="80"/>
-    </row>
-    <row r="154" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="39">
-        <v>751</v>
-      </c>
-      <c r="B154" s="40">
-        <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="C154" s="58" t="s">
-        <v>512</v>
-      </c>
-      <c r="D154" s="41" t="str">
-        <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Vessel Replacements</v>
       </c>
       <c r="E154" s="41"/>
       <c r="F154" s="41"/>
@@ -15482,14 +15542,14 @@
       <c r="N154" s="51"/>
       <c r="O154" s="68"/>
       <c r="P154" s="51"/>
-      <c r="Q154" s="106" t="s">
+      <c r="Q154" s="61" t="s">
         <v>504</v>
       </c>
-      <c r="R154" s="106" t="s">
+      <c r="R154" s="61" t="s">
         <v>504</v>
       </c>
       <c r="S154" s="51"/>
-      <c r="T154" s="106" t="s">
+      <c r="T154" s="61" t="s">
         <v>505</v>
       </c>
       <c r="U154" s="80"/>
@@ -15504,20 +15564,20 @@
       <c r="AD154" s="83"/>
       <c r="AE154" s="80"/>
     </row>
-    <row r="155" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="39">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B155" s="40">
         <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="C155" s="58" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D155" s="41" t="str">
-        <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Moderator Replacements</v>
+        <f>REPT("   ", B155*2) &amp; C155</f>
+        <v xml:space="preserve">            Annualized Vessel Replacements</v>
       </c>
       <c r="E155" s="41"/>
       <c r="F155" s="41"/>
@@ -15531,10 +15591,16 @@
       <c r="N155" s="51"/>
       <c r="O155" s="68"/>
       <c r="P155" s="51"/>
-      <c r="Q155" s="108"/>
-      <c r="R155" s="108"/>
+      <c r="Q155" s="89" t="s">
+        <v>504</v>
+      </c>
+      <c r="R155" s="89" t="s">
+        <v>504</v>
+      </c>
       <c r="S155" s="51"/>
-      <c r="T155" s="108"/>
+      <c r="T155" s="89" t="s">
+        <v>505</v>
+      </c>
       <c r="U155" s="80"/>
       <c r="V155" s="84"/>
       <c r="W155" s="84"/>
@@ -15549,18 +15615,18 @@
     </row>
     <row r="156" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A156" s="39">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B156" s="40">
         <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="C156" s="58" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D156" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Reflector Replacements</v>
+        <v xml:space="preserve">            Annualized Moderator Replacements</v>
       </c>
       <c r="E156" s="41"/>
       <c r="F156" s="41"/>
@@ -15574,10 +15640,10 @@
       <c r="N156" s="51"/>
       <c r="O156" s="68"/>
       <c r="P156" s="51"/>
-      <c r="Q156" s="108"/>
-      <c r="R156" s="108"/>
+      <c r="Q156" s="91"/>
+      <c r="R156" s="91"/>
       <c r="S156" s="51"/>
-      <c r="T156" s="108"/>
+      <c r="T156" s="91"/>
       <c r="U156" s="80"/>
       <c r="V156" s="84"/>
       <c r="W156" s="84"/>
@@ -15590,20 +15656,20 @@
       <c r="AD156" s="83"/>
       <c r="AE156" s="80"/>
     </row>
-    <row r="157" spans="1:31" ht="29" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A157" s="39">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B157" s="40">
         <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="C157" s="58" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D157" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Reactivity Control Replacements</v>
+        <v xml:space="preserve">            Annualized Reflector Replacements</v>
       </c>
       <c r="E157" s="41"/>
       <c r="F157" s="41"/>
@@ -15617,10 +15683,10 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="108"/>
-      <c r="R157" s="108"/>
+      <c r="Q157" s="91"/>
+      <c r="R157" s="91"/>
       <c r="S157" s="51"/>
-      <c r="T157" s="108"/>
+      <c r="T157" s="91"/>
       <c r="U157" s="80"/>
       <c r="V157" s="84"/>
       <c r="W157" s="84"/>
@@ -15635,18 +15701,18 @@
     </row>
     <row r="158" spans="1:31" ht="29" x14ac:dyDescent="0.2">
       <c r="A158" s="39">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B158" s="40">
         <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="C158" s="58" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D158" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Integrated Heat Transfer System Replacements</v>
+        <v xml:space="preserve">            Annualized Reactivity Control Replacements</v>
       </c>
       <c r="E158" s="41"/>
       <c r="F158" s="41"/>
@@ -15660,10 +15726,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="108"/>
-      <c r="R158" s="108"/>
+      <c r="Q158" s="91"/>
+      <c r="R158" s="91"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="108"/>
+      <c r="T158" s="91"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -15676,20 +15742,20 @@
       <c r="AD158" s="83"/>
       <c r="AE158" s="80"/>
     </row>
-    <row r="159" spans="1:31" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:31" ht="29" x14ac:dyDescent="0.2">
       <c r="A159" s="39">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B159" s="40">
         <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="C159" s="58" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D159" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">            Annualized Misc. Replacements</v>
+        <v xml:space="preserve">            Annualized Integrated Heat Transfer System Replacements</v>
       </c>
       <c r="E159" s="41"/>
       <c r="F159" s="41"/>
@@ -15703,10 +15769,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="107"/>
-      <c r="R159" s="107"/>
+      <c r="Q159" s="91"/>
+      <c r="R159" s="91"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="107"/>
+      <c r="T159" s="91"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -15719,46 +15785,37 @@
       <c r="AD159" s="83"/>
       <c r="AE159" s="80"/>
     </row>
-    <row r="160" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:31" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="39">
-        <v>78</v>
+        <v>759</v>
       </c>
       <c r="B160" s="40">
-        <f t="shared" ref="B160" si="65">IF(ISNUMBER(A160),
-    IF(AND(A160=INT(A160), MOD(A160, 10) = 0), 0,
-        IF(AND(A160=INT(A160), LEN(A160)=2), 1,
-            IF(AND(A160=INT(A160), LEN(A160)=3), 2,
-                LEN(A160) - FIND(".", A160) + 2)
-        )
-    ),
-"")</f>
-        <v>1</v>
+        <f t="shared" si="53"/>
+        <v>2</v>
       </c>
       <c r="C160" s="58" t="s">
-        <v>42</v>
+        <v>517</v>
       </c>
       <c r="D160" s="41" t="str">
-        <f t="shared" ref="D160" si="66">REPT("   ", B160*2) &amp; C160</f>
-        <v xml:space="preserve">      Annualized Decommissioning Cost</v>
+        <f t="shared" si="54"/>
+        <v xml:space="preserve">            Annualized Misc. Replacements</v>
       </c>
       <c r="E160" s="41"/>
       <c r="F160" s="41"/>
       <c r="G160" s="41"/>
       <c r="H160" s="45"/>
-      <c r="I160" s="75"/>
+      <c r="I160" s="63"/>
       <c r="J160" s="51"/>
-      <c r="K160" s="47"/>
+      <c r="K160" s="61"/>
       <c r="L160" s="51"/>
       <c r="M160" s="51"/>
       <c r="N160" s="51"/>
       <c r="O160" s="68"/>
-      <c r="P160" s="76"/>
-      <c r="Q160" s="61"/>
-      <c r="R160" s="61"/>
+      <c r="P160" s="51"/>
+      <c r="Q160" s="90"/>
+      <c r="R160" s="90"/>
       <c r="S160" s="51"/>
-      <c r="T160" s="61" t="s">
-        <v>503</v>
-      </c>
+      <c r="T160" s="90"/>
       <c r="U160" s="80"/>
       <c r="V160" s="84"/>
       <c r="W160" s="84"/>
@@ -15771,37 +15828,46 @@
       <c r="AD160" s="83"/>
       <c r="AE160" s="80"/>
     </row>
-    <row r="161" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="39">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B161" s="40">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="C161" s="74" t="s">
-        <v>43</v>
+        <f t="shared" ref="B161" si="69">IF(ISNUMBER(A161),
+    IF(AND(A161=INT(A161), MOD(A161, 10) = 0), 0,
+        IF(AND(A161=INT(A161), LEN(A161)=2), 1,
+            IF(AND(A161=INT(A161), LEN(A161)=3), 2,
+                LEN(A161) - FIND(".", A161) + 2)
+        )
+    ),
+"")</f>
+        <v>1</v>
+      </c>
+      <c r="C161" s="58" t="s">
+        <v>42</v>
       </c>
       <c r="D161" s="41" t="str">
-        <f t="shared" si="54"/>
-        <v>Annualized Fuel Cost</v>
+        <f t="shared" ref="D161" si="70">REPT("   ", B161*2) &amp; C161</f>
+        <v xml:space="preserve">      Annualized Decommissioning Cost</v>
       </c>
       <c r="E161" s="41"/>
       <c r="F161" s="41"/>
       <c r="G161" s="41"/>
-      <c r="H161" s="42"/>
-      <c r="I161" s="42"/>
-      <c r="J161" s="40"/>
-      <c r="K161" s="43"/>
-      <c r="L161" s="40"/>
-      <c r="M161" s="40"/>
-      <c r="N161" s="40"/>
-      <c r="O161" s="42"/>
-      <c r="P161" s="40"/>
-      <c r="Q161" s="43"/>
-      <c r="R161" s="40"/>
-      <c r="S161" s="40"/>
-      <c r="T161" s="40"/>
+      <c r="H161" s="45"/>
+      <c r="I161" s="75"/>
+      <c r="J161" s="51"/>
+      <c r="K161" s="47"/>
+      <c r="L161" s="51"/>
+      <c r="M161" s="51"/>
+      <c r="N161" s="51"/>
+      <c r="O161" s="68"/>
+      <c r="P161" s="76"/>
+      <c r="Q161" s="61"/>
+      <c r="R161" s="61"/>
+      <c r="S161" s="51"/>
+      <c r="T161" s="61" t="s">
+        <v>503</v>
+      </c>
       <c r="U161" s="80"/>
       <c r="V161" s="84"/>
       <c r="W161" s="84"/>
@@ -15814,225 +15880,296 @@
       <c r="AD161" s="83"/>
       <c r="AE161" s="80"/>
     </row>
-    <row r="162" spans="1:31" ht="85" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A162" s="39">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B162" s="40">
         <f t="shared" si="53"/>
-        <v>1</v>
-      </c>
-      <c r="C162" s="58" t="s">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="C162" s="74" t="s">
+        <v>43</v>
       </c>
       <c r="D162" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">      Refueling Operations</v>
-      </c>
-      <c r="E162" s="41" t="s">
-        <v>342</v>
-      </c>
+        <v>Annualized Fuel Cost</v>
+      </c>
+      <c r="E162" s="41"/>
       <c r="F162" s="41"/>
       <c r="G162" s="41"/>
-      <c r="H162" s="45"/>
-      <c r="I162" s="63">
-        <v>178500</v>
-      </c>
-      <c r="J162" s="51" t="s">
-        <v>383</v>
-      </c>
-      <c r="K162" s="61" t="s">
-        <v>384</v>
-      </c>
-      <c r="L162" s="51"/>
-      <c r="M162" s="51"/>
-      <c r="N162" s="51">
-        <v>1</v>
-      </c>
-      <c r="O162" s="68">
-        <v>2024</v>
-      </c>
-      <c r="P162" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q162" s="61"/>
-      <c r="R162" s="61" t="s">
-        <v>385</v>
-      </c>
-      <c r="S162" s="51"/>
-      <c r="T162" s="51"/>
-      <c r="U162" s="80" t="s">
-        <v>468</v>
-      </c>
-      <c r="V162" s="84">
-        <f t="shared" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="W162" s="84">
-        <f t="shared" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="X162" s="80" t="s">
-        <v>451</v>
-      </c>
-      <c r="Y162" s="83">
-        <f t="shared" si="59"/>
-        <v>160650</v>
-      </c>
-      <c r="Z162" s="83">
-        <f t="shared" si="60"/>
-        <v>232050</v>
-      </c>
-      <c r="AA162" s="80" t="s">
-        <v>451</v>
-      </c>
-      <c r="AB162" s="83" t="s">
-        <v>475</v>
-      </c>
-      <c r="AC162" s="83" t="s">
-        <v>476</v>
-      </c>
-      <c r="AD162" s="83" t="s">
-        <v>477</v>
-      </c>
-      <c r="AE162" s="80" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="163" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+      <c r="H162" s="42"/>
+      <c r="I162" s="42"/>
+      <c r="J162" s="40"/>
+      <c r="K162" s="43"/>
+      <c r="L162" s="40"/>
+      <c r="M162" s="40"/>
+      <c r="N162" s="40"/>
+      <c r="O162" s="42"/>
+      <c r="P162" s="40"/>
+      <c r="Q162" s="43"/>
+      <c r="R162" s="40"/>
+      <c r="S162" s="40"/>
+      <c r="T162" s="40"/>
+      <c r="U162" s="80"/>
+      <c r="V162" s="84"/>
+      <c r="W162" s="84"/>
+      <c r="X162" s="80"/>
+      <c r="Y162" s="83"/>
+      <c r="Z162" s="83"/>
+      <c r="AA162" s="80"/>
+      <c r="AB162" s="83"/>
+      <c r="AC162" s="83"/>
+      <c r="AD162" s="83"/>
+      <c r="AE162" s="80"/>
+    </row>
+    <row r="163" spans="1:31" ht="85" x14ac:dyDescent="0.2">
       <c r="A163" s="39">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B163" s="40">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="C163" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D163" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">      Additional Nuclear Fuel</v>
-      </c>
-      <c r="E163" s="41"/>
+        <v xml:space="preserve">      Refueling Operations</v>
+      </c>
+      <c r="E163" s="41" t="s">
+        <v>342</v>
+      </c>
       <c r="F163" s="41"/>
       <c r="G163" s="41"/>
       <c r="H163" s="45"/>
-      <c r="I163" s="63"/>
-      <c r="J163" s="51"/>
-      <c r="K163" s="61"/>
+      <c r="I163" s="63">
+        <v>178500</v>
+      </c>
+      <c r="J163" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="K163" s="61" t="s">
+        <v>384</v>
+      </c>
       <c r="L163" s="51"/>
       <c r="M163" s="51"/>
-      <c r="N163" s="51"/>
-      <c r="O163" s="68"/>
-      <c r="P163" s="51"/>
+      <c r="N163" s="51">
+        <v>1</v>
+      </c>
+      <c r="O163" s="68">
+        <v>2024</v>
+      </c>
+      <c r="P163" s="76" t="s">
+        <v>72</v>
+      </c>
       <c r="Q163" s="61"/>
-      <c r="R163" s="51"/>
+      <c r="R163" s="61" t="s">
+        <v>385</v>
+      </c>
       <c r="S163" s="51"/>
       <c r="T163" s="51"/>
-      <c r="U163" s="80"/>
-      <c r="V163" s="84"/>
-      <c r="W163" s="84"/>
-      <c r="X163" s="80"/>
-      <c r="Y163" s="83"/>
-      <c r="Z163" s="83"/>
-      <c r="AA163" s="80"/>
-      <c r="AB163" s="83"/>
-      <c r="AC163" s="83"/>
-      <c r="AD163" s="83"/>
-      <c r="AE163" s="80"/>
-    </row>
-    <row r="164" spans="1:31" ht="29" x14ac:dyDescent="0.2">
+      <c r="U163" s="80" t="s">
+        <v>468</v>
+      </c>
+      <c r="V163" s="84">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="W163" s="84">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="X163" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y163" s="83">
+        <f t="shared" si="59"/>
+        <v>160650</v>
+      </c>
+      <c r="Z163" s="83">
+        <f t="shared" si="60"/>
+        <v>232050</v>
+      </c>
+      <c r="AA163" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="AB163" s="83" t="s">
+        <v>475</v>
+      </c>
+      <c r="AC163" s="83" t="s">
+        <v>476</v>
+      </c>
+      <c r="AD163" s="83" t="s">
+        <v>477</v>
+      </c>
+      <c r="AE163" s="80" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="164" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A164" s="39">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B164" s="40">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="C164" s="58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D164" s="41" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">      Spent Fuel Management</v>
-      </c>
-      <c r="E164" s="41" t="s">
-        <v>341</v>
-      </c>
+        <v xml:space="preserve">      Additional Nuclear Fuel</v>
+      </c>
+      <c r="E164" s="41"/>
       <c r="F164" s="41"/>
       <c r="G164" s="41"/>
       <c r="H164" s="45"/>
-      <c r="I164" s="63">
-        <v>1</v>
-      </c>
-      <c r="J164" s="51" t="s">
-        <v>396</v>
-      </c>
-      <c r="K164" s="61" t="s">
-        <v>397</v>
-      </c>
+      <c r="I164" s="63"/>
+      <c r="J164" s="51"/>
+      <c r="K164" s="61"/>
       <c r="L164" s="51"/>
       <c r="M164" s="51"/>
-      <c r="N164" s="51">
-        <v>1</v>
-      </c>
-      <c r="O164" s="68">
-        <v>2024</v>
-      </c>
-      <c r="P164" s="51" t="s">
-        <v>77</v>
-      </c>
+      <c r="N164" s="51"/>
+      <c r="O164" s="68"/>
+      <c r="P164" s="51"/>
       <c r="Q164" s="61"/>
       <c r="R164" s="51"/>
       <c r="S164" s="51"/>
       <c r="T164" s="51"/>
-      <c r="U164" s="80" t="s">
+      <c r="U164" s="80"/>
+      <c r="V164" s="84"/>
+      <c r="W164" s="84"/>
+      <c r="X164" s="80"/>
+      <c r="Y164" s="83"/>
+      <c r="Z164" s="83"/>
+      <c r="AA164" s="80"/>
+      <c r="AB164" s="83"/>
+      <c r="AC164" s="83"/>
+      <c r="AD164" s="83"/>
+      <c r="AE164" s="80"/>
+    </row>
+    <row r="165" spans="1:31" ht="29" x14ac:dyDescent="0.2">
+      <c r="A165" s="39">
+        <v>83</v>
+      </c>
+      <c r="B165" s="40">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="C165" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="D165" s="41" t="str">
+        <f t="shared" si="54"/>
+        <v xml:space="preserve">      Spent Fuel Management</v>
+      </c>
+      <c r="E165" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="F165" s="41"/>
+      <c r="G165" s="41"/>
+      <c r="H165" s="45"/>
+      <c r="I165" s="63">
+        <v>1</v>
+      </c>
+      <c r="J165" s="51" t="s">
+        <v>396</v>
+      </c>
+      <c r="K165" s="61" t="s">
+        <v>397</v>
+      </c>
+      <c r="L165" s="51"/>
+      <c r="M165" s="51"/>
+      <c r="N165" s="51">
+        <v>1</v>
+      </c>
+      <c r="O165" s="68">
+        <v>2024</v>
+      </c>
+      <c r="P165" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q165" s="61"/>
+      <c r="R165" s="51"/>
+      <c r="S165" s="51"/>
+      <c r="T165" s="51"/>
+      <c r="U165" s="80" t="s">
         <v>468</v>
       </c>
-      <c r="V164" s="84">
+      <c r="V165" s="84">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="W164" s="84">
+      <c r="W165" s="84">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="X164" s="80" t="s">
-        <v>451</v>
-      </c>
-      <c r="Y164" s="83">
+      <c r="X165" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y165" s="83">
         <f t="shared" si="59"/>
         <v>0.9</v>
       </c>
-      <c r="Z164" s="83">
+      <c r="Z165" s="83">
         <f t="shared" si="60"/>
         <v>1.3</v>
       </c>
-      <c r="AA164" s="80" t="s">
-        <v>451</v>
-      </c>
-      <c r="AB164" s="83" t="s">
+      <c r="AA165" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="AB165" s="83" t="s">
         <v>475</v>
       </c>
-      <c r="AC164" s="83" t="s">
+      <c r="AC165" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="AD164" s="83" t="s">
+      <c r="AD165" s="83" t="s">
         <v>477</v>
       </c>
-      <c r="AE164" s="80" t="s">
+      <c r="AE165" s="80" t="s">
         <v>452</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z164" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
+  <autoFilter ref="A1:Z165" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="54">
-    <mergeCell ref="T107:T108"/>
-    <mergeCell ref="R154:R159"/>
-    <mergeCell ref="Q154:Q159"/>
-    <mergeCell ref="T154:T159"/>
-    <mergeCell ref="Q138:Q141"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16049,197 +16186,169 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q129:Q133"/>
     <mergeCell ref="Q122:Q127"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
-    <mergeCell ref="S26:S28"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
+    <mergeCell ref="T107:T108"/>
+    <mergeCell ref="R155:R160"/>
+    <mergeCell ref="Q155:Q160"/>
+    <mergeCell ref="T155:T160"/>
+    <mergeCell ref="Q138:Q141"/>
   </mergeCells>
-  <conditionalFormatting sqref="A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 A150:J152 S152:T152 A96:F98">
-    <cfRule type="expression" dxfId="107" priority="228">
+  <conditionalFormatting sqref="A96:F98 A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 S152:T153 A150:J153">
+    <cfRule type="expression" dxfId="8" priority="232">
+      <formula>$B96=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="233">
+      <formula>$B96=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="234">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="226">
-      <formula>$B96=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="227">
-      <formula>$B96=2</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81:K81 A1:AE52 A111:Q112 S111:T112 A150:J152 S152:T152">
-    <cfRule type="expression" dxfId="104" priority="22">
+  <conditionalFormatting sqref="A81:K81 A1:AE52 A111:Q112 S111:T112 A150:J151 S152:T153 A152:E153 G152:J153">
+    <cfRule type="expression" dxfId="5" priority="28">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132:P133">
-    <cfRule type="expression" dxfId="103" priority="175">
+    <cfRule type="expression" dxfId="109" priority="180">
+      <formula>$B132=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="181">
       <formula>$B132=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="174">
-      <formula>$B132=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="176">
+    <cfRule type="expression" dxfId="107" priority="182">
       <formula>$B132&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="177">
+    <cfRule type="expression" dxfId="106" priority="183">
       <formula>$B132=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:P143">
-    <cfRule type="expression" dxfId="99" priority="125">
+    <cfRule type="expression" dxfId="105" priority="128">
+      <formula>$B136=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="129">
+      <formula>$B136=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="130">
+      <formula>$B136&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="131">
       <formula>$B136=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="124">
-      <formula>$B136&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="123">
-      <formula>$B136=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="122">
-      <formula>$B136=3</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:S54 A108:S108 A109:AE153 A154:P159 A160:AE164 U53:AE54 U108:AE108 Q154:AE154 S155:S159 U155:AE159 A55:AE107">
-    <cfRule type="expression" dxfId="95" priority="193">
+  <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A155:P160 A161:AE165 U53:AE54 U108:AE108 Q155:AE155 S156:S160 U156:AE160 A109:AE154">
+    <cfRule type="expression" dxfId="4" priority="199">
       <formula>$B53=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="94" priority="233">
-      <formula>$B95=0</formula>
+    <cfRule type="expression" dxfId="101" priority="236">
+      <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="232">
+    <cfRule type="expression" dxfId="100" priority="237">
+      <formula>$B95=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="238">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="231">
-      <formula>$B95=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="230">
-      <formula>$B95=3</formula>
+    <cfRule type="expression" dxfId="98" priority="239">
+      <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
-    <cfRule type="expression" dxfId="90" priority="13">
+    <cfRule type="expression" dxfId="97" priority="19">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="15">
+    <cfRule type="expression" dxfId="96" priority="20">
+      <formula>$B74=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="21">
       <formula>$B74&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="14">
-      <formula>$B74=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
-    <cfRule type="expression" dxfId="87" priority="72">
+    <cfRule type="expression" dxfId="94" priority="78">
       <formula>$B83=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A99:T99 A113:T121 A128:T128 L129:T129 L130:P130 I131:P131 A134:R134 A144:T147 A148:H149 S101:T106 S107:S108 A122:B127 S122:T127 S130:T134 R138:T143 A96:F98">
-    <cfRule type="expression" dxfId="86" priority="229">
+  <conditionalFormatting sqref="A99:T99 A113:T121 A128:T128 L129:T129 L130:P130 I131:P131 A134:R134 A144:T147 A148:H149 A96:F98 S101:T106 S107:S108 A122:B127 S122:T127 S130:T134 R138:T143">
+    <cfRule type="expression" dxfId="93" priority="235">
       <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:T110 A113:T121">
-    <cfRule type="expression" dxfId="85" priority="60">
+    <cfRule type="expression" dxfId="92" priority="66">
       <formula>$B109=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="61">
+    <cfRule type="expression" dxfId="91" priority="67">
       <formula>$B109=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="62">
+    <cfRule type="expression" dxfId="90" priority="68">
       <formula>$B109&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:T110">
-    <cfRule type="expression" dxfId="82" priority="197">
+    <cfRule type="expression" dxfId="89" priority="203">
       <formula>$B109=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:T135">
-    <cfRule type="expression" dxfId="81" priority="158">
+    <cfRule type="expression" dxfId="88" priority="164">
       <formula>$B135=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="159">
+    <cfRule type="expression" dxfId="87" priority="165">
       <formula>$B135=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="160">
+    <cfRule type="expression" dxfId="86" priority="166">
       <formula>$B135&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="161">
+    <cfRule type="expression" dxfId="85" priority="167">
       <formula>$B135=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A161:T164">
-    <cfRule type="expression" dxfId="77" priority="91">
-      <formula>$B161=2</formula>
+  <conditionalFormatting sqref="A162:T165">
+    <cfRule type="expression" dxfId="84" priority="96">
+      <formula>$B162=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="90">
-      <formula>$B161=3</formula>
+    <cfRule type="expression" dxfId="83" priority="97">
+      <formula>$B162=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="93">
-      <formula>$B161=0</formula>
+    <cfRule type="expression" dxfId="82" priority="98">
+      <formula>$B162&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="92">
-      <formula>$B161&lt;2</formula>
+    <cfRule type="expression" dxfId="81" priority="99">
+      <formula>$B162=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE52 A53:S54 U53:AE54 A108:S108 U108:AE108 A109:AE153 Q154:AE154 A154:P159 S155:S159 U155:AE159 A160:AE164 A55:AE107">
-    <cfRule type="expression" dxfId="73" priority="191">
+  <conditionalFormatting sqref="A1:AE52 A53:S54 U53:AE54 A55:AE107 A108:S108 U108:AE108 Q155:AE155 A155:P160 S156:S160 U156:AE160 A161:AE165 A109:AE154">
+    <cfRule type="expression" dxfId="3" priority="197">
       <formula>$B1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="192">
+    <cfRule type="expression" dxfId="2" priority="198">
       <formula>$B1&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A109:AE153 A160:AE164 A1:AE52 A53:S54 U53:AE54 A108:S108 U108:AE108 Q154:AE154 A154:P159 S155:S159 U155:AE159 A55:AE107">
-    <cfRule type="expression" dxfId="71" priority="190">
+  <conditionalFormatting sqref="A161:AE165 A55:AE107 A1:AE52 A53:S54 U53:AE54 A108:S108 U108:AE108 Q155:AE155 A155:P160 S156:S160 U156:AE160 A109:AE154">
+    <cfRule type="expression" dxfId="1" priority="196">
       <formula>$B1=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:R122 C123:P127">
-    <cfRule type="expression" dxfId="70" priority="52">
-      <formula>$B122=0</formula>
+    <cfRule type="expression" dxfId="80" priority="55">
+      <formula>$B122=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="51">
+    <cfRule type="expression" dxfId="79" priority="56">
+      <formula>$B122=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="57">
       <formula>$B122&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="49">
-      <formula>$B122=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="50">
-      <formula>$B122=2</formula>
+    <cfRule type="expression" dxfId="77" priority="58">
+      <formula>$B122=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16249,7 +16358,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="colorScale" priority="73">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16259,7 +16368,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D122:D127">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16268,8 +16377,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D128:D164 D2:D80 D82 D84:D121">
-    <cfRule type="colorScale" priority="478">
+  <conditionalFormatting sqref="D2:D80 D82 D84:D121 D128:D165">
+    <cfRule type="colorScale" priority="484">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16279,284 +16388,294 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E122:O127">
-    <cfRule type="expression" dxfId="66" priority="48">
+    <cfRule type="expression" dxfId="76" priority="54">
       <formula>_xlfn.ISFORMULA(E122)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F52:G54">
-    <cfRule type="expression" dxfId="65" priority="6">
-      <formula>$B52=2</formula>
+  <conditionalFormatting sqref="F51:G54">
+    <cfRule type="expression" dxfId="75" priority="3">
+      <formula>$B51=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="7">
-      <formula>$B52&lt;2</formula>
+    <cfRule type="expression" dxfId="74" priority="4">
+      <formula>$B51=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="8">
-      <formula>$B52=0</formula>
+    <cfRule type="expression" dxfId="73" priority="5">
+      <formula>$B51&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="5">
-      <formula>$B52=3</formula>
+    <cfRule type="expression" dxfId="72" priority="6">
+      <formula>$B51=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="61" priority="225">
-      <formula>$B96=0</formula>
+    <cfRule type="expression" dxfId="71" priority="228">
+      <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="224">
+    <cfRule type="expression" dxfId="70" priority="229">
+      <formula>$B96=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="230">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="223">
-      <formula>$B96=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="222">
-      <formula>$B96=3</formula>
+    <cfRule type="expression" dxfId="68" priority="231">
+      <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="57" priority="28">
+    <cfRule type="expression" dxfId="67" priority="34">
       <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="29">
+    <cfRule type="expression" dxfId="66" priority="35">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="30">
+    <cfRule type="expression" dxfId="65" priority="36">
       <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="31">
+    <cfRule type="expression" dxfId="64" priority="37">
       <formula>$B5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
-    <cfRule type="expression" dxfId="53" priority="83">
+    <cfRule type="expression" dxfId="63" priority="85">
+      <formula>_xlfn.ISFORMULA(H71)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="89">
       <formula>$B71=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="79">
-      <formula>_xlfn.ISFORMULA(H71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:O1048576">
-    <cfRule type="expression" dxfId="51" priority="89">
+    <cfRule type="expression" dxfId="61" priority="95">
       <formula>_xlfn.ISFORMULA(H1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:O70">
-    <cfRule type="expression" dxfId="50" priority="84">
+    <cfRule type="expression" dxfId="60" priority="90">
       <formula>_xlfn.ISFORMULA(H68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="49" priority="77">
-      <formula>$B69&lt;2</formula>
+    <cfRule type="expression" dxfId="59" priority="81">
+      <formula>$B69=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="76">
+    <cfRule type="expression" dxfId="58" priority="82">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="75">
-      <formula>$B69=3</formula>
+    <cfRule type="expression" dxfId="57" priority="83">
+      <formula>$B69&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
-    <cfRule type="expression" dxfId="46" priority="88">
+    <cfRule type="expression" dxfId="56" priority="94">
       <formula>$B68=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="45" priority="86">
+    <cfRule type="expression" dxfId="55" priority="91">
+      <formula>$B68=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="92">
       <formula>$B68=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="85">
-      <formula>$B68=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="87">
+    <cfRule type="expression" dxfId="53" priority="93">
       <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="42" priority="21">
+    <cfRule type="expression" dxfId="52" priority="27">
       <formula>_xlfn.ISFORMULA(I81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:J149">
-    <cfRule type="expression" dxfId="41" priority="106">
+    <cfRule type="expression" dxfId="51" priority="112">
       <formula>$B149=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="107">
+    <cfRule type="expression" dxfId="50" priority="113">
       <formula>$B149=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="108">
+    <cfRule type="expression" dxfId="49" priority="114">
       <formula>$B149&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="109">
+    <cfRule type="expression" dxfId="48" priority="115">
       <formula>$B149=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I129:K130">
-    <cfRule type="expression" dxfId="37" priority="186">
+    <cfRule type="expression" dxfId="47" priority="192">
       <formula>$B129=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="189">
-      <formula>$B129=0</formula>
+    <cfRule type="expression" dxfId="46" priority="193">
+      <formula>$B129=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="188">
+    <cfRule type="expression" dxfId="45" priority="194">
       <formula>$B129&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="187">
-      <formula>$B129=2</formula>
+    <cfRule type="expression" dxfId="44" priority="195">
+      <formula>$B129=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100">
-    <cfRule type="expression" dxfId="33" priority="35">
+    <cfRule type="expression" dxfId="43" priority="41">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="425">
+    <cfRule type="expression" dxfId="42" priority="431">
       <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="426">
+    <cfRule type="expression" dxfId="41" priority="432">
       <formula>#REF!&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="427">
+    <cfRule type="expression" dxfId="40" priority="433">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="428">
+    <cfRule type="expression" dxfId="39" priority="434">
       <formula>#REF!=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
-    <cfRule type="expression" dxfId="28" priority="34">
-      <formula>$B100&lt;2</formula>
+    <cfRule type="expression" dxfId="38" priority="38">
+      <formula>$B100=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="33">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>$B100=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="32">
-      <formula>$B100=3</formula>
+    <cfRule type="expression" dxfId="36" priority="40">
+      <formula>$B100&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L81">
-    <cfRule type="expression" dxfId="25" priority="16">
+    <cfRule type="expression" dxfId="35" priority="22">
       <formula>_xlfn.ISFORMULA(L81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L81:T81">
-    <cfRule type="expression" dxfId="24" priority="17">
+    <cfRule type="expression" dxfId="34" priority="23">
       <formula>$B81=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71:O73">
-    <cfRule type="expression" dxfId="23" priority="74">
+    <cfRule type="expression" dxfId="33" priority="80">
       <formula>_xlfn.ISFORMULA(O71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:O112 E83:O83">
-    <cfRule type="expression" dxfId="22" priority="68">
+    <cfRule type="expression" dxfId="32" priority="74">
       <formula>_xlfn.ISFORMULA(E83)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O135">
-    <cfRule type="expression" dxfId="21" priority="243">
+    <cfRule type="expression" dxfId="31" priority="249">
       <formula>$B136=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="244">
+    <cfRule type="expression" dxfId="30" priority="250">
       <formula>$B136=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="245">
+    <cfRule type="expression" dxfId="29" priority="251">
       <formula>$B136&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="246">
+    <cfRule type="expression" dxfId="28" priority="252">
       <formula>$B136=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71:Q73">
-    <cfRule type="expression" dxfId="17" priority="78">
+    <cfRule type="expression" dxfId="27" priority="84">
       <formula>$B71=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q138">
-    <cfRule type="expression" dxfId="16" priority="173">
-      <formula>$B138=0</formula>
+    <cfRule type="expression" dxfId="26" priority="176">
+      <formula>$B138=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="172">
+    <cfRule type="expression" dxfId="25" priority="177">
+      <formula>$B138=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="178">
       <formula>$B138&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="171">
-      <formula>$B138=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="170">
-      <formula>$B138=3</formula>
+    <cfRule type="expression" dxfId="23" priority="179">
+      <formula>$B138=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:Q143">
-    <cfRule type="expression" dxfId="12" priority="169">
-      <formula>$B142=0</formula>
+    <cfRule type="expression" dxfId="22" priority="172">
+      <formula>$B142=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="168">
+    <cfRule type="expression" dxfId="21" priority="173">
+      <formula>$B142=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="174">
       <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="167">
-      <formula>$B142=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="166">
-      <formula>$B142=3</formula>
+    <cfRule type="expression" dxfId="19" priority="175">
+      <formula>$B142=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
-    <cfRule type="expression" dxfId="8" priority="67">
+    <cfRule type="expression" dxfId="18" priority="73">
       <formula>$B87=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q136:T137">
-    <cfRule type="expression" dxfId="7" priority="130">
+    <cfRule type="expression" dxfId="17" priority="136">
       <formula>$B136=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="131">
+    <cfRule type="expression" dxfId="16" priority="137">
       <formula>$B136=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="132">
+    <cfRule type="expression" dxfId="15" priority="138">
       <formula>$B136&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="133">
+    <cfRule type="expression" dxfId="14" priority="139">
       <formula>$B136=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S96">
-    <cfRule type="expression" dxfId="3" priority="251">
+    <cfRule type="expression" dxfId="13" priority="257">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="252">
+    <cfRule type="expression" dxfId="12" priority="258">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="253">
+    <cfRule type="expression" dxfId="11" priority="259">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="254">
+    <cfRule type="expression" dxfId="10" priority="260">
       <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F152:F153">
+    <cfRule type="expression" dxfId="9" priority="2">
+      <formula>$B152=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G152:G153">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B152=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O165:P172 O137:O164 O2:O135" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O166:P173 O2:O135 O137:O165" xr:uid="{7C199008-9AB6-6549-A861-AD474C13E949}">
       <formula1>1950</formula1>
       <formula2>2025</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9 I57:I59 I61:I63 I84 L85:L93 I89:I94 H117:H118 H121:H128 I67:I79 L71:L83 I52:I54 I135:I164 H132:H164 I96:I133 L95:L1048576 H2:H114 L1:L67 I11:I48" xr:uid="{66ABF627-CC97-3E44-B6AC-09E441BED0CD}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9 I57:I59 I61:I63 I84 L85:L93 I89:I94 H117:H118 H121:H128 I67:I79 L71:L83 I52:I54 I96:I133 I11:I48 H2:H114 L1:L67 L95:L1048576 H132:H165 I135:I165" xr:uid="{66ABF627-CC97-3E44-B6AC-09E441BED0CD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K339:K349" xr:uid="{9E6037A9-5EC7-2945-A2FE-1723BA7DEE83}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K340:K350" xr:uid="{9E6037A9-5EC7-2945-A2FE-1723BA7DEE83}">
       <formula1>"Land Area, Power MWe, Excavation Volume,  Reactor Building Slab Roof Volume,	Reactor Building  Basement Volume, Reactor Building  Exterior Walls Volume,		Turbine Building Slab Roof Volume,	Turbine Building  Basement Volume,	Turbine Building  Exterior Wall"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J165:J1048576" xr:uid="{EEDF1E2A-32DC-6242-8EBD-BD01BBD19C77}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J166:J1048576" xr:uid="{EEDF1E2A-32DC-6242-8EBD-BD01BBD19C77}">
       <formula1>"$/acres, $/MWe, $/m^3, $/MWt"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N165:N318" xr:uid="{6D536505-A5B6-E145-A4B9-9C3C8E6B8527}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N166:N319" xr:uid="{6D536505-A5B6-E145-A4B9-9C3C8E6B8527}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N128:N164 N82:N121 N2:N80" xr:uid="{1C0096F5-23AB-5A48-8F14-E27BC72A38A6}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N80 N82:N121 N128:N165" xr:uid="{1C0096F5-23AB-5A48-8F14-E27BC72A38A6}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M121 M128:M164 M82:M118 M2:M80" xr:uid="{127B7473-9D01-354E-A3BD-12180E660A5C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M121 M2:M80 M82:M118 M128:M165" xr:uid="{127B7473-9D01-354E-A3BD-12180E660A5C}">
       <formula1>"acres, MWe, m^3, MWt, Kg, Drums, kW, $, m^2, kg/s"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J128:J164 J82:J121 J2:J80" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J80 J82:J121 J128:J165" xr:uid="{0FCCEC2F-487A-5A42-9C52-ED538456C753}">
       <formula1>"$/m^2,$/MWeHour,$/FTE, $/acres, $/MWe, $/m^3, $/MWt, $/Kg, $/Drum, $/(kg.sec), $/SWU, unitless, $/kWe"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M119:M120" xr:uid="{3DD8CB7E-F66A-4C30-8943-BB08D88ABA07}">
@@ -16572,10 +16691,10 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E164" xr:uid="{E571E7A1-C2F9-2E4D-99A9-8FA0C5D45C39}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E165" xr:uid="{E571E7A1-C2F9-2E4D-99A9-8FA0C5D45C39}">
       <formula1>"standard, nonstandard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P164" xr:uid="{17DDFD40-D97D-B64B-BD3B-AEAF52F6302C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P165" xr:uid="{17DDFD40-D97D-B64B-BD3B-AEAF52F6302C}">
       <formula1>"NA, General, Labor, Material, Equipment,Lab and Mat and Equip, 'Lab and Equip"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update the cost database to resolve PRs merging conflict
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannbn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDC7B5E-1732-D844-82E6-3FDCF9732E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7060DAED-B39E-5541-87D2-477478B847E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="21100" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="544">
   <si>
     <t>Account</t>
   </si>
@@ -1805,15 +1805,6 @@
     <t>Drum Count</t>
   </si>
   <si>
-    <t>Assumed Onsite Learning Rate</t>
-  </si>
-  <si>
-    <t>FOAK to NOAK Multipliers</t>
-  </si>
-  <si>
-    <t>Assumed Number Of Units For Onsite Learning</t>
-  </si>
-  <si>
     <t>In Vessel Shield Material</t>
   </si>
   <si>
@@ -1980,6 +1971,38 @@
   </si>
   <si>
     <t>Vendor Quotes</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>FOAK to NOAK Learning Rates</t>
+  </si>
+  <si>
+    <t>Assessment of Factory Fabrication Considerations
+for Nuclear Microreactors
+ 10.1080/00295450.2023.2206779</t>
+  </si>
+  <si>
+    <t>Calculated based on Refernce Paper + Gyutae's work. Refer to TEM Slides for rationale and methodology</t>
+  </si>
+  <si>
+    <t>Factory Be</t>
+  </si>
+  <si>
+    <t>Factory BeO</t>
+  </si>
+  <si>
+    <t>Non-nuclear off-the-shelf</t>
+  </si>
+  <si>
+    <t>Park, et al., Bottom-up levelized cost estimation of low-enriched and low-pressure nuclear batteries. Nuclear Engineering and Design. 2025.</t>
+  </si>
+  <si>
+    <t>For off-the-shelf commercial components that are not produced in the FB Factory</t>
   </si>
 </sst>
 </file>
@@ -2393,7 +2416,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2616,39 +2639,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2656,6 +2646,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2674,6 +2676,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2699,6 +2722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2707,7 +2731,352 @@
     <cellStyle name="Normal 2" xfId="4" xr:uid="{E15291B7-9068-3147-AE9D-D55638463741}"/>
     <cellStyle name="Normal 2 5" xfId="3" xr:uid="{D5427F60-54E8-014E-9224-5454BAE094F2}"/>
   </cellStyles>
-  <dxfs count="110">
+  <dxfs count="165">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2769,6 +3138,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2800,12 +3196,6 @@
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2843,29 +3233,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2875,44 +3245,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2996,17 +3332,17 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -3036,15 +3372,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3058,9 +3388,15 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -3101,13 +3437,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
@@ -3116,6 +3445,13 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3140,12 +3476,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i/>
       </font>
       <fill>
@@ -3161,16 +3491,22 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3207,15 +3543,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3223,49 +3553,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3283,6 +3570,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
@@ -3292,7 +3595,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3305,9 +3608,36 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3324,10 +3654,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3337,9 +3675,28 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3419,9 +3776,22 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -3438,6 +3808,32 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3446,7 +3842,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3460,7 +3856,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3926,8 +4322,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
   <dimension ref="A1:AH165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="C161" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3952,7 +4350,7 @@
     <col min="18" max="18" width="37.1640625" style="5" customWidth="1"/>
     <col min="19" max="19" width="81.1640625" style="5" customWidth="1"/>
     <col min="20" max="20" width="18.6640625" style="5" customWidth="1"/>
-    <col min="21" max="21" width="21.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.1640625" style="5" customWidth="1"/>
     <col min="22" max="23" width="16.6640625" style="37" customWidth="1"/>
     <col min="24" max="24" width="12.5" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="16.6640625" style="37" customWidth="1"/>
@@ -4158,10 +4556,10 @@
       <c r="Q3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="92" t="s">
+      <c r="R3" s="93" t="s">
         <v>445</v>
       </c>
-      <c r="S3" s="98" t="s">
+      <c r="S3" s="95" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4248,8 +4646,8 @@
       <c r="Q4" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="92"/>
-      <c r="S4" s="98"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="95"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>468</v>
@@ -4328,10 +4726,10 @@
       <c r="Q5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="92" t="s">
+      <c r="R5" s="93" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="98" t="s">
+      <c r="S5" s="95" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4411,8 +4809,8 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="92"/>
-      <c r="S6" s="98"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="95"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>468</v>
@@ -4718,13 +5116,13 @@
       <c r="P11" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="92" t="s">
+      <c r="Q11" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="92" t="s">
+      <c r="R11" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="99" t="s">
+      <c r="S11" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -4815,9 +5213,9 @@
       <c r="P12" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="92"/>
-      <c r="R12" s="92"/>
-      <c r="S12" s="98"/>
+      <c r="Q12" s="93"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="95"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>471</v>
@@ -4899,9 +5297,9 @@
       <c r="P13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="92"/>
-      <c r="S13" s="98"/>
+      <c r="Q13" s="93"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="95"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>471</v>
@@ -5026,13 +5424,13 @@
       <c r="P15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="92" t="s">
+      <c r="Q15" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="92" t="s">
+      <c r="R15" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="99" t="s">
+      <c r="S15" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5116,9 +5514,9 @@
       <c r="P16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="92"/>
-      <c r="R16" s="92"/>
-      <c r="S16" s="98"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="95"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>471</v>
@@ -5200,9 +5598,9 @@
       <c r="P17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="92"/>
-      <c r="R17" s="92"/>
-      <c r="S17" s="98"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="93"/>
+      <c r="S17" s="95"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>471</v>
@@ -5251,7 +5649,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D18" s="41" t="str">
         <f>REPT("   ", B18*2) &amp; C18</f>
@@ -5272,16 +5670,16 @@
         <v>6491.9267043635973</v>
       </c>
       <c r="J18" s="47" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="K18" s="49" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="L18" s="48">
         <v>9373</v>
       </c>
       <c r="M18" s="47" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="N18" s="48">
         <v>1</v>
@@ -5293,13 +5691,13 @@
         <v>77</v>
       </c>
       <c r="Q18" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="R18" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S18" s="88" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="T18" s="51"/>
       <c r="U18" s="80" t="s">
@@ -5349,7 +5747,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D19" s="41" t="str">
         <f>REPT("   ", B19*2) &amp; C19</f>
@@ -5391,13 +5789,13 @@
         <v>77</v>
       </c>
       <c r="Q19" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="R19" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S19" s="88" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="T19" s="51"/>
       <c r="U19" s="80" t="s">
@@ -5566,13 +5964,13 @@
       <c r="P22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="92" t="s">
+      <c r="Q22" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="92" t="s">
+      <c r="R22" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="99" t="s">
+      <c r="S22" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5656,9 +6054,9 @@
       <c r="P23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q23" s="92"/>
-      <c r="R23" s="92"/>
-      <c r="S23" s="98"/>
+      <c r="Q23" s="93"/>
+      <c r="R23" s="93"/>
+      <c r="S23" s="95"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>471</v>
@@ -5740,9 +6138,9 @@
       <c r="P24" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="92"/>
-      <c r="R24" s="92"/>
-      <c r="S24" s="98"/>
+      <c r="Q24" s="93"/>
+      <c r="R24" s="93"/>
+      <c r="S24" s="95"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>471</v>
@@ -5867,13 +6265,13 @@
       <c r="P26" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="92" t="s">
+      <c r="Q26" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R26" s="92" t="s">
+      <c r="R26" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="99" t="s">
+      <c r="S26" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -5957,9 +6355,9 @@
       <c r="P27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" s="92"/>
-      <c r="R27" s="92"/>
-      <c r="S27" s="98"/>
+      <c r="Q27" s="93"/>
+      <c r="R27" s="93"/>
+      <c r="S27" s="95"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>471</v>
@@ -6041,9 +6439,9 @@
       <c r="P28" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="92"/>
-      <c r="R28" s="92"/>
-      <c r="S28" s="98"/>
+      <c r="Q28" s="93"/>
+      <c r="R28" s="93"/>
+      <c r="S28" s="95"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>471</v>
@@ -6092,7 +6490,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D29" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6139,7 +6537,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D30" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6163,7 +6561,7 @@
         <v>79</v>
       </c>
       <c r="K30" s="49" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="L30" s="48"/>
       <c r="M30" s="47" t="s">
@@ -6176,13 +6574,13 @@
       <c r="P30" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="92" t="s">
+      <c r="Q30" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="92" t="s">
+      <c r="R30" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="99" t="s">
+      <c r="S30" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6233,7 +6631,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D31" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6257,7 +6655,7 @@
         <v>79</v>
       </c>
       <c r="K31" s="49" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="L31" s="48"/>
       <c r="M31" s="47" t="s">
@@ -6270,9 +6668,9 @@
       <c r="P31" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="92"/>
-      <c r="R31" s="92"/>
-      <c r="S31" s="98"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="95"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>471</v>
@@ -6321,7 +6719,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D32" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6345,7 +6743,7 @@
         <v>79</v>
       </c>
       <c r="K32" s="49" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="L32" s="48"/>
       <c r="M32" s="47" t="s">
@@ -6358,9 +6756,9 @@
       <c r="P32" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="92"/>
-      <c r="R32" s="92"/>
-      <c r="S32" s="98"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="93"/>
+      <c r="S32" s="95"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>471</v>
@@ -6409,7 +6807,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D33" s="41" t="str">
         <f t="shared" si="1"/>
@@ -6430,16 +6828,16 @@
         <v>6491.9267043635973</v>
       </c>
       <c r="J33" s="47" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="K33" s="49" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="L33" s="48">
         <v>9373</v>
       </c>
       <c r="M33" s="47" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="N33" s="48">
         <v>1</v>
@@ -6451,13 +6849,13 @@
         <v>77</v>
       </c>
       <c r="Q33" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="R33" s="49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S33" s="88" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="T33" s="51"/>
       <c r="U33" s="80" t="s">
@@ -6669,13 +7067,13 @@
       <c r="P37" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q37" s="92" t="s">
+      <c r="Q37" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R37" s="92" t="s">
+      <c r="R37" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="99" t="s">
+      <c r="S37" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -6759,9 +7157,9 @@
       <c r="P38" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="92"/>
-      <c r="R38" s="92"/>
-      <c r="S38" s="98"/>
+      <c r="Q38" s="93"/>
+      <c r="R38" s="93"/>
+      <c r="S38" s="95"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>471</v>
@@ -6843,9 +7241,9 @@
       <c r="P39" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="92"/>
-      <c r="R39" s="92"/>
-      <c r="S39" s="98"/>
+      <c r="Q39" s="93"/>
+      <c r="R39" s="93"/>
+      <c r="S39" s="95"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>471</v>
@@ -6970,13 +7368,13 @@
       <c r="P41" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="92" t="s">
+      <c r="Q41" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="92" t="s">
+      <c r="R41" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="99" t="s">
+      <c r="S41" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7060,9 +7458,9 @@
       <c r="P42" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="92"/>
-      <c r="R42" s="92"/>
-      <c r="S42" s="98"/>
+      <c r="Q42" s="93"/>
+      <c r="R42" s="93"/>
+      <c r="S42" s="95"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>471</v>
@@ -7144,9 +7542,9 @@
       <c r="P43" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q43" s="92"/>
-      <c r="R43" s="92"/>
-      <c r="S43" s="98"/>
+      <c r="Q43" s="93"/>
+      <c r="R43" s="93"/>
+      <c r="S43" s="95"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>471</v>
@@ -7314,18 +7712,18 @@
       <c r="P46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="92" t="s">
+      <c r="Q46" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R46" s="92" t="s">
+      <c r="R46" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="99" t="s">
+      <c r="S46" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
       <c r="U46" s="80" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="V46" s="84">
         <f t="shared" si="4"/>
@@ -7404,12 +7802,12 @@
       <c r="P47" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="92"/>
-      <c r="R47" s="92"/>
-      <c r="S47" s="98"/>
+      <c r="Q47" s="93"/>
+      <c r="R47" s="93"/>
+      <c r="S47" s="95"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="V47" s="84">
         <f t="shared" si="4"/>
@@ -7488,12 +7886,12 @@
       <c r="P48" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q48" s="92"/>
-      <c r="R48" s="92"/>
-      <c r="S48" s="98"/>
+      <c r="Q48" s="93"/>
+      <c r="R48" s="93"/>
+      <c r="S48" s="95"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="V48" s="84">
         <f t="shared" si="4"/>
@@ -7634,7 +8032,7 @@
         <v>3</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D50" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7677,7 +8075,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D51" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7720,7 +8118,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D52" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7738,7 +8136,7 @@
         <v>79</v>
       </c>
       <c r="K52" s="58" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="L52" s="47"/>
       <c r="M52" s="47" t="s">
@@ -7751,17 +8149,17 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="95" t="s">
+      <c r="Q52" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="R52" s="95" t="s">
+      <c r="R52" s="103" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="104" t="s">
+      <c r="S52" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="100" t="s">
-        <v>507</v>
+      <c r="T52" s="89" t="s">
+        <v>504</v>
       </c>
       <c r="U52" s="80" t="s">
         <v>471</v>
@@ -7810,7 +8208,7 @@
         <v>5</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D53" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7828,7 +8226,7 @@
         <v>79</v>
       </c>
       <c r="K53" s="58" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="L53" s="47"/>
       <c r="M53" s="47" t="s">
@@ -7841,10 +8239,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="96"/>
-      <c r="R53" s="96"/>
-      <c r="S53" s="105"/>
-      <c r="T53" s="101"/>
+      <c r="Q53" s="104"/>
+      <c r="R53" s="104"/>
+      <c r="S53" s="98"/>
+      <c r="T53" s="90"/>
       <c r="U53" s="80" t="s">
         <v>471</v>
       </c>
@@ -7892,7 +8290,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D54" s="41" t="str">
         <f t="shared" si="1"/>
@@ -7910,7 +8308,7 @@
         <v>79</v>
       </c>
       <c r="K54" s="58" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="L54" s="47"/>
       <c r="M54" s="47" t="s">
@@ -7923,10 +8321,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="97"/>
-      <c r="R54" s="97"/>
-      <c r="S54" s="106"/>
-      <c r="T54" s="102"/>
+      <c r="Q54" s="105"/>
+      <c r="R54" s="105"/>
+      <c r="S54" s="99"/>
+      <c r="T54" s="91"/>
       <c r="U54" s="80" t="s">
         <v>471</v>
       </c>
@@ -8093,13 +8491,13 @@
       <c r="P57" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q57" s="92" t="s">
+      <c r="Q57" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R57" s="92" t="s">
+      <c r="R57" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="99" t="s">
+      <c r="S57" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8183,9 +8581,9 @@
       <c r="P58" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q58" s="92"/>
-      <c r="R58" s="92"/>
-      <c r="S58" s="98"/>
+      <c r="Q58" s="93"/>
+      <c r="R58" s="93"/>
+      <c r="S58" s="95"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>471</v>
@@ -8267,9 +8665,9 @@
       <c r="P59" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q59" s="92"/>
-      <c r="R59" s="92"/>
-      <c r="S59" s="98"/>
+      <c r="Q59" s="93"/>
+      <c r="R59" s="93"/>
+      <c r="S59" s="95"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>471</v>
@@ -8394,13 +8792,13 @@
       <c r="P61" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q61" s="92" t="s">
+      <c r="Q61" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="R61" s="92" t="s">
+      <c r="R61" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="99" t="s">
+      <c r="S61" s="94" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8484,9 +8882,9 @@
       <c r="P62" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q62" s="92"/>
-      <c r="R62" s="92"/>
-      <c r="S62" s="98"/>
+      <c r="Q62" s="93"/>
+      <c r="R62" s="93"/>
+      <c r="S62" s="95"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>471</v>
@@ -8568,9 +8966,9 @@
       <c r="P63" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q63" s="92"/>
-      <c r="R63" s="92"/>
-      <c r="S63" s="98"/>
+      <c r="Q63" s="93"/>
+      <c r="R63" s="93"/>
+      <c r="S63" s="95"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>471</v>
@@ -8850,7 +9248,7 @@
         <v>341</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G68" s="41" t="s">
         <v>439</v>
@@ -8877,7 +9275,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="93" t="s">
+      <c r="R68" s="92" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -8939,7 +9337,7 @@
         <v>341</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G69" s="41" t="s">
         <v>440</v>
@@ -8966,7 +9364,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="93"/>
+      <c r="R69" s="92"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9033,7 +9431,7 @@
         <v>341</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G70" s="41" t="s">
         <v>441</v>
@@ -9060,7 +9458,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="93"/>
+      <c r="R70" s="92"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9120,7 +9518,7 @@
         <v>341</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G71" s="41" t="s">
         <v>439</v>
@@ -9147,7 +9545,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="93"/>
+      <c r="R71" s="92"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9209,7 +9607,7 @@
         <v>341</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G72" s="41" t="s">
         <v>440</v>
@@ -9236,7 +9634,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="93"/>
+      <c r="R72" s="92"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9303,7 +9701,7 @@
         <v>341</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G73" s="41" t="s">
         <v>441</v>
@@ -9330,7 +9728,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="93"/>
+      <c r="R73" s="92"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9500,10 +9898,10 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="93" t="s">
+      <c r="R76" s="92" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="103" t="s">
+      <c r="S76" s="96" t="s">
         <v>447</v>
       </c>
       <c r="T76" s="61" t="s">
@@ -9590,8 +9988,8 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="93"/>
-      <c r="S77" s="103"/>
+      <c r="R77" s="92"/>
+      <c r="S77" s="96"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
         <v>450</v>
@@ -9685,11 +10083,11 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="93"/>
-      <c r="S78" s="103"/>
+      <c r="R78" s="92"/>
+      <c r="S78" s="96"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
-        <v>450</v>
+        <v>467</v>
       </c>
       <c r="V78" s="84">
         <f t="shared" si="4"/>
@@ -9779,11 +10177,11 @@
       <c r="Q79" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="R79" s="93"/>
-      <c r="S79" s="103"/>
+      <c r="R79" s="92"/>
+      <c r="S79" s="96"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
-        <v>450</v>
+        <v>467</v>
       </c>
       <c r="V79" s="84">
         <f t="shared" si="4"/>
@@ -9874,11 +10272,11 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="93"/>
-      <c r="S80" s="103"/>
+      <c r="R80" s="92"/>
+      <c r="S80" s="96"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="V80" s="84">
         <f t="shared" ref="V80:V143" si="25">0.9*$H80</f>
@@ -9973,7 +10371,7 @@
       <c r="S81" s="67"/>
       <c r="T81" s="51"/>
       <c r="U81" s="80" t="s">
-        <v>450</v>
+        <v>539</v>
       </c>
       <c r="V81" s="84">
         <f t="shared" si="25"/>
@@ -10070,7 +10468,7 @@
       <c r="S82" s="67"/>
       <c r="T82" s="51"/>
       <c r="U82" s="80" t="s">
-        <v>450</v>
+        <v>467</v>
       </c>
       <c r="V82" s="84">
         <f t="shared" si="25"/>
@@ -10299,12 +10697,12 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="103" t="s">
+      <c r="S85" s="96" t="s">
         <v>447</v>
       </c>
       <c r="T85" s="51"/>
       <c r="U85" s="80" t="s">
-        <v>467</v>
+        <v>540</v>
       </c>
       <c r="V85" s="84">
         <f t="shared" si="25"/>
@@ -10405,10 +10803,10 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="103"/>
+      <c r="S86" s="96"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
-        <v>467</v>
+        <v>539</v>
       </c>
       <c r="V86" s="84">
         <f t="shared" si="25"/>
@@ -10501,7 +10899,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="103"/>
+      <c r="S87" s="96"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>467</v>
@@ -10595,7 +10993,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="103"/>
+      <c r="S88" s="96"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>467</v>
@@ -10664,7 +11062,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="103"/>
+      <c r="S89" s="96"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -10697,7 +11095,7 @@
         <v>341</v>
       </c>
       <c r="F90" s="41" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G90" s="41" t="s">
         <v>186</v>
@@ -10714,7 +11112,7 @@
         <v>174</v>
       </c>
       <c r="K90" s="61" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="L90" s="51">
         <f>L78</f>
@@ -10736,7 +11134,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="103"/>
+      <c r="S90" s="96"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>467</v>
@@ -10795,7 +11193,7 @@
         <v>341</v>
       </c>
       <c r="F91" s="41" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G91" s="41" t="s">
         <v>331</v>
@@ -10808,7 +11206,7 @@
         <v>174</v>
       </c>
       <c r="K91" s="61" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="L91" s="51">
         <f>'Design Variables'!B43</f>
@@ -10830,7 +11228,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="103"/>
+      <c r="S91" s="96"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>467</v>
@@ -11194,13 +11592,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="93" t="s">
+      <c r="R96" s="92" t="s">
         <v>448</v>
       </c>
-      <c r="S96" s="107" t="s">
+      <c r="S96" s="100" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="93"/>
+      <c r="T96" s="92"/>
       <c r="U96" s="80" t="s">
         <v>467</v>
       </c>
@@ -11287,9 +11685,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="93"/>
-      <c r="S97" s="108"/>
-      <c r="T97" s="93"/>
+      <c r="R97" s="92"/>
+      <c r="S97" s="101"/>
+      <c r="T97" s="92"/>
       <c r="U97" s="80" t="s">
         <v>467</v>
       </c>
@@ -11377,7 +11775,7 @@
       </c>
       <c r="S98" s="69"/>
       <c r="T98" s="65" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="U98" s="80" t="s">
         <v>467</v>
@@ -11946,7 +12344,7 @@
         <v>3</v>
       </c>
       <c r="C105" s="58" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D105" s="41" t="str">
         <f t="shared" si="48"/>
@@ -11956,10 +12354,10 @@
         <v>341</v>
       </c>
       <c r="F105" s="41" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G105" s="41" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H105" s="45"/>
       <c r="I105" s="63">
@@ -11969,7 +12367,7 @@
         <v>174</v>
       </c>
       <c r="K105" s="61" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="L105" s="51"/>
       <c r="M105" s="51" t="s">
@@ -11983,16 +12381,16 @@
         <v>74</v>
       </c>
       <c r="Q105" s="61" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="R105" s="65" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="S105" s="87" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="T105" s="51" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="U105" s="80" t="s">
         <v>468</v>
@@ -12041,7 +12439,7 @@
         <v>3</v>
       </c>
       <c r="C106" s="58" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D106" s="41" t="str">
         <f t="shared" si="48"/>
@@ -12088,7 +12486,7 @@
         <v>4</v>
       </c>
       <c r="C107" s="58" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D107" s="41" t="str">
         <f t="shared" si="48"/>
@@ -12111,7 +12509,7 @@
         <v>174</v>
       </c>
       <c r="K107" s="61" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L107" s="51"/>
       <c r="M107" s="51" t="s">
@@ -12131,8 +12529,8 @@
         <v>360</v>
       </c>
       <c r="S107" s="87"/>
-      <c r="T107" s="89" t="s">
-        <v>510</v>
+      <c r="T107" s="106" t="s">
+        <v>507</v>
       </c>
       <c r="U107" s="80" t="s">
         <v>467</v>
@@ -12181,7 +12579,7 @@
         <v>4</v>
       </c>
       <c r="C108" s="58" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D108" s="41" t="str">
         <f t="shared" si="48"/>
@@ -12205,7 +12603,7 @@
         <v>174</v>
       </c>
       <c r="K108" s="61" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L108" s="51">
         <v>387000</v>
@@ -12229,7 +12627,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="90"/>
+      <c r="T108" s="107"/>
       <c r="U108" s="80" t="s">
         <v>467</v>
       </c>
@@ -13021,7 +13419,7 @@
       </c>
       <c r="T119" s="51"/>
       <c r="U119" s="80" t="s">
-        <v>467</v>
+        <v>541</v>
       </c>
       <c r="V119" s="84">
         <f t="shared" si="25"/>
@@ -13230,16 +13628,16 @@
       <c r="P122" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q122" s="94" t="s">
+      <c r="Q122" s="102" t="s">
         <v>427</v>
       </c>
-      <c r="R122" s="94" t="s">
+      <c r="R122" s="102" t="s">
         <v>365</v>
       </c>
       <c r="S122" s="51"/>
       <c r="T122" s="51"/>
       <c r="U122" s="80" t="s">
-        <v>467</v>
+        <v>541</v>
       </c>
       <c r="V122" s="84">
         <f t="shared" si="25"/>
@@ -13322,12 +13720,12 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="94"/>
-      <c r="R123" s="94"/>
+      <c r="Q123" s="102"/>
+      <c r="R123" s="102"/>
       <c r="S123" s="51"/>
       <c r="T123" s="51"/>
       <c r="U123" s="80" t="s">
-        <v>467</v>
+        <v>541</v>
       </c>
       <c r="V123" s="84">
         <f t="shared" si="25"/>
@@ -13410,12 +13808,12 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="94"/>
-      <c r="R124" s="94"/>
+      <c r="Q124" s="102"/>
+      <c r="R124" s="102"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
-        <v>467</v>
+        <v>541</v>
       </c>
       <c r="V124" s="84">
         <f t="shared" si="25"/>
@@ -13498,12 +13896,12 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="94"/>
-      <c r="R125" s="94"/>
+      <c r="Q125" s="102"/>
+      <c r="R125" s="102"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
-        <v>467</v>
+        <v>541</v>
       </c>
       <c r="V125" s="84">
         <f t="shared" si="25"/>
@@ -13586,12 +13984,12 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="94"/>
-      <c r="R126" s="94"/>
+      <c r="Q126" s="102"/>
+      <c r="R126" s="102"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
-        <v>467</v>
+        <v>541</v>
       </c>
       <c r="V126" s="84">
         <f t="shared" si="25"/>
@@ -13674,12 +14072,12 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="94"/>
-      <c r="R127" s="94"/>
+      <c r="Q127" s="102"/>
+      <c r="R127" s="102"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
-        <v>467</v>
+        <v>541</v>
       </c>
       <c r="V127" s="84">
         <f t="shared" si="25"/>
@@ -13798,10 +14196,10 @@
       <c r="P129" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q129" s="93" t="s">
+      <c r="Q129" s="92" t="s">
         <v>369</v>
       </c>
-      <c r="R129" s="93" t="s">
+      <c r="R129" s="92" t="s">
         <v>370</v>
       </c>
       <c r="S129" s="51"/>
@@ -13883,8 +14281,8 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="93"/>
-      <c r="R130" s="93"/>
+      <c r="Q130" s="92"/>
+      <c r="R130" s="92"/>
       <c r="S130" s="51"/>
       <c r="T130" s="51"/>
       <c r="U130" s="80" t="s">
@@ -13966,8 +14364,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="93"/>
-      <c r="R131" s="93"/>
+      <c r="Q131" s="92"/>
+      <c r="R131" s="92"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14051,8 +14449,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="93"/>
-      <c r="R132" s="93"/>
+      <c r="Q132" s="92"/>
+      <c r="R132" s="92"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14143,8 +14541,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="93"/>
-      <c r="R133" s="93"/>
+      <c r="Q133" s="92"/>
+      <c r="R133" s="92"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -14436,7 +14834,7 @@
       <c r="P138" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q138" s="92" t="s">
+      <c r="Q138" s="93" t="s">
         <v>364</v>
       </c>
       <c r="R138" s="48"/>
@@ -14516,7 +14914,7 @@
       <c r="P139" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q139" s="92"/>
+      <c r="Q139" s="93"/>
       <c r="R139" s="48"/>
       <c r="S139" s="48"/>
       <c r="T139" s="48"/>
@@ -14594,7 +14992,7 @@
       <c r="P140" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q140" s="92"/>
+      <c r="Q140" s="93"/>
       <c r="R140" s="51"/>
       <c r="S140" s="51"/>
       <c r="T140" s="51"/>
@@ -14672,7 +15070,7 @@
       <c r="P141" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q141" s="92"/>
+      <c r="Q141" s="93"/>
       <c r="R141" s="51"/>
       <c r="S141" s="51"/>
       <c r="T141" s="51"/>
@@ -15331,7 +15729,7 @@
         <v>2</v>
       </c>
       <c r="C152" s="58" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D152" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15341,10 +15739,10 @@
         <v>342</v>
       </c>
       <c r="F152" s="41" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G152" s="41" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H152" s="45"/>
       <c r="I152" s="63">
@@ -15354,7 +15752,7 @@
         <v>174</v>
       </c>
       <c r="K152" s="61" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="L152" s="51"/>
       <c r="M152" s="51" t="s">
@@ -15368,16 +15766,16 @@
         <v>73</v>
       </c>
       <c r="Q152" s="61" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="R152" s="65" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="S152" s="87" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="T152" s="51" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="U152" s="80" t="s">
         <v>468</v>
@@ -15433,7 +15831,7 @@
         <v>2</v>
       </c>
       <c r="C153" s="58" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D153" s="41" t="str">
         <f t="shared" ref="D153" si="65">REPT("   ", B153*2) &amp; C153</f>
@@ -15443,10 +15841,10 @@
         <v>342</v>
       </c>
       <c r="F153" s="41" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G153" s="41" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="H153" s="45"/>
       <c r="I153" s="63">
@@ -15456,7 +15854,7 @@
         <v>174</v>
       </c>
       <c r="K153" s="61" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="L153" s="51"/>
       <c r="M153" s="51" t="s">
@@ -15470,12 +15868,12 @@
         <v>73</v>
       </c>
       <c r="Q153" s="61" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="R153" s="65"/>
       <c r="S153" s="87"/>
       <c r="T153" s="51" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="U153" s="80" t="s">
         <v>468</v>
@@ -15543,14 +15941,14 @@
       <c r="O154" s="68"/>
       <c r="P154" s="51"/>
       <c r="Q154" s="61" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="R154" s="61" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="S154" s="51"/>
       <c r="T154" s="61" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="U154" s="80"/>
       <c r="V154" s="84"/>
@@ -15573,7 +15971,7 @@
         <v>2</v>
       </c>
       <c r="C155" s="58" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D155" s="41" t="str">
         <f>REPT("   ", B155*2) &amp; C155</f>
@@ -15591,15 +15989,15 @@
       <c r="N155" s="51"/>
       <c r="O155" s="68"/>
       <c r="P155" s="51"/>
-      <c r="Q155" s="89" t="s">
-        <v>504</v>
-      </c>
-      <c r="R155" s="89" t="s">
-        <v>504</v>
+      <c r="Q155" s="106" t="s">
+        <v>501</v>
+      </c>
+      <c r="R155" s="106" t="s">
+        <v>501</v>
       </c>
       <c r="S155" s="51"/>
-      <c r="T155" s="89" t="s">
-        <v>505</v>
+      <c r="T155" s="106" t="s">
+        <v>502</v>
       </c>
       <c r="U155" s="80"/>
       <c r="V155" s="84"/>
@@ -15622,7 +16020,7 @@
         <v>2</v>
       </c>
       <c r="C156" s="58" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D156" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15640,10 +16038,10 @@
       <c r="N156" s="51"/>
       <c r="O156" s="68"/>
       <c r="P156" s="51"/>
-      <c r="Q156" s="91"/>
-      <c r="R156" s="91"/>
+      <c r="Q156" s="108"/>
+      <c r="R156" s="108"/>
       <c r="S156" s="51"/>
-      <c r="T156" s="91"/>
+      <c r="T156" s="108"/>
       <c r="U156" s="80"/>
       <c r="V156" s="84"/>
       <c r="W156" s="84"/>
@@ -15665,7 +16063,7 @@
         <v>2</v>
       </c>
       <c r="C157" s="58" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D157" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15683,10 +16081,10 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="91"/>
-      <c r="R157" s="91"/>
+      <c r="Q157" s="108"/>
+      <c r="R157" s="108"/>
       <c r="S157" s="51"/>
-      <c r="T157" s="91"/>
+      <c r="T157" s="108"/>
       <c r="U157" s="80"/>
       <c r="V157" s="84"/>
       <c r="W157" s="84"/>
@@ -15708,7 +16106,7 @@
         <v>2</v>
       </c>
       <c r="C158" s="58" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D158" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15726,10 +16124,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="91"/>
-      <c r="R158" s="91"/>
+      <c r="Q158" s="108"/>
+      <c r="R158" s="108"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="91"/>
+      <c r="T158" s="108"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -15751,7 +16149,7 @@
         <v>2</v>
       </c>
       <c r="C159" s="58" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D159" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15769,10 +16167,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="91"/>
-      <c r="R159" s="91"/>
+      <c r="Q159" s="108"/>
+      <c r="R159" s="108"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="91"/>
+      <c r="T159" s="108"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -15794,7 +16192,7 @@
         <v>2</v>
       </c>
       <c r="C160" s="58" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D160" s="41" t="str">
         <f t="shared" si="54"/>
@@ -15812,10 +16210,10 @@
       <c r="N160" s="51"/>
       <c r="O160" s="68"/>
       <c r="P160" s="51"/>
-      <c r="Q160" s="90"/>
-      <c r="R160" s="90"/>
+      <c r="Q160" s="107"/>
+      <c r="R160" s="107"/>
       <c r="S160" s="51"/>
-      <c r="T160" s="90"/>
+      <c r="T160" s="107"/>
       <c r="U160" s="80"/>
       <c r="V160" s="84"/>
       <c r="W160" s="84"/>
@@ -15866,7 +16264,7 @@
       <c r="R161" s="61"/>
       <c r="S161" s="51"/>
       <c r="T161" s="61" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="U161" s="80"/>
       <c r="V161" s="84"/>
@@ -16137,39 +16535,11 @@
   </sheetData>
   <autoFilter ref="A1:Z165" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="54">
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="S26:S28"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="T107:T108"/>
+    <mergeCell ref="R155:R160"/>
+    <mergeCell ref="Q155:Q160"/>
+    <mergeCell ref="T155:T160"/>
+    <mergeCell ref="Q138:Q141"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16186,169 +16556,212 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q129:Q133"/>
     <mergeCell ref="Q122:Q127"/>
-    <mergeCell ref="T107:T108"/>
-    <mergeCell ref="R155:R160"/>
-    <mergeCell ref="Q155:Q160"/>
-    <mergeCell ref="T155:T160"/>
-    <mergeCell ref="Q138:Q141"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
   </mergeCells>
-  <conditionalFormatting sqref="A96:F98 A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 S152:T153 A150:J153">
-    <cfRule type="expression" dxfId="8" priority="232">
+  <conditionalFormatting sqref="A96:F98 A99:T99 S101:T106 S107:S108 A111:Q112 S111:T112 A122:B127 S122:T127 A128:T128 L129:T129 L130:P130 S130:T134 I131:P131 A134:R134 R138:T143 A144:T147 A148:H149 A150:J153 S152:T153">
+    <cfRule type="expression" dxfId="164" priority="290">
+      <formula>$B96&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="163" priority="289">
+      <formula>$B96=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="162" priority="288">
       <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="233">
-      <formula>$B96=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="234">
-      <formula>$B96&lt;2</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A150:J153">
+    <cfRule type="expression" dxfId="161" priority="57">
+      <formula>$B150=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81:K81 A1:AE52 A111:Q112 S111:T112 A150:J151 S152:T153 A152:E153 G152:J153">
-    <cfRule type="expression" dxfId="5" priority="28">
+  <conditionalFormatting sqref="A81:K81 A1:AE45 A111:Q112 S111:T112 S152:T153 A49:AE52 A46:T48 V46:AE48">
+    <cfRule type="expression" dxfId="160" priority="84">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132:P133">
-    <cfRule type="expression" dxfId="109" priority="180">
-      <formula>$B132=3</formula>
+    <cfRule type="expression" dxfId="159" priority="239">
+      <formula>$B132=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="181">
+    <cfRule type="expression" dxfId="158" priority="238">
+      <formula>$B132&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="157" priority="237">
       <formula>$B132=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="182">
-      <formula>$B132&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="183">
-      <formula>$B132=0</formula>
+    <cfRule type="expression" dxfId="156" priority="236">
+      <formula>$B132=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:P143">
-    <cfRule type="expression" dxfId="105" priority="128">
+    <cfRule type="expression" dxfId="155" priority="185">
+      <formula>$B136=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="187">
+      <formula>$B136=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="186">
+      <formula>$B136&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="184">
       <formula>$B136=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="129">
-      <formula>$B136=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="130">
-      <formula>$B136&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="131">
-      <formula>$B136=0</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:S54 A55:AE107 A108:S108 A155:P160 A161:AE165 U53:AE54 U108:AE108 Q155:AE155 S156:S160 U156:AE160 A109:AE154">
-    <cfRule type="expression" dxfId="4" priority="199">
+  <conditionalFormatting sqref="A53:S54 A55:AE75 A108:S108 A109:AE118 A155:P160 A161:AE165 U53:AE54 U108:AE108 Q155:AE155 S156:S160 U156:AE160 A83:AE84 A76:T82 V76:AE82 A89:AE89 A85:T88 V85:AE88 A94:AE95 A90:T93 V90:AE93 A99:AE107 A96:T98 V96:AE98 A120:AE121 A119:T119 V119:AE119 A128:AE154 A122:T127 V122:AE127">
+    <cfRule type="expression" dxfId="151" priority="255">
       <formula>$B53=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="101" priority="236">
+    <cfRule type="expression" dxfId="150" priority="292">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="237">
+    <cfRule type="expression" dxfId="149" priority="293">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="238">
+    <cfRule type="expression" dxfId="148" priority="294">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="239">
+    <cfRule type="expression" dxfId="147" priority="295">
       <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
-    <cfRule type="expression" dxfId="97" priority="19">
+    <cfRule type="expression" dxfId="146" priority="75">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="20">
+    <cfRule type="expression" dxfId="145" priority="76">
       <formula>$B74=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="21">
+    <cfRule type="expression" dxfId="144" priority="77">
       <formula>$B74&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
-    <cfRule type="expression" dxfId="94" priority="78">
+    <cfRule type="expression" dxfId="143" priority="134">
       <formula>$B83=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:T99 A113:T121 A128:T128 L129:T129 L130:P130 I131:P131 A134:R134 A144:T147 A148:H149 A96:F98 S101:T106 S107:S108 A122:B127 S122:T127 S130:T134 R138:T143">
-    <cfRule type="expression" dxfId="93" priority="235">
+    <cfRule type="expression" dxfId="142" priority="291">
       <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:T110 A113:T121">
-    <cfRule type="expression" dxfId="92" priority="66">
+    <cfRule type="expression" dxfId="141" priority="122">
       <formula>$B109=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="67">
+    <cfRule type="expression" dxfId="140" priority="124">
+      <formula>$B109&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="123">
       <formula>$B109=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="68">
-      <formula>$B109&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:T110">
-    <cfRule type="expression" dxfId="89" priority="203">
+    <cfRule type="expression" dxfId="138" priority="259">
       <formula>$B109=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:T135">
-    <cfRule type="expression" dxfId="88" priority="164">
-      <formula>$B135=3</formula>
+    <cfRule type="expression" dxfId="137" priority="223">
+      <formula>$B135=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="165">
+    <cfRule type="expression" dxfId="136" priority="222">
+      <formula>$B135&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="135" priority="221">
       <formula>$B135=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="166">
-      <formula>$B135&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="167">
-      <formula>$B135=0</formula>
+    <cfRule type="expression" dxfId="134" priority="220">
+      <formula>$B135=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A162:T165">
-    <cfRule type="expression" dxfId="84" priority="96">
+    <cfRule type="expression" dxfId="133" priority="152">
       <formula>$B162=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="97">
+    <cfRule type="expression" dxfId="132" priority="153">
       <formula>$B162=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="98">
+    <cfRule type="expression" dxfId="131" priority="155">
+      <formula>$B162=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="154">
       <formula>$B162&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="99">
-      <formula>$B162=0</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AE45 A53:S54 U53:AE54 A55:AE75 A108:S108 U108:AE108 A109:AE118 Q155:AE155 A155:P160 S156:S160 U156:AE160 A161:AE165 A49:AE52 A46:T48 V46:AE48 A83:AE84 A76:T82 V76:AE82 A89:AE89 A85:T88 V85:AE88 A94:AE95 A90:T93 V90:AE93 A99:AE107 A96:T98 V96:AE98 A120:AE121 A119:T119 V119:AE119 A128:AE154 A122:T127 V122:AE127">
+    <cfRule type="expression" dxfId="129" priority="254">
+      <formula>$B1&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="253">
+      <formula>$B1=2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE52 A53:S54 U53:AE54 A55:AE107 A108:S108 U108:AE108 Q155:AE155 A155:P160 S156:S160 U156:AE160 A161:AE165 A109:AE154">
-    <cfRule type="expression" dxfId="3" priority="197">
-      <formula>$B1=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="198">
-      <formula>$B1&lt;2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A161:AE165 A55:AE107 A1:AE52 A53:S54 U53:AE54 A108:S108 U108:AE108 Q155:AE155 A155:P160 S156:S160 U156:AE160 A109:AE154">
-    <cfRule type="expression" dxfId="1" priority="196">
+  <conditionalFormatting sqref="A109:AE118 A161:AE165 A55:AE75 A1:AE45 A53:S54 U53:AE54 A108:S108 U108:AE108 Q155:AE155 A155:P160 S156:S160 U156:AE160 A49:AE52 A46:T48 V46:AE48 A83:AE84 A76:T82 V76:AE82 A89:AE89 A85:T88 V85:AE88 A94:AE95 A90:T93 V90:AE93 A99:AE107 A96:T98 V96:AE98 A120:AE121 A119:T119 V119:AE119 A128:AE154 A122:T127 V122:AE127">
+    <cfRule type="expression" dxfId="127" priority="252">
       <formula>$B1=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:R122 C123:P127">
-    <cfRule type="expression" dxfId="80" priority="55">
+    <cfRule type="expression" dxfId="126" priority="114">
+      <formula>$B122=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="113">
+      <formula>$B122&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="112">
+      <formula>$B122=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="111">
       <formula>$B122=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="56">
-      <formula>$B122=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="57">
-      <formula>$B122&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="58">
-      <formula>$B122=0</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D80 D82 D84:D121 D128:D165">
+    <cfRule type="colorScale" priority="540">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16358,7 +16771,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="135">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16368,17 +16781,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D122:D127">
-    <cfRule type="colorScale" priority="59">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D80 D82 D84:D121 D128:D165">
-    <cfRule type="colorScale" priority="484">
+    <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16388,266 +16791,508 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E122:O127">
-    <cfRule type="expression" dxfId="76" priority="54">
+    <cfRule type="expression" dxfId="122" priority="110">
       <formula>_xlfn.ISFORMULA(E122)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:G54">
-    <cfRule type="expression" dxfId="75" priority="3">
-      <formula>$B51=3</formula>
+    <cfRule type="expression" dxfId="121" priority="61">
+      <formula>$B51&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="4">
+    <cfRule type="expression" dxfId="120" priority="62">
+      <formula>$B51=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="119" priority="60">
       <formula>$B51=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="5">
-      <formula>$B51&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="6">
-      <formula>$B51=0</formula>
+    <cfRule type="expression" dxfId="118" priority="59">
+      <formula>$B51=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="71" priority="228">
+    <cfRule type="expression" dxfId="117" priority="284">
       <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="229">
+    <cfRule type="expression" dxfId="116" priority="285">
       <formula>$B96=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="230">
+    <cfRule type="expression" dxfId="115" priority="286">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="231">
+    <cfRule type="expression" dxfId="114" priority="287">
       <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="67" priority="34">
+    <cfRule type="expression" dxfId="113" priority="90">
       <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="35">
-      <formula>$B5=2</formula>
+    <cfRule type="expression" dxfId="112" priority="93">
+      <formula>$B5=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="36">
+    <cfRule type="expression" dxfId="111" priority="92">
       <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="37">
-      <formula>$B5=0</formula>
+    <cfRule type="expression" dxfId="110" priority="91">
+      <formula>$B5=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
-    <cfRule type="expression" dxfId="63" priority="85">
+    <cfRule type="expression" dxfId="109" priority="145">
+      <formula>$B71=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="141">
       <formula>_xlfn.ISFORMULA(H71)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="89">
-      <formula>$B71=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:O1048576">
-    <cfRule type="expression" dxfId="61" priority="95">
+    <cfRule type="expression" dxfId="107" priority="151">
       <formula>_xlfn.ISFORMULA(H1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:O70">
-    <cfRule type="expression" dxfId="60" priority="90">
+    <cfRule type="expression" dxfId="106" priority="146">
       <formula>_xlfn.ISFORMULA(H68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="59" priority="81">
+    <cfRule type="expression" dxfId="105" priority="139">
+      <formula>$B69&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="137">
       <formula>$B69=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="82">
+    <cfRule type="expression" dxfId="103" priority="138">
       <formula>$B69=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="83">
-      <formula>$B69&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
-    <cfRule type="expression" dxfId="56" priority="94">
+    <cfRule type="expression" dxfId="102" priority="150">
       <formula>$B68=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="55" priority="91">
+    <cfRule type="expression" dxfId="101" priority="147">
       <formula>$B68=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="92">
+    <cfRule type="expression" dxfId="100" priority="148">
       <formula>$B68=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="93">
+    <cfRule type="expression" dxfId="99" priority="149">
       <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="52" priority="27">
+    <cfRule type="expression" dxfId="98" priority="83">
       <formula>_xlfn.ISFORMULA(I81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:J149">
-    <cfRule type="expression" dxfId="51" priority="112">
-      <formula>$B149=3</formula>
+    <cfRule type="expression" dxfId="97" priority="171">
+      <formula>$B149=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="113">
+    <cfRule type="expression" dxfId="96" priority="170">
+      <formula>$B149&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="169">
       <formula>$B149=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="114">
-      <formula>$B149&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="115">
-      <formula>$B149=0</formula>
+    <cfRule type="expression" dxfId="94" priority="168">
+      <formula>$B149=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I129:K130">
-    <cfRule type="expression" dxfId="47" priority="192">
+    <cfRule type="expression" dxfId="93" priority="248">
       <formula>$B129=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="193">
+    <cfRule type="expression" dxfId="92" priority="249">
       <formula>$B129=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="194">
+    <cfRule type="expression" dxfId="91" priority="250">
       <formula>$B129&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="195">
+    <cfRule type="expression" dxfId="90" priority="251">
       <formula>$B129=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100">
-    <cfRule type="expression" dxfId="43" priority="41">
+    <cfRule type="expression" dxfId="89" priority="487">
+      <formula>#REF!=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="97">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="431">
-      <formula>#REF!=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="432">
+    <cfRule type="expression" dxfId="87" priority="488">
       <formula>#REF!&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="433">
+    <cfRule type="expression" dxfId="86" priority="489">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="434">
+    <cfRule type="expression" dxfId="85" priority="490">
       <formula>#REF!=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
-    <cfRule type="expression" dxfId="38" priority="38">
+    <cfRule type="expression" dxfId="84" priority="94">
       <formula>$B100=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="83" priority="95">
       <formula>$B100=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="40">
+    <cfRule type="expression" dxfId="82" priority="96">
       <formula>$B100&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L81">
-    <cfRule type="expression" dxfId="35" priority="22">
+    <cfRule type="expression" dxfId="81" priority="78">
       <formula>_xlfn.ISFORMULA(L81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L81:T81">
-    <cfRule type="expression" dxfId="34" priority="23">
+    <cfRule type="expression" dxfId="80" priority="79">
       <formula>$B81=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71:O73">
-    <cfRule type="expression" dxfId="33" priority="80">
+    <cfRule type="expression" dxfId="79" priority="136">
       <formula>_xlfn.ISFORMULA(O71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:O112 E83:O83">
-    <cfRule type="expression" dxfId="32" priority="74">
+    <cfRule type="expression" dxfId="78" priority="130">
       <formula>_xlfn.ISFORMULA(E83)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O135">
-    <cfRule type="expression" dxfId="31" priority="249">
+    <cfRule type="expression" dxfId="77" priority="305">
       <formula>$B136=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="250">
-      <formula>$B136=2</formula>
+    <cfRule type="expression" dxfId="76" priority="308">
+      <formula>$B136=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="251">
+    <cfRule type="expression" dxfId="75" priority="307">
       <formula>$B136&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="252">
-      <formula>$B136=0</formula>
+    <cfRule type="expression" dxfId="74" priority="306">
+      <formula>$B136=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71:Q73">
-    <cfRule type="expression" dxfId="27" priority="84">
+    <cfRule type="expression" dxfId="73" priority="140">
       <formula>$B71=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q138">
-    <cfRule type="expression" dxfId="26" priority="176">
+    <cfRule type="expression" dxfId="72" priority="235">
+      <formula>$B138=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="232">
       <formula>$B138=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="177">
+    <cfRule type="expression" dxfId="70" priority="233">
       <formula>$B138=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="178">
+    <cfRule type="expression" dxfId="69" priority="234">
       <formula>$B138&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="179">
-      <formula>$B138=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:Q143">
-    <cfRule type="expression" dxfId="22" priority="172">
+    <cfRule type="expression" dxfId="68" priority="228">
       <formula>$B142=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="173">
+    <cfRule type="expression" dxfId="67" priority="229">
       <formula>$B142=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="174">
+    <cfRule type="expression" dxfId="66" priority="230">
       <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="175">
+    <cfRule type="expression" dxfId="65" priority="231">
       <formula>$B142=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
-    <cfRule type="expression" dxfId="18" priority="73">
+    <cfRule type="expression" dxfId="64" priority="129">
       <formula>$B87=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q136:T137">
-    <cfRule type="expression" dxfId="17" priority="136">
+    <cfRule type="expression" dxfId="63" priority="195">
+      <formula>$B136=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="193">
+      <formula>$B136=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="192">
       <formula>$B136=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="137">
-      <formula>$B136=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="138">
+    <cfRule type="expression" dxfId="60" priority="194">
       <formula>$B136&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="139">
-      <formula>$B136=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S96">
-    <cfRule type="expression" dxfId="13" priority="257">
+    <cfRule type="expression" dxfId="59" priority="313">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="258">
+    <cfRule type="expression" dxfId="58" priority="314">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="259">
+    <cfRule type="expression" dxfId="57" priority="315">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="260">
+    <cfRule type="expression" dxfId="56" priority="316">
       <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F152:F153">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>$B152=0</formula>
+  <conditionalFormatting sqref="U46:U48">
+    <cfRule type="expression" dxfId="55" priority="53">
+      <formula>$B46=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G152:G153">
+  <conditionalFormatting sqref="U46:U48">
+    <cfRule type="expression" dxfId="54" priority="55">
+      <formula>$B46=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="56">
+      <formula>$B46&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U46:U48">
+    <cfRule type="expression" dxfId="52" priority="54">
+      <formula>$B46=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U76:U77">
+    <cfRule type="expression" dxfId="51" priority="52">
+      <formula>$B76=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U76:U77">
+    <cfRule type="expression" dxfId="50" priority="50">
+      <formula>$B76=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="51">
+      <formula>$B76&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U76:U77">
+    <cfRule type="expression" dxfId="48" priority="49">
+      <formula>$B76=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U78:U79">
+    <cfRule type="expression" dxfId="47" priority="48">
+      <formula>$B78=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U78:U79">
+    <cfRule type="expression" dxfId="46" priority="46">
+      <formula>$B78=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="47">
+      <formula>$B78&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U78:U79">
+    <cfRule type="expression" dxfId="44" priority="45">
+      <formula>$B78=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U80">
+    <cfRule type="expression" dxfId="43" priority="44">
+      <formula>$B80=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U80">
+    <cfRule type="expression" dxfId="42" priority="42">
+      <formula>$B80=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="43">
+      <formula>$B80&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U80">
+    <cfRule type="expression" dxfId="40" priority="41">
+      <formula>$B80=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U81">
+    <cfRule type="expression" dxfId="39" priority="40">
+      <formula>$B81=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U81">
+    <cfRule type="expression" dxfId="38" priority="38">
+      <formula>$B81=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="39">
+      <formula>$B81&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U81">
+    <cfRule type="expression" dxfId="36" priority="37">
+      <formula>$B81=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U82">
+    <cfRule type="expression" dxfId="35" priority="36">
+      <formula>$B82=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U82">
+    <cfRule type="expression" dxfId="34" priority="34">
+      <formula>$B82=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="35">
+      <formula>$B82&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U82">
+    <cfRule type="expression" dxfId="32" priority="33">
+      <formula>$B82=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U85:U86">
+    <cfRule type="expression" dxfId="31" priority="32">
+      <formula>$B85=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U85:U86">
+    <cfRule type="expression" dxfId="30" priority="30">
+      <formula>$B85=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="31">
+      <formula>$B85&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U85:U86">
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>$B85=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U87:U88">
+    <cfRule type="expression" dxfId="27" priority="28">
+      <formula>$B87=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U87:U88">
+    <cfRule type="expression" dxfId="26" priority="26">
+      <formula>$B87=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="27">
+      <formula>$B87&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U87:U88">
+    <cfRule type="expression" dxfId="24" priority="25">
+      <formula>$B87=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U90:U91">
+    <cfRule type="expression" dxfId="23" priority="24">
+      <formula>$B90=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U90:U91">
+    <cfRule type="expression" dxfId="22" priority="22">
+      <formula>$B90=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="23">
+      <formula>$B90&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U90:U91">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>$B90=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U92:U93">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>$B92=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U92:U93">
+    <cfRule type="expression" dxfId="18" priority="18">
+      <formula>$B92=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="19">
+      <formula>$B92&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U92:U93">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>$B92=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U96:U97">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>$B96=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U96:U97">
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>$B96=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>$B96&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U96:U97">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>$B96=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U98">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>$B98=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U98">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>$B98=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>$B98&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U98">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>$B98=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U119">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$B119=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U119">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$B119=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>$B119&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U119">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>$B119=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U122:U127">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$B122=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U122:U127">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$B122=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$B122&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U122:U127">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$B152=0</formula>
+      <formula>$B122=3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
@@ -19442,10 +20087,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358A137-1626-9343-A399-452BA3D3C6F7}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19454,15 +20099,24 @@
     <col min="2" max="2" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
         <v>382</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="36" t="s">
+        <v>534</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>535</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>381</v>
       </c>
@@ -19470,7 +20124,7 @@
         <v>6.5389932052543287E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>391</v>
       </c>
@@ -19478,7 +20132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -19486,7 +20140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>393</v>
       </c>
@@ -19494,7 +20148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>394</v>
       </c>
@@ -19502,7 +20156,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>386</v>
       </c>
@@ -19510,7 +20164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>395</v>
       </c>
@@ -19518,72 +20172,120 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B9">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="116" t="s">
+        <v>536</v>
+      </c>
+      <c r="D9" s="116" t="s">
+        <v>537</v>
+      </c>
+      <c r="E9" s="116" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>468</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="116" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="116"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="116"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>469</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C11" s="116"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>472</v>
       </c>
       <c r="B12">
-        <v>0.6</v>
+        <v>0.18443169820109745</v>
       </c>
       <c r="C12" s="116"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>450</v>
       </c>
       <c r="B13">
-        <v>0.4</v>
+        <v>0.24138000000000001</v>
       </c>
       <c r="C13" s="116"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="B14">
-        <v>0.3</v>
+      <c r="B14" s="117">
+        <v>0.22962848022115534</v>
       </c>
       <c r="C14" s="116"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>481</v>
+        <v>539</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>0.41505377678599265</v>
+      </c>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="B16">
+        <v>0.39914905811401724</v>
+      </c>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B17">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="116"/>
+      <c r="D17" t="s">
+        <v>542</v>
+      </c>
+      <c r="E17" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C10:C14"/>
+  <mergeCells count="3">
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="D9:D16"/>
+    <mergeCell ref="E9:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update database to calculate coolant replacement cost (A72)  based on replacement inventory instead (CONOPs)
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user\scratch\mouse_250801\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A3403D-6F35-4C3F-A9C2-6C511A981B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F11792-4A12-420B-AE84-B79878B95A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="546">
   <si>
     <t>Account</t>
   </si>
@@ -2006,6 +2006,9 @@
   </si>
   <si>
     <t>LTMR</t>
+  </si>
+  <si>
+    <t>Replacement Coolant Inventory</t>
   </si>
 </sst>
 </file>
@@ -2643,39 +2646,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2683,6 +2653,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2701,6 +2683,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2738,14 +2741,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2790,6 +2793,13 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2799,13 +2809,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2846,7 +2849,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2859,7 +2862,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2997,6 +3000,12 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
@@ -3016,12 +3025,6 @@
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -3117,26 +3120,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
@@ -3159,6 +3142,19 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3167,6 +3163,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3290,6 +3293,116 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -3302,10 +3415,119 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3342,12 +3564,17 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
       <fill>
-        <patternFill patternType="gray0625"/>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -3360,20 +3587,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3442,121 +3655,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -3569,105 +3667,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4163,8 +4166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
   <dimension ref="A1:AH167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E54"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="13"/>
@@ -4395,10 +4398,10 @@
       <c r="Q3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="92" t="s">
+      <c r="R3" s="94" t="s">
         <v>444</v>
       </c>
-      <c r="S3" s="99" t="s">
+      <c r="S3" s="96" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4485,8 +4488,8 @@
       <c r="Q4" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="92"/>
-      <c r="S4" s="99"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="96"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>467</v>
@@ -4565,10 +4568,10 @@
       <c r="Q5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="92" t="s">
+      <c r="R5" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="99" t="s">
+      <c r="S5" s="96" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4648,8 +4651,8 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="92"/>
-      <c r="S6" s="99"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="96"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>467</v>
@@ -4955,13 +4958,13 @@
       <c r="P11" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="92" t="s">
+      <c r="Q11" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="92" t="s">
+      <c r="R11" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="100" t="s">
+      <c r="S11" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -5052,9 +5055,9 @@
       <c r="P12" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="92"/>
-      <c r="R12" s="92"/>
-      <c r="S12" s="99"/>
+      <c r="Q12" s="94"/>
+      <c r="R12" s="94"/>
+      <c r="S12" s="96"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>470</v>
@@ -5136,9 +5139,9 @@
       <c r="P13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="92"/>
-      <c r="S13" s="99"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="94"/>
+      <c r="S13" s="96"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>470</v>
@@ -5263,13 +5266,13 @@
       <c r="P15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="92" t="s">
+      <c r="Q15" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="92" t="s">
+      <c r="R15" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="100" t="s">
+      <c r="S15" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5353,9 +5356,9 @@
       <c r="P16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="92"/>
-      <c r="R16" s="92"/>
-      <c r="S16" s="99"/>
+      <c r="Q16" s="94"/>
+      <c r="R16" s="94"/>
+      <c r="S16" s="96"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>470</v>
@@ -5437,9 +5440,9 @@
       <c r="P17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="92"/>
-      <c r="R17" s="92"/>
-      <c r="S17" s="99"/>
+      <c r="Q17" s="94"/>
+      <c r="R17" s="94"/>
+      <c r="S17" s="96"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>470</v>
@@ -5803,13 +5806,13 @@
       <c r="P22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="92" t="s">
+      <c r="Q22" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="92" t="s">
+      <c r="R22" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="100" t="s">
+      <c r="S22" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5893,9 +5896,9 @@
       <c r="P23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q23" s="92"/>
-      <c r="R23" s="92"/>
-      <c r="S23" s="99"/>
+      <c r="Q23" s="94"/>
+      <c r="R23" s="94"/>
+      <c r="S23" s="96"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>470</v>
@@ -5977,9 +5980,9 @@
       <c r="P24" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="92"/>
-      <c r="R24" s="92"/>
-      <c r="S24" s="99"/>
+      <c r="Q24" s="94"/>
+      <c r="R24" s="94"/>
+      <c r="S24" s="96"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>470</v>
@@ -6104,13 +6107,13 @@
       <c r="P26" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="92" t="s">
+      <c r="Q26" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R26" s="92" t="s">
+      <c r="R26" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="100" t="s">
+      <c r="S26" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -6194,9 +6197,9 @@
       <c r="P27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" s="92"/>
-      <c r="R27" s="92"/>
-      <c r="S27" s="99"/>
+      <c r="Q27" s="94"/>
+      <c r="R27" s="94"/>
+      <c r="S27" s="96"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>470</v>
@@ -6278,9 +6281,9 @@
       <c r="P28" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="92"/>
-      <c r="R28" s="92"/>
-      <c r="S28" s="99"/>
+      <c r="Q28" s="94"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="96"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>470</v>
@@ -6413,13 +6416,13 @@
       <c r="P30" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="92" t="s">
+      <c r="Q30" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R30" s="92" t="s">
+      <c r="R30" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="100" t="s">
+      <c r="S30" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6507,9 +6510,9 @@
       <c r="P31" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="92"/>
-      <c r="R31" s="92"/>
-      <c r="S31" s="99"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="96"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>470</v>
@@ -6595,9 +6598,9 @@
       <c r="P32" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="92"/>
-      <c r="R32" s="92"/>
-      <c r="S32" s="99"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="96"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>470</v>
@@ -6906,13 +6909,13 @@
       <c r="P37" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q37" s="92" t="s">
+      <c r="Q37" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R37" s="92" t="s">
+      <c r="R37" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="100" t="s">
+      <c r="S37" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -6996,9 +6999,9 @@
       <c r="P38" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="92"/>
-      <c r="R38" s="92"/>
-      <c r="S38" s="99"/>
+      <c r="Q38" s="94"/>
+      <c r="R38" s="94"/>
+      <c r="S38" s="96"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>470</v>
@@ -7080,9 +7083,9 @@
       <c r="P39" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="92"/>
-      <c r="R39" s="92"/>
-      <c r="S39" s="99"/>
+      <c r="Q39" s="94"/>
+      <c r="R39" s="94"/>
+      <c r="S39" s="96"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>470</v>
@@ -7207,13 +7210,13 @@
       <c r="P41" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="92" t="s">
+      <c r="Q41" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="92" t="s">
+      <c r="R41" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="100" t="s">
+      <c r="S41" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7297,9 +7300,9 @@
       <c r="P42" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="92"/>
-      <c r="R42" s="92"/>
-      <c r="S42" s="99"/>
+      <c r="Q42" s="94"/>
+      <c r="R42" s="94"/>
+      <c r="S42" s="96"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>470</v>
@@ -7381,9 +7384,9 @@
       <c r="P43" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q43" s="92"/>
-      <c r="R43" s="92"/>
-      <c r="S43" s="99"/>
+      <c r="Q43" s="94"/>
+      <c r="R43" s="94"/>
+      <c r="S43" s="96"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>470</v>
@@ -7551,13 +7554,13 @@
       <c r="P46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="92" t="s">
+      <c r="Q46" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R46" s="92" t="s">
+      <c r="R46" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="100" t="s">
+      <c r="S46" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
@@ -7641,9 +7644,9 @@
       <c r="P47" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="92"/>
-      <c r="R47" s="92"/>
-      <c r="S47" s="99"/>
+      <c r="Q47" s="94"/>
+      <c r="R47" s="94"/>
+      <c r="S47" s="96"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
         <v>470</v>
@@ -7725,9 +7728,9 @@
       <c r="P48" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q48" s="92"/>
-      <c r="R48" s="92"/>
-      <c r="S48" s="99"/>
+      <c r="Q48" s="94"/>
+      <c r="R48" s="94"/>
+      <c r="S48" s="96"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
         <v>470</v>
@@ -7990,16 +7993,16 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="96" t="s">
+      <c r="Q52" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="R52" s="96" t="s">
+      <c r="R52" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="105" t="s">
+      <c r="S52" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="101" t="s">
+      <c r="T52" s="90" t="s">
         <v>503</v>
       </c>
       <c r="U52" s="80" t="s">
@@ -8082,10 +8085,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="97"/>
-      <c r="R53" s="97"/>
-      <c r="S53" s="106"/>
-      <c r="T53" s="102"/>
+      <c r="Q53" s="105"/>
+      <c r="R53" s="105"/>
+      <c r="S53" s="99"/>
+      <c r="T53" s="91"/>
       <c r="U53" s="80" t="s">
         <v>470</v>
       </c>
@@ -8166,10 +8169,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="98"/>
-      <c r="R54" s="98"/>
-      <c r="S54" s="107"/>
-      <c r="T54" s="103"/>
+      <c r="Q54" s="106"/>
+      <c r="R54" s="106"/>
+      <c r="S54" s="100"/>
+      <c r="T54" s="92"/>
       <c r="U54" s="80" t="s">
         <v>470</v>
       </c>
@@ -8336,13 +8339,13 @@
       <c r="P57" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q57" s="92" t="s">
+      <c r="Q57" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R57" s="92" t="s">
+      <c r="R57" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="100" t="s">
+      <c r="S57" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8426,9 +8429,9 @@
       <c r="P58" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q58" s="92"/>
-      <c r="R58" s="92"/>
-      <c r="S58" s="99"/>
+      <c r="Q58" s="94"/>
+      <c r="R58" s="94"/>
+      <c r="S58" s="96"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>470</v>
@@ -8510,9 +8513,9 @@
       <c r="P59" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q59" s="92"/>
-      <c r="R59" s="92"/>
-      <c r="S59" s="99"/>
+      <c r="Q59" s="94"/>
+      <c r="R59" s="94"/>
+      <c r="S59" s="96"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>470</v>
@@ -8637,13 +8640,13 @@
       <c r="P61" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q61" s="92" t="s">
+      <c r="Q61" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="R61" s="92" t="s">
+      <c r="R61" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="100" t="s">
+      <c r="S61" s="95" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8727,9 +8730,9 @@
       <c r="P62" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q62" s="92"/>
-      <c r="R62" s="92"/>
-      <c r="S62" s="99"/>
+      <c r="Q62" s="94"/>
+      <c r="R62" s="94"/>
+      <c r="S62" s="96"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>470</v>
@@ -8811,9 +8814,9 @@
       <c r="P63" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q63" s="92"/>
-      <c r="R63" s="92"/>
-      <c r="S63" s="99"/>
+      <c r="Q63" s="94"/>
+      <c r="R63" s="94"/>
+      <c r="S63" s="96"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>470</v>
@@ -9127,7 +9130,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="94" t="s">
+      <c r="R68" s="93" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -9216,7 +9219,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="94"/>
+      <c r="R69" s="93"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9310,7 +9313,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="94"/>
+      <c r="R70" s="93"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9404,7 +9407,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="94"/>
+      <c r="R71" s="93"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9493,7 +9496,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="94"/>
+      <c r="R72" s="93"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9587,7 +9590,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="94"/>
+      <c r="R73" s="93"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9757,10 +9760,10 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="94" t="s">
+      <c r="R76" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="104" t="s">
+      <c r="S76" s="97" t="s">
         <v>446</v>
       </c>
       <c r="T76" s="61" t="s">
@@ -9847,8 +9850,8 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="94"/>
-      <c r="S77" s="104"/>
+      <c r="R77" s="93"/>
+      <c r="S77" s="97"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
         <v>449</v>
@@ -9942,8 +9945,8 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="94"/>
-      <c r="S78" s="104"/>
+      <c r="R78" s="93"/>
+      <c r="S78" s="97"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
         <v>466</v>
@@ -10036,8 +10039,8 @@
       <c r="Q79" s="61" t="s">
         <v>435</v>
       </c>
-      <c r="R79" s="94"/>
-      <c r="S79" s="104"/>
+      <c r="R79" s="93"/>
+      <c r="S79" s="97"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
         <v>466</v>
@@ -10131,8 +10134,8 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="94"/>
-      <c r="S80" s="104"/>
+      <c r="R80" s="93"/>
+      <c r="S80" s="97"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
         <v>538</v>
@@ -10556,7 +10559,7 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="104" t="s">
+      <c r="S85" s="97" t="s">
         <v>446</v>
       </c>
       <c r="T85" s="51"/>
@@ -10662,7 +10665,7 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="104"/>
+      <c r="S86" s="97"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
         <v>537</v>
@@ -10758,7 +10761,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="104"/>
+      <c r="S87" s="97"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>466</v>
@@ -10852,7 +10855,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="104"/>
+      <c r="S88" s="97"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>466</v>
@@ -10921,7 +10924,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="104"/>
+      <c r="S89" s="97"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -10993,7 +10996,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="104"/>
+      <c r="S90" s="97"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>466</v>
@@ -11087,7 +11090,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="104"/>
+      <c r="S91" s="97"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>466</v>
@@ -11451,13 +11454,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="94" t="s">
+      <c r="R96" s="93" t="s">
         <v>447</v>
       </c>
-      <c r="S96" s="108" t="s">
+      <c r="S96" s="101" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="94"/>
+      <c r="T96" s="93"/>
       <c r="U96" s="80" t="s">
         <v>466</v>
       </c>
@@ -11544,9 +11547,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="94"/>
-      <c r="S97" s="109"/>
-      <c r="T97" s="94"/>
+      <c r="R97" s="93"/>
+      <c r="S97" s="102"/>
+      <c r="T97" s="93"/>
       <c r="U97" s="80" t="s">
         <v>466</v>
       </c>
@@ -12462,7 +12465,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="90" t="s">
+      <c r="T108" s="107" t="s">
         <v>506</v>
       </c>
       <c r="U108" s="80" t="s">
@@ -12560,7 +12563,7 @@
         <v>360</v>
       </c>
       <c r="S109" s="87"/>
-      <c r="T109" s="91"/>
+      <c r="T109" s="108"/>
       <c r="U109" s="80" t="s">
         <v>466</v>
       </c>
@@ -13561,10 +13564,10 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="95" t="s">
+      <c r="Q123" s="103" t="s">
         <v>426</v>
       </c>
-      <c r="R123" s="95" t="s">
+      <c r="R123" s="103" t="s">
         <v>365</v>
       </c>
       <c r="S123" s="51"/>
@@ -13653,8 +13656,8 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="95"/>
-      <c r="R124" s="95"/>
+      <c r="Q124" s="103"/>
+      <c r="R124" s="103"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
@@ -13741,8 +13744,8 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="95"/>
-      <c r="R125" s="95"/>
+      <c r="Q125" s="103"/>
+      <c r="R125" s="103"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
@@ -13829,8 +13832,8 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="95"/>
-      <c r="R126" s="95"/>
+      <c r="Q126" s="103"/>
+      <c r="R126" s="103"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
@@ -13917,8 +13920,8 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="95"/>
-      <c r="R127" s="95"/>
+      <c r="Q127" s="103"/>
+      <c r="R127" s="103"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
@@ -14005,8 +14008,8 @@
       <c r="P128" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q128" s="95"/>
-      <c r="R128" s="95"/>
+      <c r="Q128" s="103"/>
+      <c r="R128" s="103"/>
       <c r="S128" s="51"/>
       <c r="T128" s="51"/>
       <c r="U128" s="80" t="s">
@@ -14129,10 +14132,10 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="94" t="s">
+      <c r="Q130" s="93" t="s">
         <v>369</v>
       </c>
-      <c r="R130" s="94" t="s">
+      <c r="R130" s="93" t="s">
         <v>370</v>
       </c>
       <c r="S130" s="51"/>
@@ -14214,8 +14217,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="94"/>
-      <c r="R131" s="94"/>
+      <c r="Q131" s="93"/>
+      <c r="R131" s="93"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14297,8 +14300,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="94"/>
-      <c r="R132" s="94"/>
+      <c r="Q132" s="93"/>
+      <c r="R132" s="93"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14382,8 +14385,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="94"/>
-      <c r="R133" s="94"/>
+      <c r="Q133" s="93"/>
+      <c r="R133" s="93"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -14474,8 +14477,8 @@
       <c r="P134" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q134" s="94"/>
-      <c r="R134" s="94"/>
+      <c r="Q134" s="93"/>
+      <c r="R134" s="93"/>
       <c r="S134" s="51"/>
       <c r="T134" s="51"/>
       <c r="U134" s="80" t="s">
@@ -14767,7 +14770,7 @@
       <c r="P139" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q139" s="92" t="s">
+      <c r="Q139" s="94" t="s">
         <v>364</v>
       </c>
       <c r="R139" s="48"/>
@@ -14847,7 +14850,7 @@
       <c r="P140" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q140" s="92"/>
+      <c r="Q140" s="94"/>
       <c r="R140" s="48"/>
       <c r="S140" s="48"/>
       <c r="T140" s="48"/>
@@ -14925,7 +14928,7 @@
       <c r="P141" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q141" s="92"/>
+      <c r="Q141" s="94"/>
       <c r="R141" s="51"/>
       <c r="S141" s="51"/>
       <c r="T141" s="51"/>
@@ -15003,7 +15006,7 @@
       <c r="P142" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q142" s="92"/>
+      <c r="Q142" s="94"/>
       <c r="R142" s="51"/>
       <c r="S142" s="51"/>
       <c r="T142" s="51"/>
@@ -15515,7 +15518,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="151" spans="1:31" ht="78">
+    <row r="151" spans="1:31" ht="91">
       <c r="A151" s="55">
         <v>713</v>
       </c>
@@ -15685,7 +15688,7 @@
         <v>174</v>
       </c>
       <c r="K153" s="61" t="s">
-        <v>496</v>
+        <v>545</v>
       </c>
       <c r="L153" s="51"/>
       <c r="M153" s="51" t="s">
@@ -15922,14 +15925,14 @@
       <c r="N156" s="51"/>
       <c r="O156" s="68"/>
       <c r="P156" s="51"/>
-      <c r="Q156" s="90" t="s">
+      <c r="Q156" s="107" t="s">
         <v>500</v>
       </c>
-      <c r="R156" s="90" t="s">
+      <c r="R156" s="107" t="s">
         <v>500</v>
       </c>
       <c r="S156" s="51"/>
-      <c r="T156" s="90" t="s">
+      <c r="T156" s="107" t="s">
         <v>501</v>
       </c>
       <c r="U156" s="80"/>
@@ -15971,10 +15974,10 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="93"/>
-      <c r="R157" s="93"/>
+      <c r="Q157" s="109"/>
+      <c r="R157" s="109"/>
       <c r="S157" s="51"/>
-      <c r="T157" s="93"/>
+      <c r="T157" s="109"/>
       <c r="U157" s="80"/>
       <c r="V157" s="84"/>
       <c r="W157" s="84"/>
@@ -16014,10 +16017,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="93"/>
-      <c r="R158" s="93"/>
+      <c r="Q158" s="109"/>
+      <c r="R158" s="109"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="93"/>
+      <c r="T158" s="109"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -16057,10 +16060,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="93"/>
-      <c r="R159" s="93"/>
+      <c r="Q159" s="109"/>
+      <c r="R159" s="109"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="93"/>
+      <c r="T159" s="109"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -16100,10 +16103,10 @@
       <c r="N160" s="51"/>
       <c r="O160" s="68"/>
       <c r="P160" s="51"/>
-      <c r="Q160" s="93"/>
-      <c r="R160" s="93"/>
+      <c r="Q160" s="109"/>
+      <c r="R160" s="109"/>
       <c r="S160" s="51"/>
-      <c r="T160" s="93"/>
+      <c r="T160" s="109"/>
       <c r="U160" s="80"/>
       <c r="V160" s="84"/>
       <c r="W160" s="84"/>
@@ -16143,10 +16146,10 @@
       <c r="N161" s="51"/>
       <c r="O161" s="68"/>
       <c r="P161" s="51"/>
-      <c r="Q161" s="93"/>
-      <c r="R161" s="93"/>
+      <c r="Q161" s="109"/>
+      <c r="R161" s="109"/>
       <c r="S161" s="51"/>
-      <c r="T161" s="93"/>
+      <c r="T161" s="109"/>
       <c r="U161" s="80"/>
       <c r="V161" s="84"/>
       <c r="W161" s="84"/>
@@ -16186,10 +16189,10 @@
       <c r="N162" s="51"/>
       <c r="O162" s="68"/>
       <c r="P162" s="51"/>
-      <c r="Q162" s="91"/>
-      <c r="R162" s="91"/>
+      <c r="Q162" s="108"/>
+      <c r="R162" s="108"/>
       <c r="S162" s="51"/>
-      <c r="T162" s="91"/>
+      <c r="T162" s="108"/>
       <c r="U162" s="80"/>
       <c r="V162" s="84"/>
       <c r="W162" s="84"/>
@@ -16297,7 +16300,7 @@
       <c r="AD164" s="83"/>
       <c r="AE164" s="80"/>
     </row>
-    <row r="165" spans="1:31" ht="78">
+    <row r="165" spans="1:31" ht="91">
       <c r="A165" s="39">
         <v>81</v>
       </c>
@@ -16511,39 +16514,11 @@
   </sheetData>
   <autoFilter ref="A1:Z167" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="54">
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="S26:S28"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="T108:T109"/>
+    <mergeCell ref="Q139:Q142"/>
+    <mergeCell ref="Q156:Q162"/>
+    <mergeCell ref="R156:R162"/>
+    <mergeCell ref="T156:T162"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16560,11 +16535,39 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q130:Q134"/>
     <mergeCell ref="Q123:Q128"/>
-    <mergeCell ref="T108:T109"/>
-    <mergeCell ref="Q139:Q142"/>
-    <mergeCell ref="Q156:Q162"/>
-    <mergeCell ref="R156:R162"/>
-    <mergeCell ref="T156:T162"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
   </mergeCells>
   <conditionalFormatting sqref="A156:C162">
     <cfRule type="expression" dxfId="140" priority="4">
@@ -16590,11 +16593,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133:P134">
-    <cfRule type="expression" dxfId="135" priority="250">
+    <cfRule type="expression" dxfId="135" priority="251">
+      <formula>$B133=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="250">
       <formula>$B133&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="251">
-      <formula>$B133=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="133" priority="248">
       <formula>$B133=3</formula>
@@ -16618,75 +16621,73 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156:P162">
-    <cfRule type="expression" dxfId="127" priority="2">
+    <cfRule type="expression" dxfId="127" priority="1">
+      <formula>$B156=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="2">
       <formula>$B156=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="3">
+    <cfRule type="expression" dxfId="125" priority="3">
       <formula>$B156&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="1">
-      <formula>$B156=3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53:D54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A96:T99 A99:AE108 A109:S109 A110:AE119 A114:T129 A121:AE122 A129:AE155 D156:P162 A163:AE167 U53:AE54 U109:AE109 Q156:AE156 S157:S162 U157:AE162 F53:S54">
-    <cfRule type="expression" dxfId="124" priority="267">
-      <formula>$B53=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="123" priority="307">
+    <cfRule type="expression" dxfId="124" priority="304">
+      <formula>$B95=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="306">
+      <formula>$B95&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="307">
       <formula>$B95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="305">
+    <cfRule type="expression" dxfId="121" priority="305">
       <formula>$B95=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="304">
-      <formula>$B95=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="306">
-      <formula>$B95&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
-    <cfRule type="expression" dxfId="119" priority="87">
+    <cfRule type="expression" dxfId="120" priority="87">
       <formula>$B74=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="88">
+    <cfRule type="expression" dxfId="119" priority="88">
       <formula>$B74=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="89">
+    <cfRule type="expression" dxfId="118" priority="89">
       <formula>$B74&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
-    <cfRule type="expression" dxfId="116" priority="146">
+    <cfRule type="expression" dxfId="117" priority="146">
       <formula>$B83=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:T99 S101:T107 S108:S109 A112:Q113 S112:T113 A129:T129 L130:T130 L131:P131 S131:T135 I132:P132 A135:R135 R139:T144 A145:T148 A149:H150 A151:J154 S153:T154 A123:B128 S123:T128 A96:F98">
-    <cfRule type="expression" dxfId="115" priority="300">
+    <cfRule type="expression" dxfId="116" priority="300">
       <formula>$B96=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:T111 A114:T128">
+    <cfRule type="expression" dxfId="115" priority="136">
+      <formula>$B110&lt;2</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="114" priority="135">
       <formula>$B110=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="136">
-      <formula>$B110&lt;2</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:T111">
-    <cfRule type="expression" dxfId="112" priority="271">
+    <cfRule type="expression" dxfId="113" priority="271">
       <formula>$B110=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114:T128 A110:T111">
-    <cfRule type="expression" dxfId="111" priority="134">
+    <cfRule type="expression" dxfId="112" priority="134">
       <formula>$B110=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:T136">
+    <cfRule type="expression" dxfId="111" priority="234">
+      <formula>$B136&lt;2</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="110" priority="235">
       <formula>$B136=0</formula>
     </cfRule>
@@ -16696,65 +16697,65 @@
     <cfRule type="expression" dxfId="108" priority="233">
       <formula>$B136=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="234">
-      <formula>$B136&lt;2</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A164:T167">
-    <cfRule type="expression" dxfId="106" priority="166">
-      <formula>$B164&lt;2</formula>
+    <cfRule type="expression" dxfId="107" priority="167">
+      <formula>$B164=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="164">
+      <formula>$B164=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="105" priority="165">
       <formula>$B164=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="167">
-      <formula>$B164=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="164">
-      <formula>$B164=3</formula>
+    <cfRule type="expression" dxfId="104" priority="166">
+      <formula>$B164&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE45 A49:AE51 U53:AE54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A99:AE108 A109:S109 U109:AE109 A110:AE119 A120:T120 A121:AE122 A129:AE155 Q156:AE156 S157:S162 U157:AE162 A163:AE167 F53:S54 F52:AE52 A52:E54">
+  <conditionalFormatting sqref="A1:AE45 A49:AE51 F52:AE52 A52:E54 F53:S54 U53:AE54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A99:AE108 A109:S109 U109:AE109 A110:AE119 A120:T120 A121:AE122 A129:AE155 Q156:AE156 S157:S162 U157:AE162 A163:AE167">
+    <cfRule type="expression" dxfId="103" priority="265">
+      <formula>$B1=2</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="102" priority="266">
       <formula>$B1&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="265">
-      <formula>$B1=2</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AE51 A52:D52 F52:AE52 E52:E54">
-    <cfRule type="expression" dxfId="100" priority="65">
+  <conditionalFormatting sqref="A1:AE51 F52:AE52 A52:E54">
+    <cfRule type="expression" dxfId="101" priority="65">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:AE48">
-    <cfRule type="expression" dxfId="99" priority="66">
+    <cfRule type="expression" dxfId="100" priority="66">
       <formula>$B46=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="67">
+    <cfRule type="expression" dxfId="99" priority="67">
       <formula>$B46=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="68">
+    <cfRule type="expression" dxfId="98" priority="68">
       <formula>$B46&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:AE98">
+    <cfRule type="expression" dxfId="97" priority="22">
+      <formula>$B96=2</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="96" priority="21">
       <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="22">
-      <formula>$B96=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="23">
+    <cfRule type="expression" dxfId="95" priority="23">
       <formula>$B96&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:AE155 A163:AE167 A55:AE75 A83:AE84 A110:AE119 A120:T120 A121:AE122 A99:AE108 A1:AE45 A76:T82 A85:T88 A89:AE89 A90:T93 A94:AE95 A49:AE51 U53:AE54 A109:S109 U109:AE109 Q156:AE156 S157:S162 U157:AE162 F53:S54 F52:AE52 A52:E54">
-    <cfRule type="expression" dxfId="93" priority="264">
+  <conditionalFormatting sqref="A129:AE155 A163:AE167 A55:AE75 A83:AE84 A110:AE119 A120:T120 A121:AE122 A99:AE108 A1:AE45 A76:T82 A85:T88 A89:AE89 A90:T93 A94:AE95 A49:AE51 F52:AE52 F53:S54 A52:E54 U53:AE54 A109:S109 U109:AE109 Q156:AE156 S157:S162 U157:AE162">
+    <cfRule type="expression" dxfId="94" priority="264">
       <formula>$B1=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C123:R123 C124:P128">
+    <cfRule type="expression" dxfId="93" priority="126">
+      <formula>$B123=0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="92" priority="123">
       <formula>$B123=3</formula>
     </cfRule>
@@ -16763,9 +16764,6 @@
     </cfRule>
     <cfRule type="expression" dxfId="90" priority="125">
       <formula>$B123&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="126">
-      <formula>$B123=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D80 D82 D129:D167 D84:D122">
@@ -16809,36 +16807,41 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E123:O128">
-    <cfRule type="expression" dxfId="88" priority="122">
+    <cfRule type="expression" dxfId="89" priority="122">
       <formula>_xlfn.ISFORMULA(E123)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:G54">
-    <cfRule type="expression" dxfId="87" priority="72">
+    <cfRule type="expression" dxfId="88" priority="73">
+      <formula>$B51&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="74">
+      <formula>$B51=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="71">
+      <formula>$B51=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="72">
       <formula>$B51=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="73">
-      <formula>$B51&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="74">
-      <formula>$B51=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="71">
-      <formula>$B51=3</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F53:S54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A96:T99 A99:AE108 A109:S109 A110:AE119 A114:T129 A121:AE122 A129:AE155 D156:P162 A163:AE167 U53:AE54 U109:AE109 Q156:AE156 S157:S162 U157:AE162">
+    <cfRule type="expression" dxfId="84" priority="267">
+      <formula>$B53=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="83" priority="298">
+    <cfRule type="expression" dxfId="83" priority="296">
+      <formula>$B96=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="298">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="299">
+    <cfRule type="expression" dxfId="81" priority="299">
       <formula>$B96=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="297">
+    <cfRule type="expression" dxfId="80" priority="297">
       <formula>$B96=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="296">
-      <formula>$B96=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -16906,31 +16909,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I149:J150">
-    <cfRule type="expression" dxfId="63" priority="181">
+    <cfRule type="expression" dxfId="63" priority="180">
+      <formula>$B150=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="181">
       <formula>$B150=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="182">
+    <cfRule type="expression" dxfId="61" priority="182">
       <formula>$B150&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="180">
-      <formula>$B150=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="60" priority="183">
       <formula>$B150=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I130:K131">
-    <cfRule type="expression" dxfId="59" priority="262">
-      <formula>$B130&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="261">
+    <cfRule type="expression" dxfId="59" priority="261">
       <formula>$B130=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="260">
+    <cfRule type="expression" dxfId="58" priority="260">
       <formula>$B130=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="263">
+    <cfRule type="expression" dxfId="57" priority="263">
       <formula>$B130=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="262">
+      <formula>$B130&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100">
@@ -16987,17 +16990,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O136">
-    <cfRule type="expression" dxfId="42" priority="320">
-      <formula>$B137=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="319">
+    <cfRule type="expression" dxfId="42" priority="319">
       <formula>$B137&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="317">
+    <cfRule type="expression" dxfId="41" priority="317">
       <formula>$B137=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="318">
+    <cfRule type="expression" dxfId="40" priority="318">
       <formula>$B137=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="320">
+      <formula>$B137=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71:Q73">
@@ -17075,14 +17078,14 @@
     <cfRule type="expression" dxfId="19" priority="45">
       <formula>$B76=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="46">
-      <formula>$B76=2</formula>
+    <cfRule type="expression" dxfId="18" priority="47">
+      <formula>$B76&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="17" priority="48">
       <formula>$B76=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="47">
-      <formula>$B76&lt;2</formula>
+    <cfRule type="expression" dxfId="16" priority="46">
+      <formula>$B76=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U85:AE88">
@@ -17103,14 +17106,14 @@
     <cfRule type="expression" dxfId="11" priority="30">
       <formula>$B90=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="29">
-      <formula>$B90=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="31">
+    <cfRule type="expression" dxfId="10" priority="31">
       <formula>$B90&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="32">
+    <cfRule type="expression" dxfId="9" priority="32">
       <formula>$B90=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="29">
+      <formula>$B90=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U96:AE98">
@@ -17136,11 +17139,11 @@
     <cfRule type="expression" dxfId="2" priority="15">
       <formula>$B123&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="14">
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>$B123=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>$B123=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="13">
-      <formula>$B123=3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">

</xml_diff>

<commit_message>
change the packing factor to be packing fraction + add missing uncertainties + fix the parametric study of the packing fraction
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannbn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D6E3F9-1AB3-0C4A-9E68-05A013C1FC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C2C0AC-4575-0644-B793-319ACBFB52E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="19400" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-760" yWindow="1400" windowWidth="30240" windowHeight="17180" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="2" r:id="rId1"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="552">
   <si>
     <t>Account</t>
   </si>
@@ -2675,39 +2675,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2715,6 +2682,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2733,6 +2712,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2766,7 +2766,358 @@
     <cellStyle name="Normal 2" xfId="4" xr:uid="{E15291B7-9068-3147-AE9D-D55638463741}"/>
     <cellStyle name="Normal 2 5" xfId="3" xr:uid="{D5427F60-54E8-014E-9224-5454BAE094F2}"/>
   </cellStyles>
-  <dxfs count="149">
+  <dxfs count="201">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4249,10 +4600,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}">
   <dimension ref="A1:AH168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="165" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="165" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="O156" sqref="O156"/>
+      <selection pane="bottomLeft" activeCell="AE128" sqref="AE128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -4483,10 +4834,10 @@
       <c r="Q3" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="93" t="s">
+      <c r="R3" s="95" t="s">
         <v>444</v>
       </c>
-      <c r="S3" s="100" t="s">
+      <c r="S3" s="97" t="s">
         <v>56</v>
       </c>
       <c r="T3" s="51"/>
@@ -4573,8 +4924,8 @@
       <c r="Q4" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="93"/>
-      <c r="S4" s="100"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="97"/>
       <c r="T4" s="51"/>
       <c r="U4" s="80" t="s">
         <v>467</v>
@@ -4656,7 +5007,7 @@
       <c r="R5" s="90" t="s">
         <v>547</v>
       </c>
-      <c r="S5" s="100" t="s">
+      <c r="S5" s="97" t="s">
         <v>59</v>
       </c>
       <c r="T5" s="51"/>
@@ -4739,7 +5090,7 @@
       <c r="R6" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="S6" s="100"/>
+      <c r="S6" s="97"/>
       <c r="T6" s="51"/>
       <c r="U6" s="80" t="s">
         <v>467</v>
@@ -5045,13 +5396,13 @@
       <c r="P11" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q11" s="93" t="s">
+      <c r="Q11" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="93" t="s">
+      <c r="R11" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="101" t="s">
+      <c r="S11" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T11" s="51"/>
@@ -5142,9 +5493,9 @@
       <c r="P12" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="93"/>
-      <c r="S12" s="100"/>
+      <c r="Q12" s="95"/>
+      <c r="R12" s="95"/>
+      <c r="S12" s="97"/>
       <c r="T12" s="51"/>
       <c r="U12" s="80" t="s">
         <v>470</v>
@@ -5226,9 +5577,9 @@
       <c r="P13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="100"/>
+      <c r="Q13" s="95"/>
+      <c r="R13" s="95"/>
+      <c r="S13" s="97"/>
       <c r="T13" s="51"/>
       <c r="U13" s="80" t="s">
         <v>470</v>
@@ -5353,13 +5704,13 @@
       <c r="P15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="93" t="s">
+      <c r="Q15" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="93" t="s">
+      <c r="R15" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="101" t="s">
+      <c r="S15" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="51"/>
@@ -5443,9 +5794,9 @@
       <c r="P16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="100"/>
+      <c r="Q16" s="95"/>
+      <c r="R16" s="95"/>
+      <c r="S16" s="97"/>
       <c r="T16" s="51"/>
       <c r="U16" s="80" t="s">
         <v>470</v>
@@ -5527,9 +5878,9 @@
       <c r="P17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="93"/>
-      <c r="R17" s="93"/>
-      <c r="S17" s="100"/>
+      <c r="Q17" s="95"/>
+      <c r="R17" s="95"/>
+      <c r="S17" s="97"/>
       <c r="T17" s="51"/>
       <c r="U17" s="80" t="s">
         <v>470</v>
@@ -5893,13 +6244,13 @@
       <c r="P22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q22" s="93" t="s">
+      <c r="Q22" s="95" t="s">
         <v>551</v>
       </c>
-      <c r="R22" s="93" t="s">
+      <c r="R22" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S22" s="101" t="s">
+      <c r="S22" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="51"/>
@@ -5983,9 +6334,9 @@
       <c r="P23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="100"/>
+      <c r="Q23" s="95"/>
+      <c r="R23" s="95"/>
+      <c r="S23" s="97"/>
       <c r="T23" s="51"/>
       <c r="U23" s="80" t="s">
         <v>470</v>
@@ -6067,9 +6418,9 @@
       <c r="P24" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="100"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="95"/>
+      <c r="S24" s="97"/>
       <c r="T24" s="51"/>
       <c r="U24" s="80" t="s">
         <v>470</v>
@@ -6194,13 +6545,13 @@
       <c r="P26" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="93" t="s">
+      <c r="Q26" s="95" t="s">
         <v>551</v>
       </c>
-      <c r="R26" s="93" t="s">
+      <c r="R26" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S26" s="101" t="s">
+      <c r="S26" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T26" s="51"/>
@@ -6284,9 +6635,9 @@
       <c r="P27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="93"/>
-      <c r="S27" s="100"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="95"/>
+      <c r="S27" s="97"/>
       <c r="T27" s="51"/>
       <c r="U27" s="80" t="s">
         <v>470</v>
@@ -6368,9 +6719,9 @@
       <c r="P28" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="93"/>
-      <c r="S28" s="100"/>
+      <c r="Q28" s="95"/>
+      <c r="R28" s="95"/>
+      <c r="S28" s="97"/>
       <c r="T28" s="51"/>
       <c r="U28" s="80" t="s">
         <v>470</v>
@@ -6503,13 +6854,13 @@
       <c r="P30" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q30" s="93" t="s">
+      <c r="Q30" s="95" t="s">
         <v>551</v>
       </c>
-      <c r="R30" s="93" t="s">
+      <c r="R30" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S30" s="101" t="s">
+      <c r="S30" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T30" s="51"/>
@@ -6597,9 +6948,9 @@
       <c r="P31" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="100"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="95"/>
+      <c r="S31" s="97"/>
       <c r="T31" s="51"/>
       <c r="U31" s="80" t="s">
         <v>470</v>
@@ -6685,9 +7036,9 @@
       <c r="P32" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="93"/>
-      <c r="S32" s="100"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="95"/>
+      <c r="S32" s="97"/>
       <c r="T32" s="51"/>
       <c r="U32" s="80" t="s">
         <v>470</v>
@@ -6996,13 +7347,13 @@
       <c r="P37" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q37" s="93" t="s">
+      <c r="Q37" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="R37" s="93" t="s">
+      <c r="R37" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="101" t="s">
+      <c r="S37" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T37" s="51"/>
@@ -7086,9 +7437,9 @@
       <c r="P38" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="93"/>
-      <c r="R38" s="93"/>
-      <c r="S38" s="100"/>
+      <c r="Q38" s="95"/>
+      <c r="R38" s="95"/>
+      <c r="S38" s="97"/>
       <c r="T38" s="51"/>
       <c r="U38" s="80" t="s">
         <v>470</v>
@@ -7170,9 +7521,9 @@
       <c r="P39" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q39" s="93"/>
-      <c r="R39" s="93"/>
-      <c r="S39" s="100"/>
+      <c r="Q39" s="95"/>
+      <c r="R39" s="95"/>
+      <c r="S39" s="97"/>
       <c r="T39" s="51"/>
       <c r="U39" s="80" t="s">
         <v>470</v>
@@ -7297,13 +7648,13 @@
       <c r="P41" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="93" t="s">
+      <c r="Q41" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="93" t="s">
+      <c r="R41" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S41" s="101" t="s">
+      <c r="S41" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T41" s="51"/>
@@ -7387,9 +7738,9 @@
       <c r="P42" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="93"/>
-      <c r="R42" s="93"/>
-      <c r="S42" s="100"/>
+      <c r="Q42" s="95"/>
+      <c r="R42" s="95"/>
+      <c r="S42" s="97"/>
       <c r="T42" s="51"/>
       <c r="U42" s="80" t="s">
         <v>470</v>
@@ -7471,9 +7822,9 @@
       <c r="P43" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q43" s="93"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="100"/>
+      <c r="Q43" s="95"/>
+      <c r="R43" s="95"/>
+      <c r="S43" s="97"/>
       <c r="T43" s="51"/>
       <c r="U43" s="80" t="s">
         <v>470</v>
@@ -7641,13 +7992,13 @@
       <c r="P46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="93" t="s">
+      <c r="Q46" s="95" t="s">
         <v>551</v>
       </c>
-      <c r="R46" s="93" t="s">
+      <c r="R46" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S46" s="101" t="s">
+      <c r="S46" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T46" s="51"/>
@@ -7731,9 +8082,9 @@
       <c r="P47" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="93"/>
-      <c r="R47" s="93"/>
-      <c r="S47" s="100"/>
+      <c r="Q47" s="95"/>
+      <c r="R47" s="95"/>
+      <c r="S47" s="97"/>
       <c r="T47" s="51"/>
       <c r="U47" s="80" t="s">
         <v>470</v>
@@ -7815,9 +8166,9 @@
       <c r="P48" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q48" s="93"/>
-      <c r="R48" s="93"/>
-      <c r="S48" s="100"/>
+      <c r="Q48" s="95"/>
+      <c r="R48" s="95"/>
+      <c r="S48" s="97"/>
       <c r="T48" s="51"/>
       <c r="U48" s="80" t="s">
         <v>470</v>
@@ -8080,16 +8431,16 @@
       <c r="P52" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q52" s="97" t="s">
+      <c r="Q52" s="105" t="s">
         <v>551</v>
       </c>
-      <c r="R52" s="97" t="s">
+      <c r="R52" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="106" t="s">
+      <c r="S52" s="99" t="s">
         <v>84</v>
       </c>
-      <c r="T52" s="102" t="s">
+      <c r="T52" s="91" t="s">
         <v>503</v>
       </c>
       <c r="U52" s="80" t="s">
@@ -8172,10 +8523,10 @@
       <c r="P53" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="98"/>
-      <c r="R53" s="98"/>
-      <c r="S53" s="107"/>
-      <c r="T53" s="103"/>
+      <c r="Q53" s="106"/>
+      <c r="R53" s="106"/>
+      <c r="S53" s="100"/>
+      <c r="T53" s="92"/>
       <c r="U53" s="80" t="s">
         <v>470</v>
       </c>
@@ -8256,10 +8607,10 @@
       <c r="P54" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q54" s="99"/>
-      <c r="R54" s="99"/>
-      <c r="S54" s="108"/>
-      <c r="T54" s="104"/>
+      <c r="Q54" s="107"/>
+      <c r="R54" s="107"/>
+      <c r="S54" s="101"/>
+      <c r="T54" s="93"/>
       <c r="U54" s="80" t="s">
         <v>470</v>
       </c>
@@ -8426,13 +8777,13 @@
       <c r="P57" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q57" s="93" t="s">
+      <c r="Q57" s="95" t="s">
         <v>551</v>
       </c>
-      <c r="R57" s="93" t="s">
+      <c r="R57" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S57" s="101" t="s">
+      <c r="S57" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T57" s="51"/>
@@ -8516,9 +8867,9 @@
       <c r="P58" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q58" s="93"/>
-      <c r="R58" s="93"/>
-      <c r="S58" s="100"/>
+      <c r="Q58" s="95"/>
+      <c r="R58" s="95"/>
+      <c r="S58" s="97"/>
       <c r="T58" s="51"/>
       <c r="U58" s="80" t="s">
         <v>470</v>
@@ -8600,9 +8951,9 @@
       <c r="P59" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q59" s="93"/>
-      <c r="R59" s="93"/>
-      <c r="S59" s="100"/>
+      <c r="Q59" s="95"/>
+      <c r="R59" s="95"/>
+      <c r="S59" s="97"/>
       <c r="T59" s="51"/>
       <c r="U59" s="80" t="s">
         <v>470</v>
@@ -8727,13 +9078,13 @@
       <c r="P61" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q61" s="93" t="s">
+      <c r="Q61" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="R61" s="93" t="s">
+      <c r="R61" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="S61" s="101" t="s">
+      <c r="S61" s="96" t="s">
         <v>84</v>
       </c>
       <c r="T61" s="51"/>
@@ -8817,9 +9168,9 @@
       <c r="P62" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q62" s="93"/>
-      <c r="R62" s="93"/>
-      <c r="S62" s="100"/>
+      <c r="Q62" s="95"/>
+      <c r="R62" s="95"/>
+      <c r="S62" s="97"/>
       <c r="T62" s="51"/>
       <c r="U62" s="80" t="s">
         <v>470</v>
@@ -8901,9 +9252,9 @@
       <c r="P63" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="Q63" s="93"/>
-      <c r="R63" s="93"/>
-      <c r="S63" s="100"/>
+      <c r="Q63" s="95"/>
+      <c r="R63" s="95"/>
+      <c r="S63" s="97"/>
       <c r="T63" s="51"/>
       <c r="U63" s="80" t="s">
         <v>470</v>
@@ -9217,7 +9568,7 @@
       <c r="Q68" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R68" s="95" t="s">
+      <c r="R68" s="94" t="s">
         <v>350</v>
       </c>
       <c r="S68" s="58"/>
@@ -9306,7 +9657,7 @@
       <c r="Q69" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R69" s="95"/>
+      <c r="R69" s="94"/>
       <c r="S69" s="58"/>
       <c r="T69" s="51"/>
       <c r="U69" s="80" t="s">
@@ -9400,7 +9751,7 @@
       <c r="Q70" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R70" s="95"/>
+      <c r="R70" s="94"/>
       <c r="S70" s="58"/>
       <c r="T70" s="51"/>
       <c r="U70" s="80" t="s">
@@ -9494,7 +9845,7 @@
       <c r="Q71" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R71" s="95"/>
+      <c r="R71" s="94"/>
       <c r="S71" s="58"/>
       <c r="T71" s="61" t="s">
         <v>179</v>
@@ -9583,7 +9934,7 @@
       <c r="Q72" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R72" s="95"/>
+      <c r="R72" s="94"/>
       <c r="S72" s="58"/>
       <c r="T72" s="61"/>
       <c r="U72" s="80" t="s">
@@ -9677,7 +10028,7 @@
       <c r="Q73" s="61" t="s">
         <v>399</v>
       </c>
-      <c r="R73" s="95"/>
+      <c r="R73" s="94"/>
       <c r="S73" s="58"/>
       <c r="T73" s="61"/>
       <c r="U73" s="80" t="s">
@@ -9847,10 +10198,10 @@
       <c r="Q76" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R76" s="95" t="s">
+      <c r="R76" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="S76" s="105" t="s">
+      <c r="S76" s="98" t="s">
         <v>446</v>
       </c>
       <c r="T76" s="61" t="s">
@@ -9937,8 +10288,8 @@
       <c r="Q77" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R77" s="95"/>
-      <c r="S77" s="105"/>
+      <c r="R77" s="94"/>
+      <c r="S77" s="98"/>
       <c r="T77" s="51"/>
       <c r="U77" s="80" t="s">
         <v>449</v>
@@ -10032,8 +10383,8 @@
       <c r="Q78" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R78" s="95"/>
-      <c r="S78" s="105"/>
+      <c r="R78" s="94"/>
+      <c r="S78" s="98"/>
       <c r="T78" s="51"/>
       <c r="U78" s="80" t="s">
         <v>466</v>
@@ -10126,8 +10477,8 @@
       <c r="Q79" s="61" t="s">
         <v>435</v>
       </c>
-      <c r="R79" s="95"/>
-      <c r="S79" s="105"/>
+      <c r="R79" s="94"/>
+      <c r="S79" s="98"/>
       <c r="T79" s="51"/>
       <c r="U79" s="80" t="s">
         <v>466</v>
@@ -10221,8 +10572,8 @@
       <c r="Q80" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="R80" s="95"/>
-      <c r="S80" s="105"/>
+      <c r="R80" s="94"/>
+      <c r="S80" s="98"/>
       <c r="T80" s="51"/>
       <c r="U80" s="80" t="s">
         <v>538</v>
@@ -10646,7 +10997,7 @@
       <c r="R85" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S85" s="105" t="s">
+      <c r="S85" s="98" t="s">
         <v>446</v>
       </c>
       <c r="T85" s="51"/>
@@ -10752,7 +11103,7 @@
       <c r="R86" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="S86" s="105"/>
+      <c r="S86" s="98"/>
       <c r="T86" s="51"/>
       <c r="U86" s="80" t="s">
         <v>537</v>
@@ -10848,7 +11199,7 @@
       <c r="R87" s="61" t="s">
         <v>405</v>
       </c>
-      <c r="S87" s="105"/>
+      <c r="S87" s="98"/>
       <c r="T87" s="51"/>
       <c r="U87" s="80" t="s">
         <v>466</v>
@@ -10942,7 +11293,7 @@
         <v>408</v>
       </c>
       <c r="R88" s="61"/>
-      <c r="S88" s="105"/>
+      <c r="S88" s="98"/>
       <c r="T88" s="51"/>
       <c r="U88" s="80" t="s">
         <v>466</v>
@@ -11011,7 +11362,7 @@
       <c r="P89" s="51"/>
       <c r="Q89" s="61"/>
       <c r="R89" s="61"/>
-      <c r="S89" s="105"/>
+      <c r="S89" s="98"/>
       <c r="T89" s="51"/>
       <c r="U89" s="80"/>
       <c r="V89" s="84"/>
@@ -11083,7 +11434,7 @@
         <v>175</v>
       </c>
       <c r="R90" s="61"/>
-      <c r="S90" s="105"/>
+      <c r="S90" s="98"/>
       <c r="T90" s="51"/>
       <c r="U90" s="80" t="s">
         <v>466</v>
@@ -11177,7 +11528,7 @@
         <v>175</v>
       </c>
       <c r="R91" s="61"/>
-      <c r="S91" s="105"/>
+      <c r="S91" s="98"/>
       <c r="T91" s="51"/>
       <c r="U91" s="80" t="s">
         <v>466</v>
@@ -11541,13 +11892,13 @@
       <c r="Q96" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="R96" s="95" t="s">
+      <c r="R96" s="94" t="s">
         <v>447</v>
       </c>
-      <c r="S96" s="109" t="s">
+      <c r="S96" s="102" t="s">
         <v>344</v>
       </c>
-      <c r="T96" s="95"/>
+      <c r="T96" s="94"/>
       <c r="U96" s="80" t="s">
         <v>466</v>
       </c>
@@ -11634,9 +11985,9 @@
       <c r="Q97" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R97" s="95"/>
-      <c r="S97" s="110"/>
-      <c r="T97" s="95"/>
+      <c r="R97" s="94"/>
+      <c r="S97" s="103"/>
+      <c r="T97" s="94"/>
       <c r="U97" s="80" t="s">
         <v>466</v>
       </c>
@@ -12552,7 +12903,7 @@
         <v>360</v>
       </c>
       <c r="S108" s="87"/>
-      <c r="T108" s="91" t="s">
+      <c r="T108" s="108" t="s">
         <v>506</v>
       </c>
       <c r="U108" s="80" t="s">
@@ -12650,7 +13001,7 @@
         <v>360</v>
       </c>
       <c r="S109" s="87"/>
-      <c r="T109" s="92"/>
+      <c r="T109" s="109"/>
       <c r="U109" s="80" t="s">
         <v>466</v>
       </c>
@@ -13536,16 +13887,10 @@
         <v>1500000</v>
       </c>
       <c r="X121" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="Y121" s="83">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="Z121" s="83">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="Y121" s="83"/>
+      <c r="Z121" s="83"/>
       <c r="AA121" s="80" t="s">
         <v>469</v>
       </c>
@@ -13651,10 +13996,10 @@
       <c r="P123" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q123" s="96" t="s">
+      <c r="Q123" s="104" t="s">
         <v>426</v>
       </c>
-      <c r="R123" s="96" t="s">
+      <c r="R123" s="104" t="s">
         <v>365</v>
       </c>
       <c r="S123" s="51"/>
@@ -13682,19 +14027,19 @@
         <v>16391.712734282046</v>
       </c>
       <c r="AA123" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB123" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC123" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD123" s="83" t="s">
-        <v>469</v>
+        <v>450</v>
+      </c>
+      <c r="AB123" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="AC123" s="83">
+        <v>1</v>
+      </c>
+      <c r="AD123" s="83">
+        <v>0</v>
       </c>
       <c r="AE123" s="80" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="124" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -13743,8 +14088,8 @@
       <c r="P124" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q124" s="96"/>
-      <c r="R124" s="96"/>
+      <c r="Q124" s="104"/>
+      <c r="R124" s="104"/>
       <c r="S124" s="51"/>
       <c r="T124" s="51"/>
       <c r="U124" s="80" t="s">
@@ -13770,19 +14115,19 @@
         <v>13628.001565392728</v>
       </c>
       <c r="AA124" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB124" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC124" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD124" s="83" t="s">
-        <v>469</v>
+        <v>450</v>
+      </c>
+      <c r="AB124" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="AC124" s="83">
+        <v>1</v>
+      </c>
+      <c r="AD124" s="83">
+        <v>0</v>
       </c>
       <c r="AE124" s="80" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="125" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -13831,8 +14176,8 @@
       <c r="P125" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q125" s="96"/>
-      <c r="R125" s="96"/>
+      <c r="Q125" s="104"/>
+      <c r="R125" s="104"/>
       <c r="S125" s="51"/>
       <c r="T125" s="51"/>
       <c r="U125" s="80" t="s">
@@ -13858,19 +14203,19 @@
         <v>4425.2799704641247</v>
       </c>
       <c r="AA125" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB125" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC125" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD125" s="83" t="s">
-        <v>469</v>
+        <v>450</v>
+      </c>
+      <c r="AB125" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="AC125" s="83">
+        <v>1</v>
+      </c>
+      <c r="AD125" s="83">
+        <v>0</v>
       </c>
       <c r="AE125" s="80" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="126" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -13919,8 +14264,8 @@
       <c r="P126" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q126" s="96"/>
-      <c r="R126" s="96"/>
+      <c r="Q126" s="104"/>
+      <c r="R126" s="104"/>
       <c r="S126" s="51"/>
       <c r="T126" s="51"/>
       <c r="U126" s="80" t="s">
@@ -13946,19 +14291,19 @@
         <v>12708.990824658749</v>
       </c>
       <c r="AA126" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB126" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC126" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD126" s="83" t="s">
-        <v>469</v>
+        <v>450</v>
+      </c>
+      <c r="AB126" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="AC126" s="83">
+        <v>1</v>
+      </c>
+      <c r="AD126" s="83">
+        <v>0</v>
       </c>
       <c r="AE126" s="80" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="127" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -14007,8 +14352,8 @@
       <c r="P127" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q127" s="96"/>
-      <c r="R127" s="96"/>
+      <c r="Q127" s="104"/>
+      <c r="R127" s="104"/>
       <c r="S127" s="51"/>
       <c r="T127" s="51"/>
       <c r="U127" s="80" t="s">
@@ -14034,19 +14379,19 @@
         <v>68536.913265290917</v>
       </c>
       <c r="AA127" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB127" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC127" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD127" s="83" t="s">
-        <v>469</v>
+        <v>450</v>
+      </c>
+      <c r="AB127" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="AC127" s="83">
+        <v>1</v>
+      </c>
+      <c r="AD127" s="83">
+        <v>0</v>
       </c>
       <c r="AE127" s="80" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="128" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -14095,8 +14440,8 @@
       <c r="P128" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q128" s="96"/>
-      <c r="R128" s="96"/>
+      <c r="Q128" s="104"/>
+      <c r="R128" s="104"/>
       <c r="S128" s="51"/>
       <c r="T128" s="51"/>
       <c r="U128" s="80" t="s">
@@ -14122,19 +14467,19 @@
         <v>51833.042585647956</v>
       </c>
       <c r="AA128" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB128" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC128" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD128" s="83" t="s">
-        <v>469</v>
+        <v>450</v>
+      </c>
+      <c r="AB128" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="AC128" s="83">
+        <v>1</v>
+      </c>
+      <c r="AD128" s="83">
+        <v>0</v>
       </c>
       <c r="AE128" s="80" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="129" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -14219,10 +14564,10 @@
       <c r="P130" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q130" s="95" t="s">
+      <c r="Q130" s="94" t="s">
         <v>369</v>
       </c>
-      <c r="R130" s="95" t="s">
+      <c r="R130" s="94" t="s">
         <v>370</v>
       </c>
       <c r="S130" s="51"/>
@@ -14304,8 +14649,8 @@
       <c r="P131" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q131" s="95"/>
-      <c r="R131" s="95"/>
+      <c r="Q131" s="94"/>
+      <c r="R131" s="94"/>
       <c r="S131" s="51"/>
       <c r="T131" s="51"/>
       <c r="U131" s="80" t="s">
@@ -14387,8 +14732,8 @@
       <c r="P132" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q132" s="95"/>
-      <c r="R132" s="95"/>
+      <c r="Q132" s="94"/>
+      <c r="R132" s="94"/>
       <c r="S132" s="51"/>
       <c r="T132" s="51"/>
       <c r="U132" s="80" t="s">
@@ -14472,8 +14817,8 @@
       <c r="P133" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q133" s="95"/>
-      <c r="R133" s="95"/>
+      <c r="Q133" s="94"/>
+      <c r="R133" s="94"/>
       <c r="S133" s="51"/>
       <c r="T133" s="51"/>
       <c r="U133" s="80" t="s">
@@ -14564,8 +14909,8 @@
       <c r="P134" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q134" s="95"/>
-      <c r="R134" s="95"/>
+      <c r="Q134" s="94"/>
+      <c r="R134" s="94"/>
       <c r="S134" s="51"/>
       <c r="T134" s="51"/>
       <c r="U134" s="80" t="s">
@@ -14857,7 +15202,7 @@
       <c r="P139" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q139" s="93" t="s">
+      <c r="Q139" s="95" t="s">
         <v>364</v>
       </c>
       <c r="R139" s="48"/>
@@ -14937,7 +15282,7 @@
       <c r="P140" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="Q140" s="93"/>
+      <c r="Q140" s="95"/>
       <c r="R140" s="48"/>
       <c r="S140" s="48"/>
       <c r="T140" s="48"/>
@@ -15015,7 +15360,7 @@
       <c r="P141" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q141" s="93"/>
+      <c r="Q141" s="95"/>
       <c r="R141" s="51"/>
       <c r="S141" s="51"/>
       <c r="T141" s="51"/>
@@ -15093,7 +15438,7 @@
       <c r="P142" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Q142" s="93"/>
+      <c r="Q142" s="95"/>
       <c r="R142" s="51"/>
       <c r="S142" s="51"/>
       <c r="T142" s="51"/>
@@ -16080,14 +16425,14 @@
       <c r="N157" s="51"/>
       <c r="O157" s="68"/>
       <c r="P157" s="51"/>
-      <c r="Q157" s="91" t="s">
+      <c r="Q157" s="108" t="s">
         <v>500</v>
       </c>
-      <c r="R157" s="91" t="s">
+      <c r="R157" s="108" t="s">
         <v>500</v>
       </c>
       <c r="S157" s="51"/>
-      <c r="T157" s="91" t="s">
+      <c r="T157" s="108" t="s">
         <v>501</v>
       </c>
       <c r="U157" s="80"/>
@@ -16129,10 +16474,10 @@
       <c r="N158" s="51"/>
       <c r="O158" s="68"/>
       <c r="P158" s="51"/>
-      <c r="Q158" s="94"/>
-      <c r="R158" s="94"/>
+      <c r="Q158" s="110"/>
+      <c r="R158" s="110"/>
       <c r="S158" s="51"/>
-      <c r="T158" s="94"/>
+      <c r="T158" s="110"/>
       <c r="U158" s="80"/>
       <c r="V158" s="84"/>
       <c r="W158" s="84"/>
@@ -16172,10 +16517,10 @@
       <c r="N159" s="51"/>
       <c r="O159" s="68"/>
       <c r="P159" s="51"/>
-      <c r="Q159" s="94"/>
-      <c r="R159" s="94"/>
+      <c r="Q159" s="110"/>
+      <c r="R159" s="110"/>
       <c r="S159" s="51"/>
-      <c r="T159" s="94"/>
+      <c r="T159" s="110"/>
       <c r="U159" s="80"/>
       <c r="V159" s="84"/>
       <c r="W159" s="84"/>
@@ -16215,10 +16560,10 @@
       <c r="N160" s="51"/>
       <c r="O160" s="68"/>
       <c r="P160" s="51"/>
-      <c r="Q160" s="94"/>
-      <c r="R160" s="94"/>
+      <c r="Q160" s="110"/>
+      <c r="R160" s="110"/>
       <c r="S160" s="51"/>
-      <c r="T160" s="94"/>
+      <c r="T160" s="110"/>
       <c r="U160" s="80"/>
       <c r="V160" s="84"/>
       <c r="W160" s="84"/>
@@ -16258,10 +16603,10 @@
       <c r="N161" s="51"/>
       <c r="O161" s="68"/>
       <c r="P161" s="51"/>
-      <c r="Q161" s="94"/>
-      <c r="R161" s="94"/>
+      <c r="Q161" s="110"/>
+      <c r="R161" s="110"/>
       <c r="S161" s="51"/>
-      <c r="T161" s="94"/>
+      <c r="T161" s="110"/>
       <c r="U161" s="80"/>
       <c r="V161" s="84"/>
       <c r="W161" s="84"/>
@@ -16301,10 +16646,10 @@
       <c r="N162" s="51"/>
       <c r="O162" s="68"/>
       <c r="P162" s="51"/>
-      <c r="Q162" s="94"/>
-      <c r="R162" s="94"/>
+      <c r="Q162" s="110"/>
+      <c r="R162" s="110"/>
       <c r="S162" s="51"/>
-      <c r="T162" s="94"/>
+      <c r="T162" s="110"/>
       <c r="U162" s="80"/>
       <c r="V162" s="84"/>
       <c r="W162" s="84"/>
@@ -16344,10 +16689,10 @@
       <c r="N163" s="51"/>
       <c r="O163" s="68"/>
       <c r="P163" s="51"/>
-      <c r="Q163" s="92"/>
-      <c r="R163" s="92"/>
+      <c r="Q163" s="109"/>
+      <c r="R163" s="109"/>
       <c r="S163" s="51"/>
-      <c r="T163" s="92"/>
+      <c r="T163" s="109"/>
       <c r="U163" s="80"/>
       <c r="V163" s="84"/>
       <c r="W163" s="84"/>
@@ -16669,38 +17014,11 @@
   </sheetData>
   <autoFilter ref="A1:Z168" xr:uid="{F5330BDA-7164-B946-A942-FFAE4F744BBA}"/>
   <mergeCells count="53">
-    <mergeCell ref="T52:T54"/>
-    <mergeCell ref="T96:T97"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R61:R63"/>
-    <mergeCell ref="S57:S59"/>
-    <mergeCell ref="S61:S63"/>
-    <mergeCell ref="S85:S91"/>
-    <mergeCell ref="R76:R80"/>
-    <mergeCell ref="S76:S80"/>
-    <mergeCell ref="R68:R73"/>
-    <mergeCell ref="S52:S54"/>
-    <mergeCell ref="S96:S97"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="S37:S39"/>
-    <mergeCell ref="S41:S43"/>
-    <mergeCell ref="S46:S48"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="R26:R28"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="S22:S24"/>
-    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="T108:T109"/>
+    <mergeCell ref="Q139:Q142"/>
+    <mergeCell ref="Q157:Q163"/>
+    <mergeCell ref="R157:R163"/>
+    <mergeCell ref="T157:T163"/>
     <mergeCell ref="Q22:Q24"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="Q37:Q39"/>
@@ -16717,206 +17035,233 @@
     <mergeCell ref="Q61:Q63"/>
     <mergeCell ref="Q130:Q134"/>
     <mergeCell ref="Q123:Q128"/>
-    <mergeCell ref="T108:T109"/>
-    <mergeCell ref="Q139:Q142"/>
-    <mergeCell ref="Q157:Q163"/>
-    <mergeCell ref="R157:R163"/>
-    <mergeCell ref="T157:T163"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="S26:S28"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S41:S43"/>
+    <mergeCell ref="S46:S48"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R26:R28"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="T96:T97"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="S57:S59"/>
+    <mergeCell ref="S61:S63"/>
+    <mergeCell ref="S85:S91"/>
+    <mergeCell ref="R76:R80"/>
+    <mergeCell ref="S76:S80"/>
+    <mergeCell ref="R68:R73"/>
+    <mergeCell ref="S52:S54"/>
+    <mergeCell ref="S96:S97"/>
   </mergeCells>
   <conditionalFormatting sqref="A151:J155">
-    <cfRule type="expression" dxfId="148" priority="73">
+    <cfRule type="expression" dxfId="200" priority="125">
       <formula>$B151=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:K81 A112:Q113 S112:T113 S153:T155">
-    <cfRule type="expression" dxfId="147" priority="100">
+    <cfRule type="expression" dxfId="199" priority="152">
       <formula>$B81=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133:P134">
-    <cfRule type="expression" dxfId="146" priority="255">
+    <cfRule type="expression" dxfId="198" priority="307">
       <formula>$B133=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="254">
+    <cfRule type="expression" dxfId="197" priority="306">
       <formula>$B133&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="253">
+    <cfRule type="expression" dxfId="196" priority="305">
       <formula>$B133=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="252">
+    <cfRule type="expression" dxfId="195" priority="304">
       <formula>$B133=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:P144">
-    <cfRule type="expression" dxfId="142" priority="203">
+    <cfRule type="expression" dxfId="194" priority="255">
       <formula>$B137=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="200">
+    <cfRule type="expression" dxfId="193" priority="252">
       <formula>$B137=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="201">
+    <cfRule type="expression" dxfId="192" priority="253">
       <formula>$B137=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="202">
+    <cfRule type="expression" dxfId="191" priority="254">
       <formula>$B137&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A157:P163">
-    <cfRule type="expression" dxfId="138" priority="5">
+    <cfRule type="expression" dxfId="190" priority="57">
       <formula>$B157=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="6">
+    <cfRule type="expression" dxfId="189" priority="58">
       <formula>$B157=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="7">
+    <cfRule type="expression" dxfId="188" priority="59">
       <formula>$B157&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:S95">
-    <cfRule type="expression" dxfId="135" priority="308">
+    <cfRule type="expression" dxfId="187" priority="360">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="311">
+    <cfRule type="expression" dxfId="186" priority="363">
       <formula>$B95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="310">
+    <cfRule type="expression" dxfId="185" priority="362">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="309">
+    <cfRule type="expression" dxfId="184" priority="361">
       <formula>$B95=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:T94">
-    <cfRule type="expression" dxfId="131" priority="93">
+    <cfRule type="expression" dxfId="183" priority="145">
       <formula>$B74&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="92">
+    <cfRule type="expression" dxfId="182" priority="144">
       <formula>$B74=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="91">
+    <cfRule type="expression" dxfId="181" priority="143">
       <formula>$B74=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:T83">
-    <cfRule type="expression" dxfId="128" priority="150">
+    <cfRule type="expression" dxfId="180" priority="202">
       <formula>$B83=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:T99 S101:T107 S108:S109 A112:Q113 S112:T113 A129:T129 L130:T130 L131:P131 S131:T135 I132:P132 A135:R135 R139:T144 A145:T148 A149:H150 A151:J155 S153:T155 A123:B128 S123:T128 A5:Q6 A96:F98 A1:AE4 S5:AE6">
-    <cfRule type="expression" dxfId="127" priority="304">
+    <cfRule type="expression" dxfId="179" priority="356">
       <formula>$B1=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:T111 A114:T128">
-    <cfRule type="expression" dxfId="126" priority="139">
+    <cfRule type="expression" dxfId="178" priority="191">
       <formula>$B110=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="140">
+    <cfRule type="expression" dxfId="177" priority="192">
       <formula>$B110&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:T111">
-    <cfRule type="expression" dxfId="124" priority="275">
+    <cfRule type="expression" dxfId="176" priority="327">
       <formula>$B110=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114:T128 A110:T111">
-    <cfRule type="expression" dxfId="123" priority="138">
+    <cfRule type="expression" dxfId="175" priority="190">
       <formula>$B110=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:T136">
-    <cfRule type="expression" dxfId="122" priority="237">
+    <cfRule type="expression" dxfId="174" priority="289">
       <formula>$B136=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="238">
+    <cfRule type="expression" dxfId="173" priority="290">
       <formula>$B136&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="239">
+    <cfRule type="expression" dxfId="172" priority="291">
       <formula>$B136=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="236">
+    <cfRule type="expression" dxfId="171" priority="288">
       <formula>$B136=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A165:T168">
-    <cfRule type="expression" dxfId="118" priority="169">
+    <cfRule type="expression" dxfId="170" priority="221">
       <formula>$B165=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="168">
+    <cfRule type="expression" dxfId="169" priority="220">
       <formula>$B165=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="170">
+    <cfRule type="expression" dxfId="168" priority="222">
       <formula>$B165&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="171">
+    <cfRule type="expression" dxfId="167" priority="223">
       <formula>$B165=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AE4 A5:Q6 S5:AE6 A96:F98 A99:T99 S101:T107 S108:S109 A112:Q113 S112:T113 A123:B128 S123:T128 A129:T129 L130:T130 L131:P131 S131:T135 I132:P132 A135:R135 R139:T144 A145:T148 A149:H150 A151:J155 S153:T155">
-    <cfRule type="expression" dxfId="114" priority="305">
+    <cfRule type="expression" dxfId="166" priority="357">
       <formula>$B1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="306">
+    <cfRule type="expression" dxfId="165" priority="358">
       <formula>$B1&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AE4 A5:Q6 S5:AE6 A7:AE51 A157:C163">
-    <cfRule type="expression" dxfId="112" priority="8">
+    <cfRule type="expression" dxfId="164" priority="60">
       <formula>$B1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:AE48">
-    <cfRule type="expression" dxfId="111" priority="70">
+    <cfRule type="expression" dxfId="163" priority="122">
       <formula>$B7=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="71">
+    <cfRule type="expression" dxfId="162" priority="123">
       <formula>$B7=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="72">
+    <cfRule type="expression" dxfId="161" priority="124">
       <formula>$B7&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:AE51 F52:AE52 A52:E54 F53:S54 U53:AE54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A99:AE108 A109:S109 U109:AE109 A110:AE119 A120:T120 A121:AE122 A129:AE156 Q157:AE157 S158:S163 U158:AE163 A164:AE168">
-    <cfRule type="expression" dxfId="108" priority="270">
+  <conditionalFormatting sqref="A49:AE51 F52:AE52 A52:E54 F53:S54 U53:AE54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A99:AE108 A109:S109 U109:AE109 A110:AE119 A120:T120 A122:AE122 A129:AE156 Q157:AE157 S158:S163 U158:AE163 A164:AE168 A121:W121 Y121:AE121">
+    <cfRule type="expression" dxfId="160" priority="322">
       <formula>$B49&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="269">
+    <cfRule type="expression" dxfId="159" priority="321">
       <formula>$B49=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:AE98">
-    <cfRule type="expression" dxfId="106" priority="27">
+    <cfRule type="expression" dxfId="158" priority="79">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="26">
+    <cfRule type="expression" dxfId="157" priority="78">
       <formula>$B96=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="25">
+    <cfRule type="expression" dxfId="156" priority="77">
       <formula>$B96=3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:AE156 A164:AE168 A55:AE75 A83:AE84 A110:AE119 A120:T120 A121:AE122 A99:AE108 A76:T82 A85:T88 A89:AE89 A90:T93 A94:AE95 A49:AE51 F52:AE52 F53:S54 A52:E54 U53:AE54 A109:S109 U109:AE109 Q157:AE157 S158:S163 U158:AE163">
-    <cfRule type="expression" dxfId="103" priority="268">
+  <conditionalFormatting sqref="A129:AE156 A164:AE168 A55:AE75 A83:AE84 A110:AE119 A120:T120 A122:AE122 A99:AE108 A76:T82 A85:T88 A89:AE89 A90:T93 A94:AE95 A49:AE51 F52:AE52 F53:S54 A52:E54 U53:AE54 A109:S109 U109:AE109 Q157:AE157 S158:S163 U158:AE163 A121:W121 Y121:AE121">
+    <cfRule type="expression" dxfId="155" priority="320">
       <formula>$B49=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C123:R123 C124:P128">
-    <cfRule type="expression" dxfId="102" priority="130">
+    <cfRule type="expression" dxfId="154" priority="182">
       <formula>$B123=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="129">
+    <cfRule type="expression" dxfId="153" priority="181">
       <formula>$B123&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="127">
+    <cfRule type="expression" dxfId="152" priority="179">
       <formula>$B123=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="128">
+    <cfRule type="expression" dxfId="151" priority="180">
       <formula>$B123=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D80 D82 D84:D122 D129:D168">
-    <cfRule type="colorScale" priority="556">
+    <cfRule type="colorScale" priority="608">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16926,7 +17271,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="colorScale" priority="105">
+    <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16936,7 +17281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="colorScale" priority="151">
+    <cfRule type="colorScale" priority="203">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16946,7 +17291,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123:D128">
-    <cfRule type="colorScale" priority="131">
+    <cfRule type="colorScale" priority="183">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16956,376 +17301,558 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E123:O128">
-    <cfRule type="expression" dxfId="98" priority="126">
+    <cfRule type="expression" dxfId="150" priority="178">
       <formula>_xlfn.ISFORMULA(E123)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:G54">
-    <cfRule type="expression" dxfId="97" priority="75">
+    <cfRule type="expression" dxfId="149" priority="127">
       <formula>$B51=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="76">
+    <cfRule type="expression" dxfId="148" priority="128">
       <formula>$B51=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="77">
+    <cfRule type="expression" dxfId="147" priority="129">
       <formula>$B51&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="78">
+    <cfRule type="expression" dxfId="146" priority="130">
       <formula>$B51=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F53:S54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A96:T99 A99:AE108 A109:S109 A110:AE119 A114:T129 A121:AE122 A129:AE156 D157:P163 A164:AE168 U53:AE54 U109:AE109 Q157:AE157 S158:S163 U158:AE163">
-    <cfRule type="expression" dxfId="93" priority="271">
+  <conditionalFormatting sqref="F53:S54 A55:AE75 A76:T82 A83:AE84 A85:T88 A89:AE89 A90:T93 A94:AE95 A96:T99 A99:AE108 A109:S109 A110:AE119 A114:T129 A122:AE122 A129:AE156 D157:P163 A164:AE168 U53:AE54 U109:AE109 Q157:AE157 S158:S163 U158:AE163 A121:W121 Y121:AE121">
+    <cfRule type="expression" dxfId="145" priority="323">
       <formula>$B53=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:AE52 A52:E54">
-    <cfRule type="expression" dxfId="92" priority="69">
+    <cfRule type="expression" dxfId="144" priority="121">
       <formula>$B52=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G96:G97">
-    <cfRule type="expression" dxfId="91" priority="300">
+    <cfRule type="expression" dxfId="143" priority="352">
       <formula>$B96=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="303">
+    <cfRule type="expression" dxfId="142" priority="355">
       <formula>$B96=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="302">
+    <cfRule type="expression" dxfId="141" priority="354">
       <formula>$B96&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="301">
+    <cfRule type="expression" dxfId="140" priority="353">
       <formula>$B96=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="87" priority="109">
+    <cfRule type="expression" dxfId="139" priority="161">
       <formula>$B5=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="106">
+    <cfRule type="expression" dxfId="138" priority="158">
       <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="108">
+    <cfRule type="expression" dxfId="137" priority="160">
       <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="107">
+    <cfRule type="expression" dxfId="136" priority="159">
       <formula>$B5=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:J73">
-    <cfRule type="expression" dxfId="83" priority="157">
+    <cfRule type="expression" dxfId="135" priority="209">
       <formula>_xlfn.ISFORMULA(H71)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="161">
+    <cfRule type="expression" dxfId="134" priority="213">
       <formula>$B71=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:O1048576">
-    <cfRule type="expression" dxfId="81" priority="167">
+    <cfRule type="expression" dxfId="133" priority="219">
       <formula>_xlfn.ISFORMULA(H1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:O70">
-    <cfRule type="expression" dxfId="80" priority="162">
+    <cfRule type="expression" dxfId="132" priority="214">
       <formula>_xlfn.ISFORMULA(H68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:Q73">
-    <cfRule type="expression" dxfId="79" priority="153">
+    <cfRule type="expression" dxfId="131" priority="205">
       <formula>$B69=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="154">
+    <cfRule type="expression" dxfId="130" priority="206">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="155">
+    <cfRule type="expression" dxfId="129" priority="207">
       <formula>$B69&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 H69:Q70 S69:T73">
-    <cfRule type="expression" dxfId="76" priority="166">
+    <cfRule type="expression" dxfId="128" priority="218">
       <formula>$B68=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:T68 S69:T73">
-    <cfRule type="expression" dxfId="75" priority="163">
+    <cfRule type="expression" dxfId="127" priority="215">
       <formula>$B68=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="164">
+    <cfRule type="expression" dxfId="126" priority="216">
       <formula>$B68=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="165">
+    <cfRule type="expression" dxfId="125" priority="217">
       <formula>$B68&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="72" priority="99">
+    <cfRule type="expression" dxfId="124" priority="151">
       <formula>_xlfn.ISFORMULA(I81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I149:J150">
-    <cfRule type="expression" dxfId="71" priority="186">
+    <cfRule type="expression" dxfId="123" priority="238">
       <formula>$B150&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="187">
+    <cfRule type="expression" dxfId="122" priority="239">
       <formula>$B150=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="184">
+    <cfRule type="expression" dxfId="121" priority="236">
       <formula>$B150=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="185">
+    <cfRule type="expression" dxfId="120" priority="237">
       <formula>$B150=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I130:K131">
-    <cfRule type="expression" dxfId="67" priority="264">
+    <cfRule type="expression" dxfId="119" priority="316">
       <formula>$B130=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="265">
+    <cfRule type="expression" dxfId="118" priority="317">
       <formula>$B130=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="266">
+    <cfRule type="expression" dxfId="117" priority="318">
       <formula>$B130&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="267">
+    <cfRule type="expression" dxfId="116" priority="319">
       <formula>$B130=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100">
-    <cfRule type="expression" dxfId="63" priority="503">
+    <cfRule type="expression" dxfId="115" priority="555">
       <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="113">
+    <cfRule type="expression" dxfId="114" priority="165">
       <formula>$B100=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="506">
+    <cfRule type="expression" dxfId="113" priority="558">
       <formula>#REF!=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="505">
+    <cfRule type="expression" dxfId="112" priority="557">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="504">
+    <cfRule type="expression" dxfId="111" priority="556">
       <formula>#REF!&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:T100">
-    <cfRule type="expression" dxfId="58" priority="110">
+    <cfRule type="expression" dxfId="110" priority="162">
       <formula>$B100=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="111">
+    <cfRule type="expression" dxfId="109" priority="163">
       <formula>$B100=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="112">
+    <cfRule type="expression" dxfId="108" priority="164">
       <formula>$B100&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L81">
-    <cfRule type="expression" dxfId="55" priority="94">
+    <cfRule type="expression" dxfId="107" priority="146">
       <formula>_xlfn.ISFORMULA(L81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L81:T81">
-    <cfRule type="expression" dxfId="54" priority="95">
+    <cfRule type="expression" dxfId="106" priority="147">
       <formula>$B81=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L130:T130 L131:P131 I132:P132 A135:R135 A145:T148 A149:H150 A96:F98 S101:T107 S108:S109 A123:B128 S131:T135 R139:T144">
-    <cfRule type="expression" dxfId="53" priority="307">
+    <cfRule type="expression" dxfId="105" priority="359">
       <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71:O73">
-    <cfRule type="expression" dxfId="52" priority="152">
+    <cfRule type="expression" dxfId="104" priority="204">
       <formula>_xlfn.ISFORMULA(O71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:O113 E83:O83">
-    <cfRule type="expression" dxfId="51" priority="146">
+    <cfRule type="expression" dxfId="103" priority="198">
       <formula>_xlfn.ISFORMULA(E83)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O136">
-    <cfRule type="expression" dxfId="50" priority="324">
+    <cfRule type="expression" dxfId="102" priority="376">
       <formula>$B137=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="323">
+    <cfRule type="expression" dxfId="101" priority="375">
       <formula>$B137&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="322">
+    <cfRule type="expression" dxfId="100" priority="374">
       <formula>$B137=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="321">
+    <cfRule type="expression" dxfId="99" priority="373">
       <formula>$B137=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71:Q73">
-    <cfRule type="expression" dxfId="46" priority="156">
+    <cfRule type="expression" dxfId="98" priority="208">
       <formula>$B71=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q139">
-    <cfRule type="expression" dxfId="45" priority="248">
+    <cfRule type="expression" dxfId="97" priority="300">
       <formula>$B139=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="249">
+    <cfRule type="expression" dxfId="96" priority="301">
       <formula>$B139=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="250">
+    <cfRule type="expression" dxfId="95" priority="302">
       <formula>$B139&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="251">
+    <cfRule type="expression" dxfId="94" priority="303">
       <formula>$B139=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q143:Q144">
-    <cfRule type="expression" dxfId="41" priority="244">
+    <cfRule type="expression" dxfId="93" priority="296">
       <formula>$B143=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="245">
+    <cfRule type="expression" dxfId="92" priority="297">
       <formula>$B143=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="246">
+    <cfRule type="expression" dxfId="91" priority="298">
       <formula>$B143&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="247">
+    <cfRule type="expression" dxfId="90" priority="299">
       <formula>$B143=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q87:T88">
-    <cfRule type="expression" dxfId="37" priority="145">
+    <cfRule type="expression" dxfId="89" priority="197">
       <formula>$B87=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q137:T138">
-    <cfRule type="expression" dxfId="36" priority="211">
+    <cfRule type="expression" dxfId="88" priority="263">
       <formula>$B137=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="210">
+    <cfRule type="expression" dxfId="87" priority="262">
       <formula>$B137&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="209">
+    <cfRule type="expression" dxfId="86" priority="261">
       <formula>$B137=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="208">
+    <cfRule type="expression" dxfId="85" priority="260">
       <formula>$B137=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="expression" dxfId="32" priority="1">
+    <cfRule type="expression" dxfId="84" priority="53">
       <formula>$B5=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="3">
+    <cfRule type="expression" dxfId="83" priority="55">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="82" priority="54">
       <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="81" priority="56">
       <formula>$B5&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="expression" dxfId="28" priority="564">
+    <cfRule type="expression" dxfId="80" priority="616">
       <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="562">
+    <cfRule type="expression" dxfId="79" priority="614">
       <formula>$B5=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="560">
+    <cfRule type="expression" dxfId="78" priority="612">
       <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="559">
+    <cfRule type="expression" dxfId="77" priority="611">
       <formula>$B5=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S96">
-    <cfRule type="expression" dxfId="24" priority="329">
+    <cfRule type="expression" dxfId="76" priority="381">
       <formula>$B95=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="330">
+    <cfRule type="expression" dxfId="75" priority="382">
       <formula>$B95=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="331">
+    <cfRule type="expression" dxfId="74" priority="383">
       <formula>$B95&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="332">
+    <cfRule type="expression" dxfId="73" priority="384">
       <formula>$B95=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S123:AE128">
-    <cfRule type="expression" dxfId="20" priority="20">
+  <conditionalFormatting sqref="S123:Z128 AB123:AD128">
+    <cfRule type="expression" dxfId="72" priority="72">
       <formula>$B123=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U76:AE82">
-    <cfRule type="expression" dxfId="19" priority="52">
+    <cfRule type="expression" dxfId="71" priority="104">
       <formula>$B76=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="49">
+    <cfRule type="expression" dxfId="70" priority="101">
       <formula>$B76=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="51">
+    <cfRule type="expression" dxfId="69" priority="103">
       <formula>$B76&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="50">
+    <cfRule type="expression" dxfId="68" priority="102">
       <formula>$B76=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U85:AE88">
-    <cfRule type="expression" dxfId="15" priority="44">
+    <cfRule type="expression" dxfId="67" priority="96">
       <formula>$B85=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="43">
+    <cfRule type="expression" dxfId="66" priority="95">
       <formula>$B85&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="42">
+    <cfRule type="expression" dxfId="65" priority="94">
       <formula>$B85=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="41">
+    <cfRule type="expression" dxfId="64" priority="93">
       <formula>$B85=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U90:AE93">
-    <cfRule type="expression" dxfId="11" priority="36">
+    <cfRule type="expression" dxfId="63" priority="88">
       <formula>$B90=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="35">
+    <cfRule type="expression" dxfId="62" priority="87">
       <formula>$B90&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="34">
+    <cfRule type="expression" dxfId="61" priority="86">
       <formula>$B90=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="33">
+    <cfRule type="expression" dxfId="60" priority="85">
       <formula>$B90=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U96:AE98">
-    <cfRule type="expression" dxfId="7" priority="28">
+    <cfRule type="expression" dxfId="59" priority="80">
       <formula>$B96=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U120:AE120">
-    <cfRule type="expression" dxfId="6" priority="21">
+    <cfRule type="expression" dxfId="58" priority="73">
       <formula>$B120=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="22">
+    <cfRule type="expression" dxfId="57" priority="74">
       <formula>$B120=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="24">
+    <cfRule type="expression" dxfId="56" priority="76">
       <formula>$B120=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="23">
+    <cfRule type="expression" dxfId="55" priority="75">
       <formula>$B120&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U123:AE128">
-    <cfRule type="expression" dxfId="2" priority="17">
+  <conditionalFormatting sqref="U123:Z128 AB123:AD128">
+    <cfRule type="expression" dxfId="54" priority="69">
       <formula>$B123=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="18">
+    <cfRule type="expression" dxfId="53" priority="70">
       <formula>$B123=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="19">
+    <cfRule type="expression" dxfId="52" priority="71">
       <formula>$B123&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X121">
+    <cfRule type="expression" dxfId="51" priority="49">
+      <formula>$B121=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="50">
+      <formula>$B121=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="51">
+      <formula>$B121&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="52">
+      <formula>$B121=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA123">
+    <cfRule type="expression" dxfId="47" priority="45">
+      <formula>$B123=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="46">
+      <formula>$B123=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="47">
+      <formula>$B123&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="48">
+      <formula>$B123=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA124">
+    <cfRule type="expression" dxfId="43" priority="41">
+      <formula>$B124=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="42">
+      <formula>$B124=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="43">
+      <formula>$B124&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="44">
+      <formula>$B124=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA125">
+    <cfRule type="expression" dxfId="39" priority="37">
+      <formula>$B125=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="38">
+      <formula>$B125=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="39">
+      <formula>$B125&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="40">
+      <formula>$B125=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA126">
+    <cfRule type="expression" dxfId="35" priority="33">
+      <formula>$B126=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="34">
+      <formula>$B126=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="35">
+      <formula>$B126&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="36">
+      <formula>$B126=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA127">
+    <cfRule type="expression" dxfId="31" priority="29">
+      <formula>$B127=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="30">
+      <formula>$B127=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="31">
+      <formula>$B127&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="32">
+      <formula>$B127=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA128">
+    <cfRule type="expression" dxfId="27" priority="25">
+      <formula>$B128=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="26">
+      <formula>$B128=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="27">
+      <formula>$B128&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="28">
+      <formula>$B128=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE123">
+    <cfRule type="expression" dxfId="23" priority="21">
+      <formula>$B123=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="22">
+      <formula>$B123=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="23">
+      <formula>$B123&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="24">
+      <formula>$B123=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE124">
+    <cfRule type="expression" dxfId="19" priority="17">
+      <formula>$B124=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="18">
+      <formula>$B124=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="19">
+      <formula>$B124&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="20">
+      <formula>$B124=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE125">
+    <cfRule type="expression" dxfId="15" priority="13">
+      <formula>$B125=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>$B125=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="15">
+      <formula>$B125&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="16">
+      <formula>$B125=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE126">
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>$B126=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>$B126=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="11">
+      <formula>$B126&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>$B126=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE127">
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>$B127=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$B127=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="7">
+      <formula>$B127&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="8">
+      <formula>$B127=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE128">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$B128=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$B128=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$B128&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>$B128=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">

</xml_diff>